<commit_message>
Update for March, 2023
</commit_message>
<xml_diff>
--- a/statistics_files/2023/2023.g.net_borrower_lender.xlsx
+++ b/statistics_files/2023/2023.g.net_borrower_lender.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20395"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20396"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\GitHub\next_statistics\statistics_files\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E324060D-9B24-4292-882D-C408B7BA17FA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C1764D-10AB-4F97-9CD5-53CA66A4758C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" tabRatio="673" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="165">
   <si>
     <t>NET</t>
   </si>
@@ -475,6 +475,78 @@
   </si>
   <si>
     <t>2.23 : 1</t>
+  </si>
+  <si>
+    <t>1.11 : 1</t>
+  </si>
+  <si>
+    <t>0.95 : 1</t>
+  </si>
+  <si>
+    <t>1.01 : 1</t>
+  </si>
+  <si>
+    <t>0.23 : 1</t>
+  </si>
+  <si>
+    <t>0.66 : 1</t>
+  </si>
+  <si>
+    <t>1.37 : 1</t>
+  </si>
+  <si>
+    <t>0.62 : 1</t>
+  </si>
+  <si>
+    <t>2.04 : 1</t>
+  </si>
+  <si>
+    <t>0.01 : 1</t>
+  </si>
+  <si>
+    <t>0.56 : 1</t>
+  </si>
+  <si>
+    <t>2.38 : 1</t>
+  </si>
+  <si>
+    <t>4.12 : 1</t>
+  </si>
+  <si>
+    <t>1.66 : 1</t>
+  </si>
+  <si>
+    <t>0.50 : 1</t>
+  </si>
+  <si>
+    <t>0.33 : 1</t>
+  </si>
+  <si>
+    <t>0.00 : 1</t>
+  </si>
+  <si>
+    <t>2.25 : 1</t>
+  </si>
+  <si>
+    <t>0.35 : 1</t>
+  </si>
+  <si>
+    <t>0.72 : 1</t>
+  </si>
+  <si>
+    <t>0.34 : 1</t>
+  </si>
+  <si>
+    <t>1.75 : 1</t>
+  </si>
+  <si>
+    <t>2.99 : 1</t>
+  </si>
+  <si>
+    <t>0.42 : 1</t>
+  </si>
+  <si>
+    <t>0.16 : 1</t>
   </si>
 </sst>
 </file>
@@ -1384,15 +1456,15 @@
       </c>
       <c r="B2" s="2">
         <f>January!B2+February!B2+March!B2+April!B2+May!B2+June!B2+July!B2+August!B2+September!B2+October!B2+November!B2+December!B2</f>
-        <v>2708</v>
+        <v>4144</v>
       </c>
       <c r="C2" s="2">
         <f>January!C2+February!C2+March!C2+April!C2+May!C2+June!C2+July!C2+August!C2+September!C2+October!C2+November!C2+December!C2</f>
-        <v>2320</v>
+        <v>3555</v>
       </c>
       <c r="D2" s="2">
         <f>January!D2+February!D2+March!D2+April!D2+May!D2+June!D2+July!D2+August!D2+September!D2+October!D2+November!D2+December!D2</f>
-        <v>388</v>
+        <v>589</v>
       </c>
       <c r="E2" s="28" t="str">
         <f>IF(D2 &gt; 0, "We borrowed more than we lent this year", "")</f>
@@ -1413,15 +1485,15 @@
       </c>
       <c r="B3" s="4">
         <f>January!B3+February!B3+March!B3+April!B3+May!B3+June!B3+July!B3+August!B3+September!B3+October!B3+November!B3+December!B3</f>
-        <v>952</v>
+        <v>1452</v>
       </c>
       <c r="C3" s="4">
         <f>January!C3+February!C3+March!C3+April!C3+May!C3+June!C3+July!C3+August!C3+September!C3+October!C3+November!C3+December!C3</f>
-        <v>877</v>
+        <v>1407</v>
       </c>
       <c r="D3" s="4">
         <f>January!D3+February!D3+March!D3+April!D3+May!D3+June!D3+July!D3+August!D3+September!D3+October!D3+November!D3+December!D3</f>
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="E3" s="29" t="str">
         <f t="shared" ref="E3:E55" si="1">IF(D3 &gt; 0, "We borrowed more than we lent this year", "")</f>
@@ -1433,7 +1505,7 @@
       </c>
       <c r="G3" s="5" t="str">
         <f t="shared" ref="G3:G55" si="2">IF(ISERROR(ROUND(B3/C3,2)&amp;" : 1"), "", ROUND(B3/C3,2)&amp;" : 1")</f>
-        <v>1.09 : 1</v>
+        <v>1.03 : 1</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1442,15 +1514,15 @@
       </c>
       <c r="B4" s="2">
         <f>January!B4+February!B4+March!B4+April!B4+May!B4+June!B4+July!B4+August!B4+September!B4+October!B4+November!B4+December!B4</f>
-        <v>2482</v>
+        <v>3926</v>
       </c>
       <c r="C4" s="2">
         <f>January!C4+February!C4+March!C4+April!C4+May!C4+June!C4+July!C4+August!C4+September!C4+October!C4+November!C4+December!C4</f>
-        <v>2192</v>
+        <v>3491</v>
       </c>
       <c r="D4" s="2">
         <f>January!D4+February!D4+March!D4+April!D4+May!D4+June!D4+July!D4+August!D4+September!D4+October!D4+November!D4+December!D4</f>
-        <v>290</v>
+        <v>435</v>
       </c>
       <c r="E4" s="28" t="str">
         <f t="shared" si="1"/>
@@ -1462,7 +1534,7 @@
       </c>
       <c r="G4" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.13 : 1</v>
+        <v>1.12 : 1</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1471,15 +1543,15 @@
       </c>
       <c r="B5" s="4">
         <f>January!B5+February!B5+March!B5+April!B5+May!B5+June!B5+July!B5+August!B5+September!B5+October!B5+November!B5+December!B5</f>
-        <v>73</v>
+        <v>188</v>
       </c>
       <c r="C5" s="4">
         <f>January!C5+February!C5+March!C5+April!C5+May!C5+June!C5+July!C5+August!C5+September!C5+October!C5+November!C5+December!C5</f>
-        <v>257</v>
+        <v>368</v>
       </c>
       <c r="D5" s="4">
         <f>January!D5+February!D5+March!D5+April!D5+May!D5+June!D5+July!D5+August!D5+September!D5+October!D5+November!D5+December!D5</f>
-        <v>-184</v>
+        <v>-180</v>
       </c>
       <c r="E5" s="29" t="str">
         <f t="shared" si="1"/>
@@ -1491,7 +1563,7 @@
       </c>
       <c r="G5" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.28 : 1</v>
+        <v>0.51 : 1</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1500,27 +1572,27 @@
       </c>
       <c r="B6" s="2">
         <f>January!B6+February!B6+March!B6+April!B6+May!B6+June!B6+July!B6+August!B6+September!B6+October!B6+November!B6+December!B6</f>
-        <v>2655</v>
+        <v>4096</v>
       </c>
       <c r="C6" s="2">
         <f>January!C6+February!C6+March!C6+April!C6+May!C6+June!C6+July!C6+August!C6+September!C6+October!C6+November!C6+December!C6</f>
-        <v>2632</v>
+        <v>4346</v>
       </c>
       <c r="D6" s="2">
         <f>January!D6+February!D6+March!D6+April!D6+May!D6+June!D6+July!D6+August!D6+September!D6+October!D6+November!D6+December!D6</f>
-        <v>23</v>
+        <v>-250</v>
       </c>
       <c r="E6" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>We borrowed more than we lent this year</v>
+        <v/>
       </c>
       <c r="F6" s="28" t="str">
         <f t="shared" ref="F6:F55" si="3">IF(D6 &lt; 0, "We lent more than we borrowed this year", "")</f>
-        <v/>
+        <v>We lent more than we borrowed this year</v>
       </c>
       <c r="G6" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.01 : 1</v>
+        <v>0.94 : 1</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1529,15 +1601,15 @@
       </c>
       <c r="B7" s="4">
         <f>January!B7+February!B7+March!B7+April!B7+May!B7+June!B7+July!B7+August!B7+September!B7+October!B7+November!B7+December!B7</f>
-        <v>454</v>
+        <v>752</v>
       </c>
       <c r="C7" s="4">
         <f>January!C7+February!C7+March!C7+April!C7+May!C7+June!C7+July!C7+August!C7+September!C7+October!C7+November!C7+December!C7</f>
-        <v>391</v>
+        <v>706</v>
       </c>
       <c r="D7" s="4">
         <f>January!D7+February!D7+March!D7+April!D7+May!D7+June!D7+July!D7+August!D7+September!D7+October!D7+November!D7+December!D7</f>
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="E7" s="29" t="str">
         <f t="shared" si="1"/>
@@ -1549,7 +1621,7 @@
       </c>
       <c r="G7" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.16 : 1</v>
+        <v>1.07 : 1</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1558,15 +1630,15 @@
       </c>
       <c r="B8" s="2">
         <f>January!B8+February!B8+March!B8+April!B8+May!B8+June!B8+July!B8+August!B8+September!B8+October!B8+November!B8+December!B8</f>
-        <v>253</v>
+        <v>397</v>
       </c>
       <c r="C8" s="2">
         <f>January!C8+February!C8+March!C8+April!C8+May!C8+June!C8+July!C8+August!C8+September!C8+October!C8+November!C8+December!C8</f>
-        <v>382</v>
+        <v>587</v>
       </c>
       <c r="D8" s="2">
         <f>January!D8+February!D8+March!D8+April!D8+May!D8+June!D8+July!D8+August!D8+September!D8+October!D8+November!D8+December!D8</f>
-        <v>-129</v>
+        <v>-190</v>
       </c>
       <c r="E8" s="28" t="str">
         <f t="shared" si="1"/>
@@ -1578,7 +1650,7 @@
       </c>
       <c r="G8" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.66 : 1</v>
+        <v>0.68 : 1</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1587,15 +1659,15 @@
       </c>
       <c r="B9" s="4">
         <f>January!B9+February!B9+March!B9+April!B9+May!B9+June!B9+July!B9+August!B9+September!B9+October!B9+November!B9+December!B9</f>
-        <v>93</v>
+        <v>170</v>
       </c>
       <c r="C9" s="4">
         <f>January!C9+February!C9+March!C9+April!C9+May!C9+June!C9+July!C9+August!C9+September!C9+October!C9+November!C9+December!C9</f>
-        <v>172</v>
+        <v>248</v>
       </c>
       <c r="D9" s="4">
         <f>January!D9+February!D9+March!D9+April!D9+May!D9+June!D9+July!D9+August!D9+September!D9+October!D9+November!D9+December!D9</f>
-        <v>-79</v>
+        <v>-78</v>
       </c>
       <c r="E9" s="29" t="str">
         <f t="shared" si="1"/>
@@ -1607,7 +1679,7 @@
       </c>
       <c r="G9" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.54 : 1</v>
+        <v>0.69 : 1</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1616,15 +1688,15 @@
       </c>
       <c r="B10" s="2">
         <f>January!B10+February!B10+March!B10+April!B10+May!B10+June!B10+July!B10+August!B10+September!B10+October!B10+November!B10+December!B10</f>
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C10" s="2">
         <f>January!C10+February!C10+March!C10+April!C10+May!C10+June!C10+July!C10+August!C10+September!C10+October!C10+November!C10+December!C10</f>
-        <v>100</v>
+        <v>139</v>
       </c>
       <c r="D10" s="2">
         <f>January!D10+February!D10+March!D10+April!D10+May!D10+June!D10+July!D10+August!D10+September!D10+October!D10+November!D10+December!D10</f>
-        <v>-84</v>
+        <v>-114</v>
       </c>
       <c r="E10" s="28" t="str">
         <f t="shared" si="1"/>
@@ -1636,7 +1708,7 @@
       </c>
       <c r="G10" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.16 : 1</v>
+        <v>0.18 : 1</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1674,15 +1746,15 @@
       </c>
       <c r="B12" s="6">
         <f>January!B12+February!B12+March!B12+April!B12+May!B12+June!B12+July!B12+August!B12+September!B12+October!B12+November!B12+December!B12</f>
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="C12" s="6">
         <f>January!C12+February!C12+March!C12+April!C12+May!C12+June!C12+July!C12+August!C12+September!C12+October!C12+November!C12+December!C12</f>
-        <v>51</v>
+        <v>80</v>
       </c>
       <c r="D12" s="6">
         <f>January!D12+February!D12+March!D12+April!D12+May!D12+June!D12+July!D12+August!D12+September!D12+October!D12+November!D12+December!D12</f>
-        <v>-13</v>
+        <v>-23</v>
       </c>
       <c r="E12" s="30" t="str">
         <f t="shared" si="1"/>
@@ -1694,7 +1766,7 @@
       </c>
       <c r="G12" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0.75 : 1</v>
+        <v>0.71 : 1</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1703,15 +1775,15 @@
       </c>
       <c r="B13" s="6">
         <f>January!B13+February!B13+March!B13+April!B13+May!B13+June!B13+July!B13+August!B13+September!B13+October!B13+November!B13+December!B13</f>
-        <v>214</v>
+        <v>369</v>
       </c>
       <c r="C13" s="6">
         <f>January!C13+February!C13+March!C13+April!C13+May!C13+June!C13+July!C13+August!C13+September!C13+October!C13+November!C13+December!C13</f>
-        <v>170</v>
+        <v>283</v>
       </c>
       <c r="D13" s="6">
         <f>January!D13+February!D13+March!D13+April!D13+May!D13+June!D13+July!D13+August!D13+September!D13+October!D13+November!D13+December!D13</f>
-        <v>44</v>
+        <v>86</v>
       </c>
       <c r="E13" s="30" t="str">
         <f t="shared" si="1"/>
@@ -1723,7 +1795,7 @@
       </c>
       <c r="G13" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>1.26 : 1</v>
+        <v>1.3 : 1</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1732,15 +1804,15 @@
       </c>
       <c r="B14" s="6">
         <f>January!B14+February!B14+March!B14+April!B14+May!B14+June!B14+July!B14+August!B14+September!B14+October!B14+November!B14+December!B14</f>
-        <v>294</v>
+        <v>440</v>
       </c>
       <c r="C14" s="6">
         <f>January!C14+February!C14+March!C14+April!C14+May!C14+June!C14+July!C14+August!C14+September!C14+October!C14+November!C14+December!C14</f>
-        <v>564</v>
+        <v>905</v>
       </c>
       <c r="D14" s="6">
         <f>January!D14+February!D14+March!D14+April!D14+May!D14+June!D14+July!D14+August!D14+September!D14+October!D14+November!D14+December!D14</f>
-        <v>-270</v>
+        <v>-465</v>
       </c>
       <c r="E14" s="30" t="str">
         <f t="shared" si="1"/>
@@ -1752,7 +1824,7 @@
       </c>
       <c r="G14" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0.52 : 1</v>
+        <v>0.49 : 1</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1761,15 +1833,15 @@
       </c>
       <c r="B15" s="6">
         <f>January!B15+February!B15+March!B15+April!B15+May!B15+June!B15+July!B15+August!B15+September!B15+October!B15+November!B15+December!B15</f>
-        <v>118</v>
+        <v>178</v>
       </c>
       <c r="C15" s="6">
         <f>January!C15+February!C15+March!C15+April!C15+May!C15+June!C15+July!C15+August!C15+September!C15+October!C15+November!C15+December!C15</f>
-        <v>182</v>
+        <v>279</v>
       </c>
       <c r="D15" s="6">
         <f>January!D15+February!D15+March!D15+April!D15+May!D15+June!D15+July!D15+August!D15+September!D15+October!D15+November!D15+December!D15</f>
-        <v>-64</v>
+        <v>-101</v>
       </c>
       <c r="E15" s="30" t="str">
         <f t="shared" si="1"/>
@@ -1781,7 +1853,7 @@
       </c>
       <c r="G15" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0.65 : 1</v>
+        <v>0.64 : 1</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1790,15 +1862,15 @@
       </c>
       <c r="B16" s="2">
         <f>January!B16+February!B16+March!B16+April!B16+May!B16+June!B16+July!B16+August!B16+September!B16+October!B16+November!B16+December!B16</f>
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="C16" s="2">
         <f>January!C16+February!C16+March!C16+April!C16+May!C16+June!C16+July!C16+August!C16+September!C16+October!C16+November!C16+December!C16</f>
-        <v>294</v>
+        <v>398</v>
       </c>
       <c r="D16" s="2">
         <f>January!D16+February!D16+March!D16+April!D16+May!D16+June!D16+July!D16+August!D16+September!D16+October!D16+November!D16+December!D16</f>
-        <v>-217</v>
+        <v>-299</v>
       </c>
       <c r="E16" s="28" t="str">
         <f t="shared" si="1"/>
@@ -1810,7 +1882,7 @@
       </c>
       <c r="G16" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.26 : 1</v>
+        <v>0.25 : 1</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1819,15 +1891,15 @@
       </c>
       <c r="B17" s="4">
         <f>January!B17+February!B17+March!B17+April!B17+May!B17+June!B17+July!B17+August!B17+September!B17+October!B17+November!B17+December!B17</f>
-        <v>1173</v>
+        <v>1817</v>
       </c>
       <c r="C17" s="4">
         <f>January!C17+February!C17+March!C17+April!C17+May!C17+June!C17+July!C17+August!C17+September!C17+October!C17+November!C17+December!C17</f>
-        <v>943</v>
+        <v>1500</v>
       </c>
       <c r="D17" s="4">
         <f>January!D17+February!D17+March!D17+April!D17+May!D17+June!D17+July!D17+August!D17+September!D17+October!D17+November!D17+December!D17</f>
-        <v>230</v>
+        <v>317</v>
       </c>
       <c r="E17" s="29" t="str">
         <f t="shared" si="1"/>
@@ -1839,7 +1911,7 @@
       </c>
       <c r="G17" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.24 : 1</v>
+        <v>1.21 : 1</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1848,15 +1920,15 @@
       </c>
       <c r="B18" s="2">
         <f>January!B18+February!B18+March!B18+April!B18+May!B18+June!B18+July!B18+August!B18+September!B18+October!B18+November!B18+December!B18</f>
-        <v>247</v>
+        <v>389</v>
       </c>
       <c r="C18" s="2">
         <f>January!C18+February!C18+March!C18+April!C18+May!C18+June!C18+July!C18+August!C18+September!C18+October!C18+November!C18+December!C18</f>
-        <v>210</v>
+        <v>329</v>
       </c>
       <c r="D18" s="2">
         <f>January!D18+February!D18+March!D18+April!D18+May!D18+June!D18+July!D18+August!D18+September!D18+October!D18+November!D18+December!D18</f>
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="E18" s="28" t="str">
         <f t="shared" si="1"/>
@@ -1877,15 +1949,15 @@
       </c>
       <c r="B19" s="4">
         <f>January!B19+February!B19+March!B19+April!B19+May!B19+June!B19+July!B19+August!B19+September!B19+October!B19+November!B19+December!B19</f>
-        <v>1364</v>
+        <v>2094</v>
       </c>
       <c r="C19" s="4">
         <f>January!C19+February!C19+March!C19+April!C19+May!C19+June!C19+July!C19+August!C19+September!C19+October!C19+November!C19+December!C19</f>
-        <v>720</v>
+        <v>1077</v>
       </c>
       <c r="D19" s="4">
         <f>January!D19+February!D19+March!D19+April!D19+May!D19+June!D19+July!D19+August!D19+September!D19+October!D19+November!D19+December!D19</f>
-        <v>644</v>
+        <v>1017</v>
       </c>
       <c r="E19" s="29" t="str">
         <f t="shared" si="1"/>
@@ -1897,7 +1969,7 @@
       </c>
       <c r="G19" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.89 : 1</v>
+        <v>1.94 : 1</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1906,15 +1978,15 @@
       </c>
       <c r="B20" s="2">
         <f>January!B20+February!B20+March!B20+April!B20+May!B20+June!B20+July!B20+August!B20+September!B20+October!B20+November!B20+December!B20</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C20" s="2">
         <f>January!C20+February!C20+March!C20+April!C20+May!C20+June!C20+July!C20+August!C20+September!C20+October!C20+November!C20+December!C20</f>
-        <v>118</v>
+        <v>188</v>
       </c>
       <c r="D20" s="2">
         <f>January!D20+February!D20+March!D20+April!D20+May!D20+June!D20+July!D20+August!D20+September!D20+October!D20+November!D20+December!D20</f>
-        <v>-112</v>
+        <v>-181</v>
       </c>
       <c r="E20" s="28" t="str">
         <f t="shared" si="1"/>
@@ -1926,7 +1998,7 @@
       </c>
       <c r="G20" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.05 : 1</v>
+        <v>0.04 : 1</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1935,15 +2007,15 @@
       </c>
       <c r="B21" s="4">
         <f>January!B21+February!B21+March!B21+April!B21+May!B21+June!B21+July!B21+August!B21+September!B21+October!B21+November!B21+December!B21</f>
-        <v>1006</v>
+        <v>1636</v>
       </c>
       <c r="C21" s="4">
         <f>January!C21+February!C21+March!C21+April!C21+May!C21+June!C21+July!C21+August!C21+September!C21+October!C21+November!C21+December!C21</f>
-        <v>825</v>
+        <v>1284</v>
       </c>
       <c r="D21" s="4">
         <f>January!D21+February!D21+March!D21+April!D21+May!D21+June!D21+July!D21+August!D21+September!D21+October!D21+November!D21+December!D21</f>
-        <v>181</v>
+        <v>352</v>
       </c>
       <c r="E21" s="29" t="str">
         <f t="shared" si="1"/>
@@ -1955,7 +2027,7 @@
       </c>
       <c r="G21" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.22 : 1</v>
+        <v>1.27 : 1</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1964,15 +2036,15 @@
       </c>
       <c r="B22" s="2">
         <f>January!B22+February!B22+March!B22+April!B22+May!B22+June!B22+July!B22+August!B22+September!B22+October!B22+November!B22+December!B22</f>
-        <v>53</v>
+        <v>78</v>
       </c>
       <c r="C22" s="2">
         <f>January!C22+February!C22+March!C22+April!C22+May!C22+June!C22+July!C22+August!C22+September!C22+October!C22+November!C22+December!C22</f>
-        <v>157</v>
+        <v>250</v>
       </c>
       <c r="D22" s="2">
         <f>January!D22+February!D22+March!D22+April!D22+May!D22+June!D22+July!D22+August!D22+September!D22+October!D22+November!D22+December!D22</f>
-        <v>-104</v>
+        <v>-172</v>
       </c>
       <c r="E22" s="28" t="str">
         <f t="shared" si="1"/>
@@ -1984,7 +2056,7 @@
       </c>
       <c r="G22" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.34 : 1</v>
+        <v>0.31 : 1</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1993,15 +2065,15 @@
       </c>
       <c r="B23" s="4">
         <f>January!B23+February!B23+March!B23+April!B23+May!B23+June!B23+July!B23+August!B23+September!B23+October!B23+November!B23+December!B23</f>
-        <v>1307</v>
+        <v>2077</v>
       </c>
       <c r="C23" s="4">
         <f>January!C23+February!C23+March!C23+April!C23+May!C23+June!C23+July!C23+August!C23+September!C23+October!C23+November!C23+December!C23</f>
-        <v>1028</v>
+        <v>1630</v>
       </c>
       <c r="D23" s="4">
         <f>January!D23+February!D23+March!D23+April!D23+May!D23+June!D23+July!D23+August!D23+September!D23+October!D23+November!D23+December!D23</f>
-        <v>279</v>
+        <v>447</v>
       </c>
       <c r="E23" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2022,15 +2094,15 @@
       </c>
       <c r="B24" s="2">
         <f>January!B24+February!B24+March!B24+April!B24+May!B24+June!B24+July!B24+August!B24+September!B24+October!B24+November!B24+December!B24</f>
-        <v>3503</v>
+        <v>5755</v>
       </c>
       <c r="C24" s="2">
         <f>January!C24+February!C24+March!C24+April!C24+May!C24+June!C24+July!C24+August!C24+September!C24+October!C24+November!C24+December!C24</f>
-        <v>2771</v>
+        <v>4318</v>
       </c>
       <c r="D24" s="2">
         <f>January!D24+February!D24+March!D24+April!D24+May!D24+June!D24+July!D24+August!D24+September!D24+October!D24+November!D24+December!D24</f>
-        <v>732</v>
+        <v>1437</v>
       </c>
       <c r="E24" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2042,7 +2114,7 @@
       </c>
       <c r="G24" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.26 : 1</v>
+        <v>1.33 : 1</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2051,15 +2123,15 @@
       </c>
       <c r="B25" s="4">
         <f>January!B25+February!B25+March!B25+April!B25+May!B25+June!B25+July!B25+August!B25+September!B25+October!B25+November!B25+December!B25</f>
-        <v>342</v>
+        <v>555</v>
       </c>
       <c r="C25" s="4">
         <f>January!C25+February!C25+March!C25+April!C25+May!C25+June!C25+July!C25+August!C25+September!C25+October!C25+November!C25+December!C25</f>
-        <v>617</v>
+        <v>1000</v>
       </c>
       <c r="D25" s="4">
         <f>January!D25+February!D25+March!D25+April!D25+May!D25+June!D25+July!D25+August!D25+September!D25+October!D25+November!D25+December!D25</f>
-        <v>-275</v>
+        <v>-445</v>
       </c>
       <c r="E25" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2071,7 +2143,7 @@
       </c>
       <c r="G25" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.55 : 1</v>
+        <v>0.56 : 1</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2109,15 +2181,15 @@
       </c>
       <c r="B27" s="4">
         <f>January!B27+February!B27+March!B27+April!B27+May!B27+June!B27+July!B27+August!B27+September!B27+October!B27+November!B27+December!B27</f>
-        <v>504</v>
+        <v>984</v>
       </c>
       <c r="C27" s="4">
         <f>January!C27+February!C27+March!C27+April!C27+May!C27+June!C27+July!C27+August!C27+September!C27+October!C27+November!C27+December!C27</f>
-        <v>389</v>
+        <v>591</v>
       </c>
       <c r="D27" s="4">
         <f>January!D27+February!D27+March!D27+April!D27+May!D27+June!D27+July!D27+August!D27+September!D27+October!D27+November!D27+December!D27</f>
-        <v>115</v>
+        <v>393</v>
       </c>
       <c r="E27" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2129,7 +2201,7 @@
       </c>
       <c r="G27" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.3 : 1</v>
+        <v>1.66 : 1</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2138,15 +2210,15 @@
       </c>
       <c r="B28" s="2">
         <f>January!B28+February!B28+March!B28+April!B28+May!B28+June!B28+July!B28+August!B28+September!B28+October!B28+November!B28+December!B28</f>
-        <v>85</v>
+        <v>136</v>
       </c>
       <c r="C28" s="2">
         <f>January!C28+February!C28+March!C28+April!C28+May!C28+June!C28+July!C28+August!C28+September!C28+October!C28+November!C28+December!C28</f>
-        <v>165</v>
+        <v>256</v>
       </c>
       <c r="D28" s="2">
         <f>January!D28+February!D28+March!D28+April!D28+May!D28+June!D28+July!D28+August!D28+September!D28+October!D28+November!D28+December!D28</f>
-        <v>-80</v>
+        <v>-120</v>
       </c>
       <c r="E28" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2158,7 +2230,7 @@
       </c>
       <c r="G28" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.52 : 1</v>
+        <v>0.53 : 1</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2167,15 +2239,15 @@
       </c>
       <c r="B29" s="4">
         <f>January!B29+February!B29+March!B29+April!B29+May!B29+June!B29+July!B29+August!B29+September!B29+October!B29+November!B29+December!B29</f>
-        <v>1118</v>
+        <v>1708</v>
       </c>
       <c r="C29" s="4">
         <f>January!C29+February!C29+March!C29+April!C29+May!C29+June!C29+July!C29+August!C29+September!C29+October!C29+November!C29+December!C29</f>
-        <v>955</v>
+        <v>1456</v>
       </c>
       <c r="D29" s="4">
         <f>January!D29+February!D29+March!D29+April!D29+May!D29+June!D29+July!D29+August!D29+September!D29+October!D29+November!D29+December!D29</f>
-        <v>163</v>
+        <v>252</v>
       </c>
       <c r="E29" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2196,15 +2268,15 @@
       </c>
       <c r="B30" s="2">
         <f>January!B30+February!B30+March!B30+April!B30+May!B30+June!B30+July!B30+August!B30+September!B30+October!B30+November!B30+December!B30</f>
-        <v>97</v>
+        <v>167</v>
       </c>
       <c r="C30" s="2">
         <f>January!C30+February!C30+March!C30+April!C30+May!C30+June!C30+July!C30+August!C30+September!C30+October!C30+November!C30+December!C30</f>
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="D30" s="2">
         <f>January!D30+February!D30+March!D30+April!D30+May!D30+June!D30+July!D30+August!D30+September!D30+October!D30+November!D30+December!D30</f>
-        <v>33</v>
+        <v>86</v>
       </c>
       <c r="E30" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2216,7 +2288,7 @@
       </c>
       <c r="G30" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.52 : 1</v>
+        <v>2.06 : 1</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2225,15 +2297,15 @@
       </c>
       <c r="B31" s="4">
         <f>January!B31+February!B31+March!B31+April!B31+May!B31+June!B31+July!B31+August!B31+September!B31+October!B31+November!B31+December!B31</f>
-        <v>133</v>
+        <v>252</v>
       </c>
       <c r="C31" s="4">
         <f>January!C31+February!C31+March!C31+April!C31+May!C31+June!C31+July!C31+August!C31+September!C31+October!C31+November!C31+December!C31</f>
-        <v>613</v>
+        <v>907</v>
       </c>
       <c r="D31" s="4">
         <f>January!D31+February!D31+March!D31+April!D31+May!D31+June!D31+July!D31+August!D31+September!D31+October!D31+November!D31+December!D31</f>
-        <v>-480</v>
+        <v>-655</v>
       </c>
       <c r="E31" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2245,7 +2317,7 @@
       </c>
       <c r="G31" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.22 : 1</v>
+        <v>0.28 : 1</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2254,15 +2326,15 @@
       </c>
       <c r="B32" s="2">
         <f>January!B32+February!B32+March!B32+April!B32+May!B32+June!B32+July!B32+August!B32+September!B32+October!B32+November!B32+December!B32</f>
-        <v>867</v>
+        <v>1333</v>
       </c>
       <c r="C32" s="2">
         <f>January!C32+February!C32+March!C32+April!C32+May!C32+June!C32+July!C32+August!C32+September!C32+October!C32+November!C32+December!C32</f>
-        <v>1174</v>
+        <v>1958</v>
       </c>
       <c r="D32" s="2">
         <f>January!D32+February!D32+March!D32+April!D32+May!D32+June!D32+July!D32+August!D32+September!D32+October!D32+November!D32+December!D32</f>
-        <v>-307</v>
+        <v>-625</v>
       </c>
       <c r="E32" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2274,7 +2346,7 @@
       </c>
       <c r="G32" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.74 : 1</v>
+        <v>0.68 : 1</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2283,27 +2355,27 @@
       </c>
       <c r="B33" s="4">
         <f>January!B33+February!B33+March!B33+April!B33+May!B33+June!B33+July!B33+August!B33+September!B33+October!B33+November!B33+December!B33</f>
-        <v>992</v>
+        <v>1451</v>
       </c>
       <c r="C33" s="4">
         <f>January!C33+February!C33+March!C33+April!C33+May!C33+June!C33+July!C33+August!C33+September!C33+October!C33+November!C33+December!C33</f>
-        <v>945</v>
+        <v>1575</v>
       </c>
       <c r="D33" s="4">
         <f>January!D33+February!D33+March!D33+April!D33+May!D33+June!D33+July!D33+August!D33+September!D33+October!D33+November!D33+December!D33</f>
-        <v>47</v>
+        <v>-124</v>
       </c>
       <c r="E33" s="29" t="str">
         <f t="shared" si="1"/>
-        <v>We borrowed more than we lent this year</v>
+        <v/>
       </c>
       <c r="F33" s="29" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>We lent more than we borrowed this year</v>
       </c>
       <c r="G33" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.05 : 1</v>
+        <v>0.92 : 1</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2312,15 +2384,15 @@
       </c>
       <c r="B34" s="2">
         <f>January!B34+February!B34+March!B34+April!B34+May!B34+June!B34+July!B34+August!B34+September!B34+October!B34+November!B34+December!B34</f>
-        <v>475</v>
+        <v>734</v>
       </c>
       <c r="C34" s="2">
         <f>January!C34+February!C34+March!C34+April!C34+May!C34+June!C34+July!C34+August!C34+September!C34+October!C34+November!C34+December!C34</f>
-        <v>259</v>
+        <v>415</v>
       </c>
       <c r="D34" s="2">
         <f>January!D34+February!D34+March!D34+April!D34+May!D34+June!D34+July!D34+August!D34+September!D34+October!D34+November!D34+December!D34</f>
-        <v>216</v>
+        <v>319</v>
       </c>
       <c r="E34" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2332,7 +2404,7 @@
       </c>
       <c r="G34" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.83 : 1</v>
+        <v>1.77 : 1</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2341,15 +2413,15 @@
       </c>
       <c r="B35" s="4">
         <f>January!B35+February!B35+March!B35+April!B35+May!B35+June!B35+July!B35+August!B35+September!B35+October!B35+November!B35+December!B35</f>
-        <v>1708</v>
+        <v>2701</v>
       </c>
       <c r="C35" s="4">
         <f>January!C35+February!C35+March!C35+April!C35+May!C35+June!C35+July!C35+August!C35+September!C35+October!C35+November!C35+December!C35</f>
-        <v>2013</v>
+        <v>3230</v>
       </c>
       <c r="D35" s="4">
         <f>January!D35+February!D35+March!D35+April!D35+May!D35+June!D35+July!D35+August!D35+September!D35+October!D35+November!D35+December!D35</f>
-        <v>-305</v>
+        <v>-529</v>
       </c>
       <c r="E35" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2361,7 +2433,7 @@
       </c>
       <c r="G35" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.85 : 1</v>
+        <v>0.84 : 1</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2370,15 +2442,15 @@
       </c>
       <c r="B36" s="2">
         <f>January!B36+February!B36+March!B36+April!B36+May!B36+June!B36+July!B36+August!B36+September!B36+October!B36+November!B36+December!B36</f>
-        <v>414</v>
+        <v>669</v>
       </c>
       <c r="C36" s="2">
         <f>January!C36+February!C36+March!C36+April!C36+May!C36+June!C36+July!C36+August!C36+September!C36+October!C36+November!C36+December!C36</f>
-        <v>1127</v>
+        <v>1641</v>
       </c>
       <c r="D36" s="2">
         <f>January!D36+February!D36+March!D36+April!D36+May!D36+June!D36+July!D36+August!D36+September!D36+October!D36+November!D36+December!D36</f>
-        <v>-713</v>
+        <v>-972</v>
       </c>
       <c r="E36" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2390,7 +2462,7 @@
       </c>
       <c r="G36" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.37 : 1</v>
+        <v>0.41 : 1</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2399,15 +2471,15 @@
       </c>
       <c r="B37" s="4">
         <f>January!B37+February!B37+March!B37+April!B37+May!B37+June!B37+July!B37+August!B37+September!B37+October!B37+November!B37+December!B37</f>
-        <v>982</v>
+        <v>1574</v>
       </c>
       <c r="C37" s="4">
         <f>January!C37+February!C37+March!C37+April!C37+May!C37+June!C37+July!C37+August!C37+September!C37+October!C37+November!C37+December!C37</f>
-        <v>723</v>
+        <v>1163</v>
       </c>
       <c r="D37" s="4">
         <f>January!D37+February!D37+March!D37+April!D37+May!D37+June!D37+July!D37+August!D37+September!D37+October!D37+November!D37+December!D37</f>
-        <v>259</v>
+        <v>411</v>
       </c>
       <c r="E37" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2419,7 +2491,7 @@
       </c>
       <c r="G37" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.36 : 1</v>
+        <v>1.35 : 1</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2428,15 +2500,15 @@
       </c>
       <c r="B38" s="2">
         <f>January!B38+February!B38+March!B38+April!B38+May!B38+June!B38+July!B38+August!B38+September!B38+October!B38+November!B38+December!B38</f>
-        <v>155</v>
+        <v>187</v>
       </c>
       <c r="C38" s="2">
         <f>January!C38+February!C38+March!C38+April!C38+May!C38+June!C38+July!C38+August!C38+September!C38+October!C38+November!C38+December!C38</f>
-        <v>334</v>
+        <v>500</v>
       </c>
       <c r="D38" s="2">
         <f>January!D38+February!D38+March!D38+April!D38+May!D38+June!D38+July!D38+August!D38+September!D38+October!D38+November!D38+December!D38</f>
-        <v>-179</v>
+        <v>-313</v>
       </c>
       <c r="E38" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2448,7 +2520,7 @@
       </c>
       <c r="G38" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.46 : 1</v>
+        <v>0.37 : 1</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2457,15 +2529,15 @@
       </c>
       <c r="B39" s="8">
         <f>January!B39+February!B39+March!B39+April!B39+May!B39+June!B39+July!B39+August!B39+September!B39+October!B39+November!B39+December!B39</f>
-        <v>102</v>
+        <v>140</v>
       </c>
       <c r="C39" s="8">
         <f>January!C39+February!C39+March!C39+April!C39+May!C39+June!C39+July!C39+August!C39+September!C39+October!C39+November!C39+December!C39</f>
-        <v>117</v>
+        <v>193</v>
       </c>
       <c r="D39" s="8">
         <f>January!D39+February!D39+March!D39+April!D39+May!D39+June!D39+July!D39+August!D39+September!D39+October!D39+November!D39+December!D39</f>
-        <v>-15</v>
+        <v>-53</v>
       </c>
       <c r="E39" s="31" t="str">
         <f t="shared" si="1"/>
@@ -2477,7 +2549,7 @@
       </c>
       <c r="G39" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>0.87 : 1</v>
+        <v>0.73 : 1</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2486,15 +2558,15 @@
       </c>
       <c r="B40" s="8">
         <f>January!B40+February!B40+March!B40+April!B40+May!B40+June!B40+July!B40+August!B40+September!B40+October!B40+November!B40+December!B40</f>
-        <v>151</v>
+        <v>241</v>
       </c>
       <c r="C40" s="8">
         <f>January!C40+February!C40+March!C40+April!C40+May!C40+June!C40+July!C40+August!C40+September!C40+October!C40+November!C40+December!C40</f>
-        <v>247</v>
+        <v>367</v>
       </c>
       <c r="D40" s="8">
         <f>January!D40+February!D40+March!D40+April!D40+May!D40+June!D40+July!D40+August!D40+September!D40+October!D40+November!D40+December!D40</f>
-        <v>-96</v>
+        <v>-126</v>
       </c>
       <c r="E40" s="31" t="str">
         <f t="shared" si="1"/>
@@ -2506,7 +2578,7 @@
       </c>
       <c r="G40" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>0.61 : 1</v>
+        <v>0.66 : 1</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2515,15 +2587,15 @@
       </c>
       <c r="B41" s="8">
         <f>January!B41+February!B41+March!B41+April!B41+May!B41+June!B41+July!B41+August!B41+September!B41+October!B41+November!B41+December!B41</f>
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="C41" s="8">
         <f>January!C41+February!C41+March!C41+April!C41+May!C41+June!C41+July!C41+August!C41+September!C41+October!C41+November!C41+December!C41</f>
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="D41" s="8">
         <f>January!D41+February!D41+March!D41+April!D41+May!D41+June!D41+July!D41+August!D41+September!D41+October!D41+November!D41+December!D41</f>
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="E41" s="31" t="str">
         <f t="shared" si="1"/>
@@ -2535,7 +2607,7 @@
       </c>
       <c r="G41" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>1.41 : 1</v>
+        <v>1.06 : 1</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2544,15 +2616,15 @@
       </c>
       <c r="B42" s="8">
         <f>January!B42+February!B42+March!B42+April!B42+May!B42+June!B42+July!B42+August!B42+September!B42+October!B42+November!B42+December!B42</f>
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="C42" s="8">
         <f>January!C42+February!C42+March!C42+April!C42+May!C42+June!C42+July!C42+August!C42+September!C42+October!C42+November!C42+December!C42</f>
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="D42" s="8">
         <f>January!D42+February!D42+March!D42+April!D42+May!D42+June!D42+July!D42+August!D42+September!D42+October!D42+November!D42+December!D42</f>
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="E42" s="31" t="str">
         <f t="shared" si="1"/>
@@ -2564,7 +2636,7 @@
       </c>
       <c r="G42" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>3.3 : 1</v>
+        <v>1.21 : 1</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2577,11 +2649,11 @@
       </c>
       <c r="C43" s="8">
         <f>January!C43+February!C43+March!C43+April!C43+May!C43+June!C43+July!C43+August!C43+September!C43+October!C43+November!C43+December!C43</f>
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D43" s="8">
         <f>January!D43+February!D43+March!D43+April!D43+May!D43+June!D43+July!D43+August!D43+September!D43+October!D43+November!D43+December!D43</f>
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E43" s="31" t="str">
         <f t="shared" si="1"/>
@@ -2593,7 +2665,7 @@
       </c>
       <c r="G43" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>1.57 : 1</v>
+        <v>1.42 : 1</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2602,15 +2674,15 @@
       </c>
       <c r="B44" s="4">
         <f>January!B44+February!B44+March!B44+April!B44+May!B44+June!B44+July!B44+August!B44+September!B44+October!B44+November!B44+December!B44</f>
-        <v>174</v>
+        <v>356</v>
       </c>
       <c r="C44" s="4">
         <f>January!C44+February!C44+March!C44+April!C44+May!C44+June!C44+July!C44+August!C44+September!C44+October!C44+November!C44+December!C44</f>
-        <v>167</v>
+        <v>248</v>
       </c>
       <c r="D44" s="4">
         <f>January!D44+February!D44+March!D44+April!D44+May!D44+June!D44+July!D44+August!D44+September!D44+October!D44+November!D44+December!D44</f>
-        <v>7</v>
+        <v>108</v>
       </c>
       <c r="E44" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2622,7 +2694,7 @@
       </c>
       <c r="G44" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.04 : 1</v>
+        <v>1.44 : 1</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2631,15 +2703,15 @@
       </c>
       <c r="B45" s="2">
         <f>January!B45+February!B45+March!B45+April!B45+May!B45+June!B45+July!B45+August!B45+September!B45+October!B45+November!B45+December!B45</f>
-        <v>139</v>
+        <v>197</v>
       </c>
       <c r="C45" s="2">
         <f>January!C45+February!C45+March!C45+April!C45+May!C45+June!C45+July!C45+August!C45+September!C45+October!C45+November!C45+December!C45</f>
-        <v>295</v>
+        <v>461</v>
       </c>
       <c r="D45" s="2">
         <f>January!D45+February!D45+March!D45+April!D45+May!D45+June!D45+July!D45+August!D45+September!D45+October!D45+November!D45+December!D45</f>
-        <v>-156</v>
+        <v>-264</v>
       </c>
       <c r="E45" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2651,7 +2723,7 @@
       </c>
       <c r="G45" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.47 : 1</v>
+        <v>0.43 : 1</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2660,15 +2732,15 @@
       </c>
       <c r="B46" s="4">
         <f>January!B46+February!B46+March!B46+April!B46+May!B46+June!B46+July!B46+August!B46+September!B46+October!B46+November!B46+December!B46</f>
-        <v>856</v>
+        <v>1332</v>
       </c>
       <c r="C46" s="4">
         <f>January!C46+February!C46+March!C46+April!C46+May!C46+June!C46+July!C46+August!C46+September!C46+October!C46+November!C46+December!C46</f>
-        <v>1224</v>
+        <v>1881</v>
       </c>
       <c r="D46" s="4">
         <f>January!D46+February!D46+March!D46+April!D46+May!D46+June!D46+July!D46+August!D46+September!D46+October!D46+November!D46+December!D46</f>
-        <v>-368</v>
+        <v>-549</v>
       </c>
       <c r="E46" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2680,7 +2752,7 @@
       </c>
       <c r="G46" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.7 : 1</v>
+        <v>0.71 : 1</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2689,15 +2761,15 @@
       </c>
       <c r="B47" s="2">
         <f>January!B47+February!B47+March!B47+April!B47+May!B47+June!B47+July!B47+August!B47+September!B47+October!B47+November!B47+December!B47</f>
-        <v>2028</v>
+        <v>2884</v>
       </c>
       <c r="C47" s="2">
         <f>January!C47+February!C47+March!C47+April!C47+May!C47+June!C47+July!C47+August!C47+September!C47+October!C47+November!C47+December!C47</f>
-        <v>1499</v>
+        <v>2287</v>
       </c>
       <c r="D47" s="2">
         <f>January!D47+February!D47+March!D47+April!D47+May!D47+June!D47+July!D47+August!D47+September!D47+October!D47+November!D47+December!D47</f>
-        <v>529</v>
+        <v>597</v>
       </c>
       <c r="E47" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2709,7 +2781,7 @@
       </c>
       <c r="G47" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.35 : 1</v>
+        <v>1.26 : 1</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2718,15 +2790,15 @@
       </c>
       <c r="B48" s="4">
         <f>January!B48+February!B48+March!B48+April!B48+May!B48+June!B48+July!B48+August!B48+September!B48+October!B48+November!B48+December!B48</f>
-        <v>504</v>
+        <v>741</v>
       </c>
       <c r="C48" s="4">
         <f>January!C48+February!C48+March!C48+April!C48+May!C48+June!C48+July!C48+August!C48+September!C48+October!C48+November!C48+December!C48</f>
-        <v>1276</v>
+        <v>1977</v>
       </c>
       <c r="D48" s="4">
         <f>January!D48+February!D48+March!D48+April!D48+May!D48+June!D48+July!D48+August!D48+September!D48+October!D48+November!D48+December!D48</f>
-        <v>-772</v>
+        <v>-1236</v>
       </c>
       <c r="E48" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2738,7 +2810,7 @@
       </c>
       <c r="G48" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.39 : 1</v>
+        <v>0.37 : 1</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2747,15 +2819,15 @@
       </c>
       <c r="B49" s="2">
         <f>January!B49+February!B49+March!B49+April!B49+May!B49+June!B49+July!B49+August!B49+September!B49+October!B49+November!B49+December!B49</f>
-        <v>930</v>
+        <v>1258</v>
       </c>
       <c r="C49" s="2">
         <f>January!C49+February!C49+March!C49+April!C49+May!C49+June!C49+July!C49+August!C49+September!C49+October!C49+November!C49+December!C49</f>
-        <v>414</v>
+        <v>601</v>
       </c>
       <c r="D49" s="2">
         <f>January!D49+February!D49+March!D49+April!D49+May!D49+June!D49+July!D49+August!D49+September!D49+October!D49+November!D49+December!D49</f>
-        <v>516</v>
+        <v>657</v>
       </c>
       <c r="E49" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2767,7 +2839,7 @@
       </c>
       <c r="G49" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>2.25 : 1</v>
+        <v>2.09 : 1</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2776,15 +2848,15 @@
       </c>
       <c r="B50" s="4">
         <f>January!B50+February!B50+March!B50+April!B50+May!B50+June!B50+July!B50+August!B50+September!B50+October!B50+November!B50+December!B50</f>
-        <v>1639</v>
+        <v>2586</v>
       </c>
       <c r="C50" s="4">
         <f>January!C50+February!C50+March!C50+April!C50+May!C50+June!C50+July!C50+August!C50+September!C50+October!C50+November!C50+December!C50</f>
-        <v>1112</v>
+        <v>1695</v>
       </c>
       <c r="D50" s="4">
         <f>January!D50+February!D50+March!D50+April!D50+May!D50+June!D50+July!D50+August!D50+September!D50+October!D50+November!D50+December!D50</f>
-        <v>527</v>
+        <v>891</v>
       </c>
       <c r="E50" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2796,7 +2868,7 @@
       </c>
       <c r="G50" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.47 : 1</v>
+        <v>1.53 : 1</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2805,15 +2877,15 @@
       </c>
       <c r="B51" s="2">
         <f>January!B51+February!B51+March!B51+April!B51+May!B51+June!B51+July!B51+August!B51+September!B51+October!B51+November!B51+December!B51</f>
-        <v>418</v>
+        <v>735</v>
       </c>
       <c r="C51" s="2">
         <f>January!C51+February!C51+March!C51+April!C51+May!C51+June!C51+July!C51+August!C51+September!C51+October!C51+November!C51+December!C51</f>
-        <v>197</v>
+        <v>303</v>
       </c>
       <c r="D51" s="2">
         <f>January!D51+February!D51+March!D51+April!D51+May!D51+June!D51+July!D51+August!D51+September!D51+October!D51+November!D51+December!D51</f>
-        <v>221</v>
+        <v>432</v>
       </c>
       <c r="E51" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2825,7 +2897,7 @@
       </c>
       <c r="G51" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>2.12 : 1</v>
+        <v>2.43 : 1</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2834,15 +2906,15 @@
       </c>
       <c r="B52" s="4">
         <f>January!B52+February!B52+March!B52+April!B52+May!B52+June!B52+July!B52+August!B52+September!B52+October!B52+November!B52+December!B52</f>
-        <v>989</v>
+        <v>1619</v>
       </c>
       <c r="C52" s="4">
         <f>January!C52+February!C52+March!C52+April!C52+May!C52+June!C52+July!C52+August!C52+September!C52+October!C52+November!C52+December!C52</f>
-        <v>1157</v>
+        <v>1737</v>
       </c>
       <c r="D52" s="4">
         <f>January!D52+February!D52+March!D52+April!D52+May!D52+June!D52+July!D52+August!D52+September!D52+October!D52+November!D52+December!D52</f>
-        <v>-168</v>
+        <v>-118</v>
       </c>
       <c r="E52" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2854,7 +2926,7 @@
       </c>
       <c r="G52" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.85 : 1</v>
+        <v>0.93 : 1</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2863,15 +2935,15 @@
       </c>
       <c r="B53" s="2">
         <f>January!B53+February!B53+March!B53+April!B53+May!B53+June!B53+July!B53+August!B53+September!B53+October!B53+November!B53+December!B53</f>
-        <v>206</v>
+        <v>303</v>
       </c>
       <c r="C53" s="2">
         <f>January!C53+February!C53+March!C53+April!C53+May!C53+June!C53+July!C53+August!C53+September!C53+October!C53+November!C53+December!C53</f>
-        <v>354</v>
+        <v>587</v>
       </c>
       <c r="D53" s="2">
         <f>January!D53+February!D53+March!D53+April!D53+May!D53+June!D53+July!D53+August!D53+September!D53+October!D53+November!D53+December!D53</f>
-        <v>-148</v>
+        <v>-284</v>
       </c>
       <c r="E53" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2883,7 +2955,7 @@
       </c>
       <c r="G53" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.58 : 1</v>
+        <v>0.52 : 1</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2892,15 +2964,15 @@
       </c>
       <c r="B54" s="4">
         <f>January!B54+February!B54+March!B54+April!B54+May!B54+June!B54+July!B54+August!B54+September!B54+October!B54+November!B54+December!B54</f>
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="C54" s="4">
         <f>January!C54+February!C54+March!C54+April!C54+May!C54+June!C54+July!C54+August!C54+September!C54+October!C54+November!C54+December!C54</f>
-        <v>481</v>
+        <v>758</v>
       </c>
       <c r="D54" s="4">
         <f>January!D54+February!D54+March!D54+April!D54+May!D54+June!D54+July!D54+August!D54+September!D54+October!D54+November!D54+December!D54</f>
-        <v>-418</v>
+        <v>-652</v>
       </c>
       <c r="E54" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2912,7 +2984,7 @@
       </c>
       <c r="G54" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.13 : 1</v>
+        <v>0.14 : 1</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2921,15 +2993,15 @@
       </c>
       <c r="B55" s="10">
         <f>January!B55+February!B55+March!B55+April!B55+May!B55+June!B55+July!B55+August!B55+September!B55+October!B55+November!B55+December!B55</f>
-        <v>346</v>
+        <v>452</v>
       </c>
       <c r="C55" s="10">
         <f>January!C55+February!C55+March!C55+April!C55+May!C55+June!C55+July!C55+August!C55+September!C55+October!C55+November!C55+December!C55</f>
-        <v>286</v>
+        <v>338</v>
       </c>
       <c r="D55" s="10">
         <f>January!D55+February!D55+March!D55+April!D55+May!D55+June!D55+July!D55+August!D55+September!D55+October!D55+November!D55+December!D55</f>
-        <v>60</v>
+        <v>114</v>
       </c>
       <c r="E55" s="32" t="str">
         <f t="shared" si="1"/>
@@ -2941,7 +3013,7 @@
       </c>
       <c r="G55" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>1.21 : 1</v>
+        <v>1.34 : 1</v>
       </c>
     </row>
   </sheetData>
@@ -8040,108 +8112,204 @@
       <c r="A2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="28"/>
+      <c r="B2" s="18">
+        <v>1436</v>
+      </c>
+      <c r="C2" s="18">
+        <v>1235</v>
+      </c>
+      <c r="D2" s="18">
+        <v>201</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F2" s="28"/>
-      <c r="G2" s="3"/>
+      <c r="G2" s="3" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
+      <c r="B3" s="21">
+        <v>500</v>
+      </c>
+      <c r="C3" s="21">
+        <v>530</v>
+      </c>
+      <c r="D3" s="21">
+        <v>-30</v>
+      </c>
       <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="5"/>
+      <c r="F3" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="28"/>
+      <c r="B4" s="18">
+        <v>1444</v>
+      </c>
+      <c r="C4" s="18">
+        <v>1299</v>
+      </c>
+      <c r="D4" s="18">
+        <v>145</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F4" s="28"/>
-      <c r="G4" s="3"/>
+      <c r="G4" s="3" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="29"/>
+      <c r="B5" s="21">
+        <v>115</v>
+      </c>
+      <c r="C5" s="21">
+        <v>111</v>
+      </c>
+      <c r="D5" s="21">
+        <v>4</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F5" s="29"/>
-      <c r="G5" s="5"/>
+      <c r="G5" s="5" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
+      <c r="B6" s="18">
+        <v>1441</v>
+      </c>
+      <c r="C6" s="18">
+        <v>1714</v>
+      </c>
+      <c r="D6" s="18">
+        <v>-273</v>
+      </c>
       <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="3"/>
+      <c r="F6" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
+      <c r="B7" s="21">
+        <v>298</v>
+      </c>
+      <c r="C7" s="21">
+        <v>315</v>
+      </c>
+      <c r="D7" s="21">
+        <v>-17</v>
+      </c>
       <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="5"/>
+      <c r="F7" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
+      <c r="B8" s="18">
+        <v>144</v>
+      </c>
+      <c r="C8" s="18">
+        <v>205</v>
+      </c>
+      <c r="D8" s="18">
+        <v>-61</v>
+      </c>
       <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="3"/>
+      <c r="F8" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="29"/>
+      <c r="B9" s="21">
+        <v>77</v>
+      </c>
+      <c r="C9" s="21">
+        <v>76</v>
+      </c>
+      <c r="D9" s="21">
+        <v>1</v>
+      </c>
+      <c r="E9" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F9" s="29"/>
-      <c r="G9" s="5"/>
+      <c r="G9" s="5" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
+      <c r="B10" s="18">
+        <v>9</v>
+      </c>
+      <c r="C10" s="18">
+        <v>39</v>
+      </c>
+      <c r="D10" s="18">
+        <v>-30</v>
+      </c>
       <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="3"/>
+      <c r="F10" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
+      <c r="B11" s="21">
+        <v>0</v>
+      </c>
+      <c r="C11" s="21">
+        <v>0</v>
+      </c>
+      <c r="D11" s="21">
+        <v>0</v>
+      </c>
       <c r="E11" s="29"/>
       <c r="F11" s="29"/>
       <c r="G11" s="5"/>
@@ -8150,163 +8318,309 @@
       <c r="A12" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
+      <c r="B12" s="23">
+        <v>19</v>
+      </c>
+      <c r="C12" s="23">
+        <v>29</v>
+      </c>
+      <c r="D12" s="23">
+        <v>-10</v>
+      </c>
       <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="7"/>
+      <c r="F12" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="30"/>
+      <c r="B13" s="23">
+        <v>155</v>
+      </c>
+      <c r="C13" s="23">
+        <v>113</v>
+      </c>
+      <c r="D13" s="23">
+        <v>42</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>61</v>
+      </c>
       <c r="F13" s="30"/>
-      <c r="G13" s="7"/>
+      <c r="G13" s="7" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
+      <c r="B14" s="23">
+        <v>146</v>
+      </c>
+      <c r="C14" s="23">
+        <v>341</v>
+      </c>
+      <c r="D14" s="23">
+        <v>-195</v>
+      </c>
       <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="7"/>
+      <c r="F14" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
+      <c r="B15" s="23">
+        <v>60</v>
+      </c>
+      <c r="C15" s="23">
+        <v>97</v>
+      </c>
+      <c r="D15" s="23">
+        <v>-37</v>
+      </c>
       <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="7"/>
+      <c r="F15" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
+      <c r="B16" s="18">
+        <v>22</v>
+      </c>
+      <c r="C16" s="18">
+        <v>104</v>
+      </c>
+      <c r="D16" s="18">
+        <v>-82</v>
+      </c>
       <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="3"/>
+      <c r="F16" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="29"/>
+      <c r="B17" s="21">
+        <v>644</v>
+      </c>
+      <c r="C17" s="21">
+        <v>557</v>
+      </c>
+      <c r="D17" s="21">
+        <v>87</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F17" s="29"/>
-      <c r="G17" s="5"/>
+      <c r="G17" s="5" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="28"/>
+      <c r="B18" s="18">
+        <v>142</v>
+      </c>
+      <c r="C18" s="18">
+        <v>119</v>
+      </c>
+      <c r="D18" s="18">
+        <v>23</v>
+      </c>
+      <c r="E18" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F18" s="28"/>
-      <c r="G18" s="3"/>
+      <c r="G18" s="3" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="29"/>
+      <c r="B19" s="21">
+        <v>730</v>
+      </c>
+      <c r="C19" s="21">
+        <v>357</v>
+      </c>
+      <c r="D19" s="21">
+        <v>373</v>
+      </c>
+      <c r="E19" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F19" s="29"/>
-      <c r="G19" s="5"/>
+      <c r="G19" s="5" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
+      <c r="B20" s="18">
+        <v>1</v>
+      </c>
+      <c r="C20" s="18">
+        <v>70</v>
+      </c>
+      <c r="D20" s="18">
+        <v>-69</v>
+      </c>
       <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="3"/>
+      <c r="F20" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="29"/>
+      <c r="B21" s="21">
+        <v>630</v>
+      </c>
+      <c r="C21" s="21">
+        <v>459</v>
+      </c>
+      <c r="D21" s="21">
+        <v>171</v>
+      </c>
+      <c r="E21" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F21" s="29"/>
-      <c r="G21" s="5"/>
+      <c r="G21" s="5" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
+      <c r="B22" s="18">
+        <v>25</v>
+      </c>
+      <c r="C22" s="18">
+        <v>93</v>
+      </c>
+      <c r="D22" s="18">
+        <v>-68</v>
+      </c>
       <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="3"/>
+      <c r="F22" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="29"/>
+      <c r="B23" s="21">
+        <v>770</v>
+      </c>
+      <c r="C23" s="21">
+        <v>602</v>
+      </c>
+      <c r="D23" s="21">
+        <v>168</v>
+      </c>
+      <c r="E23" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F23" s="29"/>
-      <c r="G23" s="5"/>
+      <c r="G23" s="5" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="28"/>
+      <c r="B24" s="18">
+        <v>2252</v>
+      </c>
+      <c r="C24" s="18">
+        <v>1547</v>
+      </c>
+      <c r="D24" s="18">
+        <v>705</v>
+      </c>
+      <c r="E24" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F24" s="28"/>
-      <c r="G24" s="3"/>
+      <c r="G24" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
+      <c r="B25" s="21">
+        <v>213</v>
+      </c>
+      <c r="C25" s="21">
+        <v>383</v>
+      </c>
+      <c r="D25" s="21">
+        <v>-170</v>
+      </c>
       <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="5"/>
+      <c r="F25" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="26" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
+      <c r="B26" s="18">
+        <v>0</v>
+      </c>
+      <c r="C26" s="18">
+        <v>0</v>
+      </c>
+      <c r="D26" s="18">
+        <v>0</v>
+      </c>
       <c r="E26" s="28"/>
       <c r="F26" s="28"/>
       <c r="G26" s="3"/>
@@ -8315,320 +8629,610 @@
       <c r="A27" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="29"/>
+      <c r="B27" s="21">
+        <v>480</v>
+      </c>
+      <c r="C27" s="21">
+        <v>202</v>
+      </c>
+      <c r="D27" s="21">
+        <v>278</v>
+      </c>
+      <c r="E27" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F27" s="29"/>
-      <c r="G27" s="5"/>
+      <c r="G27" s="5" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
+      <c r="B28" s="18">
+        <v>51</v>
+      </c>
+      <c r="C28" s="18">
+        <v>91</v>
+      </c>
+      <c r="D28" s="18">
+        <v>-40</v>
+      </c>
       <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="3"/>
+      <c r="F28" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="29"/>
+      <c r="B29" s="21">
+        <v>590</v>
+      </c>
+      <c r="C29" s="21">
+        <v>501</v>
+      </c>
+      <c r="D29" s="21">
+        <v>89</v>
+      </c>
+      <c r="E29" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F29" s="29"/>
-      <c r="G29" s="5"/>
+      <c r="G29" s="5" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="30" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="28"/>
+      <c r="B30" s="18">
+        <v>70</v>
+      </c>
+      <c r="C30" s="18">
+        <v>17</v>
+      </c>
+      <c r="D30" s="18">
+        <v>53</v>
+      </c>
+      <c r="E30" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F30" s="28"/>
-      <c r="G30" s="3"/>
+      <c r="G30" s="3" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
+      <c r="B31" s="21">
+        <v>119</v>
+      </c>
+      <c r="C31" s="21">
+        <v>294</v>
+      </c>
+      <c r="D31" s="21">
+        <v>-175</v>
+      </c>
       <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="5"/>
+      <c r="F31" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="32" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
+      <c r="B32" s="18">
+        <v>466</v>
+      </c>
+      <c r="C32" s="18">
+        <v>784</v>
+      </c>
+      <c r="D32" s="18">
+        <v>-318</v>
+      </c>
       <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="3"/>
+      <c r="F32" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="33" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
+      <c r="B33" s="21">
+        <v>459</v>
+      </c>
+      <c r="C33" s="21">
+        <v>630</v>
+      </c>
+      <c r="D33" s="21">
+        <v>-171</v>
+      </c>
       <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="5"/>
+      <c r="F33" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="34" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="28"/>
+      <c r="B34" s="18">
+        <v>259</v>
+      </c>
+      <c r="C34" s="18">
+        <v>156</v>
+      </c>
+      <c r="D34" s="18">
+        <v>103</v>
+      </c>
+      <c r="E34" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F34" s="28"/>
-      <c r="G34" s="3"/>
+      <c r="G34" s="3" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
+      <c r="B35" s="21">
+        <v>993</v>
+      </c>
+      <c r="C35" s="21">
+        <v>1217</v>
+      </c>
+      <c r="D35" s="21">
+        <v>-224</v>
+      </c>
       <c r="E35" s="29"/>
-      <c r="F35" s="29"/>
-      <c r="G35" s="5"/>
+      <c r="F35" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="36" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
+      <c r="B36" s="18">
+        <v>255</v>
+      </c>
+      <c r="C36" s="18">
+        <v>514</v>
+      </c>
+      <c r="D36" s="18">
+        <v>-259</v>
+      </c>
       <c r="E36" s="28"/>
-      <c r="F36" s="28"/>
-      <c r="G36" s="3"/>
+      <c r="F36" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="29"/>
+      <c r="B37" s="21">
+        <v>592</v>
+      </c>
+      <c r="C37" s="21">
+        <v>440</v>
+      </c>
+      <c r="D37" s="21">
+        <v>152</v>
+      </c>
+      <c r="E37" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F37" s="29"/>
-      <c r="G37" s="5"/>
+      <c r="G37" s="5" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
+      <c r="B38" s="18">
+        <v>32</v>
+      </c>
+      <c r="C38" s="18">
+        <v>166</v>
+      </c>
+      <c r="D38" s="18">
+        <v>-134</v>
+      </c>
       <c r="E38" s="28"/>
-      <c r="F38" s="28"/>
-      <c r="G38" s="3"/>
+      <c r="F38" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="B39" s="25"/>
-      <c r="C39" s="25"/>
-      <c r="D39" s="25"/>
+      <c r="B39" s="25">
+        <v>38</v>
+      </c>
+      <c r="C39" s="25">
+        <v>76</v>
+      </c>
+      <c r="D39" s="25">
+        <v>-38</v>
+      </c>
       <c r="E39" s="31"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="9"/>
+      <c r="F39" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="B40" s="25"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
+      <c r="B40" s="25">
+        <v>90</v>
+      </c>
+      <c r="C40" s="25">
+        <v>120</v>
+      </c>
+      <c r="D40" s="25">
+        <v>-30</v>
+      </c>
       <c r="E40" s="31"/>
-      <c r="F40" s="31"/>
-      <c r="G40" s="9"/>
+      <c r="F40" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
+      <c r="B41" s="25">
+        <v>16</v>
+      </c>
+      <c r="C41" s="25">
+        <v>27</v>
+      </c>
+      <c r="D41" s="25">
+        <v>-11</v>
+      </c>
       <c r="E41" s="31"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="9"/>
+      <c r="F41" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="42" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="B42" s="25"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="25"/>
+      <c r="B42" s="25">
+        <v>8</v>
+      </c>
+      <c r="C42" s="25">
+        <v>24</v>
+      </c>
+      <c r="D42" s="25">
+        <v>-16</v>
+      </c>
       <c r="E42" s="31"/>
-      <c r="F42" s="31"/>
-      <c r="G42" s="9"/>
+      <c r="F42" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="B43" s="25"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
+      <c r="B43" s="25">
+        <v>0</v>
+      </c>
+      <c r="C43" s="25">
+        <v>3</v>
+      </c>
+      <c r="D43" s="25">
+        <v>-3</v>
+      </c>
       <c r="E43" s="31"/>
-      <c r="F43" s="31"/>
-      <c r="G43" s="9"/>
+      <c r="F43" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="44" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="B44" s="21"/>
-      <c r="C44" s="21"/>
-      <c r="D44" s="21"/>
-      <c r="E44" s="29"/>
+      <c r="B44" s="21">
+        <v>182</v>
+      </c>
+      <c r="C44" s="21">
+        <v>81</v>
+      </c>
+      <c r="D44" s="21">
+        <v>101</v>
+      </c>
+      <c r="E44" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F44" s="29"/>
-      <c r="G44" s="5"/>
+      <c r="G44" s="5" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="45" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
+      <c r="B45" s="18">
+        <v>58</v>
+      </c>
+      <c r="C45" s="18">
+        <v>166</v>
+      </c>
+      <c r="D45" s="18">
+        <v>-108</v>
+      </c>
       <c r="E45" s="28"/>
-      <c r="F45" s="28"/>
-      <c r="G45" s="3"/>
+      <c r="F45" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="46" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="B46" s="21"/>
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
+      <c r="B46" s="21">
+        <v>476</v>
+      </c>
+      <c r="C46" s="21">
+        <v>657</v>
+      </c>
+      <c r="D46" s="21">
+        <v>-181</v>
+      </c>
       <c r="E46" s="29"/>
-      <c r="F46" s="29"/>
-      <c r="G46" s="5"/>
+      <c r="F46" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="47" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="28"/>
+      <c r="B47" s="18">
+        <v>856</v>
+      </c>
+      <c r="C47" s="18">
+        <v>788</v>
+      </c>
+      <c r="D47" s="18">
+        <v>68</v>
+      </c>
+      <c r="E47" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F47" s="28"/>
-      <c r="G47" s="3"/>
+      <c r="G47" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="B48" s="21"/>
-      <c r="C48" s="21"/>
-      <c r="D48" s="21"/>
+      <c r="B48" s="21">
+        <v>237</v>
+      </c>
+      <c r="C48" s="21">
+        <v>701</v>
+      </c>
+      <c r="D48" s="21">
+        <v>-464</v>
+      </c>
       <c r="E48" s="29"/>
-      <c r="F48" s="29"/>
-      <c r="G48" s="5"/>
+      <c r="F48" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B49" s="18"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="18"/>
-      <c r="E49" s="28"/>
+      <c r="B49" s="18">
+        <v>328</v>
+      </c>
+      <c r="C49" s="18">
+        <v>187</v>
+      </c>
+      <c r="D49" s="18">
+        <v>141</v>
+      </c>
+      <c r="E49" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F49" s="28"/>
-      <c r="G49" s="3"/>
+      <c r="G49" s="3" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="B50" s="21"/>
-      <c r="C50" s="21"/>
-      <c r="D50" s="21"/>
-      <c r="E50" s="29"/>
+      <c r="B50" s="21">
+        <v>947</v>
+      </c>
+      <c r="C50" s="21">
+        <v>583</v>
+      </c>
+      <c r="D50" s="21">
+        <v>364</v>
+      </c>
+      <c r="E50" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F50" s="29"/>
-      <c r="G50" s="5"/>
+      <c r="G50" s="5" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B51" s="18"/>
-      <c r="C51" s="18"/>
-      <c r="D51" s="18"/>
-      <c r="E51" s="28"/>
+      <c r="B51" s="18">
+        <v>317</v>
+      </c>
+      <c r="C51" s="18">
+        <v>106</v>
+      </c>
+      <c r="D51" s="18">
+        <v>211</v>
+      </c>
+      <c r="E51" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F51" s="28"/>
-      <c r="G51" s="3"/>
+      <c r="G51" s="3" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="52" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="B52" s="21"/>
-      <c r="C52" s="21"/>
-      <c r="D52" s="21"/>
-      <c r="E52" s="29"/>
+      <c r="B52" s="21">
+        <v>630</v>
+      </c>
+      <c r="C52" s="21">
+        <v>580</v>
+      </c>
+      <c r="D52" s="21">
+        <v>50</v>
+      </c>
+      <c r="E52" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F52" s="29"/>
-      <c r="G52" s="5"/>
+      <c r="G52" s="5" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="53" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B53" s="18"/>
-      <c r="C53" s="18"/>
-      <c r="D53" s="18"/>
+      <c r="B53" s="18">
+        <v>97</v>
+      </c>
+      <c r="C53" s="18">
+        <v>233</v>
+      </c>
+      <c r="D53" s="18">
+        <v>-136</v>
+      </c>
       <c r="E53" s="28"/>
-      <c r="F53" s="28"/>
-      <c r="G53" s="3"/>
+      <c r="F53" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="54" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="B54" s="21"/>
-      <c r="C54" s="21"/>
-      <c r="D54" s="21"/>
+      <c r="B54" s="21">
+        <v>43</v>
+      </c>
+      <c r="C54" s="21">
+        <v>277</v>
+      </c>
+      <c r="D54" s="21">
+        <v>-234</v>
+      </c>
       <c r="E54" s="29"/>
-      <c r="F54" s="29"/>
-      <c r="G54" s="5"/>
+      <c r="F54" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="55" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="B55" s="27"/>
-      <c r="C55" s="27"/>
-      <c r="D55" s="27"/>
-      <c r="E55" s="32"/>
+      <c r="B55" s="27">
+        <v>106</v>
+      </c>
+      <c r="C55" s="27">
+        <v>52</v>
+      </c>
+      <c r="D55" s="27">
+        <v>54</v>
+      </c>
+      <c r="E55" s="32" t="s">
+        <v>61</v>
+      </c>
       <c r="F55" s="32"/>
-      <c r="G55" s="11"/>
+      <c r="G55" s="11" t="s">
+        <v>148</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G55" xr:uid="{00000000-0009-0000-0000-000003000000}"/>

</xml_diff>

<commit_message>
Update statistic files for April 2023 statistics
</commit_message>
<xml_diff>
--- a/statistics_files/2023/2023.g.net_borrower_lender.xlsx
+++ b/statistics_files/2023/2023.g.net_borrower_lender.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20396"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20397"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\GitHub\next_statistics\statistics_files\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C1764D-10AB-4F97-9CD5-53CA66A4758C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D869FF1-3834-42EA-B478-ED0361458D06}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" tabRatio="673" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1210" uniqueCount="190">
   <si>
     <t>NET</t>
   </si>
@@ -547,6 +547,81 @@
   </si>
   <si>
     <t>0.16 : 1</t>
+  </si>
+  <si>
+    <t>0.79 : 1</t>
+  </si>
+  <si>
+    <t>0.98 : 1</t>
+  </si>
+  <si>
+    <t>0.18 : 1</t>
+  </si>
+  <si>
+    <t>1.08 : 1</t>
+  </si>
+  <si>
+    <t>0.96 : 1</t>
+  </si>
+  <si>
+    <t>2.02 : 1</t>
+  </si>
+  <si>
+    <t>1.61 : 1</t>
+  </si>
+  <si>
+    <t>0.02 : 1</t>
+  </si>
+  <si>
+    <t>1.44 : 1</t>
+  </si>
+  <si>
+    <t>1.49 : 1</t>
+  </si>
+  <si>
+    <t>0.90 : 1</t>
+  </si>
+  <si>
+    <t>0.68 : 1</t>
+  </si>
+  <si>
+    <t>0.76 : 1</t>
+  </si>
+  <si>
+    <t>1.72 : 1</t>
+  </si>
+  <si>
+    <t>0.51 : 1</t>
+  </si>
+  <si>
+    <t>1.31 : 1</t>
+  </si>
+  <si>
+    <t>0.22 : 1</t>
+  </si>
+  <si>
+    <t>1.78 : 1</t>
+  </si>
+  <si>
+    <t>0.25 : 1</t>
+  </si>
+  <si>
+    <t>2.07 : 1</t>
+  </si>
+  <si>
+    <t>1.57 : 1</t>
+  </si>
+  <si>
+    <t>3.53 : 1</t>
+  </si>
+  <si>
+    <t>1.06 : 1</t>
+  </si>
+  <si>
+    <t>0.49 : 1</t>
+  </si>
+  <si>
+    <t>0.81 : 1</t>
   </si>
 </sst>
 </file>
@@ -1456,15 +1531,15 @@
       </c>
       <c r="B2" s="2">
         <f>January!B2+February!B2+March!B2+April!B2+May!B2+June!B2+July!B2+August!B2+September!B2+October!B2+November!B2+December!B2</f>
-        <v>4144</v>
+        <v>5375</v>
       </c>
       <c r="C2" s="2">
         <f>January!C2+February!C2+March!C2+April!C2+May!C2+June!C2+July!C2+August!C2+September!C2+October!C2+November!C2+December!C2</f>
-        <v>3555</v>
+        <v>4680</v>
       </c>
       <c r="D2" s="2">
         <f>January!D2+February!D2+March!D2+April!D2+May!D2+June!D2+July!D2+August!D2+September!D2+October!D2+November!D2+December!D2</f>
-        <v>589</v>
+        <v>695</v>
       </c>
       <c r="E2" s="28" t="str">
         <f>IF(D2 &gt; 0, "We borrowed more than we lent this year", "")</f>
@@ -1476,7 +1551,7 @@
       </c>
       <c r="G2" s="3" t="str">
         <f>IF(ISERROR(ROUND(B2/C2,2)&amp;" : 1"), "", ROUND(B2/C2,2)&amp;" : 1")</f>
-        <v>1.17 : 1</v>
+        <v>1.15 : 1</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1485,27 +1560,27 @@
       </c>
       <c r="B3" s="4">
         <f>January!B3+February!B3+March!B3+April!B3+May!B3+June!B3+July!B3+August!B3+September!B3+October!B3+November!B3+December!B3</f>
-        <v>1452</v>
+        <v>1900</v>
       </c>
       <c r="C3" s="4">
         <f>January!C3+February!C3+March!C3+April!C3+May!C3+June!C3+July!C3+August!C3+September!C3+October!C3+November!C3+December!C3</f>
-        <v>1407</v>
+        <v>1939</v>
       </c>
       <c r="D3" s="4">
         <f>January!D3+February!D3+March!D3+April!D3+May!D3+June!D3+July!D3+August!D3+September!D3+October!D3+November!D3+December!D3</f>
-        <v>45</v>
+        <v>-39</v>
       </c>
       <c r="E3" s="29" t="str">
         <f t="shared" ref="E3:E55" si="1">IF(D3 &gt; 0, "We borrowed more than we lent this year", "")</f>
-        <v>We borrowed more than we lent this year</v>
+        <v/>
       </c>
       <c r="F3" s="29" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>We lent more than we borrowed this year</v>
       </c>
       <c r="G3" s="5" t="str">
         <f t="shared" ref="G3:G55" si="2">IF(ISERROR(ROUND(B3/C3,2)&amp;" : 1"), "", ROUND(B3/C3,2)&amp;" : 1")</f>
-        <v>1.03 : 1</v>
+        <v>0.98 : 1</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1514,15 +1589,15 @@
       </c>
       <c r="B4" s="2">
         <f>January!B4+February!B4+March!B4+April!B4+May!B4+June!B4+July!B4+August!B4+September!B4+October!B4+November!B4+December!B4</f>
-        <v>3926</v>
+        <v>5288</v>
       </c>
       <c r="C4" s="2">
         <f>January!C4+February!C4+March!C4+April!C4+May!C4+June!C4+July!C4+August!C4+September!C4+October!C4+November!C4+December!C4</f>
-        <v>3491</v>
+        <v>4712</v>
       </c>
       <c r="D4" s="2">
         <f>January!D4+February!D4+March!D4+April!D4+May!D4+June!D4+July!D4+August!D4+September!D4+October!D4+November!D4+December!D4</f>
-        <v>435</v>
+        <v>576</v>
       </c>
       <c r="E4" s="28" t="str">
         <f t="shared" si="1"/>
@@ -1543,15 +1618,15 @@
       </c>
       <c r="B5" s="4">
         <f>January!B5+February!B5+March!B5+April!B5+May!B5+June!B5+July!B5+August!B5+September!B5+October!B5+November!B5+December!B5</f>
-        <v>188</v>
+        <v>261</v>
       </c>
       <c r="C5" s="4">
         <f>January!C5+February!C5+March!C5+April!C5+May!C5+June!C5+July!C5+August!C5+September!C5+October!C5+November!C5+December!C5</f>
-        <v>368</v>
+        <v>460</v>
       </c>
       <c r="D5" s="4">
         <f>January!D5+February!D5+March!D5+April!D5+May!D5+June!D5+July!D5+August!D5+September!D5+October!D5+November!D5+December!D5</f>
-        <v>-180</v>
+        <v>-199</v>
       </c>
       <c r="E5" s="29" t="str">
         <f t="shared" si="1"/>
@@ -1563,7 +1638,7 @@
       </c>
       <c r="G5" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.51 : 1</v>
+        <v>0.57 : 1</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1572,15 +1647,15 @@
       </c>
       <c r="B6" s="2">
         <f>January!B6+February!B6+March!B6+April!B6+May!B6+June!B6+July!B6+August!B6+September!B6+October!B6+November!B6+December!B6</f>
-        <v>4096</v>
+        <v>5463</v>
       </c>
       <c r="C6" s="2">
         <f>January!C6+February!C6+March!C6+April!C6+May!C6+June!C6+July!C6+August!C6+September!C6+October!C6+November!C6+December!C6</f>
-        <v>4346</v>
+        <v>5971</v>
       </c>
       <c r="D6" s="2">
         <f>January!D6+February!D6+March!D6+April!D6+May!D6+June!D6+July!D6+August!D6+September!D6+October!D6+November!D6+December!D6</f>
-        <v>-250</v>
+        <v>-508</v>
       </c>
       <c r="E6" s="28" t="str">
         <f t="shared" si="1"/>
@@ -1592,7 +1667,7 @@
       </c>
       <c r="G6" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.94 : 1</v>
+        <v>0.91 : 1</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1601,15 +1676,15 @@
       </c>
       <c r="B7" s="4">
         <f>January!B7+February!B7+March!B7+April!B7+May!B7+June!B7+July!B7+August!B7+September!B7+October!B7+November!B7+December!B7</f>
-        <v>752</v>
+        <v>1034</v>
       </c>
       <c r="C7" s="4">
         <f>January!C7+February!C7+March!C7+April!C7+May!C7+June!C7+July!C7+August!C7+September!C7+October!C7+November!C7+December!C7</f>
-        <v>706</v>
+        <v>887</v>
       </c>
       <c r="D7" s="4">
         <f>January!D7+February!D7+March!D7+April!D7+May!D7+June!D7+July!D7+August!D7+September!D7+October!D7+November!D7+December!D7</f>
-        <v>46</v>
+        <v>147</v>
       </c>
       <c r="E7" s="29" t="str">
         <f t="shared" si="1"/>
@@ -1621,7 +1696,7 @@
       </c>
       <c r="G7" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.07 : 1</v>
+        <v>1.17 : 1</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1630,15 +1705,15 @@
       </c>
       <c r="B8" s="2">
         <f>January!B8+February!B8+March!B8+April!B8+May!B8+June!B8+July!B8+August!B8+September!B8+October!B8+November!B8+December!B8</f>
-        <v>397</v>
+        <v>531</v>
       </c>
       <c r="C8" s="2">
         <f>January!C8+February!C8+March!C8+April!C8+May!C8+June!C8+July!C8+August!C8+September!C8+October!C8+November!C8+December!C8</f>
-        <v>587</v>
+        <v>724</v>
       </c>
       <c r="D8" s="2">
         <f>January!D8+February!D8+March!D8+April!D8+May!D8+June!D8+July!D8+August!D8+September!D8+October!D8+November!D8+December!D8</f>
-        <v>-190</v>
+        <v>-193</v>
       </c>
       <c r="E8" s="28" t="str">
         <f t="shared" si="1"/>
@@ -1650,7 +1725,7 @@
       </c>
       <c r="G8" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.68 : 1</v>
+        <v>0.73 : 1</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1659,15 +1734,15 @@
       </c>
       <c r="B9" s="4">
         <f>January!B9+February!B9+March!B9+April!B9+May!B9+June!B9+July!B9+August!B9+September!B9+October!B9+November!B9+December!B9</f>
-        <v>170</v>
+        <v>245</v>
       </c>
       <c r="C9" s="4">
         <f>January!C9+February!C9+March!C9+April!C9+May!C9+June!C9+July!C9+August!C9+September!C9+October!C9+November!C9+December!C9</f>
-        <v>248</v>
+        <v>306</v>
       </c>
       <c r="D9" s="4">
         <f>January!D9+February!D9+March!D9+April!D9+May!D9+June!D9+July!D9+August!D9+September!D9+October!D9+November!D9+December!D9</f>
-        <v>-78</v>
+        <v>-61</v>
       </c>
       <c r="E9" s="29" t="str">
         <f t="shared" si="1"/>
@@ -1679,7 +1754,7 @@
       </c>
       <c r="G9" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.69 : 1</v>
+        <v>0.8 : 1</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1688,15 +1763,15 @@
       </c>
       <c r="B10" s="2">
         <f>January!B10+February!B10+March!B10+April!B10+May!B10+June!B10+July!B10+August!B10+September!B10+October!B10+November!B10+December!B10</f>
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C10" s="2">
         <f>January!C10+February!C10+March!C10+April!C10+May!C10+June!C10+July!C10+August!C10+September!C10+October!C10+November!C10+December!C10</f>
-        <v>139</v>
+        <v>173</v>
       </c>
       <c r="D10" s="2">
         <f>January!D10+February!D10+March!D10+April!D10+May!D10+June!D10+July!D10+August!D10+September!D10+October!D10+November!D10+December!D10</f>
-        <v>-114</v>
+        <v>-142</v>
       </c>
       <c r="E10" s="28" t="str">
         <f t="shared" si="1"/>
@@ -1746,15 +1821,15 @@
       </c>
       <c r="B12" s="6">
         <f>January!B12+February!B12+March!B12+April!B12+May!B12+June!B12+July!B12+August!B12+September!B12+October!B12+November!B12+December!B12</f>
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="C12" s="6">
         <f>January!C12+February!C12+March!C12+April!C12+May!C12+June!C12+July!C12+August!C12+September!C12+October!C12+November!C12+December!C12</f>
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="D12" s="6">
         <f>January!D12+February!D12+March!D12+April!D12+May!D12+June!D12+July!D12+August!D12+September!D12+October!D12+November!D12+December!D12</f>
-        <v>-23</v>
+        <v>-28</v>
       </c>
       <c r="E12" s="30" t="str">
         <f t="shared" si="1"/>
@@ -1775,15 +1850,15 @@
       </c>
       <c r="B13" s="6">
         <f>January!B13+February!B13+March!B13+April!B13+May!B13+June!B13+July!B13+August!B13+September!B13+October!B13+November!B13+December!B13</f>
-        <v>369</v>
+        <v>460</v>
       </c>
       <c r="C13" s="6">
         <f>January!C13+February!C13+March!C13+April!C13+May!C13+June!C13+July!C13+August!C13+September!C13+October!C13+November!C13+December!C13</f>
-        <v>283</v>
+        <v>367</v>
       </c>
       <c r="D13" s="6">
         <f>January!D13+February!D13+March!D13+April!D13+May!D13+June!D13+July!D13+August!D13+September!D13+October!D13+November!D13+December!D13</f>
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="E13" s="30" t="str">
         <f t="shared" si="1"/>
@@ -1795,7 +1870,7 @@
       </c>
       <c r="G13" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>1.3 : 1</v>
+        <v>1.25 : 1</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1804,15 +1879,15 @@
       </c>
       <c r="B14" s="6">
         <f>January!B14+February!B14+March!B14+April!B14+May!B14+June!B14+July!B14+August!B14+September!B14+October!B14+November!B14+December!B14</f>
-        <v>440</v>
+        <v>569</v>
       </c>
       <c r="C14" s="6">
         <f>January!C14+February!C14+March!C14+April!C14+May!C14+June!C14+July!C14+August!C14+September!C14+October!C14+November!C14+December!C14</f>
-        <v>905</v>
+        <v>1163</v>
       </c>
       <c r="D14" s="6">
         <f>January!D14+February!D14+March!D14+April!D14+May!D14+June!D14+July!D14+August!D14+September!D14+October!D14+November!D14+December!D14</f>
-        <v>-465</v>
+        <v>-594</v>
       </c>
       <c r="E14" s="30" t="str">
         <f t="shared" si="1"/>
@@ -1833,15 +1908,15 @@
       </c>
       <c r="B15" s="6">
         <f>January!B15+February!B15+March!B15+April!B15+May!B15+June!B15+July!B15+August!B15+September!B15+October!B15+November!B15+December!B15</f>
-        <v>178</v>
+        <v>271</v>
       </c>
       <c r="C15" s="6">
         <f>January!C15+February!C15+March!C15+April!C15+May!C15+June!C15+July!C15+August!C15+September!C15+October!C15+November!C15+December!C15</f>
-        <v>279</v>
+        <v>376</v>
       </c>
       <c r="D15" s="6">
         <f>January!D15+February!D15+March!D15+April!D15+May!D15+June!D15+July!D15+August!D15+September!D15+October!D15+November!D15+December!D15</f>
-        <v>-101</v>
+        <v>-105</v>
       </c>
       <c r="E15" s="30" t="str">
         <f t="shared" si="1"/>
@@ -1853,7 +1928,7 @@
       </c>
       <c r="G15" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0.64 : 1</v>
+        <v>0.72 : 1</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1862,15 +1937,15 @@
       </c>
       <c r="B16" s="2">
         <f>January!B16+February!B16+March!B16+April!B16+May!B16+June!B16+July!B16+August!B16+September!B16+October!B16+November!B16+December!B16</f>
-        <v>99</v>
+        <v>131</v>
       </c>
       <c r="C16" s="2">
         <f>January!C16+February!C16+March!C16+April!C16+May!C16+June!C16+July!C16+August!C16+September!C16+October!C16+November!C16+December!C16</f>
-        <v>398</v>
+        <v>568</v>
       </c>
       <c r="D16" s="2">
         <f>January!D16+February!D16+March!D16+April!D16+May!D16+June!D16+July!D16+August!D16+September!D16+October!D16+November!D16+December!D16</f>
-        <v>-299</v>
+        <v>-437</v>
       </c>
       <c r="E16" s="28" t="str">
         <f t="shared" si="1"/>
@@ -1882,7 +1957,7 @@
       </c>
       <c r="G16" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.25 : 1</v>
+        <v>0.23 : 1</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1891,15 +1966,15 @@
       </c>
       <c r="B17" s="4">
         <f>January!B17+February!B17+March!B17+April!B17+May!B17+June!B17+July!B17+August!B17+September!B17+October!B17+November!B17+December!B17</f>
-        <v>1817</v>
+        <v>2429</v>
       </c>
       <c r="C17" s="4">
         <f>January!C17+February!C17+March!C17+April!C17+May!C17+June!C17+July!C17+August!C17+September!C17+October!C17+November!C17+December!C17</f>
-        <v>1500</v>
+        <v>1958</v>
       </c>
       <c r="D17" s="4">
         <f>January!D17+February!D17+March!D17+April!D17+May!D17+June!D17+July!D17+August!D17+September!D17+October!D17+November!D17+December!D17</f>
-        <v>317</v>
+        <v>471</v>
       </c>
       <c r="E17" s="29" t="str">
         <f t="shared" si="1"/>
@@ -1911,7 +1986,7 @@
       </c>
       <c r="G17" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.21 : 1</v>
+        <v>1.24 : 1</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1920,15 +1995,15 @@
       </c>
       <c r="B18" s="2">
         <f>January!B18+February!B18+March!B18+April!B18+May!B18+June!B18+July!B18+August!B18+September!B18+October!B18+November!B18+December!B18</f>
-        <v>389</v>
+        <v>561</v>
       </c>
       <c r="C18" s="2">
         <f>January!C18+February!C18+March!C18+April!C18+May!C18+June!C18+July!C18+August!C18+September!C18+October!C18+November!C18+December!C18</f>
-        <v>329</v>
+        <v>414</v>
       </c>
       <c r="D18" s="2">
         <f>January!D18+February!D18+March!D18+April!D18+May!D18+June!D18+July!D18+August!D18+September!D18+October!D18+November!D18+December!D18</f>
-        <v>60</v>
+        <v>147</v>
       </c>
       <c r="E18" s="28" t="str">
         <f t="shared" si="1"/>
@@ -1940,7 +2015,7 @@
       </c>
       <c r="G18" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.18 : 1</v>
+        <v>1.36 : 1</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1949,15 +2024,15 @@
       </c>
       <c r="B19" s="4">
         <f>January!B19+February!B19+March!B19+April!B19+May!B19+June!B19+July!B19+August!B19+September!B19+October!B19+November!B19+December!B19</f>
-        <v>2094</v>
+        <v>2729</v>
       </c>
       <c r="C19" s="4">
         <f>January!C19+February!C19+March!C19+April!C19+May!C19+June!C19+July!C19+August!C19+September!C19+October!C19+November!C19+December!C19</f>
-        <v>1077</v>
+        <v>1472</v>
       </c>
       <c r="D19" s="4">
         <f>January!D19+February!D19+March!D19+April!D19+May!D19+June!D19+July!D19+August!D19+September!D19+October!D19+November!D19+December!D19</f>
-        <v>1017</v>
+        <v>1257</v>
       </c>
       <c r="E19" s="29" t="str">
         <f t="shared" si="1"/>
@@ -1969,7 +2044,7 @@
       </c>
       <c r="G19" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.94 : 1</v>
+        <v>1.85 : 1</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1978,15 +2053,15 @@
       </c>
       <c r="B20" s="2">
         <f>January!B20+February!B20+March!B20+April!B20+May!B20+June!B20+July!B20+August!B20+September!B20+October!B20+November!B20+December!B20</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C20" s="2">
         <f>January!C20+February!C20+March!C20+April!C20+May!C20+June!C20+July!C20+August!C20+September!C20+October!C20+November!C20+December!C20</f>
-        <v>188</v>
+        <v>248</v>
       </c>
       <c r="D20" s="2">
         <f>January!D20+February!D20+March!D20+April!D20+May!D20+June!D20+July!D20+August!D20+September!D20+October!D20+November!D20+December!D20</f>
-        <v>-181</v>
+        <v>-240</v>
       </c>
       <c r="E20" s="28" t="str">
         <f t="shared" si="1"/>
@@ -1998,7 +2073,7 @@
       </c>
       <c r="G20" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.04 : 1</v>
+        <v>0.03 : 1</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2007,15 +2082,15 @@
       </c>
       <c r="B21" s="4">
         <f>January!B21+February!B21+March!B21+April!B21+May!B21+June!B21+July!B21+August!B21+September!B21+October!B21+November!B21+December!B21</f>
-        <v>1636</v>
+        <v>2142</v>
       </c>
       <c r="C21" s="4">
         <f>January!C21+February!C21+March!C21+April!C21+May!C21+June!C21+July!C21+August!C21+September!C21+October!C21+November!C21+December!C21</f>
-        <v>1284</v>
+        <v>1672</v>
       </c>
       <c r="D21" s="4">
         <f>January!D21+February!D21+March!D21+April!D21+May!D21+June!D21+July!D21+August!D21+September!D21+October!D21+November!D21+December!D21</f>
-        <v>352</v>
+        <v>470</v>
       </c>
       <c r="E21" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2027,7 +2102,7 @@
       </c>
       <c r="G21" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.27 : 1</v>
+        <v>1.28 : 1</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2036,15 +2111,15 @@
       </c>
       <c r="B22" s="2">
         <f>January!B22+February!B22+March!B22+April!B22+May!B22+June!B22+July!B22+August!B22+September!B22+October!B22+November!B22+December!B22</f>
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="C22" s="2">
         <f>January!C22+February!C22+March!C22+April!C22+May!C22+June!C22+July!C22+August!C22+September!C22+October!C22+November!C22+December!C22</f>
-        <v>250</v>
+        <v>322</v>
       </c>
       <c r="D22" s="2">
         <f>January!D22+February!D22+March!D22+April!D22+May!D22+June!D22+July!D22+August!D22+September!D22+October!D22+November!D22+December!D22</f>
-        <v>-172</v>
+        <v>-231</v>
       </c>
       <c r="E22" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2056,7 +2131,7 @@
       </c>
       <c r="G22" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.31 : 1</v>
+        <v>0.28 : 1</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2065,15 +2140,15 @@
       </c>
       <c r="B23" s="4">
         <f>January!B23+February!B23+March!B23+April!B23+May!B23+June!B23+July!B23+August!B23+September!B23+October!B23+November!B23+December!B23</f>
-        <v>2077</v>
+        <v>2788</v>
       </c>
       <c r="C23" s="4">
         <f>January!C23+February!C23+March!C23+April!C23+May!C23+June!C23+July!C23+August!C23+September!C23+October!C23+November!C23+December!C23</f>
-        <v>1630</v>
+        <v>2122</v>
       </c>
       <c r="D23" s="4">
         <f>January!D23+February!D23+March!D23+April!D23+May!D23+June!D23+July!D23+August!D23+September!D23+October!D23+November!D23+December!D23</f>
-        <v>447</v>
+        <v>666</v>
       </c>
       <c r="E23" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2085,7 +2160,7 @@
       </c>
       <c r="G23" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.27 : 1</v>
+        <v>1.31 : 1</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2094,15 +2169,15 @@
       </c>
       <c r="B24" s="2">
         <f>January!B24+February!B24+March!B24+April!B24+May!B24+June!B24+July!B24+August!B24+September!B24+October!B24+November!B24+December!B24</f>
-        <v>5755</v>
+        <v>7652</v>
       </c>
       <c r="C24" s="2">
         <f>January!C24+February!C24+March!C24+April!C24+May!C24+June!C24+July!C24+August!C24+September!C24+October!C24+November!C24+December!C24</f>
-        <v>4318</v>
+        <v>5633</v>
       </c>
       <c r="D24" s="2">
         <f>January!D24+February!D24+March!D24+April!D24+May!D24+June!D24+July!D24+August!D24+September!D24+October!D24+November!D24+December!D24</f>
-        <v>1437</v>
+        <v>2019</v>
       </c>
       <c r="E24" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2114,7 +2189,7 @@
       </c>
       <c r="G24" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.33 : 1</v>
+        <v>1.36 : 1</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2123,15 +2198,15 @@
       </c>
       <c r="B25" s="4">
         <f>January!B25+February!B25+March!B25+April!B25+May!B25+June!B25+July!B25+August!B25+September!B25+October!B25+November!B25+December!B25</f>
-        <v>555</v>
+        <v>714</v>
       </c>
       <c r="C25" s="4">
         <f>January!C25+February!C25+March!C25+April!C25+May!C25+June!C25+July!C25+August!C25+September!C25+October!C25+November!C25+December!C25</f>
-        <v>1000</v>
+        <v>1302</v>
       </c>
       <c r="D25" s="4">
         <f>January!D25+February!D25+March!D25+April!D25+May!D25+June!D25+July!D25+August!D25+September!D25+October!D25+November!D25+December!D25</f>
-        <v>-445</v>
+        <v>-588</v>
       </c>
       <c r="E25" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2143,7 +2218,7 @@
       </c>
       <c r="G25" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.56 : 1</v>
+        <v>0.55 : 1</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2181,15 +2256,15 @@
       </c>
       <c r="B27" s="4">
         <f>January!B27+February!B27+March!B27+April!B27+May!B27+June!B27+July!B27+August!B27+September!B27+October!B27+November!B27+December!B27</f>
-        <v>984</v>
+        <v>1254</v>
       </c>
       <c r="C27" s="4">
         <f>January!C27+February!C27+March!C27+April!C27+May!C27+June!C27+July!C27+August!C27+September!C27+October!C27+November!C27+December!C27</f>
-        <v>591</v>
+        <v>772</v>
       </c>
       <c r="D27" s="4">
         <f>January!D27+February!D27+March!D27+April!D27+May!D27+June!D27+July!D27+August!D27+September!D27+October!D27+November!D27+December!D27</f>
-        <v>393</v>
+        <v>482</v>
       </c>
       <c r="E27" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2201,7 +2276,7 @@
       </c>
       <c r="G27" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.66 : 1</v>
+        <v>1.62 : 1</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2210,15 +2285,15 @@
       </c>
       <c r="B28" s="2">
         <f>January!B28+February!B28+March!B28+April!B28+May!B28+June!B28+July!B28+August!B28+September!B28+October!B28+November!B28+December!B28</f>
-        <v>136</v>
+        <v>199</v>
       </c>
       <c r="C28" s="2">
         <f>January!C28+February!C28+March!C28+April!C28+May!C28+June!C28+July!C28+August!C28+September!C28+October!C28+November!C28+December!C28</f>
-        <v>256</v>
+        <v>331</v>
       </c>
       <c r="D28" s="2">
         <f>January!D28+February!D28+March!D28+April!D28+May!D28+June!D28+July!D28+August!D28+September!D28+October!D28+November!D28+December!D28</f>
-        <v>-120</v>
+        <v>-132</v>
       </c>
       <c r="E28" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2230,7 +2305,7 @@
       </c>
       <c r="G28" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.53 : 1</v>
+        <v>0.6 : 1</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2239,15 +2314,15 @@
       </c>
       <c r="B29" s="4">
         <f>January!B29+February!B29+March!B29+April!B29+May!B29+June!B29+July!B29+August!B29+September!B29+October!B29+November!B29+December!B29</f>
-        <v>1708</v>
+        <v>2165</v>
       </c>
       <c r="C29" s="4">
         <f>January!C29+February!C29+March!C29+April!C29+May!C29+June!C29+July!C29+August!C29+September!C29+October!C29+November!C29+December!C29</f>
-        <v>1456</v>
+        <v>1962</v>
       </c>
       <c r="D29" s="4">
         <f>January!D29+February!D29+March!D29+April!D29+May!D29+June!D29+July!D29+August!D29+September!D29+October!D29+November!D29+December!D29</f>
-        <v>252</v>
+        <v>203</v>
       </c>
       <c r="E29" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2259,7 +2334,7 @@
       </c>
       <c r="G29" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.17 : 1</v>
+        <v>1.1 : 1</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2268,15 +2343,15 @@
       </c>
       <c r="B30" s="2">
         <f>January!B30+February!B30+March!B30+April!B30+May!B30+June!B30+July!B30+August!B30+September!B30+October!B30+November!B30+December!B30</f>
-        <v>167</v>
+        <v>188</v>
       </c>
       <c r="C30" s="2">
         <f>January!C30+February!C30+March!C30+April!C30+May!C30+June!C30+July!C30+August!C30+September!C30+October!C30+November!C30+December!C30</f>
-        <v>81</v>
+        <v>112</v>
       </c>
       <c r="D30" s="2">
         <f>January!D30+February!D30+March!D30+April!D30+May!D30+June!D30+July!D30+August!D30+September!D30+October!D30+November!D30+December!D30</f>
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="E30" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2288,7 +2363,7 @@
       </c>
       <c r="G30" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>2.06 : 1</v>
+        <v>1.68 : 1</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2297,15 +2372,15 @@
       </c>
       <c r="B31" s="4">
         <f>January!B31+February!B31+March!B31+April!B31+May!B31+June!B31+July!B31+August!B31+September!B31+October!B31+November!B31+December!B31</f>
-        <v>252</v>
+        <v>363</v>
       </c>
       <c r="C31" s="4">
         <f>January!C31+February!C31+March!C31+April!C31+May!C31+June!C31+July!C31+August!C31+September!C31+October!C31+November!C31+December!C31</f>
-        <v>907</v>
+        <v>1220</v>
       </c>
       <c r="D31" s="4">
         <f>January!D31+February!D31+March!D31+April!D31+May!D31+June!D31+July!D31+August!D31+September!D31+October!D31+November!D31+December!D31</f>
-        <v>-655</v>
+        <v>-857</v>
       </c>
       <c r="E31" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2317,7 +2392,7 @@
       </c>
       <c r="G31" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.28 : 1</v>
+        <v>0.3 : 1</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2326,15 +2401,15 @@
       </c>
       <c r="B32" s="2">
         <f>January!B32+February!B32+March!B32+April!B32+May!B32+June!B32+July!B32+August!B32+September!B32+October!B32+November!B32+December!B32</f>
-        <v>1333</v>
+        <v>1737</v>
       </c>
       <c r="C32" s="2">
         <f>January!C32+February!C32+March!C32+April!C32+May!C32+June!C32+July!C32+August!C32+September!C32+October!C32+November!C32+December!C32</f>
-        <v>1958</v>
+        <v>2492</v>
       </c>
       <c r="D32" s="2">
         <f>January!D32+February!D32+March!D32+April!D32+May!D32+June!D32+July!D32+August!D32+September!D32+October!D32+November!D32+December!D32</f>
-        <v>-625</v>
+        <v>-755</v>
       </c>
       <c r="E32" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2346,7 +2421,7 @@
       </c>
       <c r="G32" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.68 : 1</v>
+        <v>0.7 : 1</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2355,15 +2430,15 @@
       </c>
       <c r="B33" s="4">
         <f>January!B33+February!B33+March!B33+April!B33+May!B33+June!B33+July!B33+August!B33+September!B33+October!B33+November!B33+December!B33</f>
-        <v>1451</v>
+        <v>1839</v>
       </c>
       <c r="C33" s="4">
         <f>January!C33+February!C33+March!C33+April!C33+May!C33+June!C33+July!C33+August!C33+September!C33+October!C33+November!C33+December!C33</f>
-        <v>1575</v>
+        <v>2068</v>
       </c>
       <c r="D33" s="4">
         <f>January!D33+February!D33+March!D33+April!D33+May!D33+June!D33+July!D33+August!D33+September!D33+October!D33+November!D33+December!D33</f>
-        <v>-124</v>
+        <v>-229</v>
       </c>
       <c r="E33" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2375,7 +2450,7 @@
       </c>
       <c r="G33" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.92 : 1</v>
+        <v>0.89 : 1</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2384,15 +2459,15 @@
       </c>
       <c r="B34" s="2">
         <f>January!B34+February!B34+March!B34+April!B34+May!B34+June!B34+July!B34+August!B34+September!B34+October!B34+November!B34+December!B34</f>
-        <v>734</v>
+        <v>956</v>
       </c>
       <c r="C34" s="2">
         <f>January!C34+February!C34+March!C34+April!C34+May!C34+June!C34+July!C34+August!C34+September!C34+October!C34+November!C34+December!C34</f>
-        <v>415</v>
+        <v>544</v>
       </c>
       <c r="D34" s="2">
         <f>January!D34+February!D34+March!D34+April!D34+May!D34+June!D34+July!D34+August!D34+September!D34+October!D34+November!D34+December!D34</f>
-        <v>319</v>
+        <v>412</v>
       </c>
       <c r="E34" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2404,7 +2479,7 @@
       </c>
       <c r="G34" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.77 : 1</v>
+        <v>1.76 : 1</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2413,15 +2488,15 @@
       </c>
       <c r="B35" s="4">
         <f>January!B35+February!B35+March!B35+April!B35+May!B35+June!B35+July!B35+August!B35+September!B35+October!B35+November!B35+December!B35</f>
-        <v>2701</v>
+        <v>3590</v>
       </c>
       <c r="C35" s="4">
         <f>January!C35+February!C35+March!C35+April!C35+May!C35+June!C35+July!C35+August!C35+September!C35+October!C35+November!C35+December!C35</f>
-        <v>3230</v>
+        <v>4215</v>
       </c>
       <c r="D35" s="4">
         <f>January!D35+February!D35+March!D35+April!D35+May!D35+June!D35+July!D35+August!D35+September!D35+October!D35+November!D35+December!D35</f>
-        <v>-529</v>
+        <v>-625</v>
       </c>
       <c r="E35" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2433,7 +2508,7 @@
       </c>
       <c r="G35" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.84 : 1</v>
+        <v>0.85 : 1</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2442,15 +2517,15 @@
       </c>
       <c r="B36" s="2">
         <f>January!B36+February!B36+March!B36+April!B36+May!B36+June!B36+July!B36+August!B36+September!B36+October!B36+November!B36+December!B36</f>
-        <v>669</v>
+        <v>894</v>
       </c>
       <c r="C36" s="2">
         <f>January!C36+February!C36+March!C36+April!C36+May!C36+June!C36+July!C36+August!C36+September!C36+October!C36+November!C36+December!C36</f>
-        <v>1641</v>
+        <v>2082</v>
       </c>
       <c r="D36" s="2">
         <f>January!D36+February!D36+March!D36+April!D36+May!D36+June!D36+July!D36+August!D36+September!D36+October!D36+November!D36+December!D36</f>
-        <v>-972</v>
+        <v>-1188</v>
       </c>
       <c r="E36" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2462,7 +2537,7 @@
       </c>
       <c r="G36" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.41 : 1</v>
+        <v>0.43 : 1</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2471,15 +2546,15 @@
       </c>
       <c r="B37" s="4">
         <f>January!B37+February!B37+March!B37+April!B37+May!B37+June!B37+July!B37+August!B37+September!B37+October!B37+November!B37+December!B37</f>
-        <v>1574</v>
+        <v>2051</v>
       </c>
       <c r="C37" s="4">
         <f>January!C37+February!C37+March!C37+April!C37+May!C37+June!C37+July!C37+August!C37+September!C37+October!C37+November!C37+December!C37</f>
-        <v>1163</v>
+        <v>1526</v>
       </c>
       <c r="D37" s="4">
         <f>January!D37+February!D37+March!D37+April!D37+May!D37+June!D37+July!D37+August!D37+September!D37+October!D37+November!D37+December!D37</f>
-        <v>411</v>
+        <v>525</v>
       </c>
       <c r="E37" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2491,7 +2566,7 @@
       </c>
       <c r="G37" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.35 : 1</v>
+        <v>1.34 : 1</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2500,15 +2575,15 @@
       </c>
       <c r="B38" s="2">
         <f>January!B38+February!B38+March!B38+April!B38+May!B38+June!B38+July!B38+August!B38+September!B38+October!B38+November!B38+December!B38</f>
-        <v>187</v>
+        <v>220</v>
       </c>
       <c r="C38" s="2">
         <f>January!C38+February!C38+March!C38+April!C38+May!C38+June!C38+July!C38+August!C38+September!C38+October!C38+November!C38+December!C38</f>
-        <v>500</v>
+        <v>650</v>
       </c>
       <c r="D38" s="2">
         <f>January!D38+February!D38+March!D38+April!D38+May!D38+June!D38+July!D38+August!D38+September!D38+October!D38+November!D38+December!D38</f>
-        <v>-313</v>
+        <v>-430</v>
       </c>
       <c r="E38" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2520,7 +2595,7 @@
       </c>
       <c r="G38" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.37 : 1</v>
+        <v>0.34 : 1</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2529,15 +2604,15 @@
       </c>
       <c r="B39" s="8">
         <f>January!B39+February!B39+March!B39+April!B39+May!B39+June!B39+July!B39+August!B39+September!B39+October!B39+November!B39+December!B39</f>
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C39" s="8">
         <f>January!C39+February!C39+March!C39+April!C39+May!C39+June!C39+July!C39+August!C39+September!C39+October!C39+November!C39+December!C39</f>
-        <v>193</v>
+        <v>249</v>
       </c>
       <c r="D39" s="8">
         <f>January!D39+February!D39+March!D39+April!D39+May!D39+June!D39+July!D39+August!D39+September!D39+October!D39+November!D39+December!D39</f>
-        <v>-53</v>
+        <v>-107</v>
       </c>
       <c r="E39" s="31" t="str">
         <f t="shared" si="1"/>
@@ -2549,7 +2624,7 @@
       </c>
       <c r="G39" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>0.73 : 1</v>
+        <v>0.57 : 1</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2558,15 +2633,15 @@
       </c>
       <c r="B40" s="8">
         <f>January!B40+February!B40+March!B40+April!B40+May!B40+June!B40+July!B40+August!B40+September!B40+October!B40+November!B40+December!B40</f>
-        <v>241</v>
+        <v>333</v>
       </c>
       <c r="C40" s="8">
         <f>January!C40+February!C40+March!C40+April!C40+May!C40+June!C40+July!C40+August!C40+September!C40+October!C40+November!C40+December!C40</f>
-        <v>367</v>
+        <v>515</v>
       </c>
       <c r="D40" s="8">
         <f>January!D40+February!D40+March!D40+April!D40+May!D40+June!D40+July!D40+August!D40+September!D40+October!D40+November!D40+December!D40</f>
-        <v>-126</v>
+        <v>-182</v>
       </c>
       <c r="E40" s="31" t="str">
         <f t="shared" si="1"/>
@@ -2578,7 +2653,7 @@
       </c>
       <c r="G40" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>0.66 : 1</v>
+        <v>0.65 : 1</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2587,27 +2662,27 @@
       </c>
       <c r="B41" s="8">
         <f>January!B41+February!B41+March!B41+April!B41+May!B41+June!B41+July!B41+August!B41+September!B41+October!B41+November!B41+December!B41</f>
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C41" s="8">
         <f>January!C41+February!C41+March!C41+April!C41+May!C41+June!C41+July!C41+August!C41+September!C41+October!C41+November!C41+December!C41</f>
-        <v>64</v>
+        <v>95</v>
       </c>
       <c r="D41" s="8">
         <f>January!D41+February!D41+March!D41+April!D41+May!D41+June!D41+July!D41+August!D41+September!D41+October!D41+November!D41+December!D41</f>
-        <v>4</v>
+        <v>-22</v>
       </c>
       <c r="E41" s="31" t="str">
         <f t="shared" si="1"/>
-        <v>We borrowed more than we lent this year</v>
+        <v/>
       </c>
       <c r="F41" s="31" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>We lent more than we borrowed this year</v>
       </c>
       <c r="G41" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>1.06 : 1</v>
+        <v>0.77 : 1</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2616,15 +2691,15 @@
       </c>
       <c r="B42" s="8">
         <f>January!B42+February!B42+March!B42+April!B42+May!B42+June!B42+July!B42+August!B42+September!B42+October!B42+November!B42+December!B42</f>
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C42" s="8">
         <f>January!C42+February!C42+March!C42+April!C42+May!C42+June!C42+July!C42+August!C42+September!C42+October!C42+November!C42+December!C42</f>
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D42" s="8">
         <f>January!D42+February!D42+March!D42+April!D42+May!D42+June!D42+July!D42+August!D42+September!D42+October!D42+November!D42+December!D42</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E42" s="31" t="str">
         <f t="shared" si="1"/>
@@ -2636,7 +2711,7 @@
       </c>
       <c r="G42" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>1.21 : 1</v>
+        <v>1.07 : 1</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2649,11 +2724,11 @@
       </c>
       <c r="C43" s="8">
         <f>January!C43+February!C43+March!C43+April!C43+May!C43+June!C43+July!C43+August!C43+September!C43+October!C43+November!C43+December!C43</f>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D43" s="8">
         <f>January!D43+February!D43+March!D43+April!D43+May!D43+June!D43+July!D43+August!D43+September!D43+October!D43+November!D43+December!D43</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E43" s="31" t="str">
         <f t="shared" si="1"/>
@@ -2665,7 +2740,7 @@
       </c>
       <c r="G43" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>1.42 : 1</v>
+        <v>1.38 : 1</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2674,15 +2749,15 @@
       </c>
       <c r="B44" s="4">
         <f>January!B44+February!B44+March!B44+April!B44+May!B44+June!B44+July!B44+August!B44+September!B44+October!B44+November!B44+December!B44</f>
-        <v>356</v>
+        <v>486</v>
       </c>
       <c r="C44" s="4">
         <f>January!C44+February!C44+March!C44+April!C44+May!C44+June!C44+July!C44+August!C44+September!C44+October!C44+November!C44+December!C44</f>
-        <v>248</v>
+        <v>321</v>
       </c>
       <c r="D44" s="4">
         <f>January!D44+February!D44+March!D44+April!D44+May!D44+June!D44+July!D44+August!D44+September!D44+October!D44+November!D44+December!D44</f>
-        <v>108</v>
+        <v>165</v>
       </c>
       <c r="E44" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2694,7 +2769,7 @@
       </c>
       <c r="G44" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.44 : 1</v>
+        <v>1.51 : 1</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2703,15 +2778,15 @@
       </c>
       <c r="B45" s="2">
         <f>January!B45+February!B45+March!B45+April!B45+May!B45+June!B45+July!B45+August!B45+September!B45+October!B45+November!B45+December!B45</f>
-        <v>197</v>
+        <v>271</v>
       </c>
       <c r="C45" s="2">
         <f>January!C45+February!C45+March!C45+April!C45+May!C45+June!C45+July!C45+August!C45+September!C45+October!C45+November!C45+December!C45</f>
-        <v>461</v>
+        <v>632</v>
       </c>
       <c r="D45" s="2">
         <f>January!D45+February!D45+March!D45+April!D45+May!D45+June!D45+July!D45+August!D45+September!D45+October!D45+November!D45+December!D45</f>
-        <v>-264</v>
+        <v>-361</v>
       </c>
       <c r="E45" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2732,15 +2807,15 @@
       </c>
       <c r="B46" s="4">
         <f>January!B46+February!B46+March!B46+April!B46+May!B46+June!B46+July!B46+August!B46+September!B46+October!B46+November!B46+December!B46</f>
-        <v>1332</v>
+        <v>1700</v>
       </c>
       <c r="C46" s="4">
         <f>January!C46+February!C46+March!C46+April!C46+May!C46+June!C46+July!C46+August!C46+September!C46+October!C46+November!C46+December!C46</f>
-        <v>1881</v>
+        <v>2440</v>
       </c>
       <c r="D46" s="4">
         <f>January!D46+February!D46+March!D46+April!D46+May!D46+June!D46+July!D46+August!D46+September!D46+October!D46+November!D46+December!D46</f>
-        <v>-549</v>
+        <v>-740</v>
       </c>
       <c r="E46" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2752,7 +2827,7 @@
       </c>
       <c r="G46" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.71 : 1</v>
+        <v>0.7 : 1</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2761,15 +2836,15 @@
       </c>
       <c r="B47" s="2">
         <f>January!B47+February!B47+March!B47+April!B47+May!B47+June!B47+July!B47+August!B47+September!B47+October!B47+November!B47+December!B47</f>
-        <v>2884</v>
+        <v>3799</v>
       </c>
       <c r="C47" s="2">
         <f>January!C47+February!C47+March!C47+April!C47+May!C47+June!C47+July!C47+August!C47+September!C47+October!C47+November!C47+December!C47</f>
-        <v>2287</v>
+        <v>2965</v>
       </c>
       <c r="D47" s="2">
         <f>January!D47+February!D47+March!D47+April!D47+May!D47+June!D47+July!D47+August!D47+September!D47+October!D47+November!D47+December!D47</f>
-        <v>597</v>
+        <v>834</v>
       </c>
       <c r="E47" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2781,7 +2856,7 @@
       </c>
       <c r="G47" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.26 : 1</v>
+        <v>1.28 : 1</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2790,15 +2865,15 @@
       </c>
       <c r="B48" s="4">
         <f>January!B48+February!B48+March!B48+April!B48+May!B48+June!B48+July!B48+August!B48+September!B48+October!B48+November!B48+December!B48</f>
-        <v>741</v>
+        <v>891</v>
       </c>
       <c r="C48" s="4">
         <f>January!C48+February!C48+March!C48+April!C48+May!C48+June!C48+July!C48+August!C48+September!C48+October!C48+November!C48+December!C48</f>
-        <v>1977</v>
+        <v>2582</v>
       </c>
       <c r="D48" s="4">
         <f>January!D48+February!D48+March!D48+April!D48+May!D48+June!D48+July!D48+August!D48+September!D48+October!D48+November!D48+December!D48</f>
-        <v>-1236</v>
+        <v>-1691</v>
       </c>
       <c r="E48" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2810,7 +2885,7 @@
       </c>
       <c r="G48" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.37 : 1</v>
+        <v>0.35 : 1</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2819,15 +2894,15 @@
       </c>
       <c r="B49" s="2">
         <f>January!B49+February!B49+March!B49+April!B49+May!B49+June!B49+July!B49+August!B49+September!B49+October!B49+November!B49+December!B49</f>
-        <v>1258</v>
+        <v>1607</v>
       </c>
       <c r="C49" s="2">
         <f>January!C49+February!C49+March!C49+April!C49+May!C49+June!C49+July!C49+August!C49+September!C49+October!C49+November!C49+December!C49</f>
-        <v>601</v>
+        <v>770</v>
       </c>
       <c r="D49" s="2">
         <f>January!D49+February!D49+March!D49+April!D49+May!D49+June!D49+July!D49+August!D49+September!D49+October!D49+November!D49+December!D49</f>
-        <v>657</v>
+        <v>837</v>
       </c>
       <c r="E49" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2848,15 +2923,15 @@
       </c>
       <c r="B50" s="4">
         <f>January!B50+February!B50+March!B50+April!B50+May!B50+June!B50+July!B50+August!B50+September!B50+October!B50+November!B50+December!B50</f>
-        <v>2586</v>
+        <v>3431</v>
       </c>
       <c r="C50" s="4">
         <f>January!C50+February!C50+March!C50+April!C50+May!C50+June!C50+July!C50+August!C50+September!C50+October!C50+November!C50+December!C50</f>
-        <v>1695</v>
+        <v>2234</v>
       </c>
       <c r="D50" s="4">
         <f>January!D50+February!D50+March!D50+April!D50+May!D50+June!D50+July!D50+August!D50+September!D50+October!D50+November!D50+December!D50</f>
-        <v>891</v>
+        <v>1197</v>
       </c>
       <c r="E50" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2868,7 +2943,7 @@
       </c>
       <c r="G50" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.53 : 1</v>
+        <v>1.54 : 1</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2877,15 +2952,15 @@
       </c>
       <c r="B51" s="2">
         <f>January!B51+February!B51+March!B51+April!B51+May!B51+June!B51+July!B51+August!B51+September!B51+October!B51+November!B51+December!B51</f>
-        <v>735</v>
+        <v>1035</v>
       </c>
       <c r="C51" s="2">
         <f>January!C51+February!C51+March!C51+April!C51+May!C51+June!C51+July!C51+August!C51+September!C51+October!C51+November!C51+December!C51</f>
-        <v>303</v>
+        <v>388</v>
       </c>
       <c r="D51" s="2">
         <f>January!D51+February!D51+March!D51+April!D51+May!D51+June!D51+July!D51+August!D51+September!D51+October!D51+November!D51+December!D51</f>
-        <v>432</v>
+        <v>647</v>
       </c>
       <c r="E51" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2897,7 +2972,7 @@
       </c>
       <c r="G51" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>2.43 : 1</v>
+        <v>2.67 : 1</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2906,15 +2981,15 @@
       </c>
       <c r="B52" s="4">
         <f>January!B52+February!B52+March!B52+April!B52+May!B52+June!B52+July!B52+August!B52+September!B52+October!B52+November!B52+December!B52</f>
-        <v>1619</v>
+        <v>2133</v>
       </c>
       <c r="C52" s="4">
         <f>January!C52+February!C52+March!C52+April!C52+May!C52+June!C52+July!C52+August!C52+September!C52+October!C52+November!C52+December!C52</f>
-        <v>1737</v>
+        <v>2221</v>
       </c>
       <c r="D52" s="4">
         <f>January!D52+February!D52+March!D52+April!D52+May!D52+June!D52+July!D52+August!D52+September!D52+October!D52+November!D52+December!D52</f>
-        <v>-118</v>
+        <v>-88</v>
       </c>
       <c r="E52" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2926,7 +3001,7 @@
       </c>
       <c r="G52" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.93 : 1</v>
+        <v>0.96 : 1</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2935,15 +3010,15 @@
       </c>
       <c r="B53" s="2">
         <f>January!B53+February!B53+March!B53+April!B53+May!B53+June!B53+July!B53+August!B53+September!B53+October!B53+November!B53+December!B53</f>
-        <v>303</v>
+        <v>400</v>
       </c>
       <c r="C53" s="2">
         <f>January!C53+February!C53+March!C53+April!C53+May!C53+June!C53+July!C53+August!C53+September!C53+October!C53+November!C53+December!C53</f>
-        <v>587</v>
+        <v>786</v>
       </c>
       <c r="D53" s="2">
         <f>January!D53+February!D53+March!D53+April!D53+May!D53+June!D53+July!D53+August!D53+September!D53+October!D53+November!D53+December!D53</f>
-        <v>-284</v>
+        <v>-386</v>
       </c>
       <c r="E53" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2955,7 +3030,7 @@
       </c>
       <c r="G53" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.52 : 1</v>
+        <v>0.51 : 1</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2964,15 +3039,15 @@
       </c>
       <c r="B54" s="4">
         <f>January!B54+February!B54+March!B54+April!B54+May!B54+June!B54+July!B54+August!B54+September!B54+October!B54+November!B54+December!B54</f>
-        <v>106</v>
+        <v>129</v>
       </c>
       <c r="C54" s="4">
         <f>January!C54+February!C54+March!C54+April!C54+May!C54+June!C54+July!C54+August!C54+September!C54+October!C54+November!C54+December!C54</f>
-        <v>758</v>
+        <v>987</v>
       </c>
       <c r="D54" s="4">
         <f>January!D54+February!D54+March!D54+April!D54+May!D54+June!D54+July!D54+August!D54+September!D54+October!D54+November!D54+December!D54</f>
-        <v>-652</v>
+        <v>-858</v>
       </c>
       <c r="E54" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2984,7 +3059,7 @@
       </c>
       <c r="G54" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.14 : 1</v>
+        <v>0.13 : 1</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2993,15 +3068,15 @@
       </c>
       <c r="B55" s="10">
         <f>January!B55+February!B55+March!B55+April!B55+May!B55+June!B55+July!B55+August!B55+September!B55+October!B55+November!B55+December!B55</f>
-        <v>452</v>
+        <v>603</v>
       </c>
       <c r="C55" s="10">
         <f>January!C55+February!C55+March!C55+April!C55+May!C55+June!C55+July!C55+August!C55+September!C55+October!C55+November!C55+December!C55</f>
-        <v>338</v>
+        <v>524</v>
       </c>
       <c r="D55" s="10">
         <f>January!D55+February!D55+March!D55+April!D55+May!D55+June!D55+July!D55+August!D55+September!D55+October!D55+November!D55+December!D55</f>
-        <v>114</v>
+        <v>79</v>
       </c>
       <c r="E55" s="32" t="str">
         <f t="shared" si="1"/>
@@ -3013,7 +3088,7 @@
       </c>
       <c r="G55" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>1.34 : 1</v>
+        <v>1.15 : 1</v>
       </c>
     </row>
   </sheetData>
@@ -9305,108 +9380,204 @@
       <c r="A2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="28"/>
+      <c r="B2" s="18">
+        <v>1231</v>
+      </c>
+      <c r="C2" s="18">
+        <v>1125</v>
+      </c>
+      <c r="D2" s="18">
+        <v>106</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F2" s="28"/>
-      <c r="G2" s="3"/>
+      <c r="G2" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
+      <c r="B3" s="21">
+        <v>448</v>
+      </c>
+      <c r="C3" s="21">
+        <v>532</v>
+      </c>
+      <c r="D3" s="21">
+        <v>-84</v>
+      </c>
       <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="5"/>
+      <c r="F3" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="28"/>
+      <c r="B4" s="18">
+        <v>1362</v>
+      </c>
+      <c r="C4" s="18">
+        <v>1221</v>
+      </c>
+      <c r="D4" s="18">
+        <v>141</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F4" s="28"/>
-      <c r="G4" s="3"/>
+      <c r="G4" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
+      <c r="B5" s="21">
+        <v>73</v>
+      </c>
+      <c r="C5" s="21">
+        <v>92</v>
+      </c>
+      <c r="D5" s="21">
+        <v>-19</v>
+      </c>
       <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="5"/>
+      <c r="F5" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
+      <c r="B6" s="18">
+        <v>1367</v>
+      </c>
+      <c r="C6" s="18">
+        <v>1625</v>
+      </c>
+      <c r="D6" s="18">
+        <v>-258</v>
+      </c>
       <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="3"/>
+      <c r="F6" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="29"/>
+      <c r="B7" s="21">
+        <v>282</v>
+      </c>
+      <c r="C7" s="21">
+        <v>181</v>
+      </c>
+      <c r="D7" s="21">
+        <v>101</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F7" s="29"/>
-      <c r="G7" s="5"/>
+      <c r="G7" s="5" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
+      <c r="B8" s="18">
+        <v>134</v>
+      </c>
+      <c r="C8" s="18">
+        <v>137</v>
+      </c>
+      <c r="D8" s="18">
+        <v>-3</v>
+      </c>
       <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="3"/>
+      <c r="F8" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="29"/>
+      <c r="B9" s="21">
+        <v>75</v>
+      </c>
+      <c r="C9" s="21">
+        <v>58</v>
+      </c>
+      <c r="D9" s="21">
+        <v>17</v>
+      </c>
+      <c r="E9" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F9" s="29"/>
-      <c r="G9" s="5"/>
+      <c r="G9" s="5" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
+      <c r="B10" s="18">
+        <v>6</v>
+      </c>
+      <c r="C10" s="18">
+        <v>34</v>
+      </c>
+      <c r="D10" s="18">
+        <v>-28</v>
+      </c>
       <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="3"/>
+      <c r="F10" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
+      <c r="B11" s="21">
+        <v>0</v>
+      </c>
+      <c r="C11" s="21">
+        <v>0</v>
+      </c>
+      <c r="D11" s="21">
+        <v>0</v>
+      </c>
       <c r="E11" s="29"/>
       <c r="F11" s="29"/>
       <c r="G11" s="5"/>
@@ -9415,163 +9586,309 @@
       <c r="A12" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
+      <c r="B12" s="23">
+        <v>13</v>
+      </c>
+      <c r="C12" s="23">
+        <v>18</v>
+      </c>
+      <c r="D12" s="23">
+        <v>-5</v>
+      </c>
       <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="7"/>
+      <c r="F12" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="30"/>
+      <c r="B13" s="23">
+        <v>91</v>
+      </c>
+      <c r="C13" s="23">
+        <v>84</v>
+      </c>
+      <c r="D13" s="23">
+        <v>7</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>61</v>
+      </c>
       <c r="F13" s="30"/>
-      <c r="G13" s="7"/>
+      <c r="G13" s="7" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
+      <c r="B14" s="23">
+        <v>129</v>
+      </c>
+      <c r="C14" s="23">
+        <v>258</v>
+      </c>
+      <c r="D14" s="23">
+        <v>-129</v>
+      </c>
       <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="7"/>
+      <c r="F14" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
+      <c r="B15" s="23">
+        <v>93</v>
+      </c>
+      <c r="C15" s="23">
+        <v>97</v>
+      </c>
+      <c r="D15" s="23">
+        <v>-4</v>
+      </c>
       <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="7"/>
+      <c r="F15" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
+      <c r="B16" s="18">
+        <v>32</v>
+      </c>
+      <c r="C16" s="18">
+        <v>170</v>
+      </c>
+      <c r="D16" s="18">
+        <v>-138</v>
+      </c>
       <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="3"/>
+      <c r="F16" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="29"/>
+      <c r="B17" s="21">
+        <v>612</v>
+      </c>
+      <c r="C17" s="21">
+        <v>458</v>
+      </c>
+      <c r="D17" s="21">
+        <v>154</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F17" s="29"/>
-      <c r="G17" s="5"/>
+      <c r="G17" s="5" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="28"/>
+      <c r="B18" s="18">
+        <v>172</v>
+      </c>
+      <c r="C18" s="18">
+        <v>85</v>
+      </c>
+      <c r="D18" s="18">
+        <v>87</v>
+      </c>
+      <c r="E18" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F18" s="28"/>
-      <c r="G18" s="3"/>
+      <c r="G18" s="3" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="29"/>
+      <c r="B19" s="21">
+        <v>635</v>
+      </c>
+      <c r="C19" s="21">
+        <v>395</v>
+      </c>
+      <c r="D19" s="21">
+        <v>240</v>
+      </c>
+      <c r="E19" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F19" s="29"/>
-      <c r="G19" s="5"/>
+      <c r="G19" s="5" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
+      <c r="B20" s="18">
+        <v>1</v>
+      </c>
+      <c r="C20" s="18">
+        <v>60</v>
+      </c>
+      <c r="D20" s="18">
+        <v>-59</v>
+      </c>
       <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="3"/>
+      <c r="F20" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="29"/>
+      <c r="B21" s="21">
+        <v>506</v>
+      </c>
+      <c r="C21" s="21">
+        <v>388</v>
+      </c>
+      <c r="D21" s="21">
+        <v>118</v>
+      </c>
+      <c r="E21" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F21" s="29"/>
-      <c r="G21" s="5"/>
+      <c r="G21" s="5" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
+      <c r="B22" s="18">
+        <v>13</v>
+      </c>
+      <c r="C22" s="18">
+        <v>72</v>
+      </c>
+      <c r="D22" s="18">
+        <v>-59</v>
+      </c>
       <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="3"/>
+      <c r="F22" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="29"/>
+      <c r="B23" s="21">
+        <v>711</v>
+      </c>
+      <c r="C23" s="21">
+        <v>492</v>
+      </c>
+      <c r="D23" s="21">
+        <v>219</v>
+      </c>
+      <c r="E23" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F23" s="29"/>
-      <c r="G23" s="5"/>
+      <c r="G23" s="5" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="28"/>
+      <c r="B24" s="18">
+        <v>1897</v>
+      </c>
+      <c r="C24" s="18">
+        <v>1315</v>
+      </c>
+      <c r="D24" s="18">
+        <v>582</v>
+      </c>
+      <c r="E24" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F24" s="28"/>
-      <c r="G24" s="3"/>
+      <c r="G24" s="3" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
+      <c r="B25" s="21">
+        <v>159</v>
+      </c>
+      <c r="C25" s="21">
+        <v>302</v>
+      </c>
+      <c r="D25" s="21">
+        <v>-143</v>
+      </c>
       <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="5"/>
+      <c r="F25" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="26" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
+      <c r="B26" s="18">
+        <v>0</v>
+      </c>
+      <c r="C26" s="18">
+        <v>0</v>
+      </c>
+      <c r="D26" s="18">
+        <v>0</v>
+      </c>
       <c r="E26" s="28"/>
       <c r="F26" s="28"/>
       <c r="G26" s="3"/>
@@ -9580,320 +9897,610 @@
       <c r="A27" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="29"/>
+      <c r="B27" s="21">
+        <v>270</v>
+      </c>
+      <c r="C27" s="21">
+        <v>181</v>
+      </c>
+      <c r="D27" s="21">
+        <v>89</v>
+      </c>
+      <c r="E27" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F27" s="29"/>
-      <c r="G27" s="5"/>
+      <c r="G27" s="5" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
+      <c r="B28" s="18">
+        <v>63</v>
+      </c>
+      <c r="C28" s="18">
+        <v>75</v>
+      </c>
+      <c r="D28" s="18">
+        <v>-12</v>
+      </c>
       <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="3"/>
+      <c r="F28" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
+      <c r="B29" s="21">
+        <v>457</v>
+      </c>
+      <c r="C29" s="21">
+        <v>506</v>
+      </c>
+      <c r="D29" s="21">
+        <v>-49</v>
+      </c>
       <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="5"/>
+      <c r="F29" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="30" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
+      <c r="B30" s="18">
+        <v>21</v>
+      </c>
+      <c r="C30" s="18">
+        <v>31</v>
+      </c>
+      <c r="D30" s="18">
+        <v>-10</v>
+      </c>
       <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="3"/>
+      <c r="F30" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
+      <c r="B31" s="21">
+        <v>111</v>
+      </c>
+      <c r="C31" s="21">
+        <v>313</v>
+      </c>
+      <c r="D31" s="21">
+        <v>-202</v>
+      </c>
       <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="5"/>
+      <c r="F31" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="32" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
+      <c r="B32" s="18">
+        <v>404</v>
+      </c>
+      <c r="C32" s="18">
+        <v>534</v>
+      </c>
+      <c r="D32" s="18">
+        <v>-130</v>
+      </c>
       <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="3"/>
+      <c r="F32" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="33" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
+      <c r="B33" s="21">
+        <v>388</v>
+      </c>
+      <c r="C33" s="21">
+        <v>493</v>
+      </c>
+      <c r="D33" s="21">
+        <v>-105</v>
+      </c>
       <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="5"/>
+      <c r="F33" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="34" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="28"/>
+      <c r="B34" s="18">
+        <v>222</v>
+      </c>
+      <c r="C34" s="18">
+        <v>129</v>
+      </c>
+      <c r="D34" s="18">
+        <v>93</v>
+      </c>
+      <c r="E34" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F34" s="28"/>
-      <c r="G34" s="3"/>
+      <c r="G34" s="3" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
+      <c r="B35" s="21">
+        <v>889</v>
+      </c>
+      <c r="C35" s="21">
+        <v>985</v>
+      </c>
+      <c r="D35" s="21">
+        <v>-96</v>
+      </c>
       <c r="E35" s="29"/>
-      <c r="F35" s="29"/>
-      <c r="G35" s="5"/>
+      <c r="F35" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="36" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
+      <c r="B36" s="18">
+        <v>225</v>
+      </c>
+      <c r="C36" s="18">
+        <v>441</v>
+      </c>
+      <c r="D36" s="18">
+        <v>-216</v>
+      </c>
       <c r="E36" s="28"/>
-      <c r="F36" s="28"/>
-      <c r="G36" s="3"/>
+      <c r="F36" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="29"/>
+      <c r="B37" s="21">
+        <v>477</v>
+      </c>
+      <c r="C37" s="21">
+        <v>363</v>
+      </c>
+      <c r="D37" s="21">
+        <v>114</v>
+      </c>
+      <c r="E37" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F37" s="29"/>
-      <c r="G37" s="5"/>
+      <c r="G37" s="5" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
+      <c r="B38" s="18">
+        <v>33</v>
+      </c>
+      <c r="C38" s="18">
+        <v>150</v>
+      </c>
+      <c r="D38" s="18">
+        <v>-117</v>
+      </c>
       <c r="E38" s="28"/>
-      <c r="F38" s="28"/>
-      <c r="G38" s="3"/>
+      <c r="F38" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="B39" s="25"/>
-      <c r="C39" s="25"/>
-      <c r="D39" s="25"/>
+      <c r="B39" s="25">
+        <v>2</v>
+      </c>
+      <c r="C39" s="25">
+        <v>56</v>
+      </c>
+      <c r="D39" s="25">
+        <v>-54</v>
+      </c>
       <c r="E39" s="31"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="9"/>
+      <c r="F39" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="B40" s="25"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
+      <c r="B40" s="25">
+        <v>92</v>
+      </c>
+      <c r="C40" s="25">
+        <v>148</v>
+      </c>
+      <c r="D40" s="25">
+        <v>-56</v>
+      </c>
       <c r="E40" s="31"/>
-      <c r="F40" s="31"/>
-      <c r="G40" s="9"/>
+      <c r="F40" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
+      <c r="B41" s="25">
+        <v>5</v>
+      </c>
+      <c r="C41" s="25">
+        <v>31</v>
+      </c>
+      <c r="D41" s="25">
+        <v>-26</v>
+      </c>
       <c r="E41" s="31"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="9"/>
+      <c r="F41" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="42" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="B42" s="25"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="25"/>
+      <c r="B42" s="25">
+        <v>5</v>
+      </c>
+      <c r="C42" s="25">
+        <v>9</v>
+      </c>
+      <c r="D42" s="25">
+        <v>-4</v>
+      </c>
       <c r="E42" s="31"/>
-      <c r="F42" s="31"/>
-      <c r="G42" s="9"/>
+      <c r="F42" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="B43" s="25"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
+      <c r="B43" s="25">
+        <v>0</v>
+      </c>
+      <c r="C43" s="25">
+        <v>1</v>
+      </c>
+      <c r="D43" s="25">
+        <v>-1</v>
+      </c>
       <c r="E43" s="31"/>
-      <c r="F43" s="31"/>
-      <c r="G43" s="9"/>
+      <c r="F43" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="44" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="B44" s="21"/>
-      <c r="C44" s="21"/>
-      <c r="D44" s="21"/>
-      <c r="E44" s="29"/>
+      <c r="B44" s="21">
+        <v>130</v>
+      </c>
+      <c r="C44" s="21">
+        <v>73</v>
+      </c>
+      <c r="D44" s="21">
+        <v>57</v>
+      </c>
+      <c r="E44" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F44" s="29"/>
-      <c r="G44" s="5"/>
+      <c r="G44" s="5" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="45" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
+      <c r="B45" s="18">
+        <v>74</v>
+      </c>
+      <c r="C45" s="18">
+        <v>171</v>
+      </c>
+      <c r="D45" s="18">
+        <v>-97</v>
+      </c>
       <c r="E45" s="28"/>
-      <c r="F45" s="28"/>
-      <c r="G45" s="3"/>
+      <c r="F45" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="46" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="B46" s="21"/>
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
+      <c r="B46" s="21">
+        <v>368</v>
+      </c>
+      <c r="C46" s="21">
+        <v>559</v>
+      </c>
+      <c r="D46" s="21">
+        <v>-191</v>
+      </c>
       <c r="E46" s="29"/>
-      <c r="F46" s="29"/>
-      <c r="G46" s="5"/>
+      <c r="F46" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="47" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="28"/>
+      <c r="B47" s="18">
+        <v>915</v>
+      </c>
+      <c r="C47" s="18">
+        <v>678</v>
+      </c>
+      <c r="D47" s="18">
+        <v>237</v>
+      </c>
+      <c r="E47" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F47" s="28"/>
-      <c r="G47" s="3"/>
+      <c r="G47" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="B48" s="21"/>
-      <c r="C48" s="21"/>
-      <c r="D48" s="21"/>
+      <c r="B48" s="21">
+        <v>150</v>
+      </c>
+      <c r="C48" s="21">
+        <v>605</v>
+      </c>
+      <c r="D48" s="21">
+        <v>-455</v>
+      </c>
       <c r="E48" s="29"/>
-      <c r="F48" s="29"/>
-      <c r="G48" s="5"/>
+      <c r="F48" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B49" s="18"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="18"/>
-      <c r="E49" s="28"/>
+      <c r="B49" s="18">
+        <v>349</v>
+      </c>
+      <c r="C49" s="18">
+        <v>169</v>
+      </c>
+      <c r="D49" s="18">
+        <v>180</v>
+      </c>
+      <c r="E49" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F49" s="28"/>
-      <c r="G49" s="3"/>
+      <c r="G49" s="3" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="B50" s="21"/>
-      <c r="C50" s="21"/>
-      <c r="D50" s="21"/>
-      <c r="E50" s="29"/>
+      <c r="B50" s="21">
+        <v>845</v>
+      </c>
+      <c r="C50" s="21">
+        <v>539</v>
+      </c>
+      <c r="D50" s="21">
+        <v>306</v>
+      </c>
+      <c r="E50" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F50" s="29"/>
-      <c r="G50" s="5"/>
+      <c r="G50" s="5" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B51" s="18"/>
-      <c r="C51" s="18"/>
-      <c r="D51" s="18"/>
-      <c r="E51" s="28"/>
+      <c r="B51" s="18">
+        <v>300</v>
+      </c>
+      <c r="C51" s="18">
+        <v>85</v>
+      </c>
+      <c r="D51" s="18">
+        <v>215</v>
+      </c>
+      <c r="E51" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F51" s="28"/>
-      <c r="G51" s="3"/>
+      <c r="G51" s="3" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="52" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="B52" s="21"/>
-      <c r="C52" s="21"/>
-      <c r="D52" s="21"/>
-      <c r="E52" s="29"/>
+      <c r="B52" s="21">
+        <v>514</v>
+      </c>
+      <c r="C52" s="21">
+        <v>484</v>
+      </c>
+      <c r="D52" s="21">
+        <v>30</v>
+      </c>
+      <c r="E52" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F52" s="29"/>
-      <c r="G52" s="5"/>
+      <c r="G52" s="5" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="53" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B53" s="18"/>
-      <c r="C53" s="18"/>
-      <c r="D53" s="18"/>
+      <c r="B53" s="18">
+        <v>97</v>
+      </c>
+      <c r="C53" s="18">
+        <v>199</v>
+      </c>
+      <c r="D53" s="18">
+        <v>-102</v>
+      </c>
       <c r="E53" s="28"/>
-      <c r="F53" s="28"/>
-      <c r="G53" s="3"/>
+      <c r="F53" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="54" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="B54" s="21"/>
-      <c r="C54" s="21"/>
-      <c r="D54" s="21"/>
+      <c r="B54" s="21">
+        <v>23</v>
+      </c>
+      <c r="C54" s="21">
+        <v>229</v>
+      </c>
+      <c r="D54" s="21">
+        <v>-206</v>
+      </c>
       <c r="E54" s="29"/>
-      <c r="F54" s="29"/>
-      <c r="G54" s="5"/>
+      <c r="F54" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="55" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="B55" s="27"/>
-      <c r="C55" s="27"/>
-      <c r="D55" s="27"/>
+      <c r="B55" s="27">
+        <v>151</v>
+      </c>
+      <c r="C55" s="27">
+        <v>186</v>
+      </c>
+      <c r="D55" s="27">
+        <v>-35</v>
+      </c>
       <c r="E55" s="32"/>
-      <c r="F55" s="32"/>
-      <c r="G55" s="11"/>
+      <c r="F55" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="G55" s="11" t="s">
+        <v>189</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G55" xr:uid="{00000000-0009-0000-0000-000004000000}"/>

</xml_diff>

<commit_message>
Update for August 2023
</commit_message>
<xml_diff>
--- a/statistics_files/2023/2023.g.net_borrower_lender.xlsx
+++ b/statistics_files/2023/2023.g.net_borrower_lender.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\GitHub\next_statistics\statistics_files\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3000385-D6E4-4E35-A961-D0EC6728B3B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0949BD9-B619-4823-85CC-52970FAA69F7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" tabRatio="673" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1515" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1617" uniqueCount="246">
   <si>
     <t>NET</t>
   </si>
@@ -766,6 +766,30 @@
   </si>
   <si>
     <t>0.11 : 1</t>
+  </si>
+  <si>
+    <t>2.05 : 1</t>
+  </si>
+  <si>
+    <t>0.31 : 1</t>
+  </si>
+  <si>
+    <t>0.03 : 1</t>
+  </si>
+  <si>
+    <t>1.67 : 1</t>
+  </si>
+  <si>
+    <t>1.27 : 1</t>
+  </si>
+  <si>
+    <t>1.10 : 1</t>
+  </si>
+  <si>
+    <t>1.73 : 1</t>
+  </si>
+  <si>
+    <t>1.60 : 1</t>
   </si>
 </sst>
 </file>
@@ -1675,15 +1699,15 @@
       </c>
       <c r="B2" s="2">
         <f>January!B2+February!B2+March!B2+April!B2+May!B2+June!B2+July!B2+August!B2+September!B2+October!B2+November!B2+December!B2</f>
-        <v>10376</v>
+        <v>12299</v>
       </c>
       <c r="C2" s="2">
         <f>January!C2+February!C2+March!C2+April!C2+May!C2+June!C2+July!C2+August!C2+September!C2+October!C2+November!C2+December!C2</f>
-        <v>8089</v>
+        <v>9403</v>
       </c>
       <c r="D2" s="2">
         <f>January!D2+February!D2+March!D2+April!D2+May!D2+June!D2+July!D2+August!D2+September!D2+October!D2+November!D2+December!D2</f>
-        <v>2287</v>
+        <v>2896</v>
       </c>
       <c r="E2" s="28" t="str">
         <f>IF(D2 &gt; 0, "We borrowed more than we lent this year", "")</f>
@@ -1695,7 +1719,7 @@
       </c>
       <c r="G2" s="3" t="str">
         <f>IF(ISERROR(ROUND(B2/C2,2)&amp;" : 1"), "", ROUND(B2/C2,2)&amp;" : 1")</f>
-        <v>1.28 : 1</v>
+        <v>1.31 : 1</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1704,15 +1728,15 @@
       </c>
       <c r="B3" s="4">
         <f>January!B3+February!B3+March!B3+April!B3+May!B3+June!B3+July!B3+August!B3+September!B3+October!B3+November!B3+December!B3</f>
-        <v>3395</v>
+        <v>4042</v>
       </c>
       <c r="C3" s="4">
         <f>January!C3+February!C3+March!C3+April!C3+May!C3+June!C3+July!C3+August!C3+September!C3+October!C3+November!C3+December!C3</f>
-        <v>3306</v>
+        <v>3855</v>
       </c>
       <c r="D3" s="4">
         <f>January!D3+February!D3+March!D3+April!D3+May!D3+June!D3+July!D3+August!D3+September!D3+October!D3+November!D3+December!D3</f>
-        <v>89</v>
+        <v>187</v>
       </c>
       <c r="E3" s="29" t="str">
         <f t="shared" ref="E3:E55" si="1">IF(D3 &gt; 0, "We borrowed more than we lent this year", "")</f>
@@ -1724,7 +1748,7 @@
       </c>
       <c r="G3" s="5" t="str">
         <f t="shared" ref="G3:G55" si="2">IF(ISERROR(ROUND(B3/C3,2)&amp;" : 1"), "", ROUND(B3/C3,2)&amp;" : 1")</f>
-        <v>1.03 : 1</v>
+        <v>1.05 : 1</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1733,15 +1757,15 @@
       </c>
       <c r="B4" s="2">
         <f>January!B4+February!B4+March!B4+April!B4+May!B4+June!B4+July!B4+August!B4+September!B4+October!B4+November!B4+December!B4</f>
-        <v>9303</v>
+        <v>10700</v>
       </c>
       <c r="C4" s="2">
         <f>January!C4+February!C4+March!C4+April!C4+May!C4+June!C4+July!C4+August!C4+September!C4+October!C4+November!C4+December!C4</f>
-        <v>8580</v>
+        <v>9919</v>
       </c>
       <c r="D4" s="2">
         <f>January!D4+February!D4+March!D4+April!D4+May!D4+June!D4+July!D4+August!D4+September!D4+October!D4+November!D4+December!D4</f>
-        <v>723</v>
+        <v>781</v>
       </c>
       <c r="E4" s="28" t="str">
         <f t="shared" si="1"/>
@@ -1762,15 +1786,15 @@
       </c>
       <c r="B5" s="4">
         <f>January!B5+February!B5+March!B5+April!B5+May!B5+June!B5+July!B5+August!B5+September!B5+October!B5+November!B5+December!B5</f>
-        <v>567</v>
+        <v>640</v>
       </c>
       <c r="C5" s="4">
         <f>January!C5+February!C5+March!C5+April!C5+May!C5+June!C5+July!C5+August!C5+September!C5+October!C5+November!C5+December!C5</f>
-        <v>836</v>
+        <v>986</v>
       </c>
       <c r="D5" s="4">
         <f>January!D5+February!D5+March!D5+April!D5+May!D5+June!D5+July!D5+August!D5+September!D5+October!D5+November!D5+December!D5</f>
-        <v>-269</v>
+        <v>-346</v>
       </c>
       <c r="E5" s="29" t="str">
         <f t="shared" si="1"/>
@@ -1782,7 +1806,7 @@
       </c>
       <c r="G5" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.68 : 1</v>
+        <v>0.65 : 1</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1791,15 +1815,15 @@
       </c>
       <c r="B6" s="2">
         <f>January!B6+February!B6+March!B6+April!B6+May!B6+June!B6+July!B6+August!B6+September!B6+October!B6+November!B6+December!B6</f>
-        <v>8813</v>
+        <v>10060</v>
       </c>
       <c r="C6" s="2">
         <f>January!C6+February!C6+March!C6+April!C6+May!C6+June!C6+July!C6+August!C6+September!C6+October!C6+November!C6+December!C6</f>
-        <v>10082</v>
+        <v>11736</v>
       </c>
       <c r="D6" s="2">
         <f>January!D6+February!D6+March!D6+April!D6+May!D6+June!D6+July!D6+August!D6+September!D6+October!D6+November!D6+December!D6</f>
-        <v>-1269</v>
+        <v>-1676</v>
       </c>
       <c r="E6" s="28" t="str">
         <f t="shared" si="1"/>
@@ -1811,7 +1835,7 @@
       </c>
       <c r="G6" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.87 : 1</v>
+        <v>0.86 : 1</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1820,27 +1844,27 @@
       </c>
       <c r="B7" s="4">
         <f>January!B7+February!B7+March!B7+April!B7+May!B7+June!B7+July!B7+August!B7+September!B7+October!B7+November!B7+December!B7</f>
-        <v>1566</v>
+        <v>1714</v>
       </c>
       <c r="C7" s="4">
         <f>January!C7+February!C7+March!C7+April!C7+May!C7+June!C7+July!C7+August!C7+September!C7+October!C7+November!C7+December!C7</f>
-        <v>1538</v>
+        <v>1810</v>
       </c>
       <c r="D7" s="4">
         <f>January!D7+February!D7+March!D7+April!D7+May!D7+June!D7+July!D7+August!D7+September!D7+October!D7+November!D7+December!D7</f>
-        <v>28</v>
+        <v>-96</v>
       </c>
       <c r="E7" s="29" t="str">
         <f t="shared" si="1"/>
-        <v>We borrowed more than we lent this year</v>
+        <v/>
       </c>
       <c r="F7" s="29" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>We lent more than we borrowed this year</v>
       </c>
       <c r="G7" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.02 : 1</v>
+        <v>0.95 : 1</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1849,15 +1873,15 @@
       </c>
       <c r="B8" s="2">
         <f>January!B8+February!B8+March!B8+April!B8+May!B8+June!B8+July!B8+August!B8+September!B8+October!B8+November!B8+December!B8</f>
-        <v>908</v>
+        <v>1056</v>
       </c>
       <c r="C8" s="2">
         <f>January!C8+February!C8+March!C8+April!C8+May!C8+June!C8+July!C8+August!C8+September!C8+October!C8+November!C8+December!C8</f>
-        <v>1359</v>
+        <v>1546</v>
       </c>
       <c r="D8" s="2">
         <f>January!D8+February!D8+March!D8+April!D8+May!D8+June!D8+July!D8+August!D8+September!D8+October!D8+November!D8+December!D8</f>
-        <v>-451</v>
+        <v>-490</v>
       </c>
       <c r="E8" s="28" t="str">
         <f t="shared" si="1"/>
@@ -1869,7 +1893,7 @@
       </c>
       <c r="G8" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.67 : 1</v>
+        <v>0.68 : 1</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1878,15 +1902,15 @@
       </c>
       <c r="B9" s="4">
         <f>January!B9+February!B9+March!B9+April!B9+May!B9+June!B9+July!B9+August!B9+September!B9+October!B9+November!B9+December!B9</f>
-        <v>386</v>
+        <v>419</v>
       </c>
       <c r="C9" s="4">
         <f>January!C9+February!C9+March!C9+April!C9+May!C9+June!C9+July!C9+August!C9+September!C9+October!C9+November!C9+December!C9</f>
-        <v>485</v>
+        <v>567</v>
       </c>
       <c r="D9" s="4">
         <f>January!D9+February!D9+March!D9+April!D9+May!D9+June!D9+July!D9+August!D9+September!D9+October!D9+November!D9+December!D9</f>
-        <v>-99</v>
+        <v>-148</v>
       </c>
       <c r="E9" s="29" t="str">
         <f t="shared" si="1"/>
@@ -1898,7 +1922,7 @@
       </c>
       <c r="G9" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.8 : 1</v>
+        <v>0.74 : 1</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1911,11 +1935,11 @@
       </c>
       <c r="C10" s="2">
         <f>January!C10+February!C10+March!C10+April!C10+May!C10+June!C10+July!C10+August!C10+September!C10+October!C10+November!C10+December!C10</f>
-        <v>253</v>
+        <v>298</v>
       </c>
       <c r="D10" s="2">
         <f>January!D10+February!D10+March!D10+April!D10+May!D10+June!D10+July!D10+August!D10+September!D10+October!D10+November!D10+December!D10</f>
-        <v>-214</v>
+        <v>-259</v>
       </c>
       <c r="E10" s="28" t="str">
         <f t="shared" si="1"/>
@@ -1927,7 +1951,7 @@
       </c>
       <c r="G10" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.15 : 1</v>
+        <v>0.13 : 1</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1965,15 +1989,15 @@
       </c>
       <c r="B12" s="6">
         <f>January!B12+February!B12+March!B12+April!B12+May!B12+June!B12+July!B12+August!B12+September!B12+October!B12+November!B12+December!B12</f>
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="C12" s="6">
         <f>January!C12+February!C12+March!C12+April!C12+May!C12+June!C12+July!C12+August!C12+September!C12+October!C12+November!C12+December!C12</f>
-        <v>143</v>
+        <v>173</v>
       </c>
       <c r="D12" s="6">
         <f>January!D12+February!D12+March!D12+April!D12+May!D12+June!D12+July!D12+August!D12+September!D12+October!D12+November!D12+December!D12</f>
-        <v>-27</v>
+        <v>-45</v>
       </c>
       <c r="E12" s="30" t="str">
         <f t="shared" si="1"/>
@@ -1985,7 +2009,7 @@
       </c>
       <c r="G12" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0.81 : 1</v>
+        <v>0.74 : 1</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1994,15 +2018,15 @@
       </c>
       <c r="B13" s="6">
         <f>January!B13+February!B13+March!B13+April!B13+May!B13+June!B13+July!B13+August!B13+September!B13+October!B13+November!B13+December!B13</f>
-        <v>908</v>
+        <v>1109</v>
       </c>
       <c r="C13" s="6">
         <f>January!C13+February!C13+March!C13+April!C13+May!C13+June!C13+July!C13+August!C13+September!C13+October!C13+November!C13+December!C13</f>
-        <v>603</v>
+        <v>701</v>
       </c>
       <c r="D13" s="6">
         <f>January!D13+February!D13+March!D13+April!D13+May!D13+June!D13+July!D13+August!D13+September!D13+October!D13+November!D13+December!D13</f>
-        <v>305</v>
+        <v>408</v>
       </c>
       <c r="E13" s="30" t="str">
         <f t="shared" si="1"/>
@@ -2014,7 +2038,7 @@
       </c>
       <c r="G13" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>1.51 : 1</v>
+        <v>1.58 : 1</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2023,15 +2047,15 @@
       </c>
       <c r="B14" s="6">
         <f>January!B14+February!B14+March!B14+April!B14+May!B14+June!B14+July!B14+August!B14+September!B14+October!B14+November!B14+December!B14</f>
-        <v>946</v>
+        <v>1088</v>
       </c>
       <c r="C14" s="6">
         <f>January!C14+February!C14+March!C14+April!C14+May!C14+June!C14+July!C14+August!C14+September!C14+October!C14+November!C14+December!C14</f>
-        <v>2035</v>
+        <v>2350</v>
       </c>
       <c r="D14" s="6">
         <f>January!D14+February!D14+March!D14+April!D14+May!D14+June!D14+July!D14+August!D14+September!D14+October!D14+November!D14+December!D14</f>
-        <v>-1089</v>
+        <v>-1262</v>
       </c>
       <c r="E14" s="30" t="str">
         <f t="shared" si="1"/>
@@ -2052,15 +2076,15 @@
       </c>
       <c r="B15" s="6">
         <f>January!B15+February!B15+March!B15+April!B15+May!B15+June!B15+July!B15+August!B15+September!B15+October!B15+November!B15+December!B15</f>
-        <v>572</v>
+        <v>677</v>
       </c>
       <c r="C15" s="6">
         <f>January!C15+February!C15+March!C15+April!C15+May!C15+June!C15+July!C15+August!C15+September!C15+October!C15+November!C15+December!C15</f>
-        <v>707</v>
+        <v>828</v>
       </c>
       <c r="D15" s="6">
         <f>January!D15+February!D15+March!D15+April!D15+May!D15+June!D15+July!D15+August!D15+September!D15+October!D15+November!D15+December!D15</f>
-        <v>-135</v>
+        <v>-151</v>
       </c>
       <c r="E15" s="30" t="str">
         <f t="shared" si="1"/>
@@ -2072,7 +2096,7 @@
       </c>
       <c r="G15" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0.81 : 1</v>
+        <v>0.82 : 1</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2081,15 +2105,15 @@
       </c>
       <c r="B16" s="2">
         <f>January!B16+February!B16+March!B16+April!B16+May!B16+June!B16+July!B16+August!B16+September!B16+October!B16+November!B16+December!B16</f>
-        <v>263</v>
+        <v>318</v>
       </c>
       <c r="C16" s="2">
         <f>January!C16+February!C16+March!C16+April!C16+May!C16+June!C16+July!C16+August!C16+September!C16+October!C16+November!C16+December!C16</f>
-        <v>1049</v>
+        <v>1227</v>
       </c>
       <c r="D16" s="2">
         <f>January!D16+February!D16+March!D16+April!D16+May!D16+June!D16+July!D16+August!D16+September!D16+October!D16+November!D16+December!D16</f>
-        <v>-786</v>
+        <v>-909</v>
       </c>
       <c r="E16" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2101,7 +2125,7 @@
       </c>
       <c r="G16" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.25 : 1</v>
+        <v>0.26 : 1</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2110,15 +2134,15 @@
       </c>
       <c r="B17" s="4">
         <f>January!B17+February!B17+March!B17+April!B17+May!B17+June!B17+July!B17+August!B17+September!B17+October!B17+November!B17+December!B17</f>
-        <v>4155</v>
+        <v>4805</v>
       </c>
       <c r="C17" s="4">
         <f>January!C17+February!C17+March!C17+April!C17+May!C17+June!C17+July!C17+August!C17+September!C17+October!C17+November!C17+December!C17</f>
-        <v>3292</v>
+        <v>3811</v>
       </c>
       <c r="D17" s="4">
         <f>January!D17+February!D17+March!D17+April!D17+May!D17+June!D17+July!D17+August!D17+September!D17+October!D17+November!D17+December!D17</f>
-        <v>863</v>
+        <v>994</v>
       </c>
       <c r="E17" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2139,27 +2163,27 @@
       </c>
       <c r="B18" s="2">
         <f>January!B18+February!B18+March!B18+April!B18+May!B18+June!B18+July!B18+August!B18+September!B18+October!B18+November!B18+December!B18</f>
-        <v>722</v>
+        <v>744</v>
       </c>
       <c r="C18" s="2">
         <f>January!C18+February!C18+March!C18+April!C18+May!C18+June!C18+July!C18+August!C18+September!C18+October!C18+November!C18+December!C18</f>
-        <v>693</v>
+        <v>799</v>
       </c>
       <c r="D18" s="2">
         <f>January!D18+February!D18+March!D18+April!D18+May!D18+June!D18+July!D18+August!D18+September!D18+October!D18+November!D18+December!D18</f>
-        <v>29</v>
+        <v>-55</v>
       </c>
       <c r="E18" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>We borrowed more than we lent this year</v>
+        <v/>
       </c>
       <c r="F18" s="28" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>We lent more than we borrowed this year</v>
       </c>
       <c r="G18" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.04 : 1</v>
+        <v>0.93 : 1</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2168,15 +2192,15 @@
       </c>
       <c r="B19" s="4">
         <f>January!B19+February!B19+March!B19+April!B19+May!B19+June!B19+July!B19+August!B19+September!B19+October!B19+November!B19+December!B19</f>
-        <v>4612</v>
+        <v>5250</v>
       </c>
       <c r="C19" s="4">
         <f>January!C19+February!C19+March!C19+April!C19+May!C19+June!C19+July!C19+August!C19+September!C19+October!C19+November!C19+December!C19</f>
-        <v>2727</v>
+        <v>3274</v>
       </c>
       <c r="D19" s="4">
         <f>January!D19+February!D19+March!D19+April!D19+May!D19+June!D19+July!D19+August!D19+September!D19+October!D19+November!D19+December!D19</f>
-        <v>1885</v>
+        <v>1976</v>
       </c>
       <c r="E19" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2188,7 +2212,7 @@
       </c>
       <c r="G19" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.69 : 1</v>
+        <v>1.6 : 1</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2197,15 +2221,15 @@
       </c>
       <c r="B20" s="2">
         <f>January!B20+February!B20+March!B20+April!B20+May!B20+June!B20+July!B20+August!B20+September!B20+October!B20+November!B20+December!B20</f>
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C20" s="2">
         <f>January!C20+February!C20+March!C20+April!C20+May!C20+June!C20+July!C20+August!C20+September!C20+October!C20+November!C20+December!C20</f>
-        <v>445</v>
+        <v>535</v>
       </c>
       <c r="D20" s="2">
         <f>January!D20+February!D20+March!D20+April!D20+May!D20+June!D20+July!D20+August!D20+September!D20+October!D20+November!D20+December!D20</f>
-        <v>-427</v>
+        <v>-514</v>
       </c>
       <c r="E20" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2226,15 +2250,15 @@
       </c>
       <c r="B21" s="4">
         <f>January!B21+February!B21+March!B21+April!B21+May!B21+June!B21+July!B21+August!B21+September!B21+October!B21+November!B21+December!B21</f>
-        <v>3625</v>
+        <v>4141</v>
       </c>
       <c r="C21" s="4">
         <f>January!C21+February!C21+March!C21+April!C21+May!C21+June!C21+July!C21+August!C21+September!C21+October!C21+November!C21+December!C21</f>
-        <v>2898</v>
+        <v>3370</v>
       </c>
       <c r="D21" s="4">
         <f>January!D21+February!D21+March!D21+April!D21+May!D21+June!D21+July!D21+August!D21+September!D21+October!D21+November!D21+December!D21</f>
-        <v>727</v>
+        <v>771</v>
       </c>
       <c r="E21" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2246,7 +2270,7 @@
       </c>
       <c r="G21" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.25 : 1</v>
+        <v>1.23 : 1</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2255,15 +2279,15 @@
       </c>
       <c r="B22" s="2">
         <f>January!B22+February!B22+March!B22+April!B22+May!B22+June!B22+July!B22+August!B22+September!B22+October!B22+November!B22+December!B22</f>
-        <v>173</v>
+        <v>207</v>
       </c>
       <c r="C22" s="2">
         <f>January!C22+February!C22+March!C22+April!C22+May!C22+June!C22+July!C22+August!C22+September!C22+October!C22+November!C22+December!C22</f>
-        <v>520</v>
+        <v>573</v>
       </c>
       <c r="D22" s="2">
         <f>January!D22+February!D22+March!D22+April!D22+May!D22+June!D22+July!D22+August!D22+September!D22+October!D22+November!D22+December!D22</f>
-        <v>-347</v>
+        <v>-366</v>
       </c>
       <c r="E22" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2275,7 +2299,7 @@
       </c>
       <c r="G22" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.33 : 1</v>
+        <v>0.36 : 1</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2284,15 +2308,15 @@
       </c>
       <c r="B23" s="4">
         <f>January!B23+February!B23+March!B23+April!B23+May!B23+June!B23+July!B23+August!B23+September!B23+October!B23+November!B23+December!B23</f>
-        <v>4874</v>
+        <v>5600</v>
       </c>
       <c r="C23" s="4">
         <f>January!C23+February!C23+March!C23+April!C23+May!C23+June!C23+July!C23+August!C23+September!C23+October!C23+November!C23+December!C23</f>
-        <v>3534</v>
+        <v>3970</v>
       </c>
       <c r="D23" s="4">
         <f>January!D23+February!D23+March!D23+April!D23+May!D23+June!D23+July!D23+August!D23+September!D23+October!D23+November!D23+December!D23</f>
-        <v>1340</v>
+        <v>1630</v>
       </c>
       <c r="E23" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2304,7 +2328,7 @@
       </c>
       <c r="G23" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.38 : 1</v>
+        <v>1.41 : 1</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2313,15 +2337,15 @@
       </c>
       <c r="B24" s="2">
         <f>January!B24+February!B24+March!B24+April!B24+May!B24+June!B24+July!B24+August!B24+September!B24+October!B24+November!B24+December!B24</f>
-        <v>13001</v>
+        <v>14823</v>
       </c>
       <c r="C24" s="2">
         <f>January!C24+February!C24+March!C24+April!C24+May!C24+June!C24+July!C24+August!C24+September!C24+October!C24+November!C24+December!C24</f>
-        <v>9731</v>
+        <v>11161</v>
       </c>
       <c r="D24" s="2">
         <f>January!D24+February!D24+March!D24+April!D24+May!D24+June!D24+July!D24+August!D24+September!D24+October!D24+November!D24+December!D24</f>
-        <v>3270</v>
+        <v>3662</v>
       </c>
       <c r="E24" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2333,7 +2357,7 @@
       </c>
       <c r="G24" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.34 : 1</v>
+        <v>1.33 : 1</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2342,15 +2366,15 @@
       </c>
       <c r="B25" s="4">
         <f>January!B25+February!B25+March!B25+April!B25+May!B25+June!B25+July!B25+August!B25+September!B25+October!B25+November!B25+December!B25</f>
-        <v>1280</v>
+        <v>1408</v>
       </c>
       <c r="C25" s="4">
         <f>January!C25+February!C25+March!C25+April!C25+May!C25+June!C25+July!C25+August!C25+September!C25+October!C25+November!C25+December!C25</f>
-        <v>2483</v>
+        <v>2861</v>
       </c>
       <c r="D25" s="4">
         <f>January!D25+February!D25+March!D25+April!D25+May!D25+June!D25+July!D25+August!D25+September!D25+October!D25+November!D25+December!D25</f>
-        <v>-1203</v>
+        <v>-1453</v>
       </c>
       <c r="E25" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2362,7 +2386,7 @@
       </c>
       <c r="G25" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.52 : 1</v>
+        <v>0.49 : 1</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2400,15 +2424,15 @@
       </c>
       <c r="B27" s="4">
         <f>January!B27+February!B27+March!B27+April!B27+May!B27+June!B27+July!B27+August!B27+September!B27+October!B27+November!B27+December!B27</f>
-        <v>2021</v>
+        <v>2321</v>
       </c>
       <c r="C27" s="4">
         <f>January!C27+February!C27+March!C27+April!C27+May!C27+June!C27+July!C27+August!C27+September!C27+October!C27+November!C27+December!C27</f>
-        <v>1356</v>
+        <v>1580</v>
       </c>
       <c r="D27" s="4">
         <f>January!D27+February!D27+March!D27+April!D27+May!D27+June!D27+July!D27+August!D27+September!D27+October!D27+November!D27+December!D27</f>
-        <v>665</v>
+        <v>741</v>
       </c>
       <c r="E27" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2420,7 +2444,7 @@
       </c>
       <c r="G27" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.49 : 1</v>
+        <v>1.47 : 1</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2429,15 +2453,15 @@
       </c>
       <c r="B28" s="2">
         <f>January!B28+February!B28+March!B28+April!B28+May!B28+June!B28+July!B28+August!B28+September!B28+October!B28+November!B28+December!B28</f>
-        <v>367</v>
+        <v>433</v>
       </c>
       <c r="C28" s="2">
         <f>January!C28+February!C28+March!C28+April!C28+May!C28+June!C28+July!C28+August!C28+September!C28+October!C28+November!C28+December!C28</f>
-        <v>540</v>
+        <v>589</v>
       </c>
       <c r="D28" s="2">
         <f>January!D28+February!D28+March!D28+April!D28+May!D28+June!D28+July!D28+August!D28+September!D28+October!D28+November!D28+December!D28</f>
-        <v>-173</v>
+        <v>-156</v>
       </c>
       <c r="E28" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2449,7 +2473,7 @@
       </c>
       <c r="G28" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.68 : 1</v>
+        <v>0.74 : 1</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2458,15 +2482,15 @@
       </c>
       <c r="B29" s="4">
         <f>January!B29+February!B29+March!B29+April!B29+May!B29+June!B29+July!B29+August!B29+September!B29+October!B29+November!B29+December!B29</f>
-        <v>3712</v>
+        <v>4251</v>
       </c>
       <c r="C29" s="4">
         <f>January!C29+February!C29+March!C29+April!C29+May!C29+June!C29+July!C29+August!C29+September!C29+October!C29+November!C29+December!C29</f>
-        <v>3229</v>
+        <v>3717</v>
       </c>
       <c r="D29" s="4">
         <f>January!D29+February!D29+March!D29+April!D29+May!D29+June!D29+July!D29+August!D29+September!D29+October!D29+November!D29+December!D29</f>
-        <v>483</v>
+        <v>534</v>
       </c>
       <c r="E29" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2478,7 +2502,7 @@
       </c>
       <c r="G29" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.15 : 1</v>
+        <v>1.14 : 1</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2487,15 +2511,15 @@
       </c>
       <c r="B30" s="2">
         <f>January!B30+February!B30+March!B30+April!B30+May!B30+June!B30+July!B30+August!B30+September!B30+October!B30+November!B30+December!B30</f>
-        <v>326</v>
+        <v>381</v>
       </c>
       <c r="C30" s="2">
         <f>January!C30+February!C30+March!C30+April!C30+May!C30+June!C30+July!C30+August!C30+September!C30+October!C30+November!C30+December!C30</f>
-        <v>247</v>
+        <v>282</v>
       </c>
       <c r="D30" s="2">
         <f>January!D30+February!D30+March!D30+April!D30+May!D30+June!D30+July!D30+August!D30+September!D30+October!D30+November!D30+December!D30</f>
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="E30" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2507,7 +2531,7 @@
       </c>
       <c r="G30" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.32 : 1</v>
+        <v>1.35 : 1</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2516,15 +2540,15 @@
       </c>
       <c r="B31" s="4">
         <f>January!B31+February!B31+March!B31+April!B31+May!B31+June!B31+July!B31+August!B31+September!B31+October!B31+November!B31+December!B31</f>
-        <v>528</v>
+        <v>596</v>
       </c>
       <c r="C31" s="4">
         <f>January!C31+February!C31+March!C31+April!C31+May!C31+June!C31+July!C31+August!C31+September!C31+October!C31+November!C31+December!C31</f>
-        <v>2128</v>
+        <v>2447</v>
       </c>
       <c r="D31" s="4">
         <f>January!D31+February!D31+March!D31+April!D31+May!D31+June!D31+July!D31+August!D31+September!D31+October!D31+November!D31+December!D31</f>
-        <v>-1600</v>
+        <v>-1851</v>
       </c>
       <c r="E31" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2536,7 +2560,7 @@
       </c>
       <c r="G31" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.25 : 1</v>
+        <v>0.24 : 1</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2545,15 +2569,15 @@
       </c>
       <c r="B32" s="2">
         <f>January!B32+February!B32+March!B32+April!B32+May!B32+June!B32+July!B32+August!B32+September!B32+October!B32+November!B32+December!B32</f>
-        <v>3020</v>
+        <v>3559</v>
       </c>
       <c r="C32" s="2">
         <f>January!C32+February!C32+March!C32+April!C32+May!C32+June!C32+July!C32+August!C32+September!C32+October!C32+November!C32+December!C32</f>
-        <v>3999</v>
+        <v>4539</v>
       </c>
       <c r="D32" s="2">
         <f>January!D32+February!D32+March!D32+April!D32+May!D32+June!D32+July!D32+August!D32+September!D32+October!D32+November!D32+December!D32</f>
-        <v>-979</v>
+        <v>-980</v>
       </c>
       <c r="E32" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2565,7 +2589,7 @@
       </c>
       <c r="G32" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.76 : 1</v>
+        <v>0.78 : 1</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2574,15 +2598,15 @@
       </c>
       <c r="B33" s="4">
         <f>January!B33+February!B33+March!B33+April!B33+May!B33+June!B33+July!B33+August!B33+September!B33+October!B33+November!B33+December!B33</f>
-        <v>2973</v>
+        <v>3429</v>
       </c>
       <c r="C33" s="4">
         <f>January!C33+February!C33+March!C33+April!C33+May!C33+June!C33+July!C33+August!C33+September!C33+October!C33+November!C33+December!C33</f>
-        <v>3601</v>
+        <v>4180</v>
       </c>
       <c r="D33" s="4">
         <f>January!D33+February!D33+March!D33+April!D33+May!D33+June!D33+July!D33+August!D33+September!D33+October!D33+November!D33+December!D33</f>
-        <v>-628</v>
+        <v>-751</v>
       </c>
       <c r="E33" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2594,7 +2618,7 @@
       </c>
       <c r="G33" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.83 : 1</v>
+        <v>0.82 : 1</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2603,15 +2627,15 @@
       </c>
       <c r="B34" s="2">
         <f>January!B34+February!B34+March!B34+April!B34+May!B34+June!B34+July!B34+August!B34+September!B34+October!B34+November!B34+December!B34</f>
-        <v>1537</v>
+        <v>1763</v>
       </c>
       <c r="C34" s="2">
         <f>January!C34+February!C34+March!C34+April!C34+May!C34+June!C34+July!C34+August!C34+September!C34+October!C34+November!C34+December!C34</f>
-        <v>820</v>
+        <v>939</v>
       </c>
       <c r="D34" s="2">
         <f>January!D34+February!D34+March!D34+April!D34+May!D34+June!D34+July!D34+August!D34+September!D34+October!D34+November!D34+December!D34</f>
-        <v>717</v>
+        <v>824</v>
       </c>
       <c r="E34" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2623,7 +2647,7 @@
       </c>
       <c r="G34" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.87 : 1</v>
+        <v>1.88 : 1</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2632,15 +2656,15 @@
       </c>
       <c r="B35" s="4">
         <f>January!B35+February!B35+March!B35+April!B35+May!B35+June!B35+July!B35+August!B35+September!B35+October!B35+November!B35+December!B35</f>
-        <v>6376</v>
+        <v>7614</v>
       </c>
       <c r="C35" s="4">
         <f>January!C35+February!C35+March!C35+April!C35+May!C35+June!C35+July!C35+August!C35+September!C35+October!C35+November!C35+December!C35</f>
-        <v>7096</v>
+        <v>8085</v>
       </c>
       <c r="D35" s="4">
         <f>January!D35+February!D35+March!D35+April!D35+May!D35+June!D35+July!D35+August!D35+September!D35+October!D35+November!D35+December!D35</f>
-        <v>-720</v>
+        <v>-471</v>
       </c>
       <c r="E35" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2652,7 +2676,7 @@
       </c>
       <c r="G35" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.9 : 1</v>
+        <v>0.94 : 1</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2661,15 +2685,15 @@
       </c>
       <c r="B36" s="2">
         <f>January!B36+February!B36+March!B36+April!B36+May!B36+June!B36+July!B36+August!B36+September!B36+October!B36+November!B36+December!B36</f>
-        <v>1583</v>
+        <v>1792</v>
       </c>
       <c r="C36" s="2">
         <f>January!C36+February!C36+March!C36+April!C36+May!C36+June!C36+July!C36+August!C36+September!C36+October!C36+November!C36+December!C36</f>
-        <v>3364</v>
+        <v>3825</v>
       </c>
       <c r="D36" s="2">
         <f>January!D36+February!D36+March!D36+April!D36+May!D36+June!D36+July!D36+August!D36+September!D36+October!D36+November!D36+December!D36</f>
-        <v>-1781</v>
+        <v>-2033</v>
       </c>
       <c r="E36" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2690,15 +2714,15 @@
       </c>
       <c r="B37" s="4">
         <f>January!B37+February!B37+March!B37+April!B37+May!B37+June!B37+July!B37+August!B37+September!B37+October!B37+November!B37+December!B37</f>
-        <v>3651</v>
+        <v>4153</v>
       </c>
       <c r="C37" s="4">
         <f>January!C37+February!C37+March!C37+April!C37+May!C37+June!C37+July!C37+August!C37+September!C37+October!C37+November!C37+December!C37</f>
-        <v>2553</v>
+        <v>2915</v>
       </c>
       <c r="D37" s="4">
         <f>January!D37+February!D37+March!D37+April!D37+May!D37+June!D37+July!D37+August!D37+September!D37+October!D37+November!D37+December!D37</f>
-        <v>1098</v>
+        <v>1238</v>
       </c>
       <c r="E37" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2710,7 +2734,7 @@
       </c>
       <c r="G37" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.43 : 1</v>
+        <v>1.42 : 1</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2719,15 +2743,15 @@
       </c>
       <c r="B38" s="2">
         <f>January!B38+February!B38+March!B38+April!B38+May!B38+June!B38+July!B38+August!B38+September!B38+October!B38+November!B38+December!B38</f>
-        <v>254</v>
+        <v>267</v>
       </c>
       <c r="C38" s="2">
         <f>January!C38+February!C38+March!C38+April!C38+May!C38+June!C38+July!C38+August!C38+September!C38+October!C38+November!C38+December!C38</f>
-        <v>1156</v>
+        <v>1333</v>
       </c>
       <c r="D38" s="2">
         <f>January!D38+February!D38+March!D38+April!D38+May!D38+June!D38+July!D38+August!D38+September!D38+October!D38+November!D38+December!D38</f>
-        <v>-902</v>
+        <v>-1066</v>
       </c>
       <c r="E38" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2739,7 +2763,7 @@
       </c>
       <c r="G38" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.22 : 1</v>
+        <v>0.2 : 1</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2748,15 +2772,15 @@
       </c>
       <c r="B39" s="8">
         <f>January!B39+February!B39+March!B39+April!B39+May!B39+June!B39+July!B39+August!B39+September!B39+October!B39+November!B39+December!B39</f>
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="C39" s="8">
         <f>January!C39+February!C39+March!C39+April!C39+May!C39+June!C39+July!C39+August!C39+September!C39+October!C39+November!C39+December!C39</f>
-        <v>313</v>
+        <v>341</v>
       </c>
       <c r="D39" s="8">
         <f>January!D39+February!D39+March!D39+April!D39+May!D39+June!D39+July!D39+August!D39+September!D39+October!D39+November!D39+December!D39</f>
-        <v>-170</v>
+        <v>-189</v>
       </c>
       <c r="E39" s="31" t="str">
         <f t="shared" si="1"/>
@@ -2768,7 +2792,7 @@
       </c>
       <c r="G39" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>0.46 : 1</v>
+        <v>0.45 : 1</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2777,15 +2801,15 @@
       </c>
       <c r="B40" s="8">
         <f>January!B40+February!B40+March!B40+April!B40+May!B40+June!B40+July!B40+August!B40+September!B40+October!B40+November!B40+December!B40</f>
-        <v>348</v>
+        <v>372</v>
       </c>
       <c r="C40" s="8">
         <f>January!C40+February!C40+March!C40+April!C40+May!C40+June!C40+July!C40+August!C40+September!C40+October!C40+November!C40+December!C40</f>
-        <v>611</v>
+        <v>660</v>
       </c>
       <c r="D40" s="8">
         <f>January!D40+February!D40+March!D40+April!D40+May!D40+June!D40+July!D40+August!D40+September!D40+October!D40+November!D40+December!D40</f>
-        <v>-263</v>
+        <v>-288</v>
       </c>
       <c r="E40" s="31" t="str">
         <f t="shared" si="1"/>
@@ -2797,7 +2821,7 @@
       </c>
       <c r="G40" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>0.57 : 1</v>
+        <v>0.56 : 1</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2806,15 +2830,15 @@
       </c>
       <c r="B41" s="8">
         <f>January!B41+February!B41+March!B41+April!B41+May!B41+June!B41+July!B41+August!B41+September!B41+October!B41+November!B41+December!B41</f>
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C41" s="8">
         <f>January!C41+February!C41+March!C41+April!C41+May!C41+June!C41+July!C41+August!C41+September!C41+October!C41+November!C41+December!C41</f>
-        <v>126</v>
+        <v>139</v>
       </c>
       <c r="D41" s="8">
         <f>January!D41+February!D41+March!D41+April!D41+May!D41+June!D41+July!D41+August!D41+September!D41+October!D41+November!D41+December!D41</f>
-        <v>-50</v>
+        <v>-62</v>
       </c>
       <c r="E41" s="31" t="str">
         <f t="shared" si="1"/>
@@ -2826,7 +2850,7 @@
       </c>
       <c r="G41" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>0.6 : 1</v>
+        <v>0.55 : 1</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2835,19 +2859,19 @@
       </c>
       <c r="B42" s="8">
         <f>January!B42+February!B42+March!B42+April!B42+May!B42+June!B42+July!B42+August!B42+September!B42+October!B42+November!B42+December!B42</f>
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="C42" s="8">
         <f>January!C42+February!C42+March!C42+April!C42+May!C42+June!C42+July!C42+August!C42+September!C42+October!C42+November!C42+December!C42</f>
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="D42" s="8">
         <f>January!D42+February!D42+March!D42+April!D42+May!D42+June!D42+July!D42+August!D42+September!D42+October!D42+November!D42+December!D42</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E42" s="31" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>We borrowed more than we lent this year</v>
       </c>
       <c r="F42" s="31" t="str">
         <f t="shared" si="3"/>
@@ -2855,7 +2879,7 @@
       </c>
       <c r="G42" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>1 : 1</v>
+        <v>1.14 : 1</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2893,15 +2917,15 @@
       </c>
       <c r="B44" s="4">
         <f>January!B44+February!B44+March!B44+April!B44+May!B44+June!B44+July!B44+August!B44+September!B44+October!B44+November!B44+December!B44</f>
-        <v>792</v>
+        <v>862</v>
       </c>
       <c r="C44" s="4">
         <f>January!C44+February!C44+March!C44+April!C44+May!C44+June!C44+July!C44+August!C44+September!C44+October!C44+November!C44+December!C44</f>
-        <v>545</v>
+        <v>600</v>
       </c>
       <c r="D44" s="4">
         <f>January!D44+February!D44+March!D44+April!D44+May!D44+June!D44+July!D44+August!D44+September!D44+October!D44+November!D44+December!D44</f>
-        <v>247</v>
+        <v>262</v>
       </c>
       <c r="E44" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2913,7 +2937,7 @@
       </c>
       <c r="G44" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.45 : 1</v>
+        <v>1.44 : 1</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2922,15 +2946,15 @@
       </c>
       <c r="B45" s="2">
         <f>January!B45+February!B45+March!B45+April!B45+May!B45+June!B45+July!B45+August!B45+September!B45+October!B45+November!B45+December!B45</f>
-        <v>538</v>
+        <v>608</v>
       </c>
       <c r="C45" s="2">
         <f>January!C45+February!C45+March!C45+April!C45+May!C45+June!C45+July!C45+August!C45+September!C45+October!C45+November!C45+December!C45</f>
-        <v>1095</v>
+        <v>1220</v>
       </c>
       <c r="D45" s="2">
         <f>January!D45+February!D45+March!D45+April!D45+May!D45+June!D45+July!D45+August!D45+September!D45+October!D45+November!D45+December!D45</f>
-        <v>-557</v>
+        <v>-612</v>
       </c>
       <c r="E45" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2942,7 +2966,7 @@
       </c>
       <c r="G45" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.49 : 1</v>
+        <v>0.5 : 1</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2951,15 +2975,15 @@
       </c>
       <c r="B46" s="4">
         <f>January!B46+February!B46+March!B46+April!B46+May!B46+June!B46+July!B46+August!B46+September!B46+October!B46+November!B46+December!B46</f>
-        <v>2977</v>
+        <v>3520</v>
       </c>
       <c r="C46" s="4">
         <f>January!C46+February!C46+March!C46+April!C46+May!C46+June!C46+July!C46+August!C46+September!C46+October!C46+November!C46+December!C46</f>
-        <v>4281</v>
+        <v>4932</v>
       </c>
       <c r="D46" s="4">
         <f>January!D46+February!D46+March!D46+April!D46+May!D46+June!D46+July!D46+August!D46+September!D46+October!D46+November!D46+December!D46</f>
-        <v>-1304</v>
+        <v>-1412</v>
       </c>
       <c r="E46" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2971,7 +2995,7 @@
       </c>
       <c r="G46" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.7 : 1</v>
+        <v>0.71 : 1</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2980,15 +3004,15 @@
       </c>
       <c r="B47" s="2">
         <f>January!B47+February!B47+March!B47+April!B47+May!B47+June!B47+July!B47+August!B47+September!B47+October!B47+November!B47+December!B47</f>
-        <v>6270</v>
+        <v>7129</v>
       </c>
       <c r="C47" s="2">
         <f>January!C47+February!C47+March!C47+April!C47+May!C47+June!C47+July!C47+August!C47+September!C47+October!C47+November!C47+December!C47</f>
-        <v>4639</v>
+        <v>5230</v>
       </c>
       <c r="D47" s="2">
         <f>January!D47+February!D47+March!D47+April!D47+May!D47+June!D47+July!D47+August!D47+September!D47+October!D47+November!D47+December!D47</f>
-        <v>1631</v>
+        <v>1899</v>
       </c>
       <c r="E47" s="28" t="str">
         <f t="shared" si="1"/>
@@ -3000,7 +3024,7 @@
       </c>
       <c r="G47" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.35 : 1</v>
+        <v>1.36 : 1</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3009,15 +3033,15 @@
       </c>
       <c r="B48" s="4">
         <f>January!B48+February!B48+March!B48+April!B48+May!B48+June!B48+July!B48+August!B48+September!B48+October!B48+November!B48+December!B48</f>
-        <v>1609</v>
+        <v>1836</v>
       </c>
       <c r="C48" s="4">
         <f>January!C48+February!C48+March!C48+April!C48+May!C48+June!C48+July!C48+August!C48+September!C48+October!C48+November!C48+December!C48</f>
-        <v>4497</v>
+        <v>5151</v>
       </c>
       <c r="D48" s="4">
         <f>January!D48+February!D48+March!D48+April!D48+May!D48+June!D48+July!D48+August!D48+September!D48+October!D48+November!D48+December!D48</f>
-        <v>-2888</v>
+        <v>-3315</v>
       </c>
       <c r="E48" s="29" t="str">
         <f t="shared" si="1"/>
@@ -3038,15 +3062,15 @@
       </c>
       <c r="B49" s="2">
         <f>January!B49+February!B49+March!B49+April!B49+May!B49+June!B49+July!B49+August!B49+September!B49+October!B49+November!B49+December!B49</f>
-        <v>2549</v>
+        <v>2943</v>
       </c>
       <c r="C49" s="2">
         <f>January!C49+February!C49+March!C49+April!C49+May!C49+June!C49+July!C49+August!C49+September!C49+October!C49+November!C49+December!C49</f>
-        <v>1379</v>
+        <v>1651</v>
       </c>
       <c r="D49" s="2">
         <f>January!D49+February!D49+March!D49+April!D49+May!D49+June!D49+July!D49+August!D49+September!D49+October!D49+November!D49+December!D49</f>
-        <v>1170</v>
+        <v>1292</v>
       </c>
       <c r="E49" s="28" t="str">
         <f t="shared" si="1"/>
@@ -3058,7 +3082,7 @@
       </c>
       <c r="G49" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.85 : 1</v>
+        <v>1.78 : 1</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3067,15 +3091,15 @@
       </c>
       <c r="B50" s="4">
         <f>January!B50+February!B50+March!B50+April!B50+May!B50+June!B50+July!B50+August!B50+September!B50+October!B50+November!B50+December!B50</f>
-        <v>5962</v>
+        <v>6953</v>
       </c>
       <c r="C50" s="4">
         <f>January!C50+February!C50+March!C50+April!C50+May!C50+June!C50+July!C50+August!C50+September!C50+October!C50+November!C50+December!C50</f>
-        <v>3853</v>
+        <v>4506</v>
       </c>
       <c r="D50" s="4">
         <f>January!D50+February!D50+March!D50+April!D50+May!D50+June!D50+July!D50+August!D50+September!D50+October!D50+November!D50+December!D50</f>
-        <v>2109</v>
+        <v>2447</v>
       </c>
       <c r="E50" s="29" t="str">
         <f t="shared" si="1"/>
@@ -3087,7 +3111,7 @@
       </c>
       <c r="G50" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.55 : 1</v>
+        <v>1.54 : 1</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3096,15 +3120,15 @@
       </c>
       <c r="B51" s="2">
         <f>January!B51+February!B51+March!B51+April!B51+May!B51+June!B51+July!B51+August!B51+September!B51+October!B51+November!B51+December!B51</f>
-        <v>1715</v>
+        <v>1961</v>
       </c>
       <c r="C51" s="2">
         <f>January!C51+February!C51+March!C51+April!C51+May!C51+June!C51+July!C51+August!C51+September!C51+October!C51+November!C51+December!C51</f>
-        <v>676</v>
+        <v>830</v>
       </c>
       <c r="D51" s="2">
         <f>January!D51+February!D51+March!D51+April!D51+May!D51+June!D51+July!D51+August!D51+September!D51+October!D51+November!D51+December!D51</f>
-        <v>1039</v>
+        <v>1131</v>
       </c>
       <c r="E51" s="28" t="str">
         <f t="shared" si="1"/>
@@ -3116,7 +3140,7 @@
       </c>
       <c r="G51" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>2.54 : 1</v>
+        <v>2.36 : 1</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3125,15 +3149,15 @@
       </c>
       <c r="B52" s="4">
         <f>January!B52+February!B52+March!B52+April!B52+May!B52+June!B52+July!B52+August!B52+September!B52+October!B52+November!B52+December!B52</f>
-        <v>3287</v>
+        <v>3634</v>
       </c>
       <c r="C52" s="4">
         <f>January!C52+February!C52+March!C52+April!C52+May!C52+June!C52+July!C52+August!C52+September!C52+October!C52+November!C52+December!C52</f>
-        <v>3868</v>
+        <v>4382</v>
       </c>
       <c r="D52" s="4">
         <f>January!D52+February!D52+March!D52+April!D52+May!D52+June!D52+July!D52+August!D52+September!D52+October!D52+November!D52+December!D52</f>
-        <v>-581</v>
+        <v>-748</v>
       </c>
       <c r="E52" s="29" t="str">
         <f t="shared" si="1"/>
@@ -3145,7 +3169,7 @@
       </c>
       <c r="G52" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.85 : 1</v>
+        <v>0.83 : 1</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3154,15 +3178,15 @@
       </c>
       <c r="B53" s="2">
         <f>January!B53+February!B53+March!B53+April!B53+May!B53+June!B53+July!B53+August!B53+September!B53+October!B53+November!B53+December!B53</f>
-        <v>864</v>
+        <v>1018</v>
       </c>
       <c r="C53" s="2">
         <f>January!C53+February!C53+March!C53+April!C53+May!C53+June!C53+July!C53+August!C53+September!C53+October!C53+November!C53+December!C53</f>
-        <v>1500</v>
+        <v>1757</v>
       </c>
       <c r="D53" s="2">
         <f>January!D53+February!D53+March!D53+April!D53+May!D53+June!D53+July!D53+August!D53+September!D53+October!D53+November!D53+December!D53</f>
-        <v>-636</v>
+        <v>-739</v>
       </c>
       <c r="E53" s="28" t="str">
         <f t="shared" si="1"/>
@@ -3183,15 +3207,15 @@
       </c>
       <c r="B54" s="4">
         <f>January!B54+February!B54+March!B54+April!B54+May!B54+June!B54+July!B54+August!B54+September!B54+October!B54+November!B54+December!B54</f>
-        <v>202</v>
+        <v>234</v>
       </c>
       <c r="C54" s="4">
         <f>January!C54+February!C54+March!C54+April!C54+May!C54+June!C54+July!C54+August!C54+September!C54+October!C54+November!C54+December!C54</f>
-        <v>1633</v>
+        <v>1832</v>
       </c>
       <c r="D54" s="4">
         <f>January!D54+February!D54+March!D54+April!D54+May!D54+June!D54+July!D54+August!D54+September!D54+October!D54+November!D54+December!D54</f>
-        <v>-1431</v>
+        <v>-1598</v>
       </c>
       <c r="E54" s="29" t="str">
         <f t="shared" si="1"/>
@@ -3203,7 +3227,7 @@
       </c>
       <c r="G54" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.12 : 1</v>
+        <v>0.13 : 1</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3212,15 +3236,15 @@
       </c>
       <c r="B55" s="10">
         <f>January!B55+February!B55+March!B55+April!B55+May!B55+June!B55+July!B55+August!B55+September!B55+October!B55+November!B55+December!B55</f>
-        <v>1320</v>
+        <v>1579</v>
       </c>
       <c r="C55" s="10">
         <f>January!C55+February!C55+March!C55+April!C55+May!C55+June!C55+July!C55+August!C55+September!C55+October!C55+November!C55+December!C55</f>
-        <v>1140</v>
+        <v>1333</v>
       </c>
       <c r="D55" s="10">
         <f>January!D55+February!D55+March!D55+April!D55+May!D55+June!D55+July!D55+August!D55+September!D55+October!D55+November!D55+December!D55</f>
-        <v>180</v>
+        <v>246</v>
       </c>
       <c r="E55" s="32" t="str">
         <f t="shared" si="1"/>
@@ -3232,7 +3256,7 @@
       </c>
       <c r="G55" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>1.16 : 1</v>
+        <v>1.18 : 1</v>
       </c>
     </row>
   </sheetData>
@@ -14278,108 +14302,204 @@
       <c r="A2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="28"/>
+      <c r="B2" s="18">
+        <v>1923</v>
+      </c>
+      <c r="C2" s="18">
+        <v>1314</v>
+      </c>
+      <c r="D2" s="18">
+        <v>609</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F2" s="28"/>
-      <c r="G2" s="3"/>
+      <c r="G2" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="29"/>
+      <c r="B3" s="21">
+        <v>647</v>
+      </c>
+      <c r="C3" s="21">
+        <v>549</v>
+      </c>
+      <c r="D3" s="21">
+        <v>98</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F3" s="29"/>
-      <c r="G3" s="5"/>
+      <c r="G3" s="5" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="28"/>
+      <c r="B4" s="18">
+        <v>1397</v>
+      </c>
+      <c r="C4" s="18">
+        <v>1339</v>
+      </c>
+      <c r="D4" s="18">
+        <v>58</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F4" s="28"/>
-      <c r="G4" s="3"/>
+      <c r="G4" s="3" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
+      <c r="B5" s="21">
+        <v>73</v>
+      </c>
+      <c r="C5" s="21">
+        <v>150</v>
+      </c>
+      <c r="D5" s="21">
+        <v>-77</v>
+      </c>
       <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="5"/>
+      <c r="F5" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
+      <c r="B6" s="18">
+        <v>1247</v>
+      </c>
+      <c r="C6" s="18">
+        <v>1654</v>
+      </c>
+      <c r="D6" s="18">
+        <v>-407</v>
+      </c>
       <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="3"/>
+      <c r="F6" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
+      <c r="B7" s="21">
+        <v>148</v>
+      </c>
+      <c r="C7" s="21">
+        <v>272</v>
+      </c>
+      <c r="D7" s="21">
+        <v>-124</v>
+      </c>
       <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="5"/>
+      <c r="F7" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
+      <c r="B8" s="18">
+        <v>148</v>
+      </c>
+      <c r="C8" s="18">
+        <v>187</v>
+      </c>
+      <c r="D8" s="18">
+        <v>-39</v>
+      </c>
       <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="3"/>
+      <c r="F8" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
+      <c r="B9" s="21">
+        <v>33</v>
+      </c>
+      <c r="C9" s="21">
+        <v>82</v>
+      </c>
+      <c r="D9" s="21">
+        <v>-49</v>
+      </c>
       <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="5"/>
+      <c r="F9" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
+      <c r="B10" s="18">
+        <v>0</v>
+      </c>
+      <c r="C10" s="18">
+        <v>45</v>
+      </c>
+      <c r="D10" s="18">
+        <v>-45</v>
+      </c>
       <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="3"/>
+      <c r="F10" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
+      <c r="B11" s="21">
+        <v>0</v>
+      </c>
+      <c r="C11" s="21">
+        <v>0</v>
+      </c>
+      <c r="D11" s="21">
+        <v>0</v>
+      </c>
       <c r="E11" s="29"/>
       <c r="F11" s="29"/>
       <c r="G11" s="5"/>
@@ -14388,163 +14508,309 @@
       <c r="A12" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
+      <c r="B12" s="23">
+        <v>12</v>
+      </c>
+      <c r="C12" s="23">
+        <v>30</v>
+      </c>
+      <c r="D12" s="23">
+        <v>-18</v>
+      </c>
       <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="7"/>
+      <c r="F12" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="30"/>
+      <c r="B13" s="23">
+        <v>201</v>
+      </c>
+      <c r="C13" s="23">
+        <v>98</v>
+      </c>
+      <c r="D13" s="23">
+        <v>103</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>61</v>
+      </c>
       <c r="F13" s="30"/>
-      <c r="G13" s="7"/>
+      <c r="G13" s="7" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
+      <c r="B14" s="23">
+        <v>142</v>
+      </c>
+      <c r="C14" s="23">
+        <v>315</v>
+      </c>
+      <c r="D14" s="23">
+        <v>-173</v>
+      </c>
       <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="7"/>
+      <c r="F14" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
+      <c r="B15" s="23">
+        <v>105</v>
+      </c>
+      <c r="C15" s="23">
+        <v>121</v>
+      </c>
+      <c r="D15" s="23">
+        <v>-16</v>
+      </c>
       <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="7"/>
+      <c r="F15" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
+      <c r="B16" s="18">
+        <v>55</v>
+      </c>
+      <c r="C16" s="18">
+        <v>178</v>
+      </c>
+      <c r="D16" s="18">
+        <v>-123</v>
+      </c>
       <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="3"/>
+      <c r="F16" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="29"/>
+      <c r="B17" s="21">
+        <v>650</v>
+      </c>
+      <c r="C17" s="21">
+        <v>519</v>
+      </c>
+      <c r="D17" s="21">
+        <v>131</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F17" s="29"/>
-      <c r="G17" s="5"/>
+      <c r="G17" s="5" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
+      <c r="B18" s="18">
+        <v>22</v>
+      </c>
+      <c r="C18" s="18">
+        <v>106</v>
+      </c>
+      <c r="D18" s="18">
+        <v>-84</v>
+      </c>
       <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="3"/>
+      <c r="F18" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="29"/>
+      <c r="B19" s="21">
+        <v>638</v>
+      </c>
+      <c r="C19" s="21">
+        <v>547</v>
+      </c>
+      <c r="D19" s="21">
+        <v>91</v>
+      </c>
+      <c r="E19" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F19" s="29"/>
-      <c r="G19" s="5"/>
+      <c r="G19" s="5" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
+      <c r="B20" s="18">
+        <v>3</v>
+      </c>
+      <c r="C20" s="18">
+        <v>90</v>
+      </c>
+      <c r="D20" s="18">
+        <v>-87</v>
+      </c>
       <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="3"/>
+      <c r="F20" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="29"/>
+      <c r="B21" s="21">
+        <v>516</v>
+      </c>
+      <c r="C21" s="21">
+        <v>472</v>
+      </c>
+      <c r="D21" s="21">
+        <v>44</v>
+      </c>
+      <c r="E21" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F21" s="29"/>
-      <c r="G21" s="5"/>
+      <c r="G21" s="5" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
+      <c r="B22" s="18">
+        <v>34</v>
+      </c>
+      <c r="C22" s="18">
+        <v>53</v>
+      </c>
+      <c r="D22" s="18">
+        <v>-19</v>
+      </c>
       <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="3"/>
+      <c r="F22" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="29"/>
+      <c r="B23" s="21">
+        <v>726</v>
+      </c>
+      <c r="C23" s="21">
+        <v>436</v>
+      </c>
+      <c r="D23" s="21">
+        <v>290</v>
+      </c>
+      <c r="E23" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F23" s="29"/>
-      <c r="G23" s="5"/>
+      <c r="G23" s="5" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="28"/>
+      <c r="B24" s="18">
+        <v>1822</v>
+      </c>
+      <c r="C24" s="18">
+        <v>1430</v>
+      </c>
+      <c r="D24" s="18">
+        <v>392</v>
+      </c>
+      <c r="E24" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F24" s="28"/>
-      <c r="G24" s="3"/>
+      <c r="G24" s="3" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
+      <c r="B25" s="21">
+        <v>128</v>
+      </c>
+      <c r="C25" s="21">
+        <v>378</v>
+      </c>
+      <c r="D25" s="21">
+        <v>-250</v>
+      </c>
       <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="5"/>
+      <c r="F25" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="26" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
+      <c r="B26" s="18">
+        <v>0</v>
+      </c>
+      <c r="C26" s="18">
+        <v>0</v>
+      </c>
+      <c r="D26" s="18">
+        <v>0</v>
+      </c>
       <c r="E26" s="28"/>
       <c r="F26" s="28"/>
       <c r="G26" s="3"/>
@@ -14553,185 +14819,351 @@
       <c r="A27" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="29"/>
+      <c r="B27" s="21">
+        <v>300</v>
+      </c>
+      <c r="C27" s="21">
+        <v>224</v>
+      </c>
+      <c r="D27" s="21">
+        <v>76</v>
+      </c>
+      <c r="E27" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F27" s="29"/>
-      <c r="G27" s="5"/>
+      <c r="G27" s="5" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="28"/>
+      <c r="B28" s="18">
+        <v>66</v>
+      </c>
+      <c r="C28" s="18">
+        <v>49</v>
+      </c>
+      <c r="D28" s="18">
+        <v>17</v>
+      </c>
+      <c r="E28" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F28" s="28"/>
-      <c r="G28" s="3"/>
+      <c r="G28" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="29"/>
+      <c r="B29" s="21">
+        <v>539</v>
+      </c>
+      <c r="C29" s="21">
+        <v>488</v>
+      </c>
+      <c r="D29" s="21">
+        <v>51</v>
+      </c>
+      <c r="E29" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F29" s="29"/>
-      <c r="G29" s="5"/>
+      <c r="G29" s="5" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="30" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="28"/>
+      <c r="B30" s="18">
+        <v>55</v>
+      </c>
+      <c r="C30" s="18">
+        <v>35</v>
+      </c>
+      <c r="D30" s="18">
+        <v>20</v>
+      </c>
+      <c r="E30" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F30" s="28"/>
-      <c r="G30" s="3"/>
+      <c r="G30" s="3" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
+      <c r="B31" s="21">
+        <v>68</v>
+      </c>
+      <c r="C31" s="21">
+        <v>319</v>
+      </c>
+      <c r="D31" s="21">
+        <v>-251</v>
+      </c>
       <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="5"/>
+      <c r="F31" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="32" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
+      <c r="B32" s="18">
+        <v>539</v>
+      </c>
+      <c r="C32" s="18">
+        <v>540</v>
+      </c>
+      <c r="D32" s="18">
+        <v>-1</v>
+      </c>
       <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="3"/>
+      <c r="F32" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="33" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
+      <c r="B33" s="21">
+        <v>456</v>
+      </c>
+      <c r="C33" s="21">
+        <v>579</v>
+      </c>
+      <c r="D33" s="21">
+        <v>-123</v>
+      </c>
       <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="5"/>
+      <c r="F33" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="34" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="28"/>
+      <c r="B34" s="18">
+        <v>226</v>
+      </c>
+      <c r="C34" s="18">
+        <v>119</v>
+      </c>
+      <c r="D34" s="18">
+        <v>107</v>
+      </c>
+      <c r="E34" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F34" s="28"/>
-      <c r="G34" s="3"/>
+      <c r="G34" s="3" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="29"/>
+      <c r="B35" s="21">
+        <v>1238</v>
+      </c>
+      <c r="C35" s="21">
+        <v>989</v>
+      </c>
+      <c r="D35" s="21">
+        <v>249</v>
+      </c>
+      <c r="E35" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F35" s="29"/>
-      <c r="G35" s="5"/>
+      <c r="G35" s="5" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="36" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
+      <c r="B36" s="18">
+        <v>209</v>
+      </c>
+      <c r="C36" s="18">
+        <v>461</v>
+      </c>
+      <c r="D36" s="18">
+        <v>-252</v>
+      </c>
       <c r="E36" s="28"/>
-      <c r="F36" s="28"/>
-      <c r="G36" s="3"/>
+      <c r="F36" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="29"/>
+      <c r="B37" s="21">
+        <v>502</v>
+      </c>
+      <c r="C37" s="21">
+        <v>362</v>
+      </c>
+      <c r="D37" s="21">
+        <v>140</v>
+      </c>
+      <c r="E37" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F37" s="29"/>
-      <c r="G37" s="5"/>
+      <c r="G37" s="5" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
+      <c r="B38" s="18">
+        <v>13</v>
+      </c>
+      <c r="C38" s="18">
+        <v>177</v>
+      </c>
+      <c r="D38" s="18">
+        <v>-164</v>
+      </c>
       <c r="E38" s="28"/>
-      <c r="F38" s="28"/>
-      <c r="G38" s="3"/>
+      <c r="F38" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="B39" s="25"/>
-      <c r="C39" s="25"/>
-      <c r="D39" s="25"/>
+      <c r="B39" s="25">
+        <v>9</v>
+      </c>
+      <c r="C39" s="25">
+        <v>28</v>
+      </c>
+      <c r="D39" s="25">
+        <v>-19</v>
+      </c>
       <c r="E39" s="31"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="9"/>
+      <c r="F39" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="B40" s="25"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
+      <c r="B40" s="25">
+        <v>24</v>
+      </c>
+      <c r="C40" s="25">
+        <v>49</v>
+      </c>
+      <c r="D40" s="25">
+        <v>-25</v>
+      </c>
       <c r="E40" s="31"/>
-      <c r="F40" s="31"/>
-      <c r="G40" s="9"/>
+      <c r="F40" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
+      <c r="B41" s="25">
+        <v>1</v>
+      </c>
+      <c r="C41" s="25">
+        <v>13</v>
+      </c>
+      <c r="D41" s="25">
+        <v>-12</v>
+      </c>
       <c r="E41" s="31"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="9"/>
+      <c r="F41" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="42" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="B42" s="25"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="25"/>
-      <c r="E42" s="31"/>
+      <c r="B42" s="25">
+        <v>19</v>
+      </c>
+      <c r="C42" s="25">
+        <v>11</v>
+      </c>
+      <c r="D42" s="25">
+        <v>8</v>
+      </c>
+      <c r="E42" s="31" t="s">
+        <v>61</v>
+      </c>
       <c r="F42" s="31"/>
-      <c r="G42" s="9"/>
+      <c r="G42" s="9" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="B43" s="25"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
+      <c r="B43" s="25">
+        <v>0</v>
+      </c>
+      <c r="C43" s="25">
+        <v>0</v>
+      </c>
+      <c r="D43" s="25">
+        <v>0</v>
+      </c>
       <c r="E43" s="31"/>
       <c r="F43" s="31"/>
       <c r="G43" s="9"/>
@@ -14740,133 +15172,253 @@
       <c r="A44" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="B44" s="21"/>
-      <c r="C44" s="21"/>
-      <c r="D44" s="21"/>
-      <c r="E44" s="29"/>
+      <c r="B44" s="21">
+        <v>70</v>
+      </c>
+      <c r="C44" s="21">
+        <v>55</v>
+      </c>
+      <c r="D44" s="21">
+        <v>15</v>
+      </c>
+      <c r="E44" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F44" s="29"/>
-      <c r="G44" s="5"/>
+      <c r="G44" s="5" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="45" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
+      <c r="B45" s="18">
+        <v>70</v>
+      </c>
+      <c r="C45" s="18">
+        <v>125</v>
+      </c>
+      <c r="D45" s="18">
+        <v>-55</v>
+      </c>
       <c r="E45" s="28"/>
-      <c r="F45" s="28"/>
-      <c r="G45" s="3"/>
+      <c r="F45" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="46" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="B46" s="21"/>
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
+      <c r="B46" s="21">
+        <v>543</v>
+      </c>
+      <c r="C46" s="21">
+        <v>651</v>
+      </c>
+      <c r="D46" s="21">
+        <v>-108</v>
+      </c>
       <c r="E46" s="29"/>
-      <c r="F46" s="29"/>
-      <c r="G46" s="5"/>
+      <c r="F46" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="47" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="28"/>
+      <c r="B47" s="18">
+        <v>859</v>
+      </c>
+      <c r="C47" s="18">
+        <v>591</v>
+      </c>
+      <c r="D47" s="18">
+        <v>268</v>
+      </c>
+      <c r="E47" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F47" s="28"/>
-      <c r="G47" s="3"/>
+      <c r="G47" s="3" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="B48" s="21"/>
-      <c r="C48" s="21"/>
-      <c r="D48" s="21"/>
+      <c r="B48" s="21">
+        <v>227</v>
+      </c>
+      <c r="C48" s="21">
+        <v>654</v>
+      </c>
+      <c r="D48" s="21">
+        <v>-427</v>
+      </c>
       <c r="E48" s="29"/>
-      <c r="F48" s="29"/>
-      <c r="G48" s="5"/>
+      <c r="F48" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B49" s="18"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="18"/>
-      <c r="E49" s="28"/>
+      <c r="B49" s="18">
+        <v>394</v>
+      </c>
+      <c r="C49" s="18">
+        <v>272</v>
+      </c>
+      <c r="D49" s="18">
+        <v>122</v>
+      </c>
+      <c r="E49" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F49" s="28"/>
-      <c r="G49" s="3"/>
+      <c r="G49" s="3" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="B50" s="21"/>
-      <c r="C50" s="21"/>
-      <c r="D50" s="21"/>
-      <c r="E50" s="29"/>
+      <c r="B50" s="21">
+        <v>991</v>
+      </c>
+      <c r="C50" s="21">
+        <v>653</v>
+      </c>
+      <c r="D50" s="21">
+        <v>338</v>
+      </c>
+      <c r="E50" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F50" s="29"/>
-      <c r="G50" s="5"/>
+      <c r="G50" s="5" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B51" s="18"/>
-      <c r="C51" s="18"/>
-      <c r="D51" s="18"/>
-      <c r="E51" s="28"/>
+      <c r="B51" s="18">
+        <v>246</v>
+      </c>
+      <c r="C51" s="18">
+        <v>154</v>
+      </c>
+      <c r="D51" s="18">
+        <v>92</v>
+      </c>
+      <c r="E51" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F51" s="28"/>
-      <c r="G51" s="3"/>
+      <c r="G51" s="3" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="52" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="B52" s="21"/>
-      <c r="C52" s="21"/>
-      <c r="D52" s="21"/>
+      <c r="B52" s="21">
+        <v>347</v>
+      </c>
+      <c r="C52" s="21">
+        <v>514</v>
+      </c>
+      <c r="D52" s="21">
+        <v>-167</v>
+      </c>
       <c r="E52" s="29"/>
-      <c r="F52" s="29"/>
-      <c r="G52" s="5"/>
+      <c r="F52" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="53" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B53" s="18"/>
-      <c r="C53" s="18"/>
-      <c r="D53" s="18"/>
+      <c r="B53" s="18">
+        <v>154</v>
+      </c>
+      <c r="C53" s="18">
+        <v>257</v>
+      </c>
+      <c r="D53" s="18">
+        <v>-103</v>
+      </c>
       <c r="E53" s="28"/>
-      <c r="F53" s="28"/>
-      <c r="G53" s="3"/>
+      <c r="F53" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="54" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="B54" s="21"/>
-      <c r="C54" s="21"/>
-      <c r="D54" s="21"/>
+      <c r="B54" s="21">
+        <v>32</v>
+      </c>
+      <c r="C54" s="21">
+        <v>199</v>
+      </c>
+      <c r="D54" s="21">
+        <v>-167</v>
+      </c>
       <c r="E54" s="29"/>
-      <c r="F54" s="29"/>
-      <c r="G54" s="5"/>
+      <c r="F54" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="55" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="B55" s="27"/>
-      <c r="C55" s="27"/>
-      <c r="D55" s="27"/>
-      <c r="E55" s="32"/>
+      <c r="B55" s="27">
+        <v>259</v>
+      </c>
+      <c r="C55" s="27">
+        <v>193</v>
+      </c>
+      <c r="D55" s="27">
+        <v>66</v>
+      </c>
+      <c r="E55" s="32" t="s">
+        <v>61</v>
+      </c>
       <c r="F55" s="32"/>
-      <c r="G55" s="11"/>
+      <c r="G55" s="11" t="s">
+        <v>46</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G55" xr:uid="{00000000-0009-0000-0000-000008000000}"/>

</xml_diff>

<commit_message>
Update files for September, 2023
</commit_message>
<xml_diff>
--- a/statistics_files/2023/2023.g.net_borrower_lender.xlsx
+++ b/statistics_files/2023/2023.g.net_borrower_lender.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20402"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\GitHub\next_statistics\statistics_files\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0949BD9-B619-4823-85CC-52970FAA69F7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35732D75-A9C1-4A6B-A198-00DB7DDDD321}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" tabRatio="673" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1617" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1717" uniqueCount="252">
   <si>
     <t>NET</t>
   </si>
@@ -790,6 +790,24 @@
   </si>
   <si>
     <t>1.60 : 1</t>
+  </si>
+  <si>
+    <t>0.30 : 1</t>
+  </si>
+  <si>
+    <t>1.43 : 1</t>
+  </si>
+  <si>
+    <t>0.05 : 1</t>
+  </si>
+  <si>
+    <t>1.87 : 1</t>
+  </si>
+  <si>
+    <t>1.76 : 1</t>
+  </si>
+  <si>
+    <t>0.46 : 1</t>
   </si>
 </sst>
 </file>
@@ -1699,15 +1717,15 @@
       </c>
       <c r="B2" s="2">
         <f>January!B2+February!B2+March!B2+April!B2+May!B2+June!B2+July!B2+August!B2+September!B2+October!B2+November!B2+December!B2</f>
-        <v>12299</v>
+        <v>13885</v>
       </c>
       <c r="C2" s="2">
         <f>January!C2+February!C2+March!C2+April!C2+May!C2+June!C2+July!C2+August!C2+September!C2+October!C2+November!C2+December!C2</f>
-        <v>9403</v>
+        <v>10581</v>
       </c>
       <c r="D2" s="2">
         <f>January!D2+February!D2+March!D2+April!D2+May!D2+June!D2+July!D2+August!D2+September!D2+October!D2+November!D2+December!D2</f>
-        <v>2896</v>
+        <v>3304</v>
       </c>
       <c r="E2" s="28" t="str">
         <f>IF(D2 &gt; 0, "We borrowed more than we lent this year", "")</f>
@@ -1728,15 +1746,15 @@
       </c>
       <c r="B3" s="4">
         <f>January!B3+February!B3+March!B3+April!B3+May!B3+June!B3+July!B3+August!B3+September!B3+October!B3+November!B3+December!B3</f>
-        <v>4042</v>
+        <v>4862</v>
       </c>
       <c r="C3" s="4">
         <f>January!C3+February!C3+March!C3+April!C3+May!C3+June!C3+July!C3+August!C3+September!C3+October!C3+November!C3+December!C3</f>
-        <v>3855</v>
+        <v>4392</v>
       </c>
       <c r="D3" s="4">
         <f>January!D3+February!D3+March!D3+April!D3+May!D3+June!D3+July!D3+August!D3+September!D3+October!D3+November!D3+December!D3</f>
-        <v>187</v>
+        <v>470</v>
       </c>
       <c r="E3" s="29" t="str">
         <f t="shared" ref="E3:E55" si="1">IF(D3 &gt; 0, "We borrowed more than we lent this year", "")</f>
@@ -1748,7 +1766,7 @@
       </c>
       <c r="G3" s="5" t="str">
         <f t="shared" ref="G3:G55" si="2">IF(ISERROR(ROUND(B3/C3,2)&amp;" : 1"), "", ROUND(B3/C3,2)&amp;" : 1")</f>
-        <v>1.05 : 1</v>
+        <v>1.11 : 1</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1757,15 +1775,15 @@
       </c>
       <c r="B4" s="2">
         <f>January!B4+February!B4+March!B4+April!B4+May!B4+June!B4+July!B4+August!B4+September!B4+October!B4+November!B4+December!B4</f>
-        <v>10700</v>
+        <v>11963</v>
       </c>
       <c r="C4" s="2">
         <f>January!C4+February!C4+March!C4+April!C4+May!C4+June!C4+July!C4+August!C4+September!C4+October!C4+November!C4+December!C4</f>
-        <v>9919</v>
+        <v>11285</v>
       </c>
       <c r="D4" s="2">
         <f>January!D4+February!D4+March!D4+April!D4+May!D4+June!D4+July!D4+August!D4+September!D4+October!D4+November!D4+December!D4</f>
-        <v>781</v>
+        <v>678</v>
       </c>
       <c r="E4" s="28" t="str">
         <f t="shared" si="1"/>
@@ -1777,7 +1795,7 @@
       </c>
       <c r="G4" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.08 : 1</v>
+        <v>1.06 : 1</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1786,15 +1804,15 @@
       </c>
       <c r="B5" s="4">
         <f>January!B5+February!B5+March!B5+April!B5+May!B5+June!B5+July!B5+August!B5+September!B5+October!B5+November!B5+December!B5</f>
-        <v>640</v>
+        <v>764</v>
       </c>
       <c r="C5" s="4">
         <f>January!C5+February!C5+March!C5+April!C5+May!C5+June!C5+July!C5+August!C5+September!C5+October!C5+November!C5+December!C5</f>
-        <v>986</v>
+        <v>1133</v>
       </c>
       <c r="D5" s="4">
         <f>January!D5+February!D5+March!D5+April!D5+May!D5+June!D5+July!D5+August!D5+September!D5+October!D5+November!D5+December!D5</f>
-        <v>-346</v>
+        <v>-369</v>
       </c>
       <c r="E5" s="29" t="str">
         <f t="shared" si="1"/>
@@ -1806,7 +1824,7 @@
       </c>
       <c r="G5" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.65 : 1</v>
+        <v>0.67 : 1</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1815,15 +1833,15 @@
       </c>
       <c r="B6" s="2">
         <f>January!B6+February!B6+March!B6+April!B6+May!B6+June!B6+July!B6+August!B6+September!B6+October!B6+November!B6+December!B6</f>
-        <v>10060</v>
+        <v>11375</v>
       </c>
       <c r="C6" s="2">
         <f>January!C6+February!C6+March!C6+April!C6+May!C6+June!C6+July!C6+August!C6+September!C6+October!C6+November!C6+December!C6</f>
-        <v>11736</v>
+        <v>13255</v>
       </c>
       <c r="D6" s="2">
         <f>January!D6+February!D6+March!D6+April!D6+May!D6+June!D6+July!D6+August!D6+September!D6+October!D6+November!D6+December!D6</f>
-        <v>-1676</v>
+        <v>-1880</v>
       </c>
       <c r="E6" s="28" t="str">
         <f t="shared" si="1"/>
@@ -1844,15 +1862,15 @@
       </c>
       <c r="B7" s="4">
         <f>January!B7+February!B7+March!B7+April!B7+May!B7+June!B7+July!B7+August!B7+September!B7+October!B7+November!B7+December!B7</f>
-        <v>1714</v>
+        <v>1886</v>
       </c>
       <c r="C7" s="4">
         <f>January!C7+February!C7+March!C7+April!C7+May!C7+June!C7+July!C7+August!C7+September!C7+October!C7+November!C7+December!C7</f>
-        <v>1810</v>
+        <v>2035</v>
       </c>
       <c r="D7" s="4">
         <f>January!D7+February!D7+March!D7+April!D7+May!D7+June!D7+July!D7+August!D7+September!D7+October!D7+November!D7+December!D7</f>
-        <v>-96</v>
+        <v>-149</v>
       </c>
       <c r="E7" s="29" t="str">
         <f t="shared" si="1"/>
@@ -1864,7 +1882,7 @@
       </c>
       <c r="G7" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.95 : 1</v>
+        <v>0.93 : 1</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1873,15 +1891,15 @@
       </c>
       <c r="B8" s="2">
         <f>January!B8+February!B8+March!B8+April!B8+May!B8+June!B8+July!B8+August!B8+September!B8+October!B8+November!B8+December!B8</f>
-        <v>1056</v>
+        <v>1219</v>
       </c>
       <c r="C8" s="2">
         <f>January!C8+February!C8+March!C8+April!C8+May!C8+June!C8+July!C8+August!C8+September!C8+October!C8+November!C8+December!C8</f>
-        <v>1546</v>
+        <v>1686</v>
       </c>
       <c r="D8" s="2">
         <f>January!D8+February!D8+March!D8+April!D8+May!D8+June!D8+July!D8+August!D8+September!D8+October!D8+November!D8+December!D8</f>
-        <v>-490</v>
+        <v>-467</v>
       </c>
       <c r="E8" s="28" t="str">
         <f t="shared" si="1"/>
@@ -1893,7 +1911,7 @@
       </c>
       <c r="G8" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.68 : 1</v>
+        <v>0.72 : 1</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1902,15 +1920,15 @@
       </c>
       <c r="B9" s="4">
         <f>January!B9+February!B9+March!B9+April!B9+May!B9+June!B9+July!B9+August!B9+September!B9+October!B9+November!B9+December!B9</f>
-        <v>419</v>
+        <v>456</v>
       </c>
       <c r="C9" s="4">
         <f>January!C9+February!C9+March!C9+April!C9+May!C9+June!C9+July!C9+August!C9+September!C9+October!C9+November!C9+December!C9</f>
-        <v>567</v>
+        <v>634</v>
       </c>
       <c r="D9" s="4">
         <f>January!D9+February!D9+March!D9+April!D9+May!D9+June!D9+July!D9+August!D9+September!D9+October!D9+November!D9+December!D9</f>
-        <v>-148</v>
+        <v>-178</v>
       </c>
       <c r="E9" s="29" t="str">
         <f t="shared" si="1"/>
@@ -1922,7 +1940,7 @@
       </c>
       <c r="G9" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.74 : 1</v>
+        <v>0.72 : 1</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1935,11 +1953,11 @@
       </c>
       <c r="C10" s="2">
         <f>January!C10+February!C10+March!C10+April!C10+May!C10+June!C10+July!C10+August!C10+September!C10+October!C10+November!C10+December!C10</f>
-        <v>298</v>
+        <v>356</v>
       </c>
       <c r="D10" s="2">
         <f>January!D10+February!D10+March!D10+April!D10+May!D10+June!D10+July!D10+August!D10+September!D10+October!D10+November!D10+December!D10</f>
-        <v>-259</v>
+        <v>-317</v>
       </c>
       <c r="E10" s="28" t="str">
         <f t="shared" si="1"/>
@@ -1951,7 +1969,7 @@
       </c>
       <c r="G10" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.13 : 1</v>
+        <v>0.11 : 1</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1989,15 +2007,15 @@
       </c>
       <c r="B12" s="6">
         <f>January!B12+February!B12+March!B12+April!B12+May!B12+June!B12+July!B12+August!B12+September!B12+October!B12+November!B12+December!B12</f>
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="C12" s="6">
         <f>January!C12+February!C12+March!C12+April!C12+May!C12+June!C12+July!C12+August!C12+September!C12+October!C12+November!C12+December!C12</f>
-        <v>173</v>
+        <v>210</v>
       </c>
       <c r="D12" s="6">
         <f>January!D12+February!D12+March!D12+April!D12+May!D12+June!D12+July!D12+August!D12+September!D12+October!D12+November!D12+December!D12</f>
-        <v>-45</v>
+        <v>-71</v>
       </c>
       <c r="E12" s="30" t="str">
         <f t="shared" si="1"/>
@@ -2009,7 +2027,7 @@
       </c>
       <c r="G12" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0.74 : 1</v>
+        <v>0.66 : 1</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2018,15 +2036,15 @@
       </c>
       <c r="B13" s="6">
         <f>January!B13+February!B13+March!B13+April!B13+May!B13+June!B13+July!B13+August!B13+September!B13+October!B13+November!B13+December!B13</f>
-        <v>1109</v>
+        <v>1257</v>
       </c>
       <c r="C13" s="6">
         <f>January!C13+February!C13+March!C13+April!C13+May!C13+June!C13+July!C13+August!C13+September!C13+October!C13+November!C13+December!C13</f>
-        <v>701</v>
+        <v>812</v>
       </c>
       <c r="D13" s="6">
         <f>January!D13+February!D13+March!D13+April!D13+May!D13+June!D13+July!D13+August!D13+September!D13+October!D13+November!D13+December!D13</f>
-        <v>408</v>
+        <v>445</v>
       </c>
       <c r="E13" s="30" t="str">
         <f t="shared" si="1"/>
@@ -2038,7 +2056,7 @@
       </c>
       <c r="G13" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>1.58 : 1</v>
+        <v>1.55 : 1</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2047,15 +2065,15 @@
       </c>
       <c r="B14" s="6">
         <f>January!B14+February!B14+March!B14+April!B14+May!B14+June!B14+July!B14+August!B14+September!B14+October!B14+November!B14+December!B14</f>
-        <v>1088</v>
+        <v>1196</v>
       </c>
       <c r="C14" s="6">
         <f>January!C14+February!C14+March!C14+April!C14+May!C14+June!C14+July!C14+August!C14+September!C14+October!C14+November!C14+December!C14</f>
-        <v>2350</v>
+        <v>2647</v>
       </c>
       <c r="D14" s="6">
         <f>January!D14+February!D14+March!D14+April!D14+May!D14+June!D14+July!D14+August!D14+September!D14+October!D14+November!D14+December!D14</f>
-        <v>-1262</v>
+        <v>-1451</v>
       </c>
       <c r="E14" s="30" t="str">
         <f t="shared" si="1"/>
@@ -2067,7 +2085,7 @@
       </c>
       <c r="G14" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0.46 : 1</v>
+        <v>0.45 : 1</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2076,15 +2094,15 @@
       </c>
       <c r="B15" s="6">
         <f>January!B15+February!B15+March!B15+April!B15+May!B15+June!B15+July!B15+August!B15+September!B15+October!B15+November!B15+December!B15</f>
-        <v>677</v>
+        <v>804</v>
       </c>
       <c r="C15" s="6">
         <f>January!C15+February!C15+March!C15+April!C15+May!C15+June!C15+July!C15+August!C15+September!C15+October!C15+November!C15+December!C15</f>
-        <v>828</v>
+        <v>925</v>
       </c>
       <c r="D15" s="6">
         <f>January!D15+February!D15+March!D15+April!D15+May!D15+June!D15+July!D15+August!D15+September!D15+October!D15+November!D15+December!D15</f>
-        <v>-151</v>
+        <v>-121</v>
       </c>
       <c r="E15" s="30" t="str">
         <f t="shared" si="1"/>
@@ -2096,7 +2114,7 @@
       </c>
       <c r="G15" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0.82 : 1</v>
+        <v>0.87 : 1</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2105,15 +2123,15 @@
       </c>
       <c r="B16" s="2">
         <f>January!B16+February!B16+March!B16+April!B16+May!B16+June!B16+July!B16+August!B16+September!B16+October!B16+November!B16+December!B16</f>
-        <v>318</v>
+        <v>353</v>
       </c>
       <c r="C16" s="2">
         <f>January!C16+February!C16+March!C16+April!C16+May!C16+June!C16+July!C16+August!C16+September!C16+October!C16+November!C16+December!C16</f>
-        <v>1227</v>
+        <v>1385</v>
       </c>
       <c r="D16" s="2">
         <f>January!D16+February!D16+March!D16+April!D16+May!D16+June!D16+July!D16+August!D16+September!D16+October!D16+November!D16+December!D16</f>
-        <v>-909</v>
+        <v>-1032</v>
       </c>
       <c r="E16" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2125,7 +2143,7 @@
       </c>
       <c r="G16" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.26 : 1</v>
+        <v>0.25 : 1</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2134,15 +2152,15 @@
       </c>
       <c r="B17" s="4">
         <f>January!B17+February!B17+March!B17+April!B17+May!B17+June!B17+July!B17+August!B17+September!B17+October!B17+November!B17+December!B17</f>
-        <v>4805</v>
+        <v>5546</v>
       </c>
       <c r="C17" s="4">
         <f>January!C17+February!C17+March!C17+April!C17+May!C17+June!C17+July!C17+August!C17+September!C17+October!C17+November!C17+December!C17</f>
-        <v>3811</v>
+        <v>4328</v>
       </c>
       <c r="D17" s="4">
         <f>January!D17+February!D17+March!D17+April!D17+May!D17+June!D17+July!D17+August!D17+September!D17+October!D17+November!D17+December!D17</f>
-        <v>994</v>
+        <v>1218</v>
       </c>
       <c r="E17" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2154,7 +2172,7 @@
       </c>
       <c r="G17" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.26 : 1</v>
+        <v>1.28 : 1</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2163,15 +2181,15 @@
       </c>
       <c r="B18" s="2">
         <f>January!B18+February!B18+March!B18+April!B18+May!B18+June!B18+July!B18+August!B18+September!B18+October!B18+November!B18+December!B18</f>
-        <v>744</v>
+        <v>832</v>
       </c>
       <c r="C18" s="2">
         <f>January!C18+February!C18+March!C18+April!C18+May!C18+June!C18+July!C18+August!C18+September!C18+October!C18+November!C18+December!C18</f>
-        <v>799</v>
+        <v>906</v>
       </c>
       <c r="D18" s="2">
         <f>January!D18+February!D18+March!D18+April!D18+May!D18+June!D18+July!D18+August!D18+September!D18+October!D18+November!D18+December!D18</f>
-        <v>-55</v>
+        <v>-74</v>
       </c>
       <c r="E18" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2183,7 +2201,7 @@
       </c>
       <c r="G18" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.93 : 1</v>
+        <v>0.92 : 1</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2192,15 +2210,15 @@
       </c>
       <c r="B19" s="4">
         <f>January!B19+February!B19+March!B19+April!B19+May!B19+June!B19+July!B19+August!B19+September!B19+October!B19+November!B19+December!B19</f>
-        <v>5250</v>
+        <v>5879</v>
       </c>
       <c r="C19" s="4">
         <f>January!C19+February!C19+March!C19+April!C19+May!C19+June!C19+July!C19+August!C19+September!C19+October!C19+November!C19+December!C19</f>
-        <v>3274</v>
+        <v>3773</v>
       </c>
       <c r="D19" s="4">
         <f>January!D19+February!D19+March!D19+April!D19+May!D19+June!D19+July!D19+August!D19+September!D19+October!D19+November!D19+December!D19</f>
-        <v>1976</v>
+        <v>2106</v>
       </c>
       <c r="E19" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2212,7 +2230,7 @@
       </c>
       <c r="G19" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.6 : 1</v>
+        <v>1.56 : 1</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2221,15 +2239,15 @@
       </c>
       <c r="B20" s="2">
         <f>January!B20+February!B20+March!B20+April!B20+May!B20+June!B20+July!B20+August!B20+September!B20+October!B20+November!B20+December!B20</f>
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C20" s="2">
         <f>January!C20+February!C20+March!C20+April!C20+May!C20+June!C20+July!C20+August!C20+September!C20+October!C20+November!C20+December!C20</f>
-        <v>535</v>
+        <v>609</v>
       </c>
       <c r="D20" s="2">
         <f>January!D20+February!D20+March!D20+April!D20+May!D20+June!D20+July!D20+August!D20+September!D20+October!D20+November!D20+December!D20</f>
-        <v>-514</v>
+        <v>-584</v>
       </c>
       <c r="E20" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2250,15 +2268,15 @@
       </c>
       <c r="B21" s="4">
         <f>January!B21+February!B21+March!B21+April!B21+May!B21+June!B21+July!B21+August!B21+September!B21+October!B21+November!B21+December!B21</f>
-        <v>4141</v>
+        <v>4577</v>
       </c>
       <c r="C21" s="4">
         <f>January!C21+February!C21+March!C21+April!C21+May!C21+June!C21+July!C21+August!C21+September!C21+October!C21+November!C21+December!C21</f>
-        <v>3370</v>
+        <v>3803</v>
       </c>
       <c r="D21" s="4">
         <f>January!D21+February!D21+March!D21+April!D21+May!D21+June!D21+July!D21+August!D21+September!D21+October!D21+November!D21+December!D21</f>
-        <v>771</v>
+        <v>774</v>
       </c>
       <c r="E21" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2270,7 +2288,7 @@
       </c>
       <c r="G21" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.23 : 1</v>
+        <v>1.2 : 1</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2279,15 +2297,15 @@
       </c>
       <c r="B22" s="2">
         <f>January!B22+February!B22+March!B22+April!B22+May!B22+June!B22+July!B22+August!B22+September!B22+October!B22+November!B22+December!B22</f>
-        <v>207</v>
+        <v>245</v>
       </c>
       <c r="C22" s="2">
         <f>January!C22+February!C22+March!C22+April!C22+May!C22+June!C22+July!C22+August!C22+September!C22+October!C22+November!C22+December!C22</f>
-        <v>573</v>
+        <v>663</v>
       </c>
       <c r="D22" s="2">
         <f>January!D22+February!D22+March!D22+April!D22+May!D22+June!D22+July!D22+August!D22+September!D22+October!D22+November!D22+December!D22</f>
-        <v>-366</v>
+        <v>-418</v>
       </c>
       <c r="E22" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2299,7 +2317,7 @@
       </c>
       <c r="G22" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.36 : 1</v>
+        <v>0.37 : 1</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2308,15 +2326,15 @@
       </c>
       <c r="B23" s="4">
         <f>January!B23+February!B23+March!B23+April!B23+May!B23+June!B23+July!B23+August!B23+September!B23+October!B23+November!B23+December!B23</f>
-        <v>5600</v>
+        <v>6324</v>
       </c>
       <c r="C23" s="4">
         <f>January!C23+February!C23+March!C23+April!C23+May!C23+June!C23+July!C23+August!C23+September!C23+October!C23+November!C23+December!C23</f>
-        <v>3970</v>
+        <v>4358</v>
       </c>
       <c r="D23" s="4">
         <f>January!D23+February!D23+March!D23+April!D23+May!D23+June!D23+July!D23+August!D23+September!D23+October!D23+November!D23+December!D23</f>
-        <v>1630</v>
+        <v>1966</v>
       </c>
       <c r="E23" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2328,7 +2346,7 @@
       </c>
       <c r="G23" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.41 : 1</v>
+        <v>1.45 : 1</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2337,15 +2355,15 @@
       </c>
       <c r="B24" s="2">
         <f>January!B24+February!B24+March!B24+April!B24+May!B24+June!B24+July!B24+August!B24+September!B24+October!B24+November!B24+December!B24</f>
-        <v>14823</v>
+        <v>16820</v>
       </c>
       <c r="C24" s="2">
         <f>January!C24+February!C24+March!C24+April!C24+May!C24+June!C24+July!C24+August!C24+September!C24+October!C24+November!C24+December!C24</f>
-        <v>11161</v>
+        <v>12538</v>
       </c>
       <c r="D24" s="2">
         <f>January!D24+February!D24+March!D24+April!D24+May!D24+June!D24+July!D24+August!D24+September!D24+October!D24+November!D24+December!D24</f>
-        <v>3662</v>
+        <v>4282</v>
       </c>
       <c r="E24" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2357,7 +2375,7 @@
       </c>
       <c r="G24" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.33 : 1</v>
+        <v>1.34 : 1</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2366,15 +2384,15 @@
       </c>
       <c r="B25" s="4">
         <f>January!B25+February!B25+March!B25+April!B25+May!B25+June!B25+July!B25+August!B25+September!B25+October!B25+November!B25+December!B25</f>
-        <v>1408</v>
+        <v>1584</v>
       </c>
       <c r="C25" s="4">
         <f>January!C25+February!C25+March!C25+April!C25+May!C25+June!C25+July!C25+August!C25+September!C25+October!C25+November!C25+December!C25</f>
-        <v>2861</v>
+        <v>3229</v>
       </c>
       <c r="D25" s="4">
         <f>January!D25+February!D25+March!D25+April!D25+May!D25+June!D25+July!D25+August!D25+September!D25+October!D25+November!D25+December!D25</f>
-        <v>-1453</v>
+        <v>-1645</v>
       </c>
       <c r="E25" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2424,15 +2442,15 @@
       </c>
       <c r="B27" s="4">
         <f>January!B27+February!B27+March!B27+April!B27+May!B27+June!B27+July!B27+August!B27+September!B27+October!B27+November!B27+December!B27</f>
-        <v>2321</v>
+        <v>2497</v>
       </c>
       <c r="C27" s="4">
         <f>January!C27+February!C27+March!C27+April!C27+May!C27+June!C27+July!C27+August!C27+September!C27+October!C27+November!C27+December!C27</f>
-        <v>1580</v>
+        <v>1795</v>
       </c>
       <c r="D27" s="4">
         <f>January!D27+February!D27+March!D27+April!D27+May!D27+June!D27+July!D27+August!D27+September!D27+October!D27+November!D27+December!D27</f>
-        <v>741</v>
+        <v>702</v>
       </c>
       <c r="E27" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2444,7 +2462,7 @@
       </c>
       <c r="G27" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.47 : 1</v>
+        <v>1.39 : 1</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2453,15 +2471,15 @@
       </c>
       <c r="B28" s="2">
         <f>January!B28+February!B28+March!B28+April!B28+May!B28+June!B28+July!B28+August!B28+September!B28+October!B28+November!B28+December!B28</f>
-        <v>433</v>
+        <v>484</v>
       </c>
       <c r="C28" s="2">
         <f>January!C28+February!C28+March!C28+April!C28+May!C28+June!C28+July!C28+August!C28+September!C28+October!C28+November!C28+December!C28</f>
-        <v>589</v>
+        <v>661</v>
       </c>
       <c r="D28" s="2">
         <f>January!D28+February!D28+March!D28+April!D28+May!D28+June!D28+July!D28+August!D28+September!D28+October!D28+November!D28+December!D28</f>
-        <v>-156</v>
+        <v>-177</v>
       </c>
       <c r="E28" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2473,7 +2491,7 @@
       </c>
       <c r="G28" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.74 : 1</v>
+        <v>0.73 : 1</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2482,15 +2500,15 @@
       </c>
       <c r="B29" s="4">
         <f>January!B29+February!B29+March!B29+April!B29+May!B29+June!B29+July!B29+August!B29+September!B29+October!B29+November!B29+December!B29</f>
-        <v>4251</v>
+        <v>4814</v>
       </c>
       <c r="C29" s="4">
         <f>January!C29+February!C29+March!C29+April!C29+May!C29+June!C29+July!C29+August!C29+September!C29+October!C29+November!C29+December!C29</f>
-        <v>3717</v>
+        <v>4199</v>
       </c>
       <c r="D29" s="4">
         <f>January!D29+February!D29+March!D29+April!D29+May!D29+June!D29+July!D29+August!D29+September!D29+October!D29+November!D29+December!D29</f>
-        <v>534</v>
+        <v>615</v>
       </c>
       <c r="E29" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2502,7 +2520,7 @@
       </c>
       <c r="G29" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.14 : 1</v>
+        <v>1.15 : 1</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2511,11 +2529,11 @@
       </c>
       <c r="B30" s="2">
         <f>January!B30+February!B30+March!B30+April!B30+May!B30+June!B30+July!B30+August!B30+September!B30+October!B30+November!B30+December!B30</f>
-        <v>381</v>
+        <v>420</v>
       </c>
       <c r="C30" s="2">
         <f>January!C30+February!C30+March!C30+April!C30+May!C30+June!C30+July!C30+August!C30+September!C30+October!C30+November!C30+December!C30</f>
-        <v>282</v>
+        <v>321</v>
       </c>
       <c r="D30" s="2">
         <f>January!D30+February!D30+March!D30+April!D30+May!D30+June!D30+July!D30+August!D30+September!D30+October!D30+November!D30+December!D30</f>
@@ -2531,7 +2549,7 @@
       </c>
       <c r="G30" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.35 : 1</v>
+        <v>1.31 : 1</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2540,15 +2558,15 @@
       </c>
       <c r="B31" s="4">
         <f>January!B31+February!B31+March!B31+April!B31+May!B31+June!B31+July!B31+August!B31+September!B31+October!B31+November!B31+December!B31</f>
-        <v>596</v>
+        <v>672</v>
       </c>
       <c r="C31" s="4">
         <f>January!C31+February!C31+March!C31+April!C31+May!C31+June!C31+July!C31+August!C31+September!C31+October!C31+November!C31+December!C31</f>
-        <v>2447</v>
+        <v>2706</v>
       </c>
       <c r="D31" s="4">
         <f>January!D31+February!D31+March!D31+April!D31+May!D31+June!D31+July!D31+August!D31+September!D31+October!D31+November!D31+December!D31</f>
-        <v>-1851</v>
+        <v>-2034</v>
       </c>
       <c r="E31" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2560,7 +2578,7 @@
       </c>
       <c r="G31" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.24 : 1</v>
+        <v>0.25 : 1</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2569,15 +2587,15 @@
       </c>
       <c r="B32" s="2">
         <f>January!B32+February!B32+March!B32+April!B32+May!B32+June!B32+July!B32+August!B32+September!B32+October!B32+November!B32+December!B32</f>
-        <v>3559</v>
+        <v>4016</v>
       </c>
       <c r="C32" s="2">
         <f>January!C32+February!C32+March!C32+April!C32+May!C32+June!C32+July!C32+August!C32+September!C32+October!C32+November!C32+December!C32</f>
-        <v>4539</v>
+        <v>5085</v>
       </c>
       <c r="D32" s="2">
         <f>January!D32+February!D32+March!D32+April!D32+May!D32+June!D32+July!D32+August!D32+September!D32+October!D32+November!D32+December!D32</f>
-        <v>-980</v>
+        <v>-1069</v>
       </c>
       <c r="E32" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2589,7 +2607,7 @@
       </c>
       <c r="G32" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.78 : 1</v>
+        <v>0.79 : 1</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2598,15 +2616,15 @@
       </c>
       <c r="B33" s="4">
         <f>January!B33+February!B33+March!B33+April!B33+May!B33+June!B33+July!B33+August!B33+September!B33+October!B33+November!B33+December!B33</f>
-        <v>3429</v>
+        <v>3808</v>
       </c>
       <c r="C33" s="4">
         <f>January!C33+February!C33+March!C33+April!C33+May!C33+June!C33+July!C33+August!C33+September!C33+October!C33+November!C33+December!C33</f>
-        <v>4180</v>
+        <v>4672</v>
       </c>
       <c r="D33" s="4">
         <f>January!D33+February!D33+March!D33+April!D33+May!D33+June!D33+July!D33+August!D33+September!D33+October!D33+November!D33+December!D33</f>
-        <v>-751</v>
+        <v>-864</v>
       </c>
       <c r="E33" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2627,15 +2645,15 @@
       </c>
       <c r="B34" s="2">
         <f>January!B34+February!B34+March!B34+April!B34+May!B34+June!B34+July!B34+August!B34+September!B34+October!B34+November!B34+December!B34</f>
-        <v>1763</v>
+        <v>1940</v>
       </c>
       <c r="C34" s="2">
         <f>January!C34+February!C34+March!C34+April!C34+May!C34+June!C34+July!C34+August!C34+September!C34+October!C34+November!C34+December!C34</f>
-        <v>939</v>
+        <v>1063</v>
       </c>
       <c r="D34" s="2">
         <f>January!D34+February!D34+March!D34+April!D34+May!D34+June!D34+July!D34+August!D34+September!D34+October!D34+November!D34+December!D34</f>
-        <v>824</v>
+        <v>877</v>
       </c>
       <c r="E34" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2647,7 +2665,7 @@
       </c>
       <c r="G34" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.88 : 1</v>
+        <v>1.83 : 1</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2656,15 +2674,15 @@
       </c>
       <c r="B35" s="4">
         <f>January!B35+February!B35+March!B35+April!B35+May!B35+June!B35+July!B35+August!B35+September!B35+October!B35+November!B35+December!B35</f>
-        <v>7614</v>
+        <v>8674</v>
       </c>
       <c r="C35" s="4">
         <f>January!C35+February!C35+March!C35+April!C35+May!C35+June!C35+July!C35+August!C35+September!C35+October!C35+November!C35+December!C35</f>
-        <v>8085</v>
+        <v>9101</v>
       </c>
       <c r="D35" s="4">
         <f>January!D35+February!D35+March!D35+April!D35+May!D35+June!D35+July!D35+August!D35+September!D35+October!D35+November!D35+December!D35</f>
-        <v>-471</v>
+        <v>-427</v>
       </c>
       <c r="E35" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2676,7 +2694,7 @@
       </c>
       <c r="G35" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.94 : 1</v>
+        <v>0.95 : 1</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2685,15 +2703,15 @@
       </c>
       <c r="B36" s="2">
         <f>January!B36+February!B36+March!B36+April!B36+May!B36+June!B36+July!B36+August!B36+September!B36+October!B36+November!B36+December!B36</f>
-        <v>1792</v>
+        <v>1971</v>
       </c>
       <c r="C36" s="2">
         <f>January!C36+February!C36+March!C36+April!C36+May!C36+June!C36+July!C36+August!C36+September!C36+October!C36+November!C36+December!C36</f>
-        <v>3825</v>
+        <v>4294</v>
       </c>
       <c r="D36" s="2">
         <f>January!D36+February!D36+March!D36+April!D36+May!D36+June!D36+July!D36+August!D36+September!D36+October!D36+November!D36+December!D36</f>
-        <v>-2033</v>
+        <v>-2323</v>
       </c>
       <c r="E36" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2705,7 +2723,7 @@
       </c>
       <c r="G36" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.47 : 1</v>
+        <v>0.46 : 1</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2714,15 +2732,15 @@
       </c>
       <c r="B37" s="4">
         <f>January!B37+February!B37+March!B37+April!B37+May!B37+June!B37+July!B37+August!B37+September!B37+October!B37+November!B37+December!B37</f>
-        <v>4153</v>
+        <v>4702</v>
       </c>
       <c r="C37" s="4">
         <f>January!C37+February!C37+March!C37+April!C37+May!C37+June!C37+July!C37+August!C37+September!C37+October!C37+November!C37+December!C37</f>
-        <v>2915</v>
+        <v>3227</v>
       </c>
       <c r="D37" s="4">
         <f>January!D37+February!D37+March!D37+April!D37+May!D37+June!D37+July!D37+August!D37+September!D37+October!D37+November!D37+December!D37</f>
-        <v>1238</v>
+        <v>1475</v>
       </c>
       <c r="E37" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2734,7 +2752,7 @@
       </c>
       <c r="G37" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.42 : 1</v>
+        <v>1.46 : 1</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2743,15 +2761,15 @@
       </c>
       <c r="B38" s="2">
         <f>January!B38+February!B38+March!B38+April!B38+May!B38+June!B38+July!B38+August!B38+September!B38+October!B38+November!B38+December!B38</f>
-        <v>267</v>
+        <v>287</v>
       </c>
       <c r="C38" s="2">
         <f>January!C38+February!C38+March!C38+April!C38+May!C38+June!C38+July!C38+August!C38+September!C38+October!C38+November!C38+December!C38</f>
-        <v>1333</v>
+        <v>1514</v>
       </c>
       <c r="D38" s="2">
         <f>January!D38+February!D38+March!D38+April!D38+May!D38+June!D38+July!D38+August!D38+September!D38+October!D38+November!D38+December!D38</f>
-        <v>-1066</v>
+        <v>-1227</v>
       </c>
       <c r="E38" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2763,7 +2781,7 @@
       </c>
       <c r="G38" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.2 : 1</v>
+        <v>0.19 : 1</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2772,15 +2790,15 @@
       </c>
       <c r="B39" s="8">
         <f>January!B39+February!B39+March!B39+April!B39+May!B39+June!B39+July!B39+August!B39+September!B39+October!B39+November!B39+December!B39</f>
-        <v>152</v>
+        <v>201</v>
       </c>
       <c r="C39" s="8">
         <f>January!C39+February!C39+March!C39+April!C39+May!C39+June!C39+July!C39+August!C39+September!C39+October!C39+November!C39+December!C39</f>
-        <v>341</v>
+        <v>419</v>
       </c>
       <c r="D39" s="8">
         <f>January!D39+February!D39+March!D39+April!D39+May!D39+June!D39+July!D39+August!D39+September!D39+October!D39+November!D39+December!D39</f>
-        <v>-189</v>
+        <v>-218</v>
       </c>
       <c r="E39" s="31" t="str">
         <f t="shared" si="1"/>
@@ -2792,7 +2810,7 @@
       </c>
       <c r="G39" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>0.45 : 1</v>
+        <v>0.48 : 1</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2801,15 +2819,15 @@
       </c>
       <c r="B40" s="8">
         <f>January!B40+February!B40+March!B40+April!B40+May!B40+June!B40+July!B40+August!B40+September!B40+October!B40+November!B40+December!B40</f>
-        <v>372</v>
+        <v>463</v>
       </c>
       <c r="C40" s="8">
         <f>January!C40+February!C40+March!C40+April!C40+May!C40+June!C40+July!C40+August!C40+September!C40+October!C40+November!C40+December!C40</f>
-        <v>660</v>
+        <v>791</v>
       </c>
       <c r="D40" s="8">
         <f>January!D40+February!D40+March!D40+April!D40+May!D40+June!D40+July!D40+August!D40+September!D40+October!D40+November!D40+December!D40</f>
-        <v>-288</v>
+        <v>-328</v>
       </c>
       <c r="E40" s="31" t="str">
         <f t="shared" si="1"/>
@@ -2821,7 +2839,7 @@
       </c>
       <c r="G40" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>0.56 : 1</v>
+        <v>0.59 : 1</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2830,15 +2848,15 @@
       </c>
       <c r="B41" s="8">
         <f>January!B41+February!B41+March!B41+April!B41+May!B41+June!B41+July!B41+August!B41+September!B41+October!B41+November!B41+December!B41</f>
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="C41" s="8">
         <f>January!C41+February!C41+March!C41+April!C41+May!C41+June!C41+July!C41+August!C41+September!C41+October!C41+November!C41+December!C41</f>
-        <v>139</v>
+        <v>157</v>
       </c>
       <c r="D41" s="8">
         <f>January!D41+February!D41+March!D41+April!D41+May!D41+June!D41+July!D41+August!D41+September!D41+October!D41+November!D41+December!D41</f>
-        <v>-62</v>
+        <v>-75</v>
       </c>
       <c r="E41" s="31" t="str">
         <f t="shared" si="1"/>
@@ -2850,7 +2868,7 @@
       </c>
       <c r="G41" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>0.55 : 1</v>
+        <v>0.52 : 1</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2859,11 +2877,11 @@
       </c>
       <c r="B42" s="8">
         <f>January!B42+February!B42+March!B42+April!B42+May!B42+June!B42+July!B42+August!B42+September!B42+October!B42+November!B42+December!B42</f>
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="C42" s="8">
         <f>January!C42+February!C42+March!C42+April!C42+May!C42+June!C42+July!C42+August!C42+September!C42+October!C42+November!C42+December!C42</f>
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="D42" s="8">
         <f>January!D42+February!D42+March!D42+April!D42+May!D42+June!D42+July!D42+August!D42+September!D42+October!D42+November!D42+December!D42</f>
@@ -2879,7 +2897,7 @@
       </c>
       <c r="G42" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>1.14 : 1</v>
+        <v>1.11 : 1</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2917,15 +2935,15 @@
       </c>
       <c r="B44" s="4">
         <f>January!B44+February!B44+March!B44+April!B44+May!B44+June!B44+July!B44+August!B44+September!B44+October!B44+November!B44+December!B44</f>
-        <v>862</v>
+        <v>929</v>
       </c>
       <c r="C44" s="4">
         <f>January!C44+February!C44+March!C44+April!C44+May!C44+June!C44+July!C44+August!C44+September!C44+October!C44+November!C44+December!C44</f>
-        <v>600</v>
+        <v>693</v>
       </c>
       <c r="D44" s="4">
         <f>January!D44+February!D44+March!D44+April!D44+May!D44+June!D44+July!D44+August!D44+September!D44+October!D44+November!D44+December!D44</f>
-        <v>262</v>
+        <v>236</v>
       </c>
       <c r="E44" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2937,7 +2955,7 @@
       </c>
       <c r="G44" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.44 : 1</v>
+        <v>1.34 : 1</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2946,15 +2964,15 @@
       </c>
       <c r="B45" s="2">
         <f>January!B45+February!B45+March!B45+April!B45+May!B45+June!B45+July!B45+August!B45+September!B45+October!B45+November!B45+December!B45</f>
-        <v>608</v>
+        <v>677</v>
       </c>
       <c r="C45" s="2">
         <f>January!C45+February!C45+March!C45+April!C45+May!C45+June!C45+July!C45+August!C45+September!C45+October!C45+November!C45+December!C45</f>
-        <v>1220</v>
+        <v>1392</v>
       </c>
       <c r="D45" s="2">
         <f>January!D45+February!D45+March!D45+April!D45+May!D45+June!D45+July!D45+August!D45+September!D45+October!D45+November!D45+December!D45</f>
-        <v>-612</v>
+        <v>-715</v>
       </c>
       <c r="E45" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2966,7 +2984,7 @@
       </c>
       <c r="G45" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.5 : 1</v>
+        <v>0.49 : 1</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2975,15 +2993,15 @@
       </c>
       <c r="B46" s="4">
         <f>January!B46+February!B46+March!B46+April!B46+May!B46+June!B46+July!B46+August!B46+September!B46+October!B46+November!B46+December!B46</f>
-        <v>3520</v>
+        <v>3989</v>
       </c>
       <c r="C46" s="4">
         <f>January!C46+February!C46+March!C46+April!C46+May!C46+June!C46+July!C46+August!C46+September!C46+October!C46+November!C46+December!C46</f>
-        <v>4932</v>
+        <v>5558</v>
       </c>
       <c r="D46" s="4">
         <f>January!D46+February!D46+March!D46+April!D46+May!D46+June!D46+July!D46+August!D46+September!D46+October!D46+November!D46+December!D46</f>
-        <v>-1412</v>
+        <v>-1569</v>
       </c>
       <c r="E46" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2995,7 +3013,7 @@
       </c>
       <c r="G46" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.71 : 1</v>
+        <v>0.72 : 1</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3004,15 +3022,15 @@
       </c>
       <c r="B47" s="2">
         <f>January!B47+February!B47+March!B47+April!B47+May!B47+June!B47+July!B47+August!B47+September!B47+October!B47+November!B47+December!B47</f>
-        <v>7129</v>
+        <v>8021</v>
       </c>
       <c r="C47" s="2">
         <f>January!C47+February!C47+March!C47+April!C47+May!C47+June!C47+July!C47+August!C47+September!C47+October!C47+November!C47+December!C47</f>
-        <v>5230</v>
+        <v>5936</v>
       </c>
       <c r="D47" s="2">
         <f>January!D47+February!D47+March!D47+April!D47+May!D47+June!D47+July!D47+August!D47+September!D47+October!D47+November!D47+December!D47</f>
-        <v>1899</v>
+        <v>2085</v>
       </c>
       <c r="E47" s="28" t="str">
         <f t="shared" si="1"/>
@@ -3024,7 +3042,7 @@
       </c>
       <c r="G47" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.36 : 1</v>
+        <v>1.35 : 1</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3033,15 +3051,15 @@
       </c>
       <c r="B48" s="4">
         <f>January!B48+February!B48+March!B48+April!B48+May!B48+June!B48+July!B48+August!B48+September!B48+October!B48+November!B48+December!B48</f>
-        <v>1836</v>
+        <v>2100</v>
       </c>
       <c r="C48" s="4">
         <f>January!C48+February!C48+March!C48+April!C48+May!C48+June!C48+July!C48+August!C48+September!C48+October!C48+November!C48+December!C48</f>
-        <v>5151</v>
+        <v>5781</v>
       </c>
       <c r="D48" s="4">
         <f>January!D48+February!D48+March!D48+April!D48+May!D48+June!D48+July!D48+August!D48+September!D48+October!D48+November!D48+December!D48</f>
-        <v>-3315</v>
+        <v>-3681</v>
       </c>
       <c r="E48" s="29" t="str">
         <f t="shared" si="1"/>
@@ -3062,15 +3080,15 @@
       </c>
       <c r="B49" s="2">
         <f>January!B49+February!B49+March!B49+April!B49+May!B49+June!B49+July!B49+August!B49+September!B49+October!B49+November!B49+December!B49</f>
-        <v>2943</v>
+        <v>3365</v>
       </c>
       <c r="C49" s="2">
         <f>January!C49+February!C49+March!C49+April!C49+May!C49+June!C49+July!C49+August!C49+September!C49+October!C49+November!C49+December!C49</f>
-        <v>1651</v>
+        <v>1908</v>
       </c>
       <c r="D49" s="2">
         <f>January!D49+February!D49+March!D49+April!D49+May!D49+June!D49+July!D49+August!D49+September!D49+October!D49+November!D49+December!D49</f>
-        <v>1292</v>
+        <v>1457</v>
       </c>
       <c r="E49" s="28" t="str">
         <f t="shared" si="1"/>
@@ -3082,7 +3100,7 @@
       </c>
       <c r="G49" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.78 : 1</v>
+        <v>1.76 : 1</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3091,15 +3109,15 @@
       </c>
       <c r="B50" s="4">
         <f>January!B50+February!B50+March!B50+April!B50+May!B50+June!B50+July!B50+August!B50+September!B50+October!B50+November!B50+December!B50</f>
-        <v>6953</v>
+        <v>7745</v>
       </c>
       <c r="C50" s="4">
         <f>January!C50+February!C50+March!C50+April!C50+May!C50+June!C50+July!C50+August!C50+September!C50+October!C50+November!C50+December!C50</f>
-        <v>4506</v>
+        <v>5046</v>
       </c>
       <c r="D50" s="4">
         <f>January!D50+February!D50+March!D50+April!D50+May!D50+June!D50+July!D50+August!D50+September!D50+October!D50+November!D50+December!D50</f>
-        <v>2447</v>
+        <v>2699</v>
       </c>
       <c r="E50" s="29" t="str">
         <f t="shared" si="1"/>
@@ -3111,7 +3129,7 @@
       </c>
       <c r="G50" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.54 : 1</v>
+        <v>1.53 : 1</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3120,15 +3138,15 @@
       </c>
       <c r="B51" s="2">
         <f>January!B51+February!B51+March!B51+April!B51+May!B51+June!B51+July!B51+August!B51+September!B51+October!B51+November!B51+December!B51</f>
-        <v>1961</v>
+        <v>2127</v>
       </c>
       <c r="C51" s="2">
         <f>January!C51+February!C51+March!C51+April!C51+May!C51+June!C51+July!C51+August!C51+September!C51+October!C51+November!C51+December!C51</f>
-        <v>830</v>
+        <v>976</v>
       </c>
       <c r="D51" s="2">
         <f>January!D51+February!D51+March!D51+April!D51+May!D51+June!D51+July!D51+August!D51+September!D51+October!D51+November!D51+December!D51</f>
-        <v>1131</v>
+        <v>1151</v>
       </c>
       <c r="E51" s="28" t="str">
         <f t="shared" si="1"/>
@@ -3140,7 +3158,7 @@
       </c>
       <c r="G51" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>2.36 : 1</v>
+        <v>2.18 : 1</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3149,15 +3167,15 @@
       </c>
       <c r="B52" s="4">
         <f>January!B52+February!B52+March!B52+April!B52+May!B52+June!B52+July!B52+August!B52+September!B52+October!B52+November!B52+December!B52</f>
-        <v>3634</v>
+        <v>4070</v>
       </c>
       <c r="C52" s="4">
         <f>January!C52+February!C52+March!C52+April!C52+May!C52+June!C52+July!C52+August!C52+September!C52+October!C52+November!C52+December!C52</f>
-        <v>4382</v>
+        <v>4910</v>
       </c>
       <c r="D52" s="4">
         <f>January!D52+February!D52+March!D52+April!D52+May!D52+June!D52+July!D52+August!D52+September!D52+October!D52+November!D52+December!D52</f>
-        <v>-748</v>
+        <v>-840</v>
       </c>
       <c r="E52" s="29" t="str">
         <f t="shared" si="1"/>
@@ -3178,15 +3196,15 @@
       </c>
       <c r="B53" s="2">
         <f>January!B53+February!B53+March!B53+April!B53+May!B53+June!B53+July!B53+August!B53+September!B53+October!B53+November!B53+December!B53</f>
-        <v>1018</v>
+        <v>1141</v>
       </c>
       <c r="C53" s="2">
         <f>January!C53+February!C53+March!C53+April!C53+May!C53+June!C53+July!C53+August!C53+September!C53+October!C53+November!C53+December!C53</f>
-        <v>1757</v>
+        <v>2023</v>
       </c>
       <c r="D53" s="2">
         <f>January!D53+February!D53+March!D53+April!D53+May!D53+June!D53+July!D53+August!D53+September!D53+October!D53+November!D53+December!D53</f>
-        <v>-739</v>
+        <v>-882</v>
       </c>
       <c r="E53" s="28" t="str">
         <f t="shared" si="1"/>
@@ -3198,7 +3216,7 @@
       </c>
       <c r="G53" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.58 : 1</v>
+        <v>0.56 : 1</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3207,15 +3225,15 @@
       </c>
       <c r="B54" s="4">
         <f>January!B54+February!B54+March!B54+April!B54+May!B54+June!B54+July!B54+August!B54+September!B54+October!B54+November!B54+December!B54</f>
-        <v>234</v>
+        <v>253</v>
       </c>
       <c r="C54" s="4">
         <f>January!C54+February!C54+March!C54+April!C54+May!C54+June!C54+July!C54+August!C54+September!C54+October!C54+November!C54+December!C54</f>
-        <v>1832</v>
+        <v>2063</v>
       </c>
       <c r="D54" s="4">
         <f>January!D54+February!D54+March!D54+April!D54+May!D54+June!D54+July!D54+August!D54+September!D54+October!D54+November!D54+December!D54</f>
-        <v>-1598</v>
+        <v>-1810</v>
       </c>
       <c r="E54" s="29" t="str">
         <f t="shared" si="1"/>
@@ -3227,7 +3245,7 @@
       </c>
       <c r="G54" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.13 : 1</v>
+        <v>0.12 : 1</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3236,15 +3254,15 @@
       </c>
       <c r="B55" s="10">
         <f>January!B55+February!B55+March!B55+April!B55+May!B55+June!B55+July!B55+August!B55+September!B55+October!B55+November!B55+December!B55</f>
-        <v>1579</v>
+        <v>1900</v>
       </c>
       <c r="C55" s="10">
         <f>January!C55+February!C55+March!C55+April!C55+May!C55+June!C55+July!C55+August!C55+September!C55+October!C55+November!C55+December!C55</f>
-        <v>1333</v>
+        <v>1567</v>
       </c>
       <c r="D55" s="10">
         <f>January!D55+February!D55+March!D55+April!D55+May!D55+June!D55+July!D55+August!D55+September!D55+October!D55+November!D55+December!D55</f>
-        <v>246</v>
+        <v>333</v>
       </c>
       <c r="E55" s="32" t="str">
         <f t="shared" si="1"/>
@@ -3256,7 +3274,7 @@
       </c>
       <c r="G55" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>1.18 : 1</v>
+        <v>1.21 : 1</v>
       </c>
     </row>
   </sheetData>
@@ -3329,108 +3347,204 @@
       <c r="A2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="28"/>
+      <c r="B2" s="18">
+        <v>1586</v>
+      </c>
+      <c r="C2" s="18">
+        <v>1178</v>
+      </c>
+      <c r="D2" s="18">
+        <v>408</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F2" s="28"/>
-      <c r="G2" s="3"/>
+      <c r="G2" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="29"/>
+      <c r="B3" s="21">
+        <v>820</v>
+      </c>
+      <c r="C3" s="21">
+        <v>537</v>
+      </c>
+      <c r="D3" s="21">
+        <v>283</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F3" s="29"/>
-      <c r="G3" s="5"/>
+      <c r="G3" s="5" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
+      <c r="B4" s="18">
+        <v>1263</v>
+      </c>
+      <c r="C4" s="18">
+        <v>1366</v>
+      </c>
+      <c r="D4" s="18">
+        <v>-103</v>
+      </c>
       <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="3"/>
+      <c r="F4" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
+      <c r="B5" s="21">
+        <v>124</v>
+      </c>
+      <c r="C5" s="21">
+        <v>147</v>
+      </c>
+      <c r="D5" s="21">
+        <v>-23</v>
+      </c>
       <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="5"/>
+      <c r="F5" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
+      <c r="B6" s="18">
+        <v>1315</v>
+      </c>
+      <c r="C6" s="18">
+        <v>1519</v>
+      </c>
+      <c r="D6" s="18">
+        <v>-204</v>
+      </c>
       <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="3"/>
+      <c r="F6" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
+      <c r="B7" s="21">
+        <v>172</v>
+      </c>
+      <c r="C7" s="21">
+        <v>225</v>
+      </c>
+      <c r="D7" s="21">
+        <v>-53</v>
+      </c>
       <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="5"/>
+      <c r="F7" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="28"/>
+      <c r="B8" s="18">
+        <v>163</v>
+      </c>
+      <c r="C8" s="18">
+        <v>140</v>
+      </c>
+      <c r="D8" s="18">
+        <v>23</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F8" s="28"/>
-      <c r="G8" s="3"/>
+      <c r="G8" s="3" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
+      <c r="B9" s="21">
+        <v>37</v>
+      </c>
+      <c r="C9" s="21">
+        <v>67</v>
+      </c>
+      <c r="D9" s="21">
+        <v>-30</v>
+      </c>
       <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="5"/>
+      <c r="F9" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
+      <c r="B10" s="18">
+        <v>0</v>
+      </c>
+      <c r="C10" s="18">
+        <v>58</v>
+      </c>
+      <c r="D10" s="18">
+        <v>-58</v>
+      </c>
       <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="3"/>
+      <c r="F10" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
+      <c r="B11" s="21">
+        <v>0</v>
+      </c>
+      <c r="C11" s="21">
+        <v>0</v>
+      </c>
+      <c r="D11" s="21">
+        <v>0</v>
+      </c>
       <c r="E11" s="29"/>
       <c r="F11" s="29"/>
       <c r="G11" s="5"/>
@@ -3439,163 +3553,309 @@
       <c r="A12" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
+      <c r="B12" s="23">
+        <v>11</v>
+      </c>
+      <c r="C12" s="23">
+        <v>37</v>
+      </c>
+      <c r="D12" s="23">
+        <v>-26</v>
+      </c>
       <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="7"/>
+      <c r="F12" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="30"/>
+      <c r="B13" s="23">
+        <v>148</v>
+      </c>
+      <c r="C13" s="23">
+        <v>111</v>
+      </c>
+      <c r="D13" s="23">
+        <v>37</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>61</v>
+      </c>
       <c r="F13" s="30"/>
-      <c r="G13" s="7"/>
+      <c r="G13" s="7" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
+      <c r="B14" s="23">
+        <v>108</v>
+      </c>
+      <c r="C14" s="23">
+        <v>297</v>
+      </c>
+      <c r="D14" s="23">
+        <v>-189</v>
+      </c>
       <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="7"/>
+      <c r="F14" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="30"/>
+      <c r="B15" s="23">
+        <v>127</v>
+      </c>
+      <c r="C15" s="23">
+        <v>97</v>
+      </c>
+      <c r="D15" s="23">
+        <v>30</v>
+      </c>
+      <c r="E15" s="30" t="s">
+        <v>61</v>
+      </c>
       <c r="F15" s="30"/>
-      <c r="G15" s="7"/>
+      <c r="G15" s="7" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
+      <c r="B16" s="18">
+        <v>35</v>
+      </c>
+      <c r="C16" s="18">
+        <v>158</v>
+      </c>
+      <c r="D16" s="18">
+        <v>-123</v>
+      </c>
       <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="3"/>
+      <c r="F16" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="29"/>
+      <c r="B17" s="21">
+        <v>741</v>
+      </c>
+      <c r="C17" s="21">
+        <v>517</v>
+      </c>
+      <c r="D17" s="21">
+        <v>224</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F17" s="29"/>
-      <c r="G17" s="5"/>
+      <c r="G17" s="5" t="s">
+        <v>247</v>
+      </c>
     </row>
     <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
+      <c r="B18" s="18">
+        <v>88</v>
+      </c>
+      <c r="C18" s="18">
+        <v>107</v>
+      </c>
+      <c r="D18" s="18">
+        <v>-19</v>
+      </c>
       <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="3"/>
+      <c r="F18" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="29"/>
+      <c r="B19" s="21">
+        <v>629</v>
+      </c>
+      <c r="C19" s="21">
+        <v>499</v>
+      </c>
+      <c r="D19" s="21">
+        <v>130</v>
+      </c>
+      <c r="E19" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F19" s="29"/>
-      <c r="G19" s="5"/>
+      <c r="G19" s="5" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
+      <c r="B20" s="18">
+        <v>4</v>
+      </c>
+      <c r="C20" s="18">
+        <v>74</v>
+      </c>
+      <c r="D20" s="18">
+        <v>-70</v>
+      </c>
       <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="3"/>
+      <c r="F20" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="29"/>
+      <c r="B21" s="21">
+        <v>436</v>
+      </c>
+      <c r="C21" s="21">
+        <v>433</v>
+      </c>
+      <c r="D21" s="21">
+        <v>3</v>
+      </c>
+      <c r="E21" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F21" s="29"/>
-      <c r="G21" s="5"/>
+      <c r="G21" s="5" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
+      <c r="B22" s="18">
+        <v>38</v>
+      </c>
+      <c r="C22" s="18">
+        <v>90</v>
+      </c>
+      <c r="D22" s="18">
+        <v>-52</v>
+      </c>
       <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="3"/>
+      <c r="F22" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="29"/>
+      <c r="B23" s="21">
+        <v>724</v>
+      </c>
+      <c r="C23" s="21">
+        <v>388</v>
+      </c>
+      <c r="D23" s="21">
+        <v>336</v>
+      </c>
+      <c r="E23" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F23" s="29"/>
-      <c r="G23" s="5"/>
+      <c r="G23" s="5" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="28"/>
+      <c r="B24" s="18">
+        <v>1997</v>
+      </c>
+      <c r="C24" s="18">
+        <v>1377</v>
+      </c>
+      <c r="D24" s="18">
+        <v>620</v>
+      </c>
+      <c r="E24" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F24" s="28"/>
-      <c r="G24" s="3"/>
+      <c r="G24" s="3" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
+      <c r="B25" s="21">
+        <v>176</v>
+      </c>
+      <c r="C25" s="21">
+        <v>368</v>
+      </c>
+      <c r="D25" s="21">
+        <v>-192</v>
+      </c>
       <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="5"/>
+      <c r="F25" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="26" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
+      <c r="B26" s="18">
+        <v>0</v>
+      </c>
+      <c r="C26" s="18">
+        <v>0</v>
+      </c>
+      <c r="D26" s="18">
+        <v>0</v>
+      </c>
       <c r="E26" s="28"/>
       <c r="F26" s="28"/>
       <c r="G26" s="3"/>
@@ -3604,185 +3864,347 @@
       <c r="A27" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
+      <c r="B27" s="21">
+        <v>176</v>
+      </c>
+      <c r="C27" s="21">
+        <v>215</v>
+      </c>
+      <c r="D27" s="21">
+        <v>-39</v>
+      </c>
       <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="5"/>
+      <c r="F27" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
+      <c r="B28" s="18">
+        <v>51</v>
+      </c>
+      <c r="C28" s="18">
+        <v>72</v>
+      </c>
+      <c r="D28" s="18">
+        <v>-21</v>
+      </c>
       <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="3"/>
+      <c r="F28" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="29"/>
+      <c r="B29" s="21">
+        <v>563</v>
+      </c>
+      <c r="C29" s="21">
+        <v>482</v>
+      </c>
+      <c r="D29" s="21">
+        <v>81</v>
+      </c>
+      <c r="E29" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F29" s="29"/>
-      <c r="G29" s="5"/>
+      <c r="G29" s="5" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="30" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
+      <c r="B30" s="18">
+        <v>39</v>
+      </c>
+      <c r="C30" s="18">
+        <v>39</v>
+      </c>
+      <c r="D30" s="18">
+        <v>0</v>
+      </c>
       <c r="E30" s="28"/>
       <c r="F30" s="28"/>
-      <c r="G30" s="3"/>
+      <c r="G30" s="3" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
+      <c r="B31" s="21">
+        <v>76</v>
+      </c>
+      <c r="C31" s="21">
+        <v>259</v>
+      </c>
+      <c r="D31" s="21">
+        <v>-183</v>
+      </c>
       <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="5"/>
+      <c r="F31" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="32" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
+      <c r="B32" s="18">
+        <v>457</v>
+      </c>
+      <c r="C32" s="18">
+        <v>546</v>
+      </c>
+      <c r="D32" s="18">
+        <v>-89</v>
+      </c>
       <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="3"/>
+      <c r="F32" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="33" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
+      <c r="B33" s="21">
+        <v>379</v>
+      </c>
+      <c r="C33" s="21">
+        <v>492</v>
+      </c>
+      <c r="D33" s="21">
+        <v>-113</v>
+      </c>
       <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="5"/>
+      <c r="F33" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="34" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="28"/>
+      <c r="B34" s="18">
+        <v>177</v>
+      </c>
+      <c r="C34" s="18">
+        <v>124</v>
+      </c>
+      <c r="D34" s="18">
+        <v>53</v>
+      </c>
+      <c r="E34" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F34" s="28"/>
-      <c r="G34" s="3"/>
+      <c r="G34" s="3" t="s">
+        <v>247</v>
+      </c>
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="29"/>
+      <c r="B35" s="21">
+        <v>1060</v>
+      </c>
+      <c r="C35" s="21">
+        <v>1016</v>
+      </c>
+      <c r="D35" s="21">
+        <v>44</v>
+      </c>
+      <c r="E35" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F35" s="29"/>
-      <c r="G35" s="5"/>
+      <c r="G35" s="5" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="36" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
+      <c r="B36" s="18">
+        <v>179</v>
+      </c>
+      <c r="C36" s="18">
+        <v>469</v>
+      </c>
+      <c r="D36" s="18">
+        <v>-290</v>
+      </c>
       <c r="E36" s="28"/>
-      <c r="F36" s="28"/>
-      <c r="G36" s="3"/>
+      <c r="F36" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="29"/>
+      <c r="B37" s="21">
+        <v>549</v>
+      </c>
+      <c r="C37" s="21">
+        <v>312</v>
+      </c>
+      <c r="D37" s="21">
+        <v>237</v>
+      </c>
+      <c r="E37" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F37" s="29"/>
-      <c r="G37" s="5"/>
+      <c r="G37" s="5" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
+      <c r="B38" s="18">
+        <v>20</v>
+      </c>
+      <c r="C38" s="18">
+        <v>181</v>
+      </c>
+      <c r="D38" s="18">
+        <v>-161</v>
+      </c>
       <c r="E38" s="28"/>
-      <c r="F38" s="28"/>
-      <c r="G38" s="3"/>
+      <c r="F38" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="B39" s="25"/>
-      <c r="C39" s="25"/>
-      <c r="D39" s="25"/>
+      <c r="B39" s="25">
+        <v>49</v>
+      </c>
+      <c r="C39" s="25">
+        <v>78</v>
+      </c>
+      <c r="D39" s="25">
+        <v>-29</v>
+      </c>
       <c r="E39" s="31"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="9"/>
+      <c r="F39" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="B40" s="25"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
+      <c r="B40" s="25">
+        <v>91</v>
+      </c>
+      <c r="C40" s="25">
+        <v>131</v>
+      </c>
+      <c r="D40" s="25">
+        <v>-40</v>
+      </c>
       <c r="E40" s="31"/>
-      <c r="F40" s="31"/>
-      <c r="G40" s="9"/>
+      <c r="F40" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
+      <c r="B41" s="25">
+        <v>5</v>
+      </c>
+      <c r="C41" s="25">
+        <v>18</v>
+      </c>
+      <c r="D41" s="25">
+        <v>-13</v>
+      </c>
       <c r="E41" s="31"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="9"/>
+      <c r="F41" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="42" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="B42" s="25"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="25"/>
+      <c r="B42" s="25">
+        <v>19</v>
+      </c>
+      <c r="C42" s="25">
+        <v>19</v>
+      </c>
+      <c r="D42" s="25">
+        <v>0</v>
+      </c>
       <c r="E42" s="31"/>
       <c r="F42" s="31"/>
-      <c r="G42" s="9"/>
+      <c r="G42" s="9" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="B43" s="25"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
+      <c r="B43" s="25">
+        <v>0</v>
+      </c>
+      <c r="C43" s="25">
+        <v>0</v>
+      </c>
+      <c r="D43" s="25">
+        <v>0</v>
+      </c>
       <c r="E43" s="31"/>
       <c r="F43" s="31"/>
       <c r="G43" s="9"/>
@@ -3791,133 +4213,253 @@
       <c r="A44" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="B44" s="21"/>
-      <c r="C44" s="21"/>
-      <c r="D44" s="21"/>
+      <c r="B44" s="21">
+        <v>67</v>
+      </c>
+      <c r="C44" s="21">
+        <v>93</v>
+      </c>
+      <c r="D44" s="21">
+        <v>-26</v>
+      </c>
       <c r="E44" s="29"/>
-      <c r="F44" s="29"/>
-      <c r="G44" s="5"/>
+      <c r="F44" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="45" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
+      <c r="B45" s="18">
+        <v>69</v>
+      </c>
+      <c r="C45" s="18">
+        <v>172</v>
+      </c>
+      <c r="D45" s="18">
+        <v>-103</v>
+      </c>
       <c r="E45" s="28"/>
-      <c r="F45" s="28"/>
-      <c r="G45" s="3"/>
+      <c r="F45" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="46" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="B46" s="21"/>
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
+      <c r="B46" s="21">
+        <v>469</v>
+      </c>
+      <c r="C46" s="21">
+        <v>626</v>
+      </c>
+      <c r="D46" s="21">
+        <v>-157</v>
+      </c>
       <c r="E46" s="29"/>
-      <c r="F46" s="29"/>
-      <c r="G46" s="5"/>
+      <c r="F46" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="47" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="28"/>
+      <c r="B47" s="18">
+        <v>892</v>
+      </c>
+      <c r="C47" s="18">
+        <v>706</v>
+      </c>
+      <c r="D47" s="18">
+        <v>186</v>
+      </c>
+      <c r="E47" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F47" s="28"/>
-      <c r="G47" s="3"/>
+      <c r="G47" s="3" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="B48" s="21"/>
-      <c r="C48" s="21"/>
-      <c r="D48" s="21"/>
+      <c r="B48" s="21">
+        <v>264</v>
+      </c>
+      <c r="C48" s="21">
+        <v>630</v>
+      </c>
+      <c r="D48" s="21">
+        <v>-366</v>
+      </c>
       <c r="E48" s="29"/>
-      <c r="F48" s="29"/>
-      <c r="G48" s="5"/>
+      <c r="F48" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B49" s="18"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="18"/>
-      <c r="E49" s="28"/>
+      <c r="B49" s="18">
+        <v>422</v>
+      </c>
+      <c r="C49" s="18">
+        <v>257</v>
+      </c>
+      <c r="D49" s="18">
+        <v>165</v>
+      </c>
+      <c r="E49" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F49" s="28"/>
-      <c r="G49" s="3"/>
+      <c r="G49" s="3" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="B50" s="21"/>
-      <c r="C50" s="21"/>
-      <c r="D50" s="21"/>
-      <c r="E50" s="29"/>
+      <c r="B50" s="21">
+        <v>792</v>
+      </c>
+      <c r="C50" s="21">
+        <v>540</v>
+      </c>
+      <c r="D50" s="21">
+        <v>252</v>
+      </c>
+      <c r="E50" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F50" s="29"/>
-      <c r="G50" s="5"/>
+      <c r="G50" s="5" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B51" s="18"/>
-      <c r="C51" s="18"/>
-      <c r="D51" s="18"/>
-      <c r="E51" s="28"/>
+      <c r="B51" s="18">
+        <v>166</v>
+      </c>
+      <c r="C51" s="18">
+        <v>146</v>
+      </c>
+      <c r="D51" s="18">
+        <v>20</v>
+      </c>
+      <c r="E51" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F51" s="28"/>
-      <c r="G51" s="3"/>
+      <c r="G51" s="3" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="52" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="B52" s="21"/>
-      <c r="C52" s="21"/>
-      <c r="D52" s="21"/>
+      <c r="B52" s="21">
+        <v>436</v>
+      </c>
+      <c r="C52" s="21">
+        <v>528</v>
+      </c>
+      <c r="D52" s="21">
+        <v>-92</v>
+      </c>
       <c r="E52" s="29"/>
-      <c r="F52" s="29"/>
-      <c r="G52" s="5"/>
+      <c r="F52" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="53" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B53" s="18"/>
-      <c r="C53" s="18"/>
-      <c r="D53" s="18"/>
+      <c r="B53" s="18">
+        <v>123</v>
+      </c>
+      <c r="C53" s="18">
+        <v>266</v>
+      </c>
+      <c r="D53" s="18">
+        <v>-143</v>
+      </c>
       <c r="E53" s="28"/>
-      <c r="F53" s="28"/>
-      <c r="G53" s="3"/>
+      <c r="F53" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="54" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="B54" s="21"/>
-      <c r="C54" s="21"/>
-      <c r="D54" s="21"/>
+      <c r="B54" s="21">
+        <v>19</v>
+      </c>
+      <c r="C54" s="21">
+        <v>231</v>
+      </c>
+      <c r="D54" s="21">
+        <v>-212</v>
+      </c>
       <c r="E54" s="29"/>
-      <c r="F54" s="29"/>
-      <c r="G54" s="5"/>
+      <c r="F54" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="55" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="B55" s="27"/>
-      <c r="C55" s="27"/>
-      <c r="D55" s="27"/>
-      <c r="E55" s="32"/>
+      <c r="B55" s="27">
+        <v>321</v>
+      </c>
+      <c r="C55" s="27">
+        <v>234</v>
+      </c>
+      <c r="D55" s="27">
+        <v>87</v>
+      </c>
+      <c r="E55" s="32" t="s">
+        <v>61</v>
+      </c>
       <c r="F55" s="32"/>
-      <c r="G55" s="11"/>
+      <c r="G55" s="11" t="s">
+        <v>146</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G55" xr:uid="{00000000-0009-0000-0000-000009000000}"/>

</xml_diff>

<commit_message>
Update to all statistic files for October 2023
</commit_message>
<xml_diff>
--- a/statistics_files/2023/2023.g.net_borrower_lender.xlsx
+++ b/statistics_files/2023/2023.g.net_borrower_lender.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20403"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\GitHub\next_statistics\statistics_files\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35732D75-A9C1-4A6B-A198-00DB7DDDD321}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CF10911-42C1-4434-8741-90DB73F4B2AA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" tabRatio="673" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1717" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1819" uniqueCount="255">
   <si>
     <t>NET</t>
   </si>
@@ -808,6 +808,15 @@
   </si>
   <si>
     <t>0.46 : 1</t>
+  </si>
+  <si>
+    <t>0.44 : 1</t>
+  </si>
+  <si>
+    <t>0.88 : 1</t>
+  </si>
+  <si>
+    <t>0.61 : 1</t>
   </si>
 </sst>
 </file>
@@ -1717,15 +1726,15 @@
       </c>
       <c r="B2" s="2">
         <f>January!B2+February!B2+March!B2+April!B2+May!B2+June!B2+July!B2+August!B2+September!B2+October!B2+November!B2+December!B2</f>
-        <v>13885</v>
+        <v>15673</v>
       </c>
       <c r="C2" s="2">
         <f>January!C2+February!C2+March!C2+April!C2+May!C2+June!C2+July!C2+August!C2+September!C2+October!C2+November!C2+December!C2</f>
-        <v>10581</v>
+        <v>11820</v>
       </c>
       <c r="D2" s="2">
         <f>January!D2+February!D2+March!D2+April!D2+May!D2+June!D2+July!D2+August!D2+September!D2+October!D2+November!D2+December!D2</f>
-        <v>3304</v>
+        <v>3853</v>
       </c>
       <c r="E2" s="28" t="str">
         <f>IF(D2 &gt; 0, "We borrowed more than we lent this year", "")</f>
@@ -1737,7 +1746,7 @@
       </c>
       <c r="G2" s="3" t="str">
         <f>IF(ISERROR(ROUND(B2/C2,2)&amp;" : 1"), "", ROUND(B2/C2,2)&amp;" : 1")</f>
-        <v>1.31 : 1</v>
+        <v>1.33 : 1</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1746,15 +1755,15 @@
       </c>
       <c r="B3" s="4">
         <f>January!B3+February!B3+March!B3+April!B3+May!B3+June!B3+July!B3+August!B3+September!B3+October!B3+November!B3+December!B3</f>
-        <v>4862</v>
+        <v>5403</v>
       </c>
       <c r="C3" s="4">
         <f>January!C3+February!C3+March!C3+April!C3+May!C3+June!C3+July!C3+August!C3+September!C3+October!C3+November!C3+December!C3</f>
-        <v>4392</v>
+        <v>4902</v>
       </c>
       <c r="D3" s="4">
         <f>January!D3+February!D3+March!D3+April!D3+May!D3+June!D3+July!D3+August!D3+September!D3+October!D3+November!D3+December!D3</f>
-        <v>470</v>
+        <v>501</v>
       </c>
       <c r="E3" s="29" t="str">
         <f t="shared" ref="E3:E55" si="1">IF(D3 &gt; 0, "We borrowed more than we lent this year", "")</f>
@@ -1766,7 +1775,7 @@
       </c>
       <c r="G3" s="5" t="str">
         <f t="shared" ref="G3:G55" si="2">IF(ISERROR(ROUND(B3/C3,2)&amp;" : 1"), "", ROUND(B3/C3,2)&amp;" : 1")</f>
-        <v>1.11 : 1</v>
+        <v>1.1 : 1</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1775,15 +1784,15 @@
       </c>
       <c r="B4" s="2">
         <f>January!B4+February!B4+March!B4+April!B4+May!B4+June!B4+July!B4+August!B4+September!B4+October!B4+November!B4+December!B4</f>
-        <v>11963</v>
+        <v>13069</v>
       </c>
       <c r="C4" s="2">
         <f>January!C4+February!C4+March!C4+April!C4+May!C4+June!C4+July!C4+August!C4+September!C4+October!C4+November!C4+December!C4</f>
-        <v>11285</v>
+        <v>12677</v>
       </c>
       <c r="D4" s="2">
         <f>January!D4+February!D4+March!D4+April!D4+May!D4+June!D4+July!D4+August!D4+September!D4+October!D4+November!D4+December!D4</f>
-        <v>678</v>
+        <v>392</v>
       </c>
       <c r="E4" s="28" t="str">
         <f t="shared" si="1"/>
@@ -1795,7 +1804,7 @@
       </c>
       <c r="G4" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.06 : 1</v>
+        <v>1.03 : 1</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1804,15 +1813,15 @@
       </c>
       <c r="B5" s="4">
         <f>January!B5+February!B5+March!B5+April!B5+May!B5+June!B5+July!B5+August!B5+September!B5+October!B5+November!B5+December!B5</f>
-        <v>764</v>
+        <v>846</v>
       </c>
       <c r="C5" s="4">
         <f>January!C5+February!C5+March!C5+April!C5+May!C5+June!C5+July!C5+August!C5+September!C5+October!C5+November!C5+December!C5</f>
-        <v>1133</v>
+        <v>1277</v>
       </c>
       <c r="D5" s="4">
         <f>January!D5+February!D5+March!D5+April!D5+May!D5+June!D5+July!D5+August!D5+September!D5+October!D5+November!D5+December!D5</f>
-        <v>-369</v>
+        <v>-431</v>
       </c>
       <c r="E5" s="29" t="str">
         <f t="shared" si="1"/>
@@ -1824,7 +1833,7 @@
       </c>
       <c r="G5" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.67 : 1</v>
+        <v>0.66 : 1</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1833,15 +1842,15 @@
       </c>
       <c r="B6" s="2">
         <f>January!B6+February!B6+March!B6+April!B6+May!B6+June!B6+July!B6+August!B6+September!B6+October!B6+November!B6+December!B6</f>
-        <v>11375</v>
+        <v>12624</v>
       </c>
       <c r="C6" s="2">
         <f>January!C6+February!C6+March!C6+April!C6+May!C6+June!C6+July!C6+August!C6+September!C6+October!C6+November!C6+December!C6</f>
-        <v>13255</v>
+        <v>14771</v>
       </c>
       <c r="D6" s="2">
         <f>January!D6+February!D6+March!D6+April!D6+May!D6+June!D6+July!D6+August!D6+September!D6+October!D6+November!D6+December!D6</f>
-        <v>-1880</v>
+        <v>-2147</v>
       </c>
       <c r="E6" s="28" t="str">
         <f t="shared" si="1"/>
@@ -1853,7 +1862,7 @@
       </c>
       <c r="G6" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.86 : 1</v>
+        <v>0.85 : 1</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1862,15 +1871,15 @@
       </c>
       <c r="B7" s="4">
         <f>January!B7+February!B7+March!B7+April!B7+May!B7+June!B7+July!B7+August!B7+September!B7+October!B7+November!B7+December!B7</f>
-        <v>1886</v>
+        <v>2105</v>
       </c>
       <c r="C7" s="4">
         <f>January!C7+February!C7+March!C7+April!C7+May!C7+June!C7+July!C7+August!C7+September!C7+October!C7+November!C7+December!C7</f>
-        <v>2035</v>
+        <v>2235</v>
       </c>
       <c r="D7" s="4">
         <f>January!D7+February!D7+March!D7+April!D7+May!D7+June!D7+July!D7+August!D7+September!D7+October!D7+November!D7+December!D7</f>
-        <v>-149</v>
+        <v>-130</v>
       </c>
       <c r="E7" s="29" t="str">
         <f t="shared" si="1"/>
@@ -1882,7 +1891,7 @@
       </c>
       <c r="G7" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.93 : 1</v>
+        <v>0.94 : 1</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1891,15 +1900,15 @@
       </c>
       <c r="B8" s="2">
         <f>January!B8+February!B8+March!B8+April!B8+May!B8+June!B8+July!B8+August!B8+September!B8+October!B8+November!B8+December!B8</f>
-        <v>1219</v>
+        <v>1300</v>
       </c>
       <c r="C8" s="2">
         <f>January!C8+February!C8+March!C8+April!C8+May!C8+June!C8+July!C8+August!C8+September!C8+October!C8+November!C8+December!C8</f>
-        <v>1686</v>
+        <v>1865</v>
       </c>
       <c r="D8" s="2">
         <f>January!D8+February!D8+March!D8+April!D8+May!D8+June!D8+July!D8+August!D8+September!D8+October!D8+November!D8+December!D8</f>
-        <v>-467</v>
+        <v>-565</v>
       </c>
       <c r="E8" s="28" t="str">
         <f t="shared" si="1"/>
@@ -1911,7 +1920,7 @@
       </c>
       <c r="G8" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.72 : 1</v>
+        <v>0.7 : 1</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1920,15 +1929,15 @@
       </c>
       <c r="B9" s="4">
         <f>January!B9+February!B9+March!B9+April!B9+May!B9+June!B9+July!B9+August!B9+September!B9+October!B9+November!B9+December!B9</f>
-        <v>456</v>
+        <v>508</v>
       </c>
       <c r="C9" s="4">
         <f>January!C9+February!C9+March!C9+April!C9+May!C9+June!C9+July!C9+August!C9+September!C9+October!C9+November!C9+December!C9</f>
-        <v>634</v>
+        <v>700</v>
       </c>
       <c r="D9" s="4">
         <f>January!D9+February!D9+March!D9+April!D9+May!D9+June!D9+July!D9+August!D9+September!D9+October!D9+November!D9+December!D9</f>
-        <v>-178</v>
+        <v>-192</v>
       </c>
       <c r="E9" s="29" t="str">
         <f t="shared" si="1"/>
@@ -1940,7 +1949,7 @@
       </c>
       <c r="G9" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.72 : 1</v>
+        <v>0.73 : 1</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1949,15 +1958,15 @@
       </c>
       <c r="B10" s="2">
         <f>January!B10+February!B10+March!B10+April!B10+May!B10+June!B10+July!B10+August!B10+September!B10+October!B10+November!B10+December!B10</f>
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C10" s="2">
         <f>January!C10+February!C10+March!C10+April!C10+May!C10+June!C10+July!C10+August!C10+September!C10+October!C10+November!C10+December!C10</f>
-        <v>356</v>
+        <v>413</v>
       </c>
       <c r="D10" s="2">
         <f>January!D10+February!D10+March!D10+April!D10+May!D10+June!D10+July!D10+August!D10+September!D10+October!D10+November!D10+December!D10</f>
-        <v>-317</v>
+        <v>-373</v>
       </c>
       <c r="E10" s="28" t="str">
         <f t="shared" si="1"/>
@@ -1969,7 +1978,7 @@
       </c>
       <c r="G10" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.11 : 1</v>
+        <v>0.1 : 1</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2007,15 +2016,15 @@
       </c>
       <c r="B12" s="6">
         <f>January!B12+February!B12+March!B12+April!B12+May!B12+June!B12+July!B12+August!B12+September!B12+October!B12+November!B12+December!B12</f>
-        <v>139</v>
+        <v>159</v>
       </c>
       <c r="C12" s="6">
         <f>January!C12+February!C12+March!C12+April!C12+May!C12+June!C12+July!C12+August!C12+September!C12+October!C12+November!C12+December!C12</f>
-        <v>210</v>
+        <v>233</v>
       </c>
       <c r="D12" s="6">
         <f>January!D12+February!D12+March!D12+April!D12+May!D12+June!D12+July!D12+August!D12+September!D12+October!D12+November!D12+December!D12</f>
-        <v>-71</v>
+        <v>-74</v>
       </c>
       <c r="E12" s="30" t="str">
         <f t="shared" si="1"/>
@@ -2027,7 +2036,7 @@
       </c>
       <c r="G12" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0.66 : 1</v>
+        <v>0.68 : 1</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2036,15 +2045,15 @@
       </c>
       <c r="B13" s="6">
         <f>January!B13+February!B13+March!B13+April!B13+May!B13+June!B13+July!B13+August!B13+September!B13+October!B13+November!B13+December!B13</f>
-        <v>1257</v>
+        <v>1439</v>
       </c>
       <c r="C13" s="6">
         <f>January!C13+February!C13+March!C13+April!C13+May!C13+June!C13+July!C13+August!C13+September!C13+October!C13+November!C13+December!C13</f>
-        <v>812</v>
+        <v>937</v>
       </c>
       <c r="D13" s="6">
         <f>January!D13+February!D13+March!D13+April!D13+May!D13+June!D13+July!D13+August!D13+September!D13+October!D13+November!D13+December!D13</f>
-        <v>445</v>
+        <v>502</v>
       </c>
       <c r="E13" s="30" t="str">
         <f t="shared" si="1"/>
@@ -2056,7 +2065,7 @@
       </c>
       <c r="G13" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>1.55 : 1</v>
+        <v>1.54 : 1</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2065,15 +2074,15 @@
       </c>
       <c r="B14" s="6">
         <f>January!B14+February!B14+March!B14+April!B14+May!B14+June!B14+July!B14+August!B14+September!B14+October!B14+November!B14+December!B14</f>
-        <v>1196</v>
+        <v>1315</v>
       </c>
       <c r="C14" s="6">
         <f>January!C14+February!C14+March!C14+April!C14+May!C14+June!C14+July!C14+August!C14+September!C14+October!C14+November!C14+December!C14</f>
-        <v>2647</v>
+        <v>2963</v>
       </c>
       <c r="D14" s="6">
         <f>January!D14+February!D14+March!D14+April!D14+May!D14+June!D14+July!D14+August!D14+September!D14+October!D14+November!D14+December!D14</f>
-        <v>-1451</v>
+        <v>-1648</v>
       </c>
       <c r="E14" s="30" t="str">
         <f t="shared" si="1"/>
@@ -2085,7 +2094,7 @@
       </c>
       <c r="G14" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0.45 : 1</v>
+        <v>0.44 : 1</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2094,15 +2103,15 @@
       </c>
       <c r="B15" s="6">
         <f>January!B15+February!B15+March!B15+April!B15+May!B15+June!B15+July!B15+August!B15+September!B15+October!B15+November!B15+December!B15</f>
-        <v>804</v>
+        <v>889</v>
       </c>
       <c r="C15" s="6">
         <f>January!C15+February!C15+March!C15+April!C15+May!C15+June!C15+July!C15+August!C15+September!C15+October!C15+November!C15+December!C15</f>
-        <v>925</v>
+        <v>1048</v>
       </c>
       <c r="D15" s="6">
         <f>January!D15+February!D15+March!D15+April!D15+May!D15+June!D15+July!D15+August!D15+September!D15+October!D15+November!D15+December!D15</f>
-        <v>-121</v>
+        <v>-159</v>
       </c>
       <c r="E15" s="30" t="str">
         <f t="shared" si="1"/>
@@ -2114,7 +2123,7 @@
       </c>
       <c r="G15" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0.87 : 1</v>
+        <v>0.85 : 1</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2123,15 +2132,15 @@
       </c>
       <c r="B16" s="2">
         <f>January!B16+February!B16+March!B16+April!B16+May!B16+June!B16+July!B16+August!B16+September!B16+October!B16+November!B16+December!B16</f>
-        <v>353</v>
+        <v>374</v>
       </c>
       <c r="C16" s="2">
         <f>January!C16+February!C16+March!C16+April!C16+May!C16+June!C16+July!C16+August!C16+September!C16+October!C16+November!C16+December!C16</f>
-        <v>1385</v>
+        <v>1529</v>
       </c>
       <c r="D16" s="2">
         <f>January!D16+February!D16+March!D16+April!D16+May!D16+June!D16+July!D16+August!D16+September!D16+October!D16+November!D16+December!D16</f>
-        <v>-1032</v>
+        <v>-1155</v>
       </c>
       <c r="E16" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2143,7 +2152,7 @@
       </c>
       <c r="G16" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.25 : 1</v>
+        <v>0.24 : 1</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2152,15 +2161,15 @@
       </c>
       <c r="B17" s="4">
         <f>January!B17+February!B17+March!B17+April!B17+May!B17+June!B17+July!B17+August!B17+September!B17+October!B17+November!B17+December!B17</f>
-        <v>5546</v>
+        <v>6315</v>
       </c>
       <c r="C17" s="4">
         <f>January!C17+February!C17+March!C17+April!C17+May!C17+June!C17+July!C17+August!C17+September!C17+October!C17+November!C17+December!C17</f>
-        <v>4328</v>
+        <v>4808</v>
       </c>
       <c r="D17" s="4">
         <f>January!D17+February!D17+March!D17+April!D17+May!D17+June!D17+July!D17+August!D17+September!D17+October!D17+November!D17+December!D17</f>
-        <v>1218</v>
+        <v>1507</v>
       </c>
       <c r="E17" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2172,7 +2181,7 @@
       </c>
       <c r="G17" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.28 : 1</v>
+        <v>1.31 : 1</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2181,15 +2190,15 @@
       </c>
       <c r="B18" s="2">
         <f>January!B18+February!B18+March!B18+April!B18+May!B18+June!B18+July!B18+August!B18+September!B18+October!B18+November!B18+December!B18</f>
-        <v>832</v>
+        <v>906</v>
       </c>
       <c r="C18" s="2">
         <f>January!C18+February!C18+March!C18+April!C18+May!C18+June!C18+July!C18+August!C18+September!C18+October!C18+November!C18+December!C18</f>
-        <v>906</v>
+        <v>1024</v>
       </c>
       <c r="D18" s="2">
         <f>January!D18+February!D18+March!D18+April!D18+May!D18+June!D18+July!D18+August!D18+September!D18+October!D18+November!D18+December!D18</f>
-        <v>-74</v>
+        <v>-118</v>
       </c>
       <c r="E18" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2201,7 +2210,7 @@
       </c>
       <c r="G18" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.92 : 1</v>
+        <v>0.88 : 1</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2210,15 +2219,15 @@
       </c>
       <c r="B19" s="4">
         <f>January!B19+February!B19+March!B19+April!B19+May!B19+June!B19+July!B19+August!B19+September!B19+October!B19+November!B19+December!B19</f>
-        <v>5879</v>
+        <v>6498</v>
       </c>
       <c r="C19" s="4">
         <f>January!C19+February!C19+March!C19+April!C19+May!C19+June!C19+July!C19+August!C19+September!C19+October!C19+November!C19+December!C19</f>
-        <v>3773</v>
+        <v>4133</v>
       </c>
       <c r="D19" s="4">
         <f>January!D19+February!D19+March!D19+April!D19+May!D19+June!D19+July!D19+August!D19+September!D19+October!D19+November!D19+December!D19</f>
-        <v>2106</v>
+        <v>2365</v>
       </c>
       <c r="E19" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2230,7 +2239,7 @@
       </c>
       <c r="G19" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.56 : 1</v>
+        <v>1.57 : 1</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2239,15 +2248,15 @@
       </c>
       <c r="B20" s="2">
         <f>January!B20+February!B20+March!B20+April!B20+May!B20+June!B20+July!B20+August!B20+September!B20+October!B20+November!B20+December!B20</f>
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="C20" s="2">
         <f>January!C20+February!C20+March!C20+April!C20+May!C20+June!C20+July!C20+August!C20+September!C20+October!C20+November!C20+December!C20</f>
-        <v>609</v>
+        <v>681</v>
       </c>
       <c r="D20" s="2">
         <f>January!D20+February!D20+March!D20+April!D20+May!D20+June!D20+July!D20+August!D20+September!D20+October!D20+November!D20+December!D20</f>
-        <v>-584</v>
+        <v>-645</v>
       </c>
       <c r="E20" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2259,7 +2268,7 @@
       </c>
       <c r="G20" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.04 : 1</v>
+        <v>0.05 : 1</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2268,15 +2277,15 @@
       </c>
       <c r="B21" s="4">
         <f>January!B21+February!B21+March!B21+April!B21+May!B21+June!B21+July!B21+August!B21+September!B21+October!B21+November!B21+December!B21</f>
-        <v>4577</v>
+        <v>5018</v>
       </c>
       <c r="C21" s="4">
         <f>January!C21+February!C21+March!C21+April!C21+May!C21+June!C21+July!C21+August!C21+September!C21+October!C21+November!C21+December!C21</f>
-        <v>3803</v>
+        <v>4259</v>
       </c>
       <c r="D21" s="4">
         <f>January!D21+February!D21+March!D21+April!D21+May!D21+June!D21+July!D21+August!D21+September!D21+October!D21+November!D21+December!D21</f>
-        <v>774</v>
+        <v>759</v>
       </c>
       <c r="E21" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2288,7 +2297,7 @@
       </c>
       <c r="G21" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.2 : 1</v>
+        <v>1.18 : 1</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2297,15 +2306,15 @@
       </c>
       <c r="B22" s="2">
         <f>January!B22+February!B22+March!B22+April!B22+May!B22+June!B22+July!B22+August!B22+September!B22+October!B22+November!B22+December!B22</f>
-        <v>245</v>
+        <v>293</v>
       </c>
       <c r="C22" s="2">
         <f>January!C22+February!C22+March!C22+April!C22+May!C22+June!C22+July!C22+August!C22+September!C22+October!C22+November!C22+December!C22</f>
-        <v>663</v>
+        <v>771</v>
       </c>
       <c r="D22" s="2">
         <f>January!D22+February!D22+March!D22+April!D22+May!D22+June!D22+July!D22+August!D22+September!D22+October!D22+November!D22+December!D22</f>
-        <v>-418</v>
+        <v>-478</v>
       </c>
       <c r="E22" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2317,7 +2326,7 @@
       </c>
       <c r="G22" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.37 : 1</v>
+        <v>0.38 : 1</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2326,15 +2335,15 @@
       </c>
       <c r="B23" s="4">
         <f>January!B23+February!B23+March!B23+April!B23+May!B23+June!B23+July!B23+August!B23+September!B23+October!B23+November!B23+December!B23</f>
-        <v>6324</v>
+        <v>7100</v>
       </c>
       <c r="C23" s="4">
         <f>January!C23+February!C23+March!C23+April!C23+May!C23+June!C23+July!C23+August!C23+September!C23+October!C23+November!C23+December!C23</f>
-        <v>4358</v>
+        <v>4772</v>
       </c>
       <c r="D23" s="4">
         <f>January!D23+February!D23+March!D23+April!D23+May!D23+June!D23+July!D23+August!D23+September!D23+October!D23+November!D23+December!D23</f>
-        <v>1966</v>
+        <v>2328</v>
       </c>
       <c r="E23" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2346,7 +2355,7 @@
       </c>
       <c r="G23" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.45 : 1</v>
+        <v>1.49 : 1</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2355,15 +2364,15 @@
       </c>
       <c r="B24" s="2">
         <f>January!B24+February!B24+March!B24+April!B24+May!B24+June!B24+July!B24+August!B24+September!B24+October!B24+November!B24+December!B24</f>
-        <v>16820</v>
+        <v>18530</v>
       </c>
       <c r="C24" s="2">
         <f>January!C24+February!C24+March!C24+April!C24+May!C24+June!C24+July!C24+August!C24+September!C24+October!C24+November!C24+December!C24</f>
-        <v>12538</v>
+        <v>13899</v>
       </c>
       <c r="D24" s="2">
         <f>January!D24+February!D24+March!D24+April!D24+May!D24+June!D24+July!D24+August!D24+September!D24+October!D24+November!D24+December!D24</f>
-        <v>4282</v>
+        <v>4631</v>
       </c>
       <c r="E24" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2375,7 +2384,7 @@
       </c>
       <c r="G24" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.34 : 1</v>
+        <v>1.33 : 1</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2384,15 +2393,15 @@
       </c>
       <c r="B25" s="4">
         <f>January!B25+February!B25+March!B25+April!B25+May!B25+June!B25+July!B25+August!B25+September!B25+October!B25+November!B25+December!B25</f>
-        <v>1584</v>
+        <v>1772</v>
       </c>
       <c r="C25" s="4">
         <f>January!C25+February!C25+March!C25+April!C25+May!C25+June!C25+July!C25+August!C25+September!C25+October!C25+November!C25+December!C25</f>
-        <v>3229</v>
+        <v>3583</v>
       </c>
       <c r="D25" s="4">
         <f>January!D25+February!D25+March!D25+April!D25+May!D25+June!D25+July!D25+August!D25+September!D25+October!D25+November!D25+December!D25</f>
-        <v>-1645</v>
+        <v>-1811</v>
       </c>
       <c r="E25" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2442,15 +2451,15 @@
       </c>
       <c r="B27" s="4">
         <f>January!B27+February!B27+March!B27+April!B27+May!B27+June!B27+July!B27+August!B27+September!B27+October!B27+November!B27+December!B27</f>
-        <v>2497</v>
+        <v>2731</v>
       </c>
       <c r="C27" s="4">
         <f>January!C27+February!C27+March!C27+April!C27+May!C27+June!C27+July!C27+August!C27+September!C27+October!C27+November!C27+December!C27</f>
-        <v>1795</v>
+        <v>2014</v>
       </c>
       <c r="D27" s="4">
         <f>January!D27+February!D27+March!D27+April!D27+May!D27+June!D27+July!D27+August!D27+September!D27+October!D27+November!D27+December!D27</f>
-        <v>702</v>
+        <v>717</v>
       </c>
       <c r="E27" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2462,7 +2471,7 @@
       </c>
       <c r="G27" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.39 : 1</v>
+        <v>1.36 : 1</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2471,15 +2480,15 @@
       </c>
       <c r="B28" s="2">
         <f>January!B28+February!B28+March!B28+April!B28+May!B28+June!B28+July!B28+August!B28+September!B28+October!B28+November!B28+December!B28</f>
-        <v>484</v>
+        <v>525</v>
       </c>
       <c r="C28" s="2">
         <f>January!C28+February!C28+March!C28+April!C28+May!C28+June!C28+July!C28+August!C28+September!C28+October!C28+November!C28+December!C28</f>
-        <v>661</v>
+        <v>720</v>
       </c>
       <c r="D28" s="2">
         <f>January!D28+February!D28+March!D28+April!D28+May!D28+June!D28+July!D28+August!D28+September!D28+October!D28+November!D28+December!D28</f>
-        <v>-177</v>
+        <v>-195</v>
       </c>
       <c r="E28" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2500,15 +2509,15 @@
       </c>
       <c r="B29" s="4">
         <f>January!B29+February!B29+March!B29+April!B29+May!B29+June!B29+July!B29+August!B29+September!B29+October!B29+November!B29+December!B29</f>
-        <v>4814</v>
+        <v>5397</v>
       </c>
       <c r="C29" s="4">
         <f>January!C29+February!C29+March!C29+April!C29+May!C29+June!C29+July!C29+August!C29+September!C29+October!C29+November!C29+December!C29</f>
-        <v>4199</v>
+        <v>4690</v>
       </c>
       <c r="D29" s="4">
         <f>January!D29+February!D29+March!D29+April!D29+May!D29+June!D29+July!D29+August!D29+September!D29+October!D29+November!D29+December!D29</f>
-        <v>615</v>
+        <v>707</v>
       </c>
       <c r="E29" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2529,15 +2538,15 @@
       </c>
       <c r="B30" s="2">
         <f>January!B30+February!B30+March!B30+April!B30+May!B30+June!B30+July!B30+August!B30+September!B30+October!B30+November!B30+December!B30</f>
-        <v>420</v>
+        <v>456</v>
       </c>
       <c r="C30" s="2">
         <f>January!C30+February!C30+March!C30+April!C30+May!C30+June!C30+July!C30+August!C30+September!C30+October!C30+November!C30+December!C30</f>
-        <v>321</v>
+        <v>362</v>
       </c>
       <c r="D30" s="2">
         <f>January!D30+February!D30+March!D30+April!D30+May!D30+June!D30+July!D30+August!D30+September!D30+October!D30+November!D30+December!D30</f>
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E30" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2549,7 +2558,7 @@
       </c>
       <c r="G30" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.31 : 1</v>
+        <v>1.26 : 1</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2558,15 +2567,15 @@
       </c>
       <c r="B31" s="4">
         <f>January!B31+February!B31+March!B31+April!B31+May!B31+June!B31+July!B31+August!B31+September!B31+October!B31+November!B31+December!B31</f>
-        <v>672</v>
+        <v>788</v>
       </c>
       <c r="C31" s="4">
         <f>January!C31+February!C31+March!C31+April!C31+May!C31+June!C31+July!C31+August!C31+September!C31+October!C31+November!C31+December!C31</f>
-        <v>2706</v>
+        <v>2994</v>
       </c>
       <c r="D31" s="4">
         <f>January!D31+February!D31+March!D31+April!D31+May!D31+June!D31+July!D31+August!D31+September!D31+October!D31+November!D31+December!D31</f>
-        <v>-2034</v>
+        <v>-2206</v>
       </c>
       <c r="E31" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2578,7 +2587,7 @@
       </c>
       <c r="G31" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.25 : 1</v>
+        <v>0.26 : 1</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2587,15 +2596,15 @@
       </c>
       <c r="B32" s="2">
         <f>January!B32+February!B32+March!B32+April!B32+May!B32+June!B32+July!B32+August!B32+September!B32+October!B32+November!B32+December!B32</f>
-        <v>4016</v>
+        <v>4501</v>
       </c>
       <c r="C32" s="2">
         <f>January!C32+February!C32+March!C32+April!C32+May!C32+June!C32+July!C32+August!C32+September!C32+October!C32+November!C32+December!C32</f>
-        <v>5085</v>
+        <v>5642</v>
       </c>
       <c r="D32" s="2">
         <f>January!D32+February!D32+March!D32+April!D32+May!D32+June!D32+July!D32+August!D32+September!D32+October!D32+November!D32+December!D32</f>
-        <v>-1069</v>
+        <v>-1141</v>
       </c>
       <c r="E32" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2607,7 +2616,7 @@
       </c>
       <c r="G32" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.79 : 1</v>
+        <v>0.8 : 1</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2616,15 +2625,15 @@
       </c>
       <c r="B33" s="4">
         <f>January!B33+February!B33+March!B33+April!B33+May!B33+June!B33+July!B33+August!B33+September!B33+October!B33+November!B33+December!B33</f>
-        <v>3808</v>
+        <v>4236</v>
       </c>
       <c r="C33" s="4">
         <f>January!C33+February!C33+March!C33+April!C33+May!C33+June!C33+July!C33+August!C33+September!C33+October!C33+November!C33+December!C33</f>
-        <v>4672</v>
+        <v>5149</v>
       </c>
       <c r="D33" s="4">
         <f>January!D33+February!D33+March!D33+April!D33+May!D33+June!D33+July!D33+August!D33+September!D33+October!D33+November!D33+December!D33</f>
-        <v>-864</v>
+        <v>-913</v>
       </c>
       <c r="E33" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2645,15 +2654,15 @@
       </c>
       <c r="B34" s="2">
         <f>January!B34+February!B34+March!B34+April!B34+May!B34+June!B34+July!B34+August!B34+September!B34+October!B34+November!B34+December!B34</f>
-        <v>1940</v>
+        <v>2121</v>
       </c>
       <c r="C34" s="2">
         <f>January!C34+February!C34+March!C34+April!C34+May!C34+June!C34+July!C34+August!C34+September!C34+October!C34+November!C34+December!C34</f>
-        <v>1063</v>
+        <v>1182</v>
       </c>
       <c r="D34" s="2">
         <f>January!D34+February!D34+March!D34+April!D34+May!D34+June!D34+July!D34+August!D34+September!D34+October!D34+November!D34+December!D34</f>
-        <v>877</v>
+        <v>939</v>
       </c>
       <c r="E34" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2665,7 +2674,7 @@
       </c>
       <c r="G34" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.83 : 1</v>
+        <v>1.79 : 1</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2674,15 +2683,15 @@
       </c>
       <c r="B35" s="4">
         <f>January!B35+February!B35+March!B35+April!B35+May!B35+June!B35+July!B35+August!B35+September!B35+October!B35+November!B35+December!B35</f>
-        <v>8674</v>
+        <v>9586</v>
       </c>
       <c r="C35" s="4">
         <f>January!C35+February!C35+March!C35+April!C35+May!C35+June!C35+July!C35+August!C35+September!C35+October!C35+November!C35+December!C35</f>
-        <v>9101</v>
+        <v>10142</v>
       </c>
       <c r="D35" s="4">
         <f>January!D35+February!D35+March!D35+April!D35+May!D35+June!D35+July!D35+August!D35+September!D35+October!D35+November!D35+December!D35</f>
-        <v>-427</v>
+        <v>-556</v>
       </c>
       <c r="E35" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2703,15 +2712,15 @@
       </c>
       <c r="B36" s="2">
         <f>January!B36+February!B36+March!B36+April!B36+May!B36+June!B36+July!B36+August!B36+September!B36+October!B36+November!B36+December!B36</f>
-        <v>1971</v>
+        <v>2169</v>
       </c>
       <c r="C36" s="2">
         <f>January!C36+February!C36+March!C36+April!C36+May!C36+June!C36+July!C36+August!C36+September!C36+October!C36+November!C36+December!C36</f>
-        <v>4294</v>
+        <v>4791</v>
       </c>
       <c r="D36" s="2">
         <f>January!D36+February!D36+March!D36+April!D36+May!D36+June!D36+July!D36+August!D36+September!D36+October!D36+November!D36+December!D36</f>
-        <v>-2323</v>
+        <v>-2622</v>
       </c>
       <c r="E36" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2723,7 +2732,7 @@
       </c>
       <c r="G36" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.46 : 1</v>
+        <v>0.45 : 1</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2732,15 +2741,15 @@
       </c>
       <c r="B37" s="4">
         <f>January!B37+February!B37+March!B37+April!B37+May!B37+June!B37+July!B37+August!B37+September!B37+October!B37+November!B37+December!B37</f>
-        <v>4702</v>
+        <v>5196</v>
       </c>
       <c r="C37" s="4">
         <f>January!C37+February!C37+March!C37+April!C37+May!C37+June!C37+July!C37+August!C37+September!C37+October!C37+November!C37+December!C37</f>
-        <v>3227</v>
+        <v>3560</v>
       </c>
       <c r="D37" s="4">
         <f>January!D37+February!D37+March!D37+April!D37+May!D37+June!D37+July!D37+August!D37+September!D37+October!D37+November!D37+December!D37</f>
-        <v>1475</v>
+        <v>1636</v>
       </c>
       <c r="E37" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2761,15 +2770,15 @@
       </c>
       <c r="B38" s="2">
         <f>January!B38+February!B38+March!B38+April!B38+May!B38+June!B38+July!B38+August!B38+September!B38+October!B38+November!B38+December!B38</f>
-        <v>287</v>
+        <v>307</v>
       </c>
       <c r="C38" s="2">
         <f>January!C38+February!C38+March!C38+April!C38+May!C38+June!C38+July!C38+August!C38+September!C38+October!C38+November!C38+December!C38</f>
-        <v>1514</v>
+        <v>1691</v>
       </c>
       <c r="D38" s="2">
         <f>January!D38+February!D38+March!D38+April!D38+May!D38+June!D38+July!D38+August!D38+September!D38+October!D38+November!D38+December!D38</f>
-        <v>-1227</v>
+        <v>-1384</v>
       </c>
       <c r="E38" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2781,7 +2790,7 @@
       </c>
       <c r="G38" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.19 : 1</v>
+        <v>0.18 : 1</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2790,15 +2799,15 @@
       </c>
       <c r="B39" s="8">
         <f>January!B39+February!B39+March!B39+April!B39+May!B39+June!B39+July!B39+August!B39+September!B39+October!B39+November!B39+December!B39</f>
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="C39" s="8">
         <f>January!C39+February!C39+March!C39+April!C39+May!C39+June!C39+July!C39+August!C39+September!C39+October!C39+November!C39+December!C39</f>
-        <v>419</v>
+        <v>483</v>
       </c>
       <c r="D39" s="8">
         <f>January!D39+February!D39+March!D39+April!D39+May!D39+June!D39+July!D39+August!D39+September!D39+October!D39+November!D39+December!D39</f>
-        <v>-218</v>
+        <v>-274</v>
       </c>
       <c r="E39" s="31" t="str">
         <f t="shared" si="1"/>
@@ -2810,7 +2819,7 @@
       </c>
       <c r="G39" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>0.48 : 1</v>
+        <v>0.43 : 1</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2819,15 +2828,15 @@
       </c>
       <c r="B40" s="8">
         <f>January!B40+February!B40+March!B40+April!B40+May!B40+June!B40+July!B40+August!B40+September!B40+October!B40+November!B40+December!B40</f>
-        <v>463</v>
+        <v>573</v>
       </c>
       <c r="C40" s="8">
         <f>January!C40+February!C40+March!C40+April!C40+May!C40+June!C40+July!C40+August!C40+September!C40+October!C40+November!C40+December!C40</f>
-        <v>791</v>
+        <v>898</v>
       </c>
       <c r="D40" s="8">
         <f>January!D40+February!D40+March!D40+April!D40+May!D40+June!D40+July!D40+August!D40+September!D40+October!D40+November!D40+December!D40</f>
-        <v>-328</v>
+        <v>-325</v>
       </c>
       <c r="E40" s="31" t="str">
         <f t="shared" si="1"/>
@@ -2839,7 +2848,7 @@
       </c>
       <c r="G40" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>0.59 : 1</v>
+        <v>0.64 : 1</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2848,15 +2857,15 @@
       </c>
       <c r="B41" s="8">
         <f>January!B41+February!B41+March!B41+April!B41+May!B41+June!B41+July!B41+August!B41+September!B41+October!B41+November!B41+December!B41</f>
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C41" s="8">
         <f>January!C41+February!C41+March!C41+April!C41+May!C41+June!C41+July!C41+August!C41+September!C41+October!C41+November!C41+December!C41</f>
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="D41" s="8">
         <f>January!D41+February!D41+March!D41+April!D41+May!D41+June!D41+July!D41+August!D41+September!D41+October!D41+November!D41+December!D41</f>
-        <v>-75</v>
+        <v>-94</v>
       </c>
       <c r="E41" s="31" t="str">
         <f t="shared" si="1"/>
@@ -2868,7 +2877,7 @@
       </c>
       <c r="G41" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>0.52 : 1</v>
+        <v>0.47 : 1</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2877,27 +2886,27 @@
       </c>
       <c r="B42" s="8">
         <f>January!B42+February!B42+March!B42+April!B42+May!B42+June!B42+July!B42+August!B42+September!B42+October!B42+November!B42+December!B42</f>
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="C42" s="8">
         <f>January!C42+February!C42+March!C42+April!C42+May!C42+June!C42+July!C42+August!C42+September!C42+October!C42+November!C42+December!C42</f>
-        <v>76</v>
+        <v>111</v>
       </c>
       <c r="D42" s="8">
         <f>January!D42+February!D42+March!D42+April!D42+May!D42+June!D42+July!D42+August!D42+September!D42+October!D42+November!D42+December!D42</f>
-        <v>8</v>
+        <v>-1</v>
       </c>
       <c r="E42" s="31" t="str">
         <f t="shared" si="1"/>
-        <v>We borrowed more than we lent this year</v>
+        <v/>
       </c>
       <c r="F42" s="31" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>We lent more than we borrowed this year</v>
       </c>
       <c r="G42" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>1.11 : 1</v>
+        <v>0.99 : 1</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2935,15 +2944,15 @@
       </c>
       <c r="B44" s="4">
         <f>January!B44+February!B44+March!B44+April!B44+May!B44+June!B44+July!B44+August!B44+September!B44+October!B44+November!B44+December!B44</f>
-        <v>929</v>
+        <v>1022</v>
       </c>
       <c r="C44" s="4">
         <f>January!C44+February!C44+March!C44+April!C44+May!C44+June!C44+July!C44+August!C44+September!C44+October!C44+November!C44+December!C44</f>
-        <v>693</v>
+        <v>769</v>
       </c>
       <c r="D44" s="4">
         <f>January!D44+February!D44+March!D44+April!D44+May!D44+June!D44+July!D44+August!D44+September!D44+October!D44+November!D44+December!D44</f>
-        <v>236</v>
+        <v>253</v>
       </c>
       <c r="E44" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2955,7 +2964,7 @@
       </c>
       <c r="G44" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.34 : 1</v>
+        <v>1.33 : 1</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2964,15 +2973,15 @@
       </c>
       <c r="B45" s="2">
         <f>January!B45+February!B45+March!B45+April!B45+May!B45+June!B45+July!B45+August!B45+September!B45+October!B45+November!B45+December!B45</f>
-        <v>677</v>
+        <v>766</v>
       </c>
       <c r="C45" s="2">
         <f>January!C45+February!C45+March!C45+April!C45+May!C45+June!C45+July!C45+August!C45+September!C45+October!C45+November!C45+December!C45</f>
-        <v>1392</v>
+        <v>1572</v>
       </c>
       <c r="D45" s="2">
         <f>January!D45+February!D45+March!D45+April!D45+May!D45+June!D45+July!D45+August!D45+September!D45+October!D45+November!D45+December!D45</f>
-        <v>-715</v>
+        <v>-806</v>
       </c>
       <c r="E45" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2993,15 +3002,15 @@
       </c>
       <c r="B46" s="4">
         <f>January!B46+February!B46+March!B46+April!B46+May!B46+June!B46+July!B46+August!B46+September!B46+October!B46+November!B46+December!B46</f>
-        <v>3989</v>
+        <v>4442</v>
       </c>
       <c r="C46" s="4">
         <f>January!C46+February!C46+March!C46+April!C46+May!C46+June!C46+July!C46+August!C46+September!C46+October!C46+November!C46+December!C46</f>
-        <v>5558</v>
+        <v>6234</v>
       </c>
       <c r="D46" s="4">
         <f>January!D46+February!D46+March!D46+April!D46+May!D46+June!D46+July!D46+August!D46+September!D46+October!D46+November!D46+December!D46</f>
-        <v>-1569</v>
+        <v>-1792</v>
       </c>
       <c r="E46" s="29" t="str">
         <f t="shared" si="1"/>
@@ -3013,7 +3022,7 @@
       </c>
       <c r="G46" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.72 : 1</v>
+        <v>0.71 : 1</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3022,15 +3031,15 @@
       </c>
       <c r="B47" s="2">
         <f>January!B47+February!B47+March!B47+April!B47+May!B47+June!B47+July!B47+August!B47+September!B47+October!B47+November!B47+December!B47</f>
-        <v>8021</v>
+        <v>9027</v>
       </c>
       <c r="C47" s="2">
         <f>January!C47+February!C47+March!C47+April!C47+May!C47+June!C47+July!C47+August!C47+September!C47+October!C47+November!C47+December!C47</f>
-        <v>5936</v>
+        <v>6633</v>
       </c>
       <c r="D47" s="2">
         <f>January!D47+February!D47+March!D47+April!D47+May!D47+June!D47+July!D47+August!D47+September!D47+October!D47+November!D47+December!D47</f>
-        <v>2085</v>
+        <v>2394</v>
       </c>
       <c r="E47" s="28" t="str">
         <f t="shared" si="1"/>
@@ -3042,7 +3051,7 @@
       </c>
       <c r="G47" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.35 : 1</v>
+        <v>1.36 : 1</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3051,15 +3060,15 @@
       </c>
       <c r="B48" s="4">
         <f>January!B48+February!B48+March!B48+April!B48+May!B48+June!B48+July!B48+August!B48+September!B48+October!B48+November!B48+December!B48</f>
-        <v>2100</v>
+        <v>2432</v>
       </c>
       <c r="C48" s="4">
         <f>January!C48+February!C48+March!C48+April!C48+May!C48+June!C48+July!C48+August!C48+September!C48+October!C48+November!C48+December!C48</f>
-        <v>5781</v>
+        <v>6324</v>
       </c>
       <c r="D48" s="4">
         <f>January!D48+February!D48+March!D48+April!D48+May!D48+June!D48+July!D48+August!D48+September!D48+October!D48+November!D48+December!D48</f>
-        <v>-3681</v>
+        <v>-3892</v>
       </c>
       <c r="E48" s="29" t="str">
         <f t="shared" si="1"/>
@@ -3071,7 +3080,7 @@
       </c>
       <c r="G48" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.36 : 1</v>
+        <v>0.38 : 1</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3080,15 +3089,15 @@
       </c>
       <c r="B49" s="2">
         <f>January!B49+February!B49+March!B49+April!B49+May!B49+June!B49+July!B49+August!B49+September!B49+October!B49+November!B49+December!B49</f>
-        <v>3365</v>
+        <v>3780</v>
       </c>
       <c r="C49" s="2">
         <f>January!C49+February!C49+March!C49+April!C49+May!C49+June!C49+July!C49+August!C49+September!C49+October!C49+November!C49+December!C49</f>
-        <v>1908</v>
+        <v>2174</v>
       </c>
       <c r="D49" s="2">
         <f>January!D49+February!D49+March!D49+April!D49+May!D49+June!D49+July!D49+August!D49+September!D49+October!D49+November!D49+December!D49</f>
-        <v>1457</v>
+        <v>1606</v>
       </c>
       <c r="E49" s="28" t="str">
         <f t="shared" si="1"/>
@@ -3100,7 +3109,7 @@
       </c>
       <c r="G49" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.76 : 1</v>
+        <v>1.74 : 1</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3109,15 +3118,15 @@
       </c>
       <c r="B50" s="4">
         <f>January!B50+February!B50+March!B50+April!B50+May!B50+June!B50+July!B50+August!B50+September!B50+October!B50+November!B50+December!B50</f>
-        <v>7745</v>
+        <v>8760</v>
       </c>
       <c r="C50" s="4">
         <f>January!C50+February!C50+March!C50+April!C50+May!C50+June!C50+July!C50+August!C50+September!C50+October!C50+November!C50+December!C50</f>
-        <v>5046</v>
+        <v>5537</v>
       </c>
       <c r="D50" s="4">
         <f>January!D50+February!D50+March!D50+April!D50+May!D50+June!D50+July!D50+August!D50+September!D50+October!D50+November!D50+December!D50</f>
-        <v>2699</v>
+        <v>3223</v>
       </c>
       <c r="E50" s="29" t="str">
         <f t="shared" si="1"/>
@@ -3129,7 +3138,7 @@
       </c>
       <c r="G50" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.53 : 1</v>
+        <v>1.58 : 1</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3138,15 +3147,15 @@
       </c>
       <c r="B51" s="2">
         <f>January!B51+February!B51+March!B51+April!B51+May!B51+June!B51+July!B51+August!B51+September!B51+October!B51+November!B51+December!B51</f>
-        <v>2127</v>
+        <v>2341</v>
       </c>
       <c r="C51" s="2">
         <f>January!C51+February!C51+March!C51+April!C51+May!C51+June!C51+July!C51+August!C51+September!C51+October!C51+November!C51+December!C51</f>
-        <v>976</v>
+        <v>1134</v>
       </c>
       <c r="D51" s="2">
         <f>January!D51+February!D51+March!D51+April!D51+May!D51+June!D51+July!D51+August!D51+September!D51+October!D51+November!D51+December!D51</f>
-        <v>1151</v>
+        <v>1207</v>
       </c>
       <c r="E51" s="28" t="str">
         <f t="shared" si="1"/>
@@ -3158,7 +3167,7 @@
       </c>
       <c r="G51" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>2.18 : 1</v>
+        <v>2.06 : 1</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3167,15 +3176,15 @@
       </c>
       <c r="B52" s="4">
         <f>January!B52+February!B52+March!B52+April!B52+May!B52+June!B52+July!B52+August!B52+September!B52+October!B52+November!B52+December!B52</f>
-        <v>4070</v>
+        <v>4478</v>
       </c>
       <c r="C52" s="4">
         <f>January!C52+February!C52+March!C52+April!C52+May!C52+June!C52+July!C52+August!C52+September!C52+October!C52+November!C52+December!C52</f>
-        <v>4910</v>
+        <v>5420</v>
       </c>
       <c r="D52" s="4">
         <f>January!D52+February!D52+March!D52+April!D52+May!D52+June!D52+July!D52+August!D52+September!D52+October!D52+November!D52+December!D52</f>
-        <v>-840</v>
+        <v>-942</v>
       </c>
       <c r="E52" s="29" t="str">
         <f t="shared" si="1"/>
@@ -3196,15 +3205,15 @@
       </c>
       <c r="B53" s="2">
         <f>January!B53+February!B53+March!B53+April!B53+May!B53+June!B53+July!B53+August!B53+September!B53+October!B53+November!B53+December!B53</f>
-        <v>1141</v>
+        <v>1261</v>
       </c>
       <c r="C53" s="2">
         <f>January!C53+February!C53+March!C53+April!C53+May!C53+June!C53+July!C53+August!C53+September!C53+October!C53+November!C53+December!C53</f>
-        <v>2023</v>
+        <v>2273</v>
       </c>
       <c r="D53" s="2">
         <f>January!D53+February!D53+March!D53+April!D53+May!D53+June!D53+July!D53+August!D53+September!D53+October!D53+November!D53+December!D53</f>
-        <v>-882</v>
+        <v>-1012</v>
       </c>
       <c r="E53" s="28" t="str">
         <f t="shared" si="1"/>
@@ -3216,7 +3225,7 @@
       </c>
       <c r="G53" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.56 : 1</v>
+        <v>0.55 : 1</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3225,15 +3234,15 @@
       </c>
       <c r="B54" s="4">
         <f>January!B54+February!B54+March!B54+April!B54+May!B54+June!B54+July!B54+August!B54+September!B54+October!B54+November!B54+December!B54</f>
-        <v>253</v>
+        <v>282</v>
       </c>
       <c r="C54" s="4">
         <f>January!C54+February!C54+March!C54+April!C54+May!C54+June!C54+July!C54+August!C54+September!C54+October!C54+November!C54+December!C54</f>
-        <v>2063</v>
+        <v>2281</v>
       </c>
       <c r="D54" s="4">
         <f>January!D54+February!D54+March!D54+April!D54+May!D54+June!D54+July!D54+August!D54+September!D54+October!D54+November!D54+December!D54</f>
-        <v>-1810</v>
+        <v>-1999</v>
       </c>
       <c r="E54" s="29" t="str">
         <f t="shared" si="1"/>
@@ -3254,15 +3263,15 @@
       </c>
       <c r="B55" s="10">
         <f>January!B55+February!B55+March!B55+April!B55+May!B55+June!B55+July!B55+August!B55+September!B55+October!B55+November!B55+December!B55</f>
-        <v>1900</v>
+        <v>2229</v>
       </c>
       <c r="C55" s="10">
         <f>January!C55+February!C55+March!C55+April!C55+May!C55+June!C55+July!C55+August!C55+September!C55+October!C55+November!C55+December!C55</f>
-        <v>1567</v>
+        <v>1778</v>
       </c>
       <c r="D55" s="10">
         <f>January!D55+February!D55+March!D55+April!D55+May!D55+June!D55+July!D55+August!D55+September!D55+October!D55+November!D55+December!D55</f>
-        <v>333</v>
+        <v>451</v>
       </c>
       <c r="E55" s="32" t="str">
         <f t="shared" si="1"/>
@@ -3274,7 +3283,7 @@
       </c>
       <c r="G55" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>1.21 : 1</v>
+        <v>1.25 : 1</v>
       </c>
     </row>
   </sheetData>
@@ -4531,108 +4540,204 @@
       <c r="A2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="28"/>
+      <c r="B2" s="18">
+        <v>1788</v>
+      </c>
+      <c r="C2" s="18">
+        <v>1239</v>
+      </c>
+      <c r="D2" s="18">
+        <v>549</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F2" s="28"/>
-      <c r="G2" s="3"/>
+      <c r="G2" s="3" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="29"/>
+      <c r="B3" s="21">
+        <v>541</v>
+      </c>
+      <c r="C3" s="21">
+        <v>510</v>
+      </c>
+      <c r="D3" s="21">
+        <v>31</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F3" s="29"/>
-      <c r="G3" s="5"/>
+      <c r="G3" s="5" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
+      <c r="B4" s="18">
+        <v>1106</v>
+      </c>
+      <c r="C4" s="18">
+        <v>1392</v>
+      </c>
+      <c r="D4" s="18">
+        <v>-286</v>
+      </c>
       <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="3"/>
+      <c r="F4" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
+      <c r="B5" s="21">
+        <v>82</v>
+      </c>
+      <c r="C5" s="21">
+        <v>144</v>
+      </c>
+      <c r="D5" s="21">
+        <v>-62</v>
+      </c>
       <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="5"/>
+      <c r="F5" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
+      <c r="B6" s="18">
+        <v>1249</v>
+      </c>
+      <c r="C6" s="18">
+        <v>1516</v>
+      </c>
+      <c r="D6" s="18">
+        <v>-267</v>
+      </c>
       <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="3"/>
+      <c r="F6" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="29"/>
+      <c r="B7" s="21">
+        <v>219</v>
+      </c>
+      <c r="C7" s="21">
+        <v>200</v>
+      </c>
+      <c r="D7" s="21">
+        <v>19</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F7" s="29"/>
-      <c r="G7" s="5"/>
+      <c r="G7" s="5" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
+      <c r="B8" s="18">
+        <v>81</v>
+      </c>
+      <c r="C8" s="18">
+        <v>179</v>
+      </c>
+      <c r="D8" s="18">
+        <v>-98</v>
+      </c>
       <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="3"/>
+      <c r="F8" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
+      <c r="B9" s="21">
+        <v>52</v>
+      </c>
+      <c r="C9" s="21">
+        <v>66</v>
+      </c>
+      <c r="D9" s="21">
+        <v>-14</v>
+      </c>
       <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="5"/>
+      <c r="F9" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
+      <c r="B10" s="18">
+        <v>1</v>
+      </c>
+      <c r="C10" s="18">
+        <v>57</v>
+      </c>
+      <c r="D10" s="18">
+        <v>-56</v>
+      </c>
       <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="3"/>
+      <c r="F10" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
+      <c r="B11" s="21">
+        <v>0</v>
+      </c>
+      <c r="C11" s="21">
+        <v>0</v>
+      </c>
+      <c r="D11" s="21">
+        <v>0</v>
+      </c>
       <c r="E11" s="29"/>
       <c r="F11" s="29"/>
       <c r="G11" s="5"/>
@@ -4641,163 +4746,309 @@
       <c r="A12" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
+      <c r="B12" s="23">
+        <v>20</v>
+      </c>
+      <c r="C12" s="23">
+        <v>23</v>
+      </c>
+      <c r="D12" s="23">
+        <v>-3</v>
+      </c>
       <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="7"/>
+      <c r="F12" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="30"/>
+      <c r="B13" s="23">
+        <v>182</v>
+      </c>
+      <c r="C13" s="23">
+        <v>125</v>
+      </c>
+      <c r="D13" s="23">
+        <v>57</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>61</v>
+      </c>
       <c r="F13" s="30"/>
-      <c r="G13" s="7"/>
+      <c r="G13" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
+      <c r="B14" s="23">
+        <v>119</v>
+      </c>
+      <c r="C14" s="23">
+        <v>316</v>
+      </c>
+      <c r="D14" s="23">
+        <v>-197</v>
+      </c>
       <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="7"/>
+      <c r="F14" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
+      <c r="B15" s="23">
+        <v>85</v>
+      </c>
+      <c r="C15" s="23">
+        <v>123</v>
+      </c>
+      <c r="D15" s="23">
+        <v>-38</v>
+      </c>
       <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="7"/>
+      <c r="F15" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
+      <c r="B16" s="18">
+        <v>21</v>
+      </c>
+      <c r="C16" s="18">
+        <v>144</v>
+      </c>
+      <c r="D16" s="18">
+        <v>-123</v>
+      </c>
       <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="3"/>
+      <c r="F16" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="29"/>
+      <c r="B17" s="21">
+        <v>769</v>
+      </c>
+      <c r="C17" s="21">
+        <v>480</v>
+      </c>
+      <c r="D17" s="21">
+        <v>289</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F17" s="29"/>
-      <c r="G17" s="5"/>
+      <c r="G17" s="5" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
+      <c r="B18" s="18">
+        <v>74</v>
+      </c>
+      <c r="C18" s="18">
+        <v>118</v>
+      </c>
+      <c r="D18" s="18">
+        <v>-44</v>
+      </c>
       <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="3"/>
+      <c r="F18" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="29"/>
+      <c r="B19" s="21">
+        <v>619</v>
+      </c>
+      <c r="C19" s="21">
+        <v>360</v>
+      </c>
+      <c r="D19" s="21">
+        <v>259</v>
+      </c>
+      <c r="E19" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F19" s="29"/>
-      <c r="G19" s="5"/>
+      <c r="G19" s="5" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
+      <c r="B20" s="18">
+        <v>11</v>
+      </c>
+      <c r="C20" s="18">
+        <v>72</v>
+      </c>
+      <c r="D20" s="18">
+        <v>-61</v>
+      </c>
       <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="3"/>
+      <c r="F20" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
+      <c r="B21" s="21">
+        <v>441</v>
+      </c>
+      <c r="C21" s="21">
+        <v>456</v>
+      </c>
+      <c r="D21" s="21">
+        <v>-15</v>
+      </c>
       <c r="E21" s="29"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="5"/>
+      <c r="F21" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
+      <c r="B22" s="18">
+        <v>48</v>
+      </c>
+      <c r="C22" s="18">
+        <v>108</v>
+      </c>
+      <c r="D22" s="18">
+        <v>-60</v>
+      </c>
       <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="3"/>
+      <c r="F22" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="29"/>
+      <c r="B23" s="21">
+        <v>776</v>
+      </c>
+      <c r="C23" s="21">
+        <v>414</v>
+      </c>
+      <c r="D23" s="21">
+        <v>362</v>
+      </c>
+      <c r="E23" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F23" s="29"/>
-      <c r="G23" s="5"/>
+      <c r="G23" s="5" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="28"/>
+      <c r="B24" s="18">
+        <v>1710</v>
+      </c>
+      <c r="C24" s="18">
+        <v>1361</v>
+      </c>
+      <c r="D24" s="18">
+        <v>349</v>
+      </c>
+      <c r="E24" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F24" s="28"/>
-      <c r="G24" s="3"/>
+      <c r="G24" s="3" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
+      <c r="B25" s="21">
+        <v>188</v>
+      </c>
+      <c r="C25" s="21">
+        <v>354</v>
+      </c>
+      <c r="D25" s="21">
+        <v>-166</v>
+      </c>
       <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="5"/>
+      <c r="F25" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="26" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
+      <c r="B26" s="18">
+        <v>0</v>
+      </c>
+      <c r="C26" s="18">
+        <v>0</v>
+      </c>
+      <c r="D26" s="18">
+        <v>0</v>
+      </c>
       <c r="E26" s="28"/>
       <c r="F26" s="28"/>
       <c r="G26" s="3"/>
@@ -4806,185 +5057,351 @@
       <c r="A27" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="29"/>
+      <c r="B27" s="21">
+        <v>234</v>
+      </c>
+      <c r="C27" s="21">
+        <v>219</v>
+      </c>
+      <c r="D27" s="21">
+        <v>15</v>
+      </c>
+      <c r="E27" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F27" s="29"/>
-      <c r="G27" s="5"/>
+      <c r="G27" s="5" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
+      <c r="B28" s="18">
+        <v>41</v>
+      </c>
+      <c r="C28" s="18">
+        <v>59</v>
+      </c>
+      <c r="D28" s="18">
+        <v>-18</v>
+      </c>
       <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="3"/>
+      <c r="F28" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="29"/>
+      <c r="B29" s="21">
+        <v>583</v>
+      </c>
+      <c r="C29" s="21">
+        <v>491</v>
+      </c>
+      <c r="D29" s="21">
+        <v>92</v>
+      </c>
+      <c r="E29" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F29" s="29"/>
-      <c r="G29" s="5"/>
+      <c r="G29" s="5" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="30" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
+      <c r="B30" s="18">
+        <v>36</v>
+      </c>
+      <c r="C30" s="18">
+        <v>41</v>
+      </c>
+      <c r="D30" s="18">
+        <v>-5</v>
+      </c>
       <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="3"/>
+      <c r="F30" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
+      <c r="B31" s="21">
+        <v>116</v>
+      </c>
+      <c r="C31" s="21">
+        <v>288</v>
+      </c>
+      <c r="D31" s="21">
+        <v>-172</v>
+      </c>
       <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="5"/>
+      <c r="F31" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="32" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
+      <c r="B32" s="18">
+        <v>485</v>
+      </c>
+      <c r="C32" s="18">
+        <v>557</v>
+      </c>
+      <c r="D32" s="18">
+        <v>-72</v>
+      </c>
       <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="3"/>
+      <c r="F32" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="33" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
+      <c r="B33" s="21">
+        <v>428</v>
+      </c>
+      <c r="C33" s="21">
+        <v>477</v>
+      </c>
+      <c r="D33" s="21">
+        <v>-49</v>
+      </c>
       <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="5"/>
+      <c r="F33" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="34" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="28"/>
+      <c r="B34" s="18">
+        <v>181</v>
+      </c>
+      <c r="C34" s="18">
+        <v>119</v>
+      </c>
+      <c r="D34" s="18">
+        <v>62</v>
+      </c>
+      <c r="E34" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F34" s="28"/>
-      <c r="G34" s="3"/>
+      <c r="G34" s="3" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
+      <c r="B35" s="21">
+        <v>912</v>
+      </c>
+      <c r="C35" s="21">
+        <v>1041</v>
+      </c>
+      <c r="D35" s="21">
+        <v>-129</v>
+      </c>
       <c r="E35" s="29"/>
-      <c r="F35" s="29"/>
-      <c r="G35" s="5"/>
+      <c r="F35" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="36" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
+      <c r="B36" s="18">
+        <v>198</v>
+      </c>
+      <c r="C36" s="18">
+        <v>497</v>
+      </c>
+      <c r="D36" s="18">
+        <v>-299</v>
+      </c>
       <c r="E36" s="28"/>
-      <c r="F36" s="28"/>
-      <c r="G36" s="3"/>
+      <c r="F36" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="29"/>
+      <c r="B37" s="21">
+        <v>494</v>
+      </c>
+      <c r="C37" s="21">
+        <v>333</v>
+      </c>
+      <c r="D37" s="21">
+        <v>161</v>
+      </c>
+      <c r="E37" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F37" s="29"/>
-      <c r="G37" s="5"/>
+      <c r="G37" s="5" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
+      <c r="B38" s="18">
+        <v>20</v>
+      </c>
+      <c r="C38" s="18">
+        <v>177</v>
+      </c>
+      <c r="D38" s="18">
+        <v>-157</v>
+      </c>
       <c r="E38" s="28"/>
-      <c r="F38" s="28"/>
-      <c r="G38" s="3"/>
+      <c r="F38" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="B39" s="25"/>
-      <c r="C39" s="25"/>
-      <c r="D39" s="25"/>
+      <c r="B39" s="25">
+        <v>8</v>
+      </c>
+      <c r="C39" s="25">
+        <v>64</v>
+      </c>
+      <c r="D39" s="25">
+        <v>-56</v>
+      </c>
       <c r="E39" s="31"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="9"/>
+      <c r="F39" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="B40" s="25"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="31"/>
+      <c r="B40" s="25">
+        <v>110</v>
+      </c>
+      <c r="C40" s="25">
+        <v>107</v>
+      </c>
+      <c r="D40" s="25">
+        <v>3</v>
+      </c>
+      <c r="E40" s="31" t="s">
+        <v>61</v>
+      </c>
       <c r="F40" s="31"/>
-      <c r="G40" s="9"/>
+      <c r="G40" s="9" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
+      <c r="B41" s="25">
+        <v>3</v>
+      </c>
+      <c r="C41" s="25">
+        <v>22</v>
+      </c>
+      <c r="D41" s="25">
+        <v>-19</v>
+      </c>
       <c r="E41" s="31"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="9"/>
+      <c r="F41" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="42" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="B42" s="25"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="25"/>
+      <c r="B42" s="25">
+        <v>26</v>
+      </c>
+      <c r="C42" s="25">
+        <v>35</v>
+      </c>
+      <c r="D42" s="25">
+        <v>-9</v>
+      </c>
       <c r="E42" s="31"/>
-      <c r="F42" s="31"/>
-      <c r="G42" s="9"/>
+      <c r="F42" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="B43" s="25"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
+      <c r="B43" s="25">
+        <v>0</v>
+      </c>
+      <c r="C43" s="25">
+        <v>0</v>
+      </c>
+      <c r="D43" s="25">
+        <v>0</v>
+      </c>
       <c r="E43" s="31"/>
       <c r="F43" s="31"/>
       <c r="G43" s="9"/>
@@ -4993,133 +5410,253 @@
       <c r="A44" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="B44" s="21"/>
-      <c r="C44" s="21"/>
-      <c r="D44" s="21"/>
-      <c r="E44" s="29"/>
+      <c r="B44" s="21">
+        <v>93</v>
+      </c>
+      <c r="C44" s="21">
+        <v>76</v>
+      </c>
+      <c r="D44" s="21">
+        <v>17</v>
+      </c>
+      <c r="E44" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F44" s="29"/>
-      <c r="G44" s="5"/>
+      <c r="G44" s="5" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="45" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
+      <c r="B45" s="18">
+        <v>89</v>
+      </c>
+      <c r="C45" s="18">
+        <v>180</v>
+      </c>
+      <c r="D45" s="18">
+        <v>-91</v>
+      </c>
       <c r="E45" s="28"/>
-      <c r="F45" s="28"/>
-      <c r="G45" s="3"/>
+      <c r="F45" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="46" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="B46" s="21"/>
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
+      <c r="B46" s="21">
+        <v>453</v>
+      </c>
+      <c r="C46" s="21">
+        <v>676</v>
+      </c>
+      <c r="D46" s="21">
+        <v>-223</v>
+      </c>
       <c r="E46" s="29"/>
-      <c r="F46" s="29"/>
-      <c r="G46" s="5"/>
+      <c r="F46" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="47" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="28"/>
+      <c r="B47" s="18">
+        <v>1006</v>
+      </c>
+      <c r="C47" s="18">
+        <v>697</v>
+      </c>
+      <c r="D47" s="18">
+        <v>309</v>
+      </c>
+      <c r="E47" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F47" s="28"/>
-      <c r="G47" s="3"/>
+      <c r="G47" s="3" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="B48" s="21"/>
-      <c r="C48" s="21"/>
-      <c r="D48" s="21"/>
+      <c r="B48" s="21">
+        <v>332</v>
+      </c>
+      <c r="C48" s="21">
+        <v>543</v>
+      </c>
+      <c r="D48" s="21">
+        <v>-211</v>
+      </c>
       <c r="E48" s="29"/>
-      <c r="F48" s="29"/>
-      <c r="G48" s="5"/>
+      <c r="F48" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>254</v>
+      </c>
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B49" s="18"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="18"/>
-      <c r="E49" s="28"/>
+      <c r="B49" s="18">
+        <v>415</v>
+      </c>
+      <c r="C49" s="18">
+        <v>266</v>
+      </c>
+      <c r="D49" s="18">
+        <v>149</v>
+      </c>
+      <c r="E49" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F49" s="28"/>
-      <c r="G49" s="3"/>
+      <c r="G49" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="B50" s="21"/>
-      <c r="C50" s="21"/>
-      <c r="D50" s="21"/>
-      <c r="E50" s="29"/>
+      <c r="B50" s="21">
+        <v>1015</v>
+      </c>
+      <c r="C50" s="21">
+        <v>491</v>
+      </c>
+      <c r="D50" s="21">
+        <v>524</v>
+      </c>
+      <c r="E50" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F50" s="29"/>
-      <c r="G50" s="5"/>
+      <c r="G50" s="5" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B51" s="18"/>
-      <c r="C51" s="18"/>
-      <c r="D51" s="18"/>
-      <c r="E51" s="28"/>
+      <c r="B51" s="18">
+        <v>214</v>
+      </c>
+      <c r="C51" s="18">
+        <v>158</v>
+      </c>
+      <c r="D51" s="18">
+        <v>56</v>
+      </c>
+      <c r="E51" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F51" s="28"/>
-      <c r="G51" s="3"/>
+      <c r="G51" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="52" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="B52" s="21"/>
-      <c r="C52" s="21"/>
-      <c r="D52" s="21"/>
+      <c r="B52" s="21">
+        <v>408</v>
+      </c>
+      <c r="C52" s="21">
+        <v>510</v>
+      </c>
+      <c r="D52" s="21">
+        <v>-102</v>
+      </c>
       <c r="E52" s="29"/>
-      <c r="F52" s="29"/>
-      <c r="G52" s="5"/>
+      <c r="F52" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="53" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B53" s="18"/>
-      <c r="C53" s="18"/>
-      <c r="D53" s="18"/>
+      <c r="B53" s="18">
+        <v>120</v>
+      </c>
+      <c r="C53" s="18">
+        <v>250</v>
+      </c>
+      <c r="D53" s="18">
+        <v>-130</v>
+      </c>
       <c r="E53" s="28"/>
-      <c r="F53" s="28"/>
-      <c r="G53" s="3"/>
+      <c r="F53" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="54" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="B54" s="21"/>
-      <c r="C54" s="21"/>
-      <c r="D54" s="21"/>
+      <c r="B54" s="21">
+        <v>29</v>
+      </c>
+      <c r="C54" s="21">
+        <v>218</v>
+      </c>
+      <c r="D54" s="21">
+        <v>-189</v>
+      </c>
       <c r="E54" s="29"/>
-      <c r="F54" s="29"/>
-      <c r="G54" s="5"/>
+      <c r="F54" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="55" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="B55" s="27"/>
-      <c r="C55" s="27"/>
-      <c r="D55" s="27"/>
-      <c r="E55" s="32"/>
+      <c r="B55" s="27">
+        <v>329</v>
+      </c>
+      <c r="C55" s="27">
+        <v>211</v>
+      </c>
+      <c r="D55" s="27">
+        <v>118</v>
+      </c>
+      <c r="E55" s="32" t="s">
+        <v>61</v>
+      </c>
       <c r="F55" s="32"/>
-      <c r="G55" s="11"/>
+      <c r="G55" s="11" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G55" xr:uid="{00000000-0009-0000-0000-00000A000000}"/>

</xml_diff>

<commit_message>
Update all statistic files for November 2023
</commit_message>
<xml_diff>
--- a/statistics_files/2023/2023.g.net_borrower_lender.xlsx
+++ b/statistics_files/2023/2023.g.net_borrower_lender.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20403"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20404"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\GitHub\next_statistics\statistics_files\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CF10911-42C1-4434-8741-90DB73F4B2AA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8458D3B0-F905-4D21-8E88-FA5FB8655D43}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" tabRatio="673" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1819" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1921" uniqueCount="259">
   <si>
     <t>NET</t>
   </si>
@@ -817,6 +817,18 @@
   </si>
   <si>
     <t>0.61 : 1</t>
+  </si>
+  <si>
+    <t>1.21 : 1</t>
+  </si>
+  <si>
+    <t>0.39 : 1</t>
+  </si>
+  <si>
+    <t>2.19 : 1</t>
+  </si>
+  <si>
+    <t>1.94 : 1</t>
   </si>
 </sst>
 </file>
@@ -1726,15 +1738,15 @@
       </c>
       <c r="B2" s="2">
         <f>January!B2+February!B2+March!B2+April!B2+May!B2+June!B2+July!B2+August!B2+September!B2+October!B2+November!B2+December!B2</f>
-        <v>15673</v>
+        <v>17141</v>
       </c>
       <c r="C2" s="2">
         <f>January!C2+February!C2+March!C2+April!C2+May!C2+June!C2+July!C2+August!C2+September!C2+October!C2+November!C2+December!C2</f>
-        <v>11820</v>
+        <v>13031</v>
       </c>
       <c r="D2" s="2">
         <f>January!D2+February!D2+March!D2+April!D2+May!D2+June!D2+July!D2+August!D2+September!D2+October!D2+November!D2+December!D2</f>
-        <v>3853</v>
+        <v>4110</v>
       </c>
       <c r="E2" s="28" t="str">
         <f>IF(D2 &gt; 0, "We borrowed more than we lent this year", "")</f>
@@ -1746,7 +1758,7 @@
       </c>
       <c r="G2" s="3" t="str">
         <f>IF(ISERROR(ROUND(B2/C2,2)&amp;" : 1"), "", ROUND(B2/C2,2)&amp;" : 1")</f>
-        <v>1.33 : 1</v>
+        <v>1.32 : 1</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1755,15 +1767,15 @@
       </c>
       <c r="B3" s="4">
         <f>January!B3+February!B3+March!B3+April!B3+May!B3+June!B3+July!B3+August!B3+September!B3+October!B3+November!B3+December!B3</f>
-        <v>5403</v>
+        <v>5853</v>
       </c>
       <c r="C3" s="4">
         <f>January!C3+February!C3+March!C3+April!C3+May!C3+June!C3+July!C3+August!C3+September!C3+October!C3+November!C3+December!C3</f>
-        <v>4902</v>
+        <v>5333</v>
       </c>
       <c r="D3" s="4">
         <f>January!D3+February!D3+March!D3+April!D3+May!D3+June!D3+July!D3+August!D3+September!D3+October!D3+November!D3+December!D3</f>
-        <v>501</v>
+        <v>520</v>
       </c>
       <c r="E3" s="29" t="str">
         <f t="shared" ref="E3:E55" si="1">IF(D3 &gt; 0, "We borrowed more than we lent this year", "")</f>
@@ -1784,15 +1796,15 @@
       </c>
       <c r="B4" s="2">
         <f>January!B4+February!B4+March!B4+April!B4+May!B4+June!B4+July!B4+August!B4+September!B4+October!B4+November!B4+December!B4</f>
-        <v>13069</v>
+        <v>14161</v>
       </c>
       <c r="C4" s="2">
         <f>January!C4+February!C4+March!C4+April!C4+May!C4+June!C4+July!C4+August!C4+September!C4+October!C4+November!C4+December!C4</f>
-        <v>12677</v>
+        <v>14095</v>
       </c>
       <c r="D4" s="2">
         <f>January!D4+February!D4+March!D4+April!D4+May!D4+June!D4+July!D4+August!D4+September!D4+October!D4+November!D4+December!D4</f>
-        <v>392</v>
+        <v>66</v>
       </c>
       <c r="E4" s="28" t="str">
         <f t="shared" si="1"/>
@@ -1804,7 +1816,7 @@
       </c>
       <c r="G4" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.03 : 1</v>
+        <v>1 : 1</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1813,15 +1825,15 @@
       </c>
       <c r="B5" s="4">
         <f>January!B5+February!B5+March!B5+April!B5+May!B5+June!B5+July!B5+August!B5+September!B5+October!B5+November!B5+December!B5</f>
-        <v>846</v>
+        <v>868</v>
       </c>
       <c r="C5" s="4">
         <f>January!C5+February!C5+March!C5+April!C5+May!C5+June!C5+July!C5+August!C5+September!C5+October!C5+November!C5+December!C5</f>
-        <v>1277</v>
+        <v>1432</v>
       </c>
       <c r="D5" s="4">
         <f>January!D5+February!D5+March!D5+April!D5+May!D5+June!D5+July!D5+August!D5+September!D5+October!D5+November!D5+December!D5</f>
-        <v>-431</v>
+        <v>-564</v>
       </c>
       <c r="E5" s="29" t="str">
         <f t="shared" si="1"/>
@@ -1833,7 +1845,7 @@
       </c>
       <c r="G5" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.66 : 1</v>
+        <v>0.61 : 1</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1842,15 +1854,15 @@
       </c>
       <c r="B6" s="2">
         <f>January!B6+February!B6+March!B6+April!B6+May!B6+June!B6+July!B6+August!B6+September!B6+October!B6+November!B6+December!B6</f>
-        <v>12624</v>
+        <v>13765</v>
       </c>
       <c r="C6" s="2">
         <f>January!C6+February!C6+March!C6+April!C6+May!C6+June!C6+July!C6+August!C6+September!C6+October!C6+November!C6+December!C6</f>
-        <v>14771</v>
+        <v>16061</v>
       </c>
       <c r="D6" s="2">
         <f>January!D6+February!D6+March!D6+April!D6+May!D6+June!D6+July!D6+August!D6+September!D6+October!D6+November!D6+December!D6</f>
-        <v>-2147</v>
+        <v>-2296</v>
       </c>
       <c r="E6" s="28" t="str">
         <f t="shared" si="1"/>
@@ -1862,7 +1874,7 @@
       </c>
       <c r="G6" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.85 : 1</v>
+        <v>0.86 : 1</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1871,15 +1883,15 @@
       </c>
       <c r="B7" s="4">
         <f>January!B7+February!B7+March!B7+April!B7+May!B7+June!B7+July!B7+August!B7+September!B7+October!B7+November!B7+December!B7</f>
-        <v>2105</v>
+        <v>2348</v>
       </c>
       <c r="C7" s="4">
         <f>January!C7+February!C7+March!C7+April!C7+May!C7+June!C7+July!C7+August!C7+September!C7+October!C7+November!C7+December!C7</f>
-        <v>2235</v>
+        <v>2386</v>
       </c>
       <c r="D7" s="4">
         <f>January!D7+February!D7+March!D7+April!D7+May!D7+June!D7+July!D7+August!D7+September!D7+October!D7+November!D7+December!D7</f>
-        <v>-130</v>
+        <v>-38</v>
       </c>
       <c r="E7" s="29" t="str">
         <f t="shared" si="1"/>
@@ -1891,7 +1903,7 @@
       </c>
       <c r="G7" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.94 : 1</v>
+        <v>0.98 : 1</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1900,15 +1912,15 @@
       </c>
       <c r="B8" s="2">
         <f>January!B8+February!B8+March!B8+April!B8+May!B8+June!B8+July!B8+August!B8+September!B8+October!B8+November!B8+December!B8</f>
-        <v>1300</v>
+        <v>1370</v>
       </c>
       <c r="C8" s="2">
         <f>January!C8+February!C8+March!C8+April!C8+May!C8+June!C8+July!C8+August!C8+September!C8+October!C8+November!C8+December!C8</f>
-        <v>1865</v>
+        <v>2044</v>
       </c>
       <c r="D8" s="2">
         <f>January!D8+February!D8+March!D8+April!D8+May!D8+June!D8+July!D8+August!D8+September!D8+October!D8+November!D8+December!D8</f>
-        <v>-565</v>
+        <v>-674</v>
       </c>
       <c r="E8" s="28" t="str">
         <f t="shared" si="1"/>
@@ -1920,7 +1932,7 @@
       </c>
       <c r="G8" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.7 : 1</v>
+        <v>0.67 : 1</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1929,15 +1941,15 @@
       </c>
       <c r="B9" s="4">
         <f>January!B9+February!B9+March!B9+April!B9+May!B9+June!B9+July!B9+August!B9+September!B9+October!B9+November!B9+December!B9</f>
-        <v>508</v>
+        <v>578</v>
       </c>
       <c r="C9" s="4">
         <f>January!C9+February!C9+March!C9+April!C9+May!C9+June!C9+July!C9+August!C9+September!C9+October!C9+November!C9+December!C9</f>
-        <v>700</v>
+        <v>772</v>
       </c>
       <c r="D9" s="4">
         <f>January!D9+February!D9+March!D9+April!D9+May!D9+June!D9+July!D9+August!D9+September!D9+October!D9+November!D9+December!D9</f>
-        <v>-192</v>
+        <v>-194</v>
       </c>
       <c r="E9" s="29" t="str">
         <f t="shared" si="1"/>
@@ -1949,7 +1961,7 @@
       </c>
       <c r="G9" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.73 : 1</v>
+        <v>0.75 : 1</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1958,15 +1970,15 @@
       </c>
       <c r="B10" s="2">
         <f>January!B10+February!B10+March!B10+April!B10+May!B10+June!B10+July!B10+August!B10+September!B10+October!B10+November!B10+December!B10</f>
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C10" s="2">
         <f>January!C10+February!C10+March!C10+April!C10+May!C10+June!C10+July!C10+August!C10+September!C10+October!C10+November!C10+December!C10</f>
-        <v>413</v>
+        <v>467</v>
       </c>
       <c r="D10" s="2">
         <f>January!D10+February!D10+March!D10+April!D10+May!D10+June!D10+July!D10+August!D10+September!D10+October!D10+November!D10+December!D10</f>
-        <v>-373</v>
+        <v>-425</v>
       </c>
       <c r="E10" s="28" t="str">
         <f t="shared" si="1"/>
@@ -1978,7 +1990,7 @@
       </c>
       <c r="G10" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.1 : 1</v>
+        <v>0.09 : 1</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2016,15 +2028,15 @@
       </c>
       <c r="B12" s="6">
         <f>January!B12+February!B12+March!B12+April!B12+May!B12+June!B12+July!B12+August!B12+September!B12+October!B12+November!B12+December!B12</f>
-        <v>159</v>
+        <v>200</v>
       </c>
       <c r="C12" s="6">
         <f>January!C12+February!C12+March!C12+April!C12+May!C12+June!C12+July!C12+August!C12+September!C12+October!C12+November!C12+December!C12</f>
-        <v>233</v>
+        <v>258</v>
       </c>
       <c r="D12" s="6">
         <f>January!D12+February!D12+March!D12+April!D12+May!D12+June!D12+July!D12+August!D12+September!D12+October!D12+November!D12+December!D12</f>
-        <v>-74</v>
+        <v>-58</v>
       </c>
       <c r="E12" s="30" t="str">
         <f t="shared" si="1"/>
@@ -2036,7 +2048,7 @@
       </c>
       <c r="G12" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0.68 : 1</v>
+        <v>0.78 : 1</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2045,15 +2057,15 @@
       </c>
       <c r="B13" s="6">
         <f>January!B13+February!B13+March!B13+April!B13+May!B13+June!B13+July!B13+August!B13+September!B13+October!B13+November!B13+December!B13</f>
-        <v>1439</v>
+        <v>1621</v>
       </c>
       <c r="C13" s="6">
         <f>January!C13+February!C13+March!C13+April!C13+May!C13+June!C13+July!C13+August!C13+September!C13+October!C13+November!C13+December!C13</f>
-        <v>937</v>
+        <v>1020</v>
       </c>
       <c r="D13" s="6">
         <f>January!D13+February!D13+March!D13+April!D13+May!D13+June!D13+July!D13+August!D13+September!D13+October!D13+November!D13+December!D13</f>
-        <v>502</v>
+        <v>601</v>
       </c>
       <c r="E13" s="30" t="str">
         <f t="shared" si="1"/>
@@ -2065,7 +2077,7 @@
       </c>
       <c r="G13" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>1.54 : 1</v>
+        <v>1.59 : 1</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2074,15 +2086,15 @@
       </c>
       <c r="B14" s="6">
         <f>January!B14+February!B14+March!B14+April!B14+May!B14+June!B14+July!B14+August!B14+September!B14+October!B14+November!B14+December!B14</f>
-        <v>1315</v>
+        <v>1443</v>
       </c>
       <c r="C14" s="6">
         <f>January!C14+February!C14+March!C14+April!C14+May!C14+June!C14+July!C14+August!C14+September!C14+October!C14+November!C14+December!C14</f>
-        <v>2963</v>
+        <v>3225</v>
       </c>
       <c r="D14" s="6">
         <f>January!D14+February!D14+March!D14+April!D14+May!D14+June!D14+July!D14+August!D14+September!D14+October!D14+November!D14+December!D14</f>
-        <v>-1648</v>
+        <v>-1782</v>
       </c>
       <c r="E14" s="30" t="str">
         <f t="shared" si="1"/>
@@ -2094,7 +2106,7 @@
       </c>
       <c r="G14" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0.44 : 1</v>
+        <v>0.45 : 1</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2103,15 +2115,15 @@
       </c>
       <c r="B15" s="6">
         <f>January!B15+February!B15+March!B15+April!B15+May!B15+June!B15+July!B15+August!B15+September!B15+October!B15+November!B15+December!B15</f>
-        <v>889</v>
+        <v>986</v>
       </c>
       <c r="C15" s="6">
         <f>January!C15+February!C15+March!C15+April!C15+May!C15+June!C15+July!C15+August!C15+September!C15+October!C15+November!C15+December!C15</f>
-        <v>1048</v>
+        <v>1138</v>
       </c>
       <c r="D15" s="6">
         <f>January!D15+February!D15+March!D15+April!D15+May!D15+June!D15+July!D15+August!D15+September!D15+October!D15+November!D15+December!D15</f>
-        <v>-159</v>
+        <v>-152</v>
       </c>
       <c r="E15" s="30" t="str">
         <f t="shared" si="1"/>
@@ -2123,7 +2135,7 @@
       </c>
       <c r="G15" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0.85 : 1</v>
+        <v>0.87 : 1</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2132,15 +2144,15 @@
       </c>
       <c r="B16" s="2">
         <f>January!B16+February!B16+March!B16+April!B16+May!B16+June!B16+July!B16+August!B16+September!B16+October!B16+November!B16+December!B16</f>
-        <v>374</v>
+        <v>393</v>
       </c>
       <c r="C16" s="2">
         <f>January!C16+February!C16+March!C16+April!C16+May!C16+June!C16+July!C16+August!C16+September!C16+October!C16+November!C16+December!C16</f>
-        <v>1529</v>
+        <v>1670</v>
       </c>
       <c r="D16" s="2">
         <f>January!D16+February!D16+March!D16+April!D16+May!D16+June!D16+July!D16+August!D16+September!D16+October!D16+November!D16+December!D16</f>
-        <v>-1155</v>
+        <v>-1277</v>
       </c>
       <c r="E16" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2161,15 +2173,15 @@
       </c>
       <c r="B17" s="4">
         <f>January!B17+February!B17+March!B17+April!B17+May!B17+June!B17+July!B17+August!B17+September!B17+October!B17+November!B17+December!B17</f>
-        <v>6315</v>
+        <v>6908</v>
       </c>
       <c r="C17" s="4">
         <f>January!C17+February!C17+March!C17+April!C17+May!C17+June!C17+July!C17+August!C17+September!C17+October!C17+November!C17+December!C17</f>
-        <v>4808</v>
+        <v>5260</v>
       </c>
       <c r="D17" s="4">
         <f>January!D17+February!D17+March!D17+April!D17+May!D17+June!D17+July!D17+August!D17+September!D17+October!D17+November!D17+December!D17</f>
-        <v>1507</v>
+        <v>1648</v>
       </c>
       <c r="E17" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2190,15 +2202,15 @@
       </c>
       <c r="B18" s="2">
         <f>January!B18+February!B18+March!B18+April!B18+May!B18+June!B18+July!B18+August!B18+September!B18+October!B18+November!B18+December!B18</f>
-        <v>906</v>
+        <v>973</v>
       </c>
       <c r="C18" s="2">
         <f>January!C18+February!C18+March!C18+April!C18+May!C18+June!C18+July!C18+August!C18+September!C18+October!C18+November!C18+December!C18</f>
-        <v>1024</v>
+        <v>1133</v>
       </c>
       <c r="D18" s="2">
         <f>January!D18+February!D18+March!D18+April!D18+May!D18+June!D18+July!D18+August!D18+September!D18+October!D18+November!D18+December!D18</f>
-        <v>-118</v>
+        <v>-160</v>
       </c>
       <c r="E18" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2210,7 +2222,7 @@
       </c>
       <c r="G18" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.88 : 1</v>
+        <v>0.86 : 1</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2219,15 +2231,15 @@
       </c>
       <c r="B19" s="4">
         <f>January!B19+February!B19+March!B19+April!B19+May!B19+June!B19+July!B19+August!B19+September!B19+October!B19+November!B19+December!B19</f>
-        <v>6498</v>
+        <v>7127</v>
       </c>
       <c r="C19" s="4">
         <f>January!C19+February!C19+March!C19+April!C19+May!C19+June!C19+July!C19+August!C19+September!C19+October!C19+November!C19+December!C19</f>
-        <v>4133</v>
+        <v>4512</v>
       </c>
       <c r="D19" s="4">
         <f>January!D19+February!D19+March!D19+April!D19+May!D19+June!D19+July!D19+August!D19+September!D19+October!D19+November!D19+December!D19</f>
-        <v>2365</v>
+        <v>2615</v>
       </c>
       <c r="E19" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2239,7 +2251,7 @@
       </c>
       <c r="G19" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.57 : 1</v>
+        <v>1.58 : 1</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2248,15 +2260,15 @@
       </c>
       <c r="B20" s="2">
         <f>January!B20+February!B20+March!B20+April!B20+May!B20+June!B20+July!B20+August!B20+September!B20+October!B20+November!B20+December!B20</f>
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C20" s="2">
         <f>January!C20+February!C20+March!C20+April!C20+May!C20+June!C20+July!C20+August!C20+September!C20+October!C20+November!C20+December!C20</f>
-        <v>681</v>
+        <v>749</v>
       </c>
       <c r="D20" s="2">
         <f>January!D20+February!D20+March!D20+April!D20+May!D20+June!D20+July!D20+August!D20+September!D20+October!D20+November!D20+December!D20</f>
-        <v>-645</v>
+        <v>-709</v>
       </c>
       <c r="E20" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2277,15 +2289,15 @@
       </c>
       <c r="B21" s="4">
         <f>January!B21+February!B21+March!B21+April!B21+May!B21+June!B21+July!B21+August!B21+September!B21+October!B21+November!B21+December!B21</f>
-        <v>5018</v>
+        <v>5423</v>
       </c>
       <c r="C21" s="4">
         <f>January!C21+February!C21+March!C21+April!C21+May!C21+June!C21+July!C21+August!C21+September!C21+October!C21+November!C21+December!C21</f>
-        <v>4259</v>
+        <v>4681</v>
       </c>
       <c r="D21" s="4">
         <f>January!D21+February!D21+March!D21+April!D21+May!D21+June!D21+July!D21+August!D21+September!D21+October!D21+November!D21+December!D21</f>
-        <v>759</v>
+        <v>742</v>
       </c>
       <c r="E21" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2297,7 +2309,7 @@
       </c>
       <c r="G21" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.18 : 1</v>
+        <v>1.16 : 1</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2306,15 +2318,15 @@
       </c>
       <c r="B22" s="2">
         <f>January!B22+February!B22+March!B22+April!B22+May!B22+June!B22+July!B22+August!B22+September!B22+October!B22+November!B22+December!B22</f>
-        <v>293</v>
+        <v>324</v>
       </c>
       <c r="C22" s="2">
         <f>January!C22+February!C22+March!C22+April!C22+May!C22+June!C22+July!C22+August!C22+September!C22+October!C22+November!C22+December!C22</f>
-        <v>771</v>
+        <v>899</v>
       </c>
       <c r="D22" s="2">
         <f>January!D22+February!D22+March!D22+April!D22+May!D22+June!D22+July!D22+August!D22+September!D22+October!D22+November!D22+December!D22</f>
-        <v>-478</v>
+        <v>-575</v>
       </c>
       <c r="E22" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2326,7 +2338,7 @@
       </c>
       <c r="G22" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.38 : 1</v>
+        <v>0.36 : 1</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2335,15 +2347,15 @@
       </c>
       <c r="B23" s="4">
         <f>January!B23+February!B23+March!B23+April!B23+May!B23+June!B23+July!B23+August!B23+September!B23+October!B23+November!B23+December!B23</f>
-        <v>7100</v>
+        <v>7866</v>
       </c>
       <c r="C23" s="4">
         <f>January!C23+February!C23+March!C23+April!C23+May!C23+June!C23+July!C23+August!C23+September!C23+October!C23+November!C23+December!C23</f>
-        <v>4772</v>
+        <v>5226</v>
       </c>
       <c r="D23" s="4">
         <f>January!D23+February!D23+March!D23+April!D23+May!D23+June!D23+July!D23+August!D23+September!D23+October!D23+November!D23+December!D23</f>
-        <v>2328</v>
+        <v>2640</v>
       </c>
       <c r="E23" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2355,7 +2367,7 @@
       </c>
       <c r="G23" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.49 : 1</v>
+        <v>1.51 : 1</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2364,15 +2376,15 @@
       </c>
       <c r="B24" s="2">
         <f>January!B24+February!B24+March!B24+April!B24+May!B24+June!B24+July!B24+August!B24+September!B24+October!B24+November!B24+December!B24</f>
-        <v>18530</v>
+        <v>20553</v>
       </c>
       <c r="C24" s="2">
         <f>January!C24+February!C24+March!C24+April!C24+May!C24+June!C24+July!C24+August!C24+September!C24+October!C24+November!C24+December!C24</f>
-        <v>13899</v>
+        <v>15108</v>
       </c>
       <c r="D24" s="2">
         <f>January!D24+February!D24+March!D24+April!D24+May!D24+June!D24+July!D24+August!D24+September!D24+October!D24+November!D24+December!D24</f>
-        <v>4631</v>
+        <v>5445</v>
       </c>
       <c r="E24" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2384,7 +2396,7 @@
       </c>
       <c r="G24" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.33 : 1</v>
+        <v>1.36 : 1</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2393,15 +2405,15 @@
       </c>
       <c r="B25" s="4">
         <f>January!B25+February!B25+March!B25+April!B25+May!B25+June!B25+July!B25+August!B25+September!B25+October!B25+November!B25+December!B25</f>
-        <v>1772</v>
+        <v>1980</v>
       </c>
       <c r="C25" s="4">
         <f>January!C25+February!C25+March!C25+April!C25+May!C25+June!C25+July!C25+August!C25+September!C25+October!C25+November!C25+December!C25</f>
-        <v>3583</v>
+        <v>3951</v>
       </c>
       <c r="D25" s="4">
         <f>January!D25+February!D25+March!D25+April!D25+May!D25+June!D25+July!D25+August!D25+September!D25+October!D25+November!D25+December!D25</f>
-        <v>-1811</v>
+        <v>-1971</v>
       </c>
       <c r="E25" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2413,7 +2425,7 @@
       </c>
       <c r="G25" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.49 : 1</v>
+        <v>0.5 : 1</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2451,15 +2463,15 @@
       </c>
       <c r="B27" s="4">
         <f>January!B27+February!B27+March!B27+April!B27+May!B27+June!B27+July!B27+August!B27+September!B27+October!B27+November!B27+December!B27</f>
-        <v>2731</v>
+        <v>3009</v>
       </c>
       <c r="C27" s="4">
         <f>January!C27+February!C27+March!C27+April!C27+May!C27+June!C27+July!C27+August!C27+September!C27+October!C27+November!C27+December!C27</f>
-        <v>2014</v>
+        <v>2223</v>
       </c>
       <c r="D27" s="4">
         <f>January!D27+February!D27+March!D27+April!D27+May!D27+June!D27+July!D27+August!D27+September!D27+October!D27+November!D27+December!D27</f>
-        <v>717</v>
+        <v>786</v>
       </c>
       <c r="E27" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2471,7 +2483,7 @@
       </c>
       <c r="G27" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.36 : 1</v>
+        <v>1.35 : 1</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2480,15 +2492,15 @@
       </c>
       <c r="B28" s="2">
         <f>January!B28+February!B28+March!B28+April!B28+May!B28+June!B28+July!B28+August!B28+September!B28+October!B28+November!B28+December!B28</f>
-        <v>525</v>
+        <v>569</v>
       </c>
       <c r="C28" s="2">
         <f>January!C28+February!C28+March!C28+April!C28+May!C28+June!C28+July!C28+August!C28+September!C28+October!C28+November!C28+December!C28</f>
-        <v>720</v>
+        <v>819</v>
       </c>
       <c r="D28" s="2">
         <f>January!D28+February!D28+March!D28+April!D28+May!D28+June!D28+July!D28+August!D28+September!D28+October!D28+November!D28+December!D28</f>
-        <v>-195</v>
+        <v>-250</v>
       </c>
       <c r="E28" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2500,7 +2512,7 @@
       </c>
       <c r="G28" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.73 : 1</v>
+        <v>0.69 : 1</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2509,15 +2521,15 @@
       </c>
       <c r="B29" s="4">
         <f>January!B29+February!B29+March!B29+April!B29+May!B29+June!B29+July!B29+August!B29+September!B29+October!B29+November!B29+December!B29</f>
-        <v>5397</v>
+        <v>5967</v>
       </c>
       <c r="C29" s="4">
         <f>January!C29+February!C29+March!C29+April!C29+May!C29+June!C29+July!C29+August!C29+September!C29+October!C29+November!C29+December!C29</f>
-        <v>4690</v>
+        <v>5178</v>
       </c>
       <c r="D29" s="4">
         <f>January!D29+February!D29+March!D29+April!D29+May!D29+June!D29+July!D29+August!D29+September!D29+October!D29+November!D29+December!D29</f>
-        <v>707</v>
+        <v>789</v>
       </c>
       <c r="E29" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2538,15 +2550,15 @@
       </c>
       <c r="B30" s="2">
         <f>January!B30+February!B30+March!B30+April!B30+May!B30+June!B30+July!B30+August!B30+September!B30+October!B30+November!B30+December!B30</f>
-        <v>456</v>
+        <v>480</v>
       </c>
       <c r="C30" s="2">
         <f>January!C30+February!C30+March!C30+April!C30+May!C30+June!C30+July!C30+August!C30+September!C30+October!C30+November!C30+December!C30</f>
-        <v>362</v>
+        <v>394</v>
       </c>
       <c r="D30" s="2">
         <f>January!D30+February!D30+March!D30+April!D30+May!D30+June!D30+July!D30+August!D30+September!D30+October!D30+November!D30+December!D30</f>
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="E30" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2558,7 +2570,7 @@
       </c>
       <c r="G30" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.26 : 1</v>
+        <v>1.22 : 1</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2567,15 +2579,15 @@
       </c>
       <c r="B31" s="4">
         <f>January!B31+February!B31+March!B31+April!B31+May!B31+June!B31+July!B31+August!B31+September!B31+October!B31+November!B31+December!B31</f>
-        <v>788</v>
+        <v>874</v>
       </c>
       <c r="C31" s="4">
         <f>January!C31+February!C31+March!C31+April!C31+May!C31+June!C31+July!C31+August!C31+September!C31+October!C31+November!C31+December!C31</f>
-        <v>2994</v>
+        <v>3287</v>
       </c>
       <c r="D31" s="4">
         <f>January!D31+February!D31+March!D31+April!D31+May!D31+June!D31+July!D31+August!D31+September!D31+October!D31+November!D31+December!D31</f>
-        <v>-2206</v>
+        <v>-2413</v>
       </c>
       <c r="E31" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2587,7 +2599,7 @@
       </c>
       <c r="G31" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.26 : 1</v>
+        <v>0.27 : 1</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2596,15 +2608,15 @@
       </c>
       <c r="B32" s="2">
         <f>January!B32+February!B32+March!B32+April!B32+May!B32+June!B32+July!B32+August!B32+September!B32+October!B32+November!B32+December!B32</f>
-        <v>4501</v>
+        <v>4920</v>
       </c>
       <c r="C32" s="2">
         <f>January!C32+February!C32+March!C32+April!C32+May!C32+June!C32+July!C32+August!C32+September!C32+October!C32+November!C32+December!C32</f>
-        <v>5642</v>
+        <v>6200</v>
       </c>
       <c r="D32" s="2">
         <f>January!D32+February!D32+March!D32+April!D32+May!D32+June!D32+July!D32+August!D32+September!D32+October!D32+November!D32+December!D32</f>
-        <v>-1141</v>
+        <v>-1280</v>
       </c>
       <c r="E32" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2616,7 +2628,7 @@
       </c>
       <c r="G32" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.8 : 1</v>
+        <v>0.79 : 1</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2625,15 +2637,15 @@
       </c>
       <c r="B33" s="4">
         <f>January!B33+February!B33+March!B33+April!B33+May!B33+June!B33+July!B33+August!B33+September!B33+October!B33+November!B33+December!B33</f>
-        <v>4236</v>
+        <v>4580</v>
       </c>
       <c r="C33" s="4">
         <f>January!C33+February!C33+March!C33+April!C33+May!C33+June!C33+July!C33+August!C33+September!C33+October!C33+November!C33+December!C33</f>
-        <v>5149</v>
+        <v>5566</v>
       </c>
       <c r="D33" s="4">
         <f>January!D33+February!D33+March!D33+April!D33+May!D33+June!D33+July!D33+August!D33+September!D33+October!D33+November!D33+December!D33</f>
-        <v>-913</v>
+        <v>-986</v>
       </c>
       <c r="E33" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2654,15 +2666,15 @@
       </c>
       <c r="B34" s="2">
         <f>January!B34+February!B34+March!B34+April!B34+May!B34+June!B34+July!B34+August!B34+September!B34+October!B34+November!B34+December!B34</f>
-        <v>2121</v>
+        <v>2337</v>
       </c>
       <c r="C34" s="2">
         <f>January!C34+February!C34+March!C34+April!C34+May!C34+June!C34+July!C34+August!C34+September!C34+October!C34+November!C34+December!C34</f>
-        <v>1182</v>
+        <v>1311</v>
       </c>
       <c r="D34" s="2">
         <f>January!D34+February!D34+March!D34+April!D34+May!D34+June!D34+July!D34+August!D34+September!D34+October!D34+November!D34+December!D34</f>
-        <v>939</v>
+        <v>1026</v>
       </c>
       <c r="E34" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2674,7 +2686,7 @@
       </c>
       <c r="G34" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.79 : 1</v>
+        <v>1.78 : 1</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2683,15 +2695,15 @@
       </c>
       <c r="B35" s="4">
         <f>January!B35+February!B35+March!B35+April!B35+May!B35+June!B35+July!B35+August!B35+September!B35+October!B35+November!B35+December!B35</f>
-        <v>9586</v>
+        <v>10439</v>
       </c>
       <c r="C35" s="4">
         <f>January!C35+February!C35+March!C35+April!C35+May!C35+June!C35+July!C35+August!C35+September!C35+October!C35+November!C35+December!C35</f>
-        <v>10142</v>
+        <v>11100</v>
       </c>
       <c r="D35" s="4">
         <f>January!D35+February!D35+March!D35+April!D35+May!D35+June!D35+July!D35+August!D35+September!D35+October!D35+November!D35+December!D35</f>
-        <v>-556</v>
+        <v>-661</v>
       </c>
       <c r="E35" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2703,7 +2715,7 @@
       </c>
       <c r="G35" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.95 : 1</v>
+        <v>0.94 : 1</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2712,15 +2724,15 @@
       </c>
       <c r="B36" s="2">
         <f>January!B36+February!B36+March!B36+April!B36+May!B36+June!B36+July!B36+August!B36+September!B36+October!B36+November!B36+December!B36</f>
-        <v>2169</v>
+        <v>2361</v>
       </c>
       <c r="C36" s="2">
         <f>January!C36+February!C36+March!C36+April!C36+May!C36+June!C36+July!C36+August!C36+September!C36+October!C36+November!C36+December!C36</f>
-        <v>4791</v>
+        <v>5211</v>
       </c>
       <c r="D36" s="2">
         <f>January!D36+February!D36+March!D36+April!D36+May!D36+June!D36+July!D36+August!D36+September!D36+October!D36+November!D36+December!D36</f>
-        <v>-2622</v>
+        <v>-2850</v>
       </c>
       <c r="E36" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2741,15 +2753,15 @@
       </c>
       <c r="B37" s="4">
         <f>January!B37+February!B37+March!B37+April!B37+May!B37+June!B37+July!B37+August!B37+September!B37+October!B37+November!B37+December!B37</f>
-        <v>5196</v>
+        <v>5631</v>
       </c>
       <c r="C37" s="4">
         <f>January!C37+February!C37+March!C37+April!C37+May!C37+June!C37+July!C37+August!C37+September!C37+October!C37+November!C37+December!C37</f>
-        <v>3560</v>
+        <v>3897</v>
       </c>
       <c r="D37" s="4">
         <f>January!D37+February!D37+March!D37+April!D37+May!D37+June!D37+July!D37+August!D37+September!D37+October!D37+November!D37+December!D37</f>
-        <v>1636</v>
+        <v>1734</v>
       </c>
       <c r="E37" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2761,7 +2773,7 @@
       </c>
       <c r="G37" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.46 : 1</v>
+        <v>1.44 : 1</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2770,15 +2782,15 @@
       </c>
       <c r="B38" s="2">
         <f>January!B38+February!B38+March!B38+April!B38+May!B38+June!B38+July!B38+August!B38+September!B38+October!B38+November!B38+December!B38</f>
-        <v>307</v>
+        <v>326</v>
       </c>
       <c r="C38" s="2">
         <f>January!C38+February!C38+March!C38+April!C38+May!C38+June!C38+July!C38+August!C38+September!C38+October!C38+November!C38+December!C38</f>
-        <v>1691</v>
+        <v>1866</v>
       </c>
       <c r="D38" s="2">
         <f>January!D38+February!D38+March!D38+April!D38+May!D38+June!D38+July!D38+August!D38+September!D38+October!D38+November!D38+December!D38</f>
-        <v>-1384</v>
+        <v>-1540</v>
       </c>
       <c r="E38" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2790,7 +2802,7 @@
       </c>
       <c r="G38" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.18 : 1</v>
+        <v>0.17 : 1</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2799,15 +2811,15 @@
       </c>
       <c r="B39" s="8">
         <f>January!B39+February!B39+March!B39+April!B39+May!B39+June!B39+July!B39+August!B39+September!B39+October!B39+November!B39+December!B39</f>
-        <v>209</v>
+        <v>244</v>
       </c>
       <c r="C39" s="8">
         <f>January!C39+February!C39+March!C39+April!C39+May!C39+June!C39+July!C39+August!C39+September!C39+October!C39+November!C39+December!C39</f>
-        <v>483</v>
+        <v>559</v>
       </c>
       <c r="D39" s="8">
         <f>January!D39+February!D39+March!D39+April!D39+May!D39+June!D39+July!D39+August!D39+September!D39+October!D39+November!D39+December!D39</f>
-        <v>-274</v>
+        <v>-315</v>
       </c>
       <c r="E39" s="31" t="str">
         <f t="shared" si="1"/>
@@ -2819,7 +2831,7 @@
       </c>
       <c r="G39" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>0.43 : 1</v>
+        <v>0.44 : 1</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2828,15 +2840,15 @@
       </c>
       <c r="B40" s="8">
         <f>January!B40+February!B40+March!B40+April!B40+May!B40+June!B40+July!B40+August!B40+September!B40+October!B40+November!B40+December!B40</f>
-        <v>573</v>
+        <v>659</v>
       </c>
       <c r="C40" s="8">
         <f>January!C40+February!C40+March!C40+April!C40+May!C40+June!C40+July!C40+August!C40+September!C40+October!C40+November!C40+December!C40</f>
-        <v>898</v>
+        <v>1016</v>
       </c>
       <c r="D40" s="8">
         <f>January!D40+February!D40+March!D40+April!D40+May!D40+June!D40+July!D40+August!D40+September!D40+October!D40+November!D40+December!D40</f>
-        <v>-325</v>
+        <v>-357</v>
       </c>
       <c r="E40" s="31" t="str">
         <f t="shared" si="1"/>
@@ -2848,7 +2860,7 @@
       </c>
       <c r="G40" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>0.64 : 1</v>
+        <v>0.65 : 1</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2857,15 +2869,15 @@
       </c>
       <c r="B41" s="8">
         <f>January!B41+February!B41+March!B41+April!B41+May!B41+June!B41+July!B41+August!B41+September!B41+October!B41+November!B41+December!B41</f>
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C41" s="8">
         <f>January!C41+February!C41+March!C41+April!C41+May!C41+June!C41+July!C41+August!C41+September!C41+October!C41+November!C41+December!C41</f>
-        <v>179</v>
+        <v>222</v>
       </c>
       <c r="D41" s="8">
         <f>January!D41+February!D41+March!D41+April!D41+May!D41+June!D41+July!D41+August!D41+September!D41+October!D41+November!D41+December!D41</f>
-        <v>-94</v>
+        <v>-135</v>
       </c>
       <c r="E41" s="31" t="str">
         <f t="shared" si="1"/>
@@ -2877,7 +2889,7 @@
       </c>
       <c r="G41" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>0.47 : 1</v>
+        <v>0.39 : 1</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2886,15 +2898,15 @@
       </c>
       <c r="B42" s="8">
         <f>January!B42+February!B42+March!B42+April!B42+May!B42+June!B42+July!B42+August!B42+September!B42+October!B42+November!B42+December!B42</f>
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="C42" s="8">
         <f>January!C42+February!C42+March!C42+April!C42+May!C42+June!C42+July!C42+August!C42+September!C42+October!C42+November!C42+December!C42</f>
-        <v>111</v>
+        <v>132</v>
       </c>
       <c r="D42" s="8">
         <f>January!D42+February!D42+March!D42+April!D42+May!D42+June!D42+July!D42+August!D42+September!D42+October!D42+November!D42+December!D42</f>
-        <v>-1</v>
+        <v>-7</v>
       </c>
       <c r="E42" s="31" t="str">
         <f t="shared" si="1"/>
@@ -2906,7 +2918,7 @@
       </c>
       <c r="G42" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>0.99 : 1</v>
+        <v>0.95 : 1</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2944,15 +2956,15 @@
       </c>
       <c r="B44" s="4">
         <f>January!B44+February!B44+March!B44+April!B44+May!B44+June!B44+July!B44+August!B44+September!B44+October!B44+November!B44+December!B44</f>
-        <v>1022</v>
+        <v>1096</v>
       </c>
       <c r="C44" s="4">
         <f>January!C44+February!C44+March!C44+April!C44+May!C44+June!C44+July!C44+August!C44+September!C44+October!C44+November!C44+December!C44</f>
-        <v>769</v>
+        <v>858</v>
       </c>
       <c r="D44" s="4">
         <f>January!D44+February!D44+March!D44+April!D44+May!D44+June!D44+July!D44+August!D44+September!D44+October!D44+November!D44+December!D44</f>
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="E44" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2964,7 +2976,7 @@
       </c>
       <c r="G44" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.33 : 1</v>
+        <v>1.28 : 1</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2973,15 +2985,15 @@
       </c>
       <c r="B45" s="2">
         <f>January!B45+February!B45+March!B45+April!B45+May!B45+June!B45+July!B45+August!B45+September!B45+October!B45+November!B45+December!B45</f>
-        <v>766</v>
+        <v>843</v>
       </c>
       <c r="C45" s="2">
         <f>January!C45+February!C45+March!C45+April!C45+May!C45+June!C45+July!C45+August!C45+September!C45+October!C45+November!C45+December!C45</f>
-        <v>1572</v>
+        <v>1745</v>
       </c>
       <c r="D45" s="2">
         <f>January!D45+February!D45+March!D45+April!D45+May!D45+June!D45+July!D45+August!D45+September!D45+October!D45+November!D45+December!D45</f>
-        <v>-806</v>
+        <v>-902</v>
       </c>
       <c r="E45" s="28" t="str">
         <f t="shared" si="1"/>
@@ -2993,7 +3005,7 @@
       </c>
       <c r="G45" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.49 : 1</v>
+        <v>0.48 : 1</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3002,15 +3014,15 @@
       </c>
       <c r="B46" s="4">
         <f>January!B46+February!B46+March!B46+April!B46+May!B46+June!B46+July!B46+August!B46+September!B46+October!B46+November!B46+December!B46</f>
-        <v>4442</v>
+        <v>4949</v>
       </c>
       <c r="C46" s="4">
         <f>January!C46+February!C46+March!C46+April!C46+May!C46+June!C46+July!C46+August!C46+September!C46+October!C46+November!C46+December!C46</f>
-        <v>6234</v>
+        <v>6758</v>
       </c>
       <c r="D46" s="4">
         <f>January!D46+February!D46+March!D46+April!D46+May!D46+June!D46+July!D46+August!D46+September!D46+October!D46+November!D46+December!D46</f>
-        <v>-1792</v>
+        <v>-1809</v>
       </c>
       <c r="E46" s="29" t="str">
         <f t="shared" si="1"/>
@@ -3022,7 +3034,7 @@
       </c>
       <c r="G46" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.71 : 1</v>
+        <v>0.73 : 1</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3031,15 +3043,15 @@
       </c>
       <c r="B47" s="2">
         <f>January!B47+February!B47+March!B47+April!B47+May!B47+June!B47+July!B47+August!B47+September!B47+October!B47+November!B47+December!B47</f>
-        <v>9027</v>
+        <v>9957</v>
       </c>
       <c r="C47" s="2">
         <f>January!C47+February!C47+March!C47+April!C47+May!C47+June!C47+July!C47+August!C47+September!C47+October!C47+November!C47+December!C47</f>
-        <v>6633</v>
+        <v>7357</v>
       </c>
       <c r="D47" s="2">
         <f>January!D47+February!D47+March!D47+April!D47+May!D47+June!D47+July!D47+August!D47+September!D47+October!D47+November!D47+December!D47</f>
-        <v>2394</v>
+        <v>2600</v>
       </c>
       <c r="E47" s="28" t="str">
         <f t="shared" si="1"/>
@@ -3051,7 +3063,7 @@
       </c>
       <c r="G47" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.36 : 1</v>
+        <v>1.35 : 1</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3060,15 +3072,15 @@
       </c>
       <c r="B48" s="4">
         <f>January!B48+February!B48+March!B48+April!B48+May!B48+June!B48+July!B48+August!B48+September!B48+October!B48+November!B48+December!B48</f>
-        <v>2432</v>
+        <v>2661</v>
       </c>
       <c r="C48" s="4">
         <f>January!C48+February!C48+March!C48+April!C48+May!C48+June!C48+July!C48+August!C48+September!C48+October!C48+November!C48+December!C48</f>
-        <v>6324</v>
+        <v>6896</v>
       </c>
       <c r="D48" s="4">
         <f>January!D48+February!D48+March!D48+April!D48+May!D48+June!D48+July!D48+August!D48+September!D48+October!D48+November!D48+December!D48</f>
-        <v>-3892</v>
+        <v>-4235</v>
       </c>
       <c r="E48" s="29" t="str">
         <f t="shared" si="1"/>
@@ -3080,7 +3092,7 @@
       </c>
       <c r="G48" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.38 : 1</v>
+        <v>0.39 : 1</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3089,15 +3101,15 @@
       </c>
       <c r="B49" s="2">
         <f>January!B49+February!B49+March!B49+April!B49+May!B49+June!B49+July!B49+August!B49+September!B49+October!B49+November!B49+December!B49</f>
-        <v>3780</v>
+        <v>4237</v>
       </c>
       <c r="C49" s="2">
         <f>January!C49+February!C49+March!C49+April!C49+May!C49+June!C49+July!C49+August!C49+September!C49+October!C49+November!C49+December!C49</f>
-        <v>2174</v>
+        <v>2410</v>
       </c>
       <c r="D49" s="2">
         <f>January!D49+February!D49+March!D49+April!D49+May!D49+June!D49+July!D49+August!D49+September!D49+October!D49+November!D49+December!D49</f>
-        <v>1606</v>
+        <v>1827</v>
       </c>
       <c r="E49" s="28" t="str">
         <f t="shared" si="1"/>
@@ -3109,7 +3121,7 @@
       </c>
       <c r="G49" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.74 : 1</v>
+        <v>1.76 : 1</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3118,15 +3130,15 @@
       </c>
       <c r="B50" s="4">
         <f>January!B50+February!B50+March!B50+April!B50+May!B50+June!B50+July!B50+August!B50+September!B50+October!B50+November!B50+December!B50</f>
-        <v>8760</v>
+        <v>9803</v>
       </c>
       <c r="C50" s="4">
         <f>January!C50+February!C50+March!C50+April!C50+May!C50+June!C50+July!C50+August!C50+September!C50+October!C50+November!C50+December!C50</f>
-        <v>5537</v>
+        <v>6042</v>
       </c>
       <c r="D50" s="4">
         <f>January!D50+February!D50+March!D50+April!D50+May!D50+June!D50+July!D50+August!D50+September!D50+October!D50+November!D50+December!D50</f>
-        <v>3223</v>
+        <v>3761</v>
       </c>
       <c r="E50" s="29" t="str">
         <f t="shared" si="1"/>
@@ -3138,7 +3150,7 @@
       </c>
       <c r="G50" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.58 : 1</v>
+        <v>1.62 : 1</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3147,15 +3159,15 @@
       </c>
       <c r="B51" s="2">
         <f>January!B51+February!B51+March!B51+April!B51+May!B51+June!B51+July!B51+August!B51+September!B51+October!B51+November!B51+December!B51</f>
-        <v>2341</v>
+        <v>2504</v>
       </c>
       <c r="C51" s="2">
         <f>January!C51+February!C51+March!C51+April!C51+May!C51+June!C51+July!C51+August!C51+September!C51+October!C51+November!C51+December!C51</f>
-        <v>1134</v>
+        <v>1320</v>
       </c>
       <c r="D51" s="2">
         <f>January!D51+February!D51+March!D51+April!D51+May!D51+June!D51+July!D51+August!D51+September!D51+October!D51+November!D51+December!D51</f>
-        <v>1207</v>
+        <v>1184</v>
       </c>
       <c r="E51" s="28" t="str">
         <f t="shared" si="1"/>
@@ -3167,7 +3179,7 @@
       </c>
       <c r="G51" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>2.06 : 1</v>
+        <v>1.9 : 1</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3176,15 +3188,15 @@
       </c>
       <c r="B52" s="4">
         <f>January!B52+February!B52+March!B52+April!B52+May!B52+June!B52+July!B52+August!B52+September!B52+October!B52+November!B52+December!B52</f>
-        <v>4478</v>
+        <v>4936</v>
       </c>
       <c r="C52" s="4">
         <f>January!C52+February!C52+March!C52+April!C52+May!C52+June!C52+July!C52+August!C52+September!C52+October!C52+November!C52+December!C52</f>
-        <v>5420</v>
+        <v>5895</v>
       </c>
       <c r="D52" s="4">
         <f>January!D52+February!D52+March!D52+April!D52+May!D52+June!D52+July!D52+August!D52+September!D52+October!D52+November!D52+December!D52</f>
-        <v>-942</v>
+        <v>-959</v>
       </c>
       <c r="E52" s="29" t="str">
         <f t="shared" si="1"/>
@@ -3196,7 +3208,7 @@
       </c>
       <c r="G52" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.83 : 1</v>
+        <v>0.84 : 1</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3205,15 +3217,15 @@
       </c>
       <c r="B53" s="2">
         <f>January!B53+February!B53+March!B53+April!B53+May!B53+June!B53+July!B53+August!B53+September!B53+October!B53+November!B53+December!B53</f>
-        <v>1261</v>
+        <v>1361</v>
       </c>
       <c r="C53" s="2">
         <f>January!C53+February!C53+March!C53+April!C53+May!C53+June!C53+July!C53+August!C53+September!C53+October!C53+November!C53+December!C53</f>
-        <v>2273</v>
+        <v>2520</v>
       </c>
       <c r="D53" s="2">
         <f>January!D53+February!D53+March!D53+April!D53+May!D53+June!D53+July!D53+August!D53+September!D53+October!D53+November!D53+December!D53</f>
-        <v>-1012</v>
+        <v>-1159</v>
       </c>
       <c r="E53" s="28" t="str">
         <f t="shared" si="1"/>
@@ -3225,7 +3237,7 @@
       </c>
       <c r="G53" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.55 : 1</v>
+        <v>0.54 : 1</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3234,15 +3246,15 @@
       </c>
       <c r="B54" s="4">
         <f>January!B54+February!B54+March!B54+April!B54+May!B54+June!B54+July!B54+August!B54+September!B54+October!B54+November!B54+December!B54</f>
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="C54" s="4">
         <f>January!C54+February!C54+March!C54+April!C54+May!C54+June!C54+July!C54+August!C54+September!C54+October!C54+November!C54+December!C54</f>
-        <v>2281</v>
+        <v>2536</v>
       </c>
       <c r="D54" s="4">
         <f>January!D54+February!D54+March!D54+April!D54+May!D54+June!D54+July!D54+August!D54+September!D54+October!D54+November!D54+December!D54</f>
-        <v>-1999</v>
+        <v>-2251</v>
       </c>
       <c r="E54" s="29" t="str">
         <f t="shared" si="1"/>
@@ -3254,7 +3266,7 @@
       </c>
       <c r="G54" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.12 : 1</v>
+        <v>0.11 : 1</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3263,15 +3275,15 @@
       </c>
       <c r="B55" s="10">
         <f>January!B55+February!B55+March!B55+April!B55+May!B55+June!B55+July!B55+August!B55+September!B55+October!B55+November!B55+December!B55</f>
-        <v>2229</v>
+        <v>2569</v>
       </c>
       <c r="C55" s="10">
         <f>January!C55+February!C55+March!C55+April!C55+May!C55+June!C55+July!C55+August!C55+September!C55+October!C55+November!C55+December!C55</f>
-        <v>1778</v>
+        <v>2018</v>
       </c>
       <c r="D55" s="10">
         <f>January!D55+February!D55+March!D55+April!D55+May!D55+June!D55+July!D55+August!D55+September!D55+October!D55+November!D55+December!D55</f>
-        <v>451</v>
+        <v>551</v>
       </c>
       <c r="E55" s="32" t="str">
         <f t="shared" si="1"/>
@@ -3283,7 +3295,7 @@
       </c>
       <c r="G55" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>1.25 : 1</v>
+        <v>1.27 : 1</v>
       </c>
     </row>
   </sheetData>
@@ -5726,108 +5738,204 @@
       <c r="A2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="28"/>
+      <c r="B2" s="18">
+        <v>1468</v>
+      </c>
+      <c r="C2" s="18">
+        <v>1211</v>
+      </c>
+      <c r="D2" s="18">
+        <v>257</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F2" s="28"/>
-      <c r="G2" s="3"/>
+      <c r="G2" s="3" t="s">
+        <v>255</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="29"/>
+      <c r="B3" s="21">
+        <v>450</v>
+      </c>
+      <c r="C3" s="21">
+        <v>431</v>
+      </c>
+      <c r="D3" s="21">
+        <v>19</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F3" s="29"/>
-      <c r="G3" s="5"/>
+      <c r="G3" s="5" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
+      <c r="B4" s="18">
+        <v>1092</v>
+      </c>
+      <c r="C4" s="18">
+        <v>1418</v>
+      </c>
+      <c r="D4" s="18">
+        <v>-326</v>
+      </c>
       <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="3"/>
+      <c r="F4" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
+      <c r="B5" s="21">
+        <v>22</v>
+      </c>
+      <c r="C5" s="21">
+        <v>155</v>
+      </c>
+      <c r="D5" s="21">
+        <v>-133</v>
+      </c>
       <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="5"/>
+      <c r="F5" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
+      <c r="B6" s="18">
+        <v>1141</v>
+      </c>
+      <c r="C6" s="18">
+        <v>1290</v>
+      </c>
+      <c r="D6" s="18">
+        <v>-149</v>
+      </c>
       <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="3"/>
+      <c r="F6" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="29"/>
+      <c r="B7" s="21">
+        <v>243</v>
+      </c>
+      <c r="C7" s="21">
+        <v>151</v>
+      </c>
+      <c r="D7" s="21">
+        <v>92</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F7" s="29"/>
-      <c r="G7" s="5"/>
+      <c r="G7" s="5" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
+      <c r="B8" s="18">
+        <v>70</v>
+      </c>
+      <c r="C8" s="18">
+        <v>179</v>
+      </c>
+      <c r="D8" s="18">
+        <v>-109</v>
+      </c>
       <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="3"/>
+      <c r="F8" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
+      <c r="B9" s="21">
+        <v>70</v>
+      </c>
+      <c r="C9" s="21">
+        <v>72</v>
+      </c>
+      <c r="D9" s="21">
+        <v>-2</v>
+      </c>
       <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="5"/>
+      <c r="F9" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
+      <c r="B10" s="18">
+        <v>2</v>
+      </c>
+      <c r="C10" s="18">
+        <v>54</v>
+      </c>
+      <c r="D10" s="18">
+        <v>-52</v>
+      </c>
       <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="3"/>
+      <c r="F10" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
+      <c r="B11" s="21">
+        <v>0</v>
+      </c>
+      <c r="C11" s="21">
+        <v>0</v>
+      </c>
+      <c r="D11" s="21">
+        <v>0</v>
+      </c>
       <c r="E11" s="29"/>
       <c r="F11" s="29"/>
       <c r="G11" s="5"/>
@@ -5836,163 +5944,309 @@
       <c r="A12" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="30"/>
+      <c r="B12" s="23">
+        <v>41</v>
+      </c>
+      <c r="C12" s="23">
+        <v>25</v>
+      </c>
+      <c r="D12" s="23">
+        <v>16</v>
+      </c>
+      <c r="E12" s="30" t="s">
+        <v>61</v>
+      </c>
       <c r="F12" s="30"/>
-      <c r="G12" s="7"/>
+      <c r="G12" s="7" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="30"/>
+      <c r="B13" s="23">
+        <v>182</v>
+      </c>
+      <c r="C13" s="23">
+        <v>83</v>
+      </c>
+      <c r="D13" s="23">
+        <v>99</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>61</v>
+      </c>
       <c r="F13" s="30"/>
-      <c r="G13" s="7"/>
+      <c r="G13" s="7" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
+      <c r="B14" s="23">
+        <v>128</v>
+      </c>
+      <c r="C14" s="23">
+        <v>262</v>
+      </c>
+      <c r="D14" s="23">
+        <v>-134</v>
+      </c>
       <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="7"/>
+      <c r="F14" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="30"/>
+      <c r="B15" s="23">
+        <v>97</v>
+      </c>
+      <c r="C15" s="23">
+        <v>90</v>
+      </c>
+      <c r="D15" s="23">
+        <v>7</v>
+      </c>
+      <c r="E15" s="30" t="s">
+        <v>61</v>
+      </c>
       <c r="F15" s="30"/>
-      <c r="G15" s="7"/>
+      <c r="G15" s="7" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
+      <c r="B16" s="18">
+        <v>19</v>
+      </c>
+      <c r="C16" s="18">
+        <v>141</v>
+      </c>
+      <c r="D16" s="18">
+        <v>-122</v>
+      </c>
       <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="3"/>
+      <c r="F16" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="29"/>
+      <c r="B17" s="21">
+        <v>593</v>
+      </c>
+      <c r="C17" s="21">
+        <v>452</v>
+      </c>
+      <c r="D17" s="21">
+        <v>141</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F17" s="29"/>
-      <c r="G17" s="5"/>
+      <c r="G17" s="5" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
+      <c r="B18" s="18">
+        <v>67</v>
+      </c>
+      <c r="C18" s="18">
+        <v>109</v>
+      </c>
+      <c r="D18" s="18">
+        <v>-42</v>
+      </c>
       <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="3"/>
+      <c r="F18" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>254</v>
+      </c>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="29"/>
+      <c r="B19" s="21">
+        <v>629</v>
+      </c>
+      <c r="C19" s="21">
+        <v>379</v>
+      </c>
+      <c r="D19" s="21">
+        <v>250</v>
+      </c>
+      <c r="E19" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F19" s="29"/>
-      <c r="G19" s="5"/>
+      <c r="G19" s="5" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
+      <c r="B20" s="18">
+        <v>4</v>
+      </c>
+      <c r="C20" s="18">
+        <v>68</v>
+      </c>
+      <c r="D20" s="18">
+        <v>-64</v>
+      </c>
       <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="3"/>
+      <c r="F20" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
+      <c r="B21" s="21">
+        <v>405</v>
+      </c>
+      <c r="C21" s="21">
+        <v>422</v>
+      </c>
+      <c r="D21" s="21">
+        <v>-17</v>
+      </c>
       <c r="E21" s="29"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="5"/>
+      <c r="F21" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
+      <c r="B22" s="18">
+        <v>31</v>
+      </c>
+      <c r="C22" s="18">
+        <v>128</v>
+      </c>
+      <c r="D22" s="18">
+        <v>-97</v>
+      </c>
       <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="3"/>
+      <c r="F22" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="29"/>
+      <c r="B23" s="21">
+        <v>766</v>
+      </c>
+      <c r="C23" s="21">
+        <v>454</v>
+      </c>
+      <c r="D23" s="21">
+        <v>312</v>
+      </c>
+      <c r="E23" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F23" s="29"/>
-      <c r="G23" s="5"/>
+      <c r="G23" s="5" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="28"/>
+      <c r="B24" s="18">
+        <v>2023</v>
+      </c>
+      <c r="C24" s="18">
+        <v>1209</v>
+      </c>
+      <c r="D24" s="18">
+        <v>814</v>
+      </c>
+      <c r="E24" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F24" s="28"/>
-      <c r="G24" s="3"/>
+      <c r="G24" s="3" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
+      <c r="B25" s="21">
+        <v>208</v>
+      </c>
+      <c r="C25" s="21">
+        <v>368</v>
+      </c>
+      <c r="D25" s="21">
+        <v>-160</v>
+      </c>
       <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="5"/>
+      <c r="F25" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="26" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
+      <c r="B26" s="18">
+        <v>0</v>
+      </c>
+      <c r="C26" s="18">
+        <v>0</v>
+      </c>
+      <c r="D26" s="18">
+        <v>0</v>
+      </c>
       <c r="E26" s="28"/>
       <c r="F26" s="28"/>
       <c r="G26" s="3"/>
@@ -6001,185 +6255,351 @@
       <c r="A27" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="29"/>
+      <c r="B27" s="21">
+        <v>278</v>
+      </c>
+      <c r="C27" s="21">
+        <v>209</v>
+      </c>
+      <c r="D27" s="21">
+        <v>69</v>
+      </c>
+      <c r="E27" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F27" s="29"/>
-      <c r="G27" s="5"/>
+      <c r="G27" s="5" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
+      <c r="B28" s="18">
+        <v>44</v>
+      </c>
+      <c r="C28" s="18">
+        <v>99</v>
+      </c>
+      <c r="D28" s="18">
+        <v>-55</v>
+      </c>
       <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="3"/>
+      <c r="F28" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="29"/>
+      <c r="B29" s="21">
+        <v>570</v>
+      </c>
+      <c r="C29" s="21">
+        <v>488</v>
+      </c>
+      <c r="D29" s="21">
+        <v>82</v>
+      </c>
+      <c r="E29" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F29" s="29"/>
-      <c r="G29" s="5"/>
+      <c r="G29" s="5" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="30" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
+      <c r="B30" s="18">
+        <v>24</v>
+      </c>
+      <c r="C30" s="18">
+        <v>32</v>
+      </c>
+      <c r="D30" s="18">
+        <v>-8</v>
+      </c>
       <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="3"/>
+      <c r="F30" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
+      <c r="B31" s="21">
+        <v>86</v>
+      </c>
+      <c r="C31" s="21">
+        <v>293</v>
+      </c>
+      <c r="D31" s="21">
+        <v>-207</v>
+      </c>
       <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="5"/>
+      <c r="F31" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="32" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
+      <c r="B32" s="18">
+        <v>419</v>
+      </c>
+      <c r="C32" s="18">
+        <v>558</v>
+      </c>
+      <c r="D32" s="18">
+        <v>-139</v>
+      </c>
       <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="3"/>
+      <c r="F32" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="33" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
+      <c r="B33" s="21">
+        <v>344</v>
+      </c>
+      <c r="C33" s="21">
+        <v>417</v>
+      </c>
+      <c r="D33" s="21">
+        <v>-73</v>
+      </c>
       <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="5"/>
+      <c r="F33" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="34" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="28"/>
+      <c r="B34" s="18">
+        <v>216</v>
+      </c>
+      <c r="C34" s="18">
+        <v>129</v>
+      </c>
+      <c r="D34" s="18">
+        <v>87</v>
+      </c>
+      <c r="E34" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F34" s="28"/>
-      <c r="G34" s="3"/>
+      <c r="G34" s="3" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
+      <c r="B35" s="21">
+        <v>853</v>
+      </c>
+      <c r="C35" s="21">
+        <v>958</v>
+      </c>
+      <c r="D35" s="21">
+        <v>-105</v>
+      </c>
       <c r="E35" s="29"/>
-      <c r="F35" s="29"/>
-      <c r="G35" s="5"/>
+      <c r="F35" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="36" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
+      <c r="B36" s="18">
+        <v>192</v>
+      </c>
+      <c r="C36" s="18">
+        <v>420</v>
+      </c>
+      <c r="D36" s="18">
+        <v>-228</v>
+      </c>
       <c r="E36" s="28"/>
-      <c r="F36" s="28"/>
-      <c r="G36" s="3"/>
+      <c r="F36" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="29"/>
+      <c r="B37" s="21">
+        <v>435</v>
+      </c>
+      <c r="C37" s="21">
+        <v>337</v>
+      </c>
+      <c r="D37" s="21">
+        <v>98</v>
+      </c>
+      <c r="E37" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F37" s="29"/>
-      <c r="G37" s="5"/>
+      <c r="G37" s="5" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
+      <c r="B38" s="18">
+        <v>19</v>
+      </c>
+      <c r="C38" s="18">
+        <v>175</v>
+      </c>
+      <c r="D38" s="18">
+        <v>-156</v>
+      </c>
       <c r="E38" s="28"/>
-      <c r="F38" s="28"/>
-      <c r="G38" s="3"/>
+      <c r="F38" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="B39" s="25"/>
-      <c r="C39" s="25"/>
-      <c r="D39" s="25"/>
+      <c r="B39" s="25">
+        <v>35</v>
+      </c>
+      <c r="C39" s="25">
+        <v>76</v>
+      </c>
+      <c r="D39" s="25">
+        <v>-41</v>
+      </c>
       <c r="E39" s="31"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="9"/>
+      <c r="F39" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="B40" s="25"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
+      <c r="B40" s="25">
+        <v>86</v>
+      </c>
+      <c r="C40" s="25">
+        <v>118</v>
+      </c>
+      <c r="D40" s="25">
+        <v>-32</v>
+      </c>
       <c r="E40" s="31"/>
-      <c r="F40" s="31"/>
-      <c r="G40" s="9"/>
+      <c r="F40" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
+      <c r="B41" s="25">
+        <v>2</v>
+      </c>
+      <c r="C41" s="25">
+        <v>43</v>
+      </c>
+      <c r="D41" s="25">
+        <v>-41</v>
+      </c>
       <c r="E41" s="31"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="9"/>
+      <c r="F41" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="42" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="B42" s="25"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="25"/>
+      <c r="B42" s="25">
+        <v>15</v>
+      </c>
+      <c r="C42" s="25">
+        <v>21</v>
+      </c>
+      <c r="D42" s="25">
+        <v>-6</v>
+      </c>
       <c r="E42" s="31"/>
-      <c r="F42" s="31"/>
-      <c r="G42" s="9"/>
+      <c r="F42" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="B43" s="25"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
+      <c r="B43" s="25">
+        <v>0</v>
+      </c>
+      <c r="C43" s="25">
+        <v>0</v>
+      </c>
+      <c r="D43" s="25">
+        <v>0</v>
+      </c>
       <c r="E43" s="31"/>
       <c r="F43" s="31"/>
       <c r="G43" s="9"/>
@@ -6188,133 +6608,253 @@
       <c r="A44" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="B44" s="21"/>
-      <c r="C44" s="21"/>
-      <c r="D44" s="21"/>
+      <c r="B44" s="21">
+        <v>74</v>
+      </c>
+      <c r="C44" s="21">
+        <v>89</v>
+      </c>
+      <c r="D44" s="21">
+        <v>-15</v>
+      </c>
       <c r="E44" s="29"/>
-      <c r="F44" s="29"/>
-      <c r="G44" s="5"/>
+      <c r="F44" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="45" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
+      <c r="B45" s="18">
+        <v>77</v>
+      </c>
+      <c r="C45" s="18">
+        <v>173</v>
+      </c>
+      <c r="D45" s="18">
+        <v>-96</v>
+      </c>
       <c r="E45" s="28"/>
-      <c r="F45" s="28"/>
-      <c r="G45" s="3"/>
+      <c r="F45" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="46" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="B46" s="21"/>
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
+      <c r="B46" s="21">
+        <v>507</v>
+      </c>
+      <c r="C46" s="21">
+        <v>524</v>
+      </c>
+      <c r="D46" s="21">
+        <v>-17</v>
+      </c>
       <c r="E46" s="29"/>
-      <c r="F46" s="29"/>
-      <c r="G46" s="5"/>
+      <c r="F46" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="47" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="28"/>
+      <c r="B47" s="18">
+        <v>930</v>
+      </c>
+      <c r="C47" s="18">
+        <v>724</v>
+      </c>
+      <c r="D47" s="18">
+        <v>206</v>
+      </c>
+      <c r="E47" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F47" s="28"/>
-      <c r="G47" s="3"/>
+      <c r="G47" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="B48" s="21"/>
-      <c r="C48" s="21"/>
-      <c r="D48" s="21"/>
+      <c r="B48" s="21">
+        <v>229</v>
+      </c>
+      <c r="C48" s="21">
+        <v>572</v>
+      </c>
+      <c r="D48" s="21">
+        <v>-343</v>
+      </c>
       <c r="E48" s="29"/>
-      <c r="F48" s="29"/>
-      <c r="G48" s="5"/>
+      <c r="F48" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B49" s="18"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="18"/>
-      <c r="E49" s="28"/>
+      <c r="B49" s="18">
+        <v>457</v>
+      </c>
+      <c r="C49" s="18">
+        <v>236</v>
+      </c>
+      <c r="D49" s="18">
+        <v>221</v>
+      </c>
+      <c r="E49" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F49" s="28"/>
-      <c r="G49" s="3"/>
+      <c r="G49" s="3" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="B50" s="21"/>
-      <c r="C50" s="21"/>
-      <c r="D50" s="21"/>
-      <c r="E50" s="29"/>
+      <c r="B50" s="21">
+        <v>1043</v>
+      </c>
+      <c r="C50" s="21">
+        <v>505</v>
+      </c>
+      <c r="D50" s="21">
+        <v>538</v>
+      </c>
+      <c r="E50" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F50" s="29"/>
-      <c r="G50" s="5"/>
+      <c r="G50" s="5" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B51" s="18"/>
-      <c r="C51" s="18"/>
-      <c r="D51" s="18"/>
+      <c r="B51" s="18">
+        <v>163</v>
+      </c>
+      <c r="C51" s="18">
+        <v>186</v>
+      </c>
+      <c r="D51" s="18">
+        <v>-23</v>
+      </c>
       <c r="E51" s="28"/>
-      <c r="F51" s="28"/>
-      <c r="G51" s="3"/>
+      <c r="F51" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="52" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="B52" s="21"/>
-      <c r="C52" s="21"/>
-      <c r="D52" s="21"/>
+      <c r="B52" s="21">
+        <v>458</v>
+      </c>
+      <c r="C52" s="21">
+        <v>475</v>
+      </c>
+      <c r="D52" s="21">
+        <v>-17</v>
+      </c>
       <c r="E52" s="29"/>
-      <c r="F52" s="29"/>
-      <c r="G52" s="5"/>
+      <c r="F52" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="53" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B53" s="18"/>
-      <c r="C53" s="18"/>
-      <c r="D53" s="18"/>
+      <c r="B53" s="18">
+        <v>100</v>
+      </c>
+      <c r="C53" s="18">
+        <v>247</v>
+      </c>
+      <c r="D53" s="18">
+        <v>-147</v>
+      </c>
       <c r="E53" s="28"/>
-      <c r="F53" s="28"/>
-      <c r="G53" s="3"/>
+      <c r="F53" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="54" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="B54" s="21"/>
-      <c r="C54" s="21"/>
-      <c r="D54" s="21"/>
+      <c r="B54" s="21">
+        <v>3</v>
+      </c>
+      <c r="C54" s="21">
+        <v>255</v>
+      </c>
+      <c r="D54" s="21">
+        <v>-252</v>
+      </c>
       <c r="E54" s="29"/>
-      <c r="F54" s="29"/>
-      <c r="G54" s="5"/>
+      <c r="F54" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="55" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="B55" s="27"/>
-      <c r="C55" s="27"/>
-      <c r="D55" s="27"/>
-      <c r="E55" s="32"/>
+      <c r="B55" s="27">
+        <v>340</v>
+      </c>
+      <c r="C55" s="27">
+        <v>240</v>
+      </c>
+      <c r="D55" s="27">
+        <v>100</v>
+      </c>
+      <c r="E55" s="32" t="s">
+        <v>61</v>
+      </c>
       <c r="F55" s="32"/>
-      <c r="G55" s="11"/>
+      <c r="G55" s="11" t="s">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G55" xr:uid="{00000000-0009-0000-0000-00000B000000}"/>

</xml_diff>